<commit_message>
lol it wasnt right, good now
</commit_message>
<xml_diff>
--- a/Clash.xlsx
+++ b/Clash.xlsx
@@ -179,7 +179,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="22">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -273,11 +273,13 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6"/>
   </cellStyleXfs>
-  <cellXfs count="265">
+  <cellXfs count="292">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -629,6 +631,37 @@
     <xf numFmtId="164" fontId="5" fillId="20" borderId="21" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="5" fillId="24" borderId="21" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="5" fillId="23" borderId="21" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="5" fillId="18" borderId="22" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="5" fillId="19" borderId="22" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="5" fillId="21" borderId="22" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="6" fillId="18" borderId="22" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="6" fillId="19" borderId="22" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="6" fillId="21" borderId="22" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="6" fillId="22" borderId="22" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="5" fillId="22" borderId="22" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="5" fillId="25" borderId="22" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="5" fillId="24" borderId="22" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="5" fillId="20" borderId="22" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="6" fillId="18" borderId="23" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="18" borderId="23" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="19" borderId="23" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="6" fillId="24" borderId="23" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="6" fillId="21" borderId="23" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="21" borderId="23" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="22" borderId="23" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="6" fillId="25" borderId="23" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="5" fillId="21" borderId="23" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="5" fillId="22" borderId="23" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="5" fillId="25" borderId="23" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="5" fillId="18" borderId="23" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="5" fillId="19" borderId="23" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="5" fillId="20" borderId="23" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="5" fillId="24" borderId="23" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="5" fillId="23" borderId="23" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1149,15 +1182,15 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="249" t="inlineStr">
+      <c r="A4" s="276" t="inlineStr">
         <is>
           <t>#YRGRRJQCY</t>
         </is>
       </c>
-      <c r="B4" s="249" t="n">
+      <c r="B4" s="276" t="n">
         <v>1341</v>
       </c>
-      <c r="C4" s="250" t="n">
+      <c r="C4" s="277" t="n">
         <v>1</v>
       </c>
       <c r="D4" s="116" t="inlineStr">
@@ -1165,31 +1198,31 @@
           <t>DoubleSpice</t>
         </is>
       </c>
-      <c r="E4" s="251" t="n">
+      <c r="E4" s="278" t="n">
         <v>6</v>
       </c>
       <c r="F4" s="116" t="n">
         <v>14095</v>
       </c>
-      <c r="G4" s="252" t="n">
+      <c r="G4" s="279" t="n">
         <v>0</v>
       </c>
       <c r="H4" s="119" t="n">
         <v>60</v>
       </c>
-      <c r="I4" s="251" t="n">
+      <c r="I4" s="278" t="n">
         <v>6</v>
       </c>
       <c r="J4" s="116" t="n">
         <v>12379</v>
       </c>
-      <c r="K4" s="251" t="n">
+      <c r="K4" s="278" t="n">
         <v>6</v>
       </c>
       <c r="L4" s="116" t="n">
         <v>8256</v>
       </c>
-      <c r="M4" s="251" t="n">
+      <c r="M4" s="278" t="n">
         <v>6</v>
       </c>
       <c r="N4" s="116" t="n">
@@ -1197,15 +1230,15 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="253" t="inlineStr">
+      <c r="A5" s="280" t="inlineStr">
         <is>
           <t>#90U0VPU9U</t>
         </is>
       </c>
-      <c r="B5" s="253" t="n">
+      <c r="B5" s="280" t="n">
         <v>2542</v>
       </c>
-      <c r="C5" s="254" t="n">
+      <c r="C5" s="281" t="n">
         <v>2</v>
       </c>
       <c r="D5" s="122" t="inlineStr">
@@ -1213,31 +1246,31 @@
           <t>KYANI7E</t>
         </is>
       </c>
-      <c r="E5" s="255" t="n">
+      <c r="E5" s="282" t="n">
         <v>6</v>
       </c>
       <c r="F5" s="122" t="n">
         <v>12144</v>
       </c>
-      <c r="G5" s="256" t="n">
+      <c r="G5" s="283" t="n">
         <v>46</v>
       </c>
       <c r="H5" s="125" t="n">
         <v>4</v>
       </c>
-      <c r="I5" s="255" t="n">
+      <c r="I5" s="282" t="n">
         <v>6</v>
       </c>
       <c r="J5" s="122" t="n">
         <v>12835</v>
       </c>
-      <c r="K5" s="255" t="n">
+      <c r="K5" s="282" t="n">
         <v>6</v>
       </c>
       <c r="L5" s="122" t="n">
         <v>7696</v>
       </c>
-      <c r="M5" s="255" t="n">
+      <c r="M5" s="282" t="n">
         <v>6</v>
       </c>
       <c r="N5" s="122" t="n">
@@ -1245,15 +1278,15 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="249" t="inlineStr">
+      <c r="A6" s="276" t="inlineStr">
         <is>
           <t>#YJ20CRJYQ</t>
         </is>
       </c>
-      <c r="B6" s="249" t="n">
+      <c r="B6" s="276" t="n">
         <v>1392</v>
       </c>
-      <c r="C6" s="250" t="n">
+      <c r="C6" s="277" t="n">
         <v>3</v>
       </c>
       <c r="D6" s="116" t="inlineStr">
@@ -1261,31 +1294,31 @@
           <t>UnluckGod</t>
         </is>
       </c>
-      <c r="E6" s="251" t="n">
+      <c r="E6" s="278" t="n">
         <v>6</v>
       </c>
       <c r="F6" s="116" t="n">
         <v>11999</v>
       </c>
-      <c r="G6" s="252" t="n">
+      <c r="G6" s="279" t="n">
         <v>0</v>
       </c>
       <c r="H6" s="119" t="n">
         <v>61</v>
       </c>
-      <c r="I6" s="251" t="n">
+      <c r="I6" s="278" t="n">
         <v>6</v>
       </c>
       <c r="J6" s="116" t="n">
         <v>12972</v>
       </c>
-      <c r="K6" s="251" t="n">
+      <c r="K6" s="278" t="n">
         <v>6</v>
       </c>
       <c r="L6" s="116" t="n">
         <v>8286</v>
       </c>
-      <c r="M6" s="251" t="n">
+      <c r="M6" s="278" t="n">
         <v>6</v>
       </c>
       <c r="N6" s="116" t="n">
@@ -1293,15 +1326,15 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="253" t="inlineStr">
+      <c r="A7" s="280" t="inlineStr">
         <is>
           <t>#QUV2GP88U</t>
         </is>
       </c>
-      <c r="B7" s="253" t="n">
+      <c r="B7" s="280" t="n">
         <v>723</v>
       </c>
-      <c r="C7" s="254" t="n">
+      <c r="C7" s="281" t="n">
         <v>4</v>
       </c>
       <c r="D7" s="122" t="inlineStr">
@@ -1309,31 +1342,31 @@
           <t>Nico Robin</t>
         </is>
       </c>
-      <c r="E7" s="255" t="n">
+      <c r="E7" s="282" t="n">
         <v>6</v>
       </c>
       <c r="F7" s="122" t="n">
         <v>11338</v>
       </c>
-      <c r="G7" s="256" t="n">
+      <c r="G7" s="283" t="n">
         <v>0</v>
       </c>
       <c r="H7" s="125" t="n">
         <v>0</v>
       </c>
-      <c r="I7" s="255" t="n">
+      <c r="I7" s="282" t="n">
         <v>6</v>
       </c>
       <c r="J7" s="122" t="n">
         <v>10997</v>
       </c>
-      <c r="K7" s="255" t="n">
+      <c r="K7" s="282" t="n">
         <v>6</v>
       </c>
       <c r="L7" s="122" t="n">
         <v>11087</v>
       </c>
-      <c r="M7" s="255" t="n">
+      <c r="M7" s="282" t="n">
         <v>6</v>
       </c>
       <c r="N7" s="122" t="n">
@@ -1341,15 +1374,15 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="249" t="inlineStr">
+      <c r="A8" s="276" t="inlineStr">
         <is>
           <t>#QLJ2U20Y2</t>
         </is>
       </c>
-      <c r="B8" s="249" t="n">
+      <c r="B8" s="276" t="n">
         <v>1458</v>
       </c>
-      <c r="C8" s="250" t="n">
+      <c r="C8" s="277" t="n">
         <v>5</v>
       </c>
       <c r="D8" s="116" t="inlineStr">
@@ -1357,31 +1390,31 @@
           <t>DeadLeaf</t>
         </is>
       </c>
-      <c r="E8" s="251" t="n">
+      <c r="E8" s="278" t="n">
         <v>6</v>
       </c>
       <c r="F8" s="116" t="n">
         <v>11140</v>
       </c>
-      <c r="G8" s="252" t="n">
+      <c r="G8" s="279" t="n">
         <v>0</v>
       </c>
       <c r="H8" s="119" t="n">
         <v>30</v>
       </c>
-      <c r="I8" s="251" t="n">
+      <c r="I8" s="278" t="n">
         <v>6</v>
       </c>
       <c r="J8" s="116" t="n">
         <v>15509</v>
       </c>
-      <c r="K8" s="251" t="n">
+      <c r="K8" s="278" t="n">
         <v>6</v>
       </c>
       <c r="L8" s="116" t="n">
         <v>8567</v>
       </c>
-      <c r="M8" s="251" t="n">
+      <c r="M8" s="278" t="n">
         <v>6</v>
       </c>
       <c r="N8" s="116" t="n">
@@ -1389,15 +1422,15 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="253" t="inlineStr">
+      <c r="A9" s="280" t="inlineStr">
         <is>
           <t>#Q8CLCUCC2</t>
         </is>
       </c>
-      <c r="B9" s="253" t="n">
+      <c r="B9" s="280" t="n">
         <v>1327</v>
       </c>
-      <c r="C9" s="254" t="n">
+      <c r="C9" s="281" t="n">
         <v>6</v>
       </c>
       <c r="D9" s="122" t="inlineStr">
@@ -1405,31 +1438,31 @@
           <t>Moxxi</t>
         </is>
       </c>
-      <c r="E9" s="255" t="n">
+      <c r="E9" s="282" t="n">
         <v>6</v>
       </c>
       <c r="F9" s="122" t="n">
         <v>11010</v>
       </c>
-      <c r="G9" s="256" t="n">
+      <c r="G9" s="283" t="n">
         <v>0</v>
       </c>
       <c r="H9" s="125" t="n">
         <v>60</v>
       </c>
-      <c r="I9" s="255" t="n">
+      <c r="I9" s="282" t="n">
         <v>6</v>
       </c>
       <c r="J9" s="122" t="n">
         <v>13857</v>
       </c>
-      <c r="K9" s="255" t="n">
+      <c r="K9" s="282" t="n">
         <v>6</v>
       </c>
       <c r="L9" s="122" t="n">
         <v>7905</v>
       </c>
-      <c r="M9" s="255" t="n">
+      <c r="M9" s="282" t="n">
         <v>6</v>
       </c>
       <c r="N9" s="122" t="n">
@@ -1437,15 +1470,15 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="249" t="inlineStr">
+      <c r="A10" s="276" t="inlineStr">
         <is>
           <t>#QCV22VP0G</t>
         </is>
       </c>
-      <c r="B10" s="249" t="n">
+      <c r="B10" s="276" t="n">
         <v>730</v>
       </c>
-      <c r="C10" s="250" t="n">
+      <c r="C10" s="277" t="n">
         <v>7</v>
       </c>
       <c r="D10" s="116" t="inlineStr">
@@ -1453,31 +1486,31 @@
           <t>Nami</t>
         </is>
       </c>
-      <c r="E10" s="251" t="n">
+      <c r="E10" s="278" t="n">
         <v>6</v>
       </c>
       <c r="F10" s="116" t="n">
         <v>10769</v>
       </c>
-      <c r="G10" s="252" t="n">
+      <c r="G10" s="279" t="n">
         <v>0</v>
       </c>
       <c r="H10" s="119" t="n">
         <v>0</v>
       </c>
-      <c r="I10" s="251" t="n">
+      <c r="I10" s="278" t="n">
         <v>6</v>
       </c>
       <c r="J10" s="116" t="n">
         <v>12486</v>
       </c>
-      <c r="K10" s="251" t="n">
+      <c r="K10" s="278" t="n">
         <v>6</v>
       </c>
       <c r="L10" s="116" t="n">
         <v>8472</v>
       </c>
-      <c r="M10" s="251" t="n">
+      <c r="M10" s="278" t="n">
         <v>6</v>
       </c>
       <c r="N10" s="116" t="n">
@@ -1485,15 +1518,15 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="253" t="inlineStr">
+      <c r="A11" s="280" t="inlineStr">
         <is>
           <t>#QUG8QQJ92</t>
         </is>
       </c>
-      <c r="B11" s="253" t="n">
+      <c r="B11" s="280" t="n">
         <v>957</v>
       </c>
-      <c r="C11" s="254" t="n">
+      <c r="C11" s="281" t="n">
         <v>8</v>
       </c>
       <c r="D11" s="122" t="inlineStr">
@@ -1501,31 +1534,31 @@
           <t>Karma</t>
         </is>
       </c>
-      <c r="E11" s="255" t="n">
+      <c r="E11" s="282" t="n">
         <v>6</v>
       </c>
       <c r="F11" s="122" t="n">
         <v>10003</v>
       </c>
-      <c r="G11" s="256" t="n">
+      <c r="G11" s="283" t="n">
         <v>0</v>
       </c>
       <c r="H11" s="125" t="n">
         <v>0</v>
       </c>
-      <c r="I11" s="255" t="n">
+      <c r="I11" s="282" t="n">
         <v>6</v>
       </c>
       <c r="J11" s="122" t="n">
         <v>10595</v>
       </c>
-      <c r="K11" s="255" t="n">
+      <c r="K11" s="282" t="n">
         <v>6</v>
       </c>
       <c r="L11" s="122" t="n">
         <v>9240</v>
       </c>
-      <c r="M11" s="255" t="n">
+      <c r="M11" s="282" t="n">
         <v>6</v>
       </c>
       <c r="N11" s="122" t="n">
@@ -1533,15 +1566,15 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="249" t="inlineStr">
+      <c r="A12" s="276" t="inlineStr">
         <is>
           <t>#QLR088LC9</t>
         </is>
       </c>
-      <c r="B12" s="249" t="n">
+      <c r="B12" s="276" t="n">
         <v>731</v>
       </c>
-      <c r="C12" s="250" t="n">
+      <c r="C12" s="277" t="n">
         <v>9</v>
       </c>
       <c r="D12" s="116" t="inlineStr">
@@ -1549,31 +1582,31 @@
           <t>Sanji</t>
         </is>
       </c>
-      <c r="E12" s="251" t="n">
+      <c r="E12" s="278" t="n">
         <v>6</v>
       </c>
       <c r="F12" s="116" t="n">
         <v>9550</v>
       </c>
-      <c r="G12" s="252" t="n">
+      <c r="G12" s="279" t="n">
         <v>0</v>
       </c>
       <c r="H12" s="119" t="n">
         <v>0</v>
       </c>
-      <c r="I12" s="251" t="n">
+      <c r="I12" s="278" t="n">
         <v>6</v>
       </c>
       <c r="J12" s="116" t="n">
         <v>9138</v>
       </c>
-      <c r="K12" s="251" t="n">
+      <c r="K12" s="278" t="n">
         <v>6</v>
       </c>
       <c r="L12" s="116" t="n">
         <v>8897</v>
       </c>
-      <c r="M12" s="251" t="n">
+      <c r="M12" s="278" t="n">
         <v>6</v>
       </c>
       <c r="N12" s="116" t="n">
@@ -1581,15 +1614,15 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="257" t="inlineStr">
+      <c r="A13" s="284" t="inlineStr">
         <is>
           <t>#G0JPUQGYR</t>
         </is>
       </c>
-      <c r="B13" s="257" t="n">
+      <c r="B13" s="284" t="n">
         <v>1297</v>
       </c>
-      <c r="C13" s="254" t="n">
+      <c r="C13" s="281" t="n">
         <v>10</v>
       </c>
       <c r="D13" s="127" t="inlineStr">
@@ -1597,31 +1630,31 @@
           <t>Collin</t>
         </is>
       </c>
-      <c r="E13" s="258" t="n">
+      <c r="E13" s="285" t="n">
         <v>6</v>
       </c>
       <c r="F13" s="127" t="n">
         <v>9238</v>
       </c>
-      <c r="G13" s="259" t="n">
+      <c r="G13" s="286" t="n">
         <v>20</v>
       </c>
       <c r="H13" s="130" t="n">
         <v>0</v>
       </c>
-      <c r="I13" s="258" t="n">
+      <c r="I13" s="285" t="n">
         <v>6</v>
       </c>
       <c r="J13" s="127" t="n">
         <v>7756</v>
       </c>
-      <c r="K13" s="258" t="n">
+      <c r="K13" s="285" t="n">
         <v>6</v>
       </c>
       <c r="L13" s="131" t="n">
         <v>5943</v>
       </c>
-      <c r="M13" s="258" t="n">
+      <c r="M13" s="285" t="n">
         <v>6</v>
       </c>
       <c r="N13" s="127" t="n">
@@ -1629,15 +1662,15 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="249" t="inlineStr">
+      <c r="A14" s="276" t="inlineStr">
         <is>
           <t>#QUYG0PQC8</t>
         </is>
       </c>
-      <c r="B14" s="249" t="n">
+      <c r="B14" s="276" t="n">
         <v>919</v>
       </c>
-      <c r="C14" s="250" t="n">
+      <c r="C14" s="277" t="n">
         <v>11</v>
       </c>
       <c r="D14" s="116" t="inlineStr">
@@ -1645,31 +1678,31 @@
           <t>Luffy</t>
         </is>
       </c>
-      <c r="E14" s="251" t="n">
+      <c r="E14" s="278" t="n">
         <v>6</v>
       </c>
       <c r="F14" s="116" t="n">
         <v>9114</v>
       </c>
-      <c r="G14" s="252" t="n">
+      <c r="G14" s="279" t="n">
         <v>0</v>
       </c>
       <c r="H14" s="119" t="n">
         <v>0</v>
       </c>
-      <c r="I14" s="251" t="n">
+      <c r="I14" s="278" t="n">
         <v>6</v>
       </c>
       <c r="J14" s="116" t="n">
         <v>13385</v>
       </c>
-      <c r="K14" s="251" t="n">
+      <c r="K14" s="278" t="n">
         <v>6</v>
       </c>
       <c r="L14" s="116" t="n">
         <v>7877</v>
       </c>
-      <c r="M14" s="251" t="n">
+      <c r="M14" s="278" t="n">
         <v>6</v>
       </c>
       <c r="N14" s="116" t="n">
@@ -1677,15 +1710,15 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="253" t="inlineStr">
+      <c r="A15" s="280" t="inlineStr">
         <is>
           <t>#G0QPVJY9L</t>
         </is>
       </c>
-      <c r="B15" s="253" t="n">
+      <c r="B15" s="280" t="n">
         <v>759</v>
       </c>
-      <c r="C15" s="254" t="n">
+      <c r="C15" s="281" t="n">
         <v>12</v>
       </c>
       <c r="D15" s="122" t="inlineStr">
@@ -1693,31 +1726,31 @@
           <t>Zoro</t>
         </is>
       </c>
-      <c r="E15" s="255" t="n">
+      <c r="E15" s="282" t="n">
         <v>6</v>
       </c>
       <c r="F15" s="122" t="n">
         <v>8855</v>
       </c>
-      <c r="G15" s="256" t="n">
+      <c r="G15" s="283" t="n">
         <v>0</v>
       </c>
       <c r="H15" s="125" t="n">
         <v>0</v>
       </c>
-      <c r="I15" s="255" t="n">
+      <c r="I15" s="282" t="n">
         <v>6</v>
       </c>
       <c r="J15" s="122" t="n">
         <v>10965</v>
       </c>
-      <c r="K15" s="255" t="n">
+      <c r="K15" s="282" t="n">
         <v>6</v>
       </c>
       <c r="L15" s="122" t="n">
         <v>7905</v>
       </c>
-      <c r="M15" s="255" t="n">
+      <c r="M15" s="282" t="n">
         <v>6</v>
       </c>
       <c r="N15" s="122" t="n">
@@ -1725,15 +1758,15 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="260" t="inlineStr">
+      <c r="A16" s="287" t="inlineStr">
         <is>
           <t>#98JG2UJQL</t>
         </is>
       </c>
-      <c r="B16" s="260" t="n">
+      <c r="B16" s="287" t="n">
         <v>2961</v>
       </c>
-      <c r="C16" s="250" t="n">
+      <c r="C16" s="277" t="n">
         <v>13</v>
       </c>
       <c r="D16" s="133" t="inlineStr">
@@ -1741,31 +1774,31 @@
           <t>Dragonux</t>
         </is>
       </c>
-      <c r="E16" s="261" t="n">
+      <c r="E16" s="288" t="n">
         <v>6</v>
       </c>
       <c r="F16" s="133" t="n">
         <v>8750</v>
       </c>
-      <c r="G16" s="262" t="n">
+      <c r="G16" s="289" t="n">
         <v>211</v>
       </c>
       <c r="H16" s="136" t="n">
         <v>0</v>
       </c>
-      <c r="I16" s="261" t="n">
+      <c r="I16" s="288" t="n">
         <v>6</v>
       </c>
       <c r="J16" s="133" t="n">
         <v>10865</v>
       </c>
-      <c r="K16" s="261" t="n">
+      <c r="K16" s="288" t="n">
         <v>6</v>
       </c>
       <c r="L16" s="133" t="n">
         <v>8025</v>
       </c>
-      <c r="M16" s="261" t="n">
+      <c r="M16" s="288" t="n">
         <v>6</v>
       </c>
       <c r="N16" s="133" t="n">
@@ -1773,15 +1806,15 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="257" t="inlineStr">
+      <c r="A17" s="284" t="inlineStr">
         <is>
           <t>#82QLQCJRJ</t>
         </is>
       </c>
-      <c r="B17" s="257" t="n">
+      <c r="B17" s="284" t="n">
         <v>2914</v>
       </c>
-      <c r="C17" s="254" t="n">
+      <c r="C17" s="281" t="n">
         <v>14</v>
       </c>
       <c r="D17" s="127" t="inlineStr">
@@ -1789,31 +1822,31 @@
           <t>Raging Fury</t>
         </is>
       </c>
-      <c r="E17" s="258" t="n">
+      <c r="E17" s="285" t="n">
         <v>6</v>
       </c>
       <c r="F17" s="127" t="n">
         <v>7115</v>
       </c>
-      <c r="G17" s="259" t="n">
+      <c r="G17" s="286" t="n">
         <v>0</v>
       </c>
       <c r="H17" s="130" t="n">
         <v>0</v>
       </c>
-      <c r="I17" s="259" t="n">
+      <c r="I17" s="286" t="n">
         <v>2</v>
       </c>
       <c r="J17" s="137" t="n">
         <v>2320</v>
       </c>
-      <c r="K17" s="258" t="n">
+      <c r="K17" s="285" t="n">
         <v>6</v>
       </c>
       <c r="L17" s="131" t="n">
         <v>4920</v>
       </c>
-      <c r="M17" s="258" t="n">
+      <c r="M17" s="285" t="n">
         <v>6</v>
       </c>
       <c r="N17" s="131" t="n">
@@ -1821,15 +1854,15 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="260" t="inlineStr">
+      <c r="A18" s="287" t="inlineStr">
         <is>
           <t>#QRPRYR8LL</t>
         </is>
       </c>
-      <c r="B18" s="260" t="n">
+      <c r="B18" s="287" t="n">
         <v>1027</v>
       </c>
-      <c r="C18" s="250" t="n">
+      <c r="C18" s="277" t="n">
         <v>15</v>
       </c>
       <c r="D18" s="133" t="inlineStr">
@@ -1837,31 +1870,31 @@
           <t>FidelCashflow</t>
         </is>
       </c>
-      <c r="E18" s="261" t="n">
+      <c r="E18" s="288" t="n">
         <v>6</v>
       </c>
       <c r="F18" s="133" t="n">
         <v>6547</v>
       </c>
-      <c r="G18" s="263" t="n">
+      <c r="G18" s="290" t="n">
         <v>4</v>
       </c>
       <c r="H18" s="136" t="n">
         <v>0</v>
       </c>
-      <c r="I18" s="261" t="n">
+      <c r="I18" s="288" t="n">
         <v>6</v>
       </c>
       <c r="J18" s="133" t="n">
         <v>6811</v>
       </c>
-      <c r="K18" s="261" t="n">
+      <c r="K18" s="288" t="n">
         <v>6</v>
       </c>
       <c r="L18" s="139" t="n">
         <v>4239</v>
       </c>
-      <c r="M18" s="261" t="n">
+      <c r="M18" s="288" t="n">
         <v>6</v>
       </c>
       <c r="N18" s="139" t="n">
@@ -1869,15 +1902,15 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="257" t="inlineStr">
+      <c r="A19" s="284" t="inlineStr">
         <is>
           <t>#QLG0VJG2J</t>
         </is>
       </c>
-      <c r="B19" s="257" t="n">
+      <c r="B19" s="284" t="n">
         <v>1050</v>
       </c>
-      <c r="C19" s="254" t="n">
+      <c r="C19" s="281" t="n">
         <v>16</v>
       </c>
       <c r="D19" s="131" t="inlineStr">
@@ -1885,35 +1918,35 @@
           <t>PocketRocket</t>
         </is>
       </c>
-      <c r="E19" s="264" t="n">
+      <c r="E19" s="291" t="n">
         <v>4</v>
       </c>
       <c r="F19" s="131" t="n">
         <v>5215</v>
       </c>
-      <c r="G19" s="259" t="n">
+      <c r="G19" s="286" t="n">
         <v>20</v>
       </c>
       <c r="H19" s="130" t="n">
         <v>0</v>
       </c>
-      <c r="I19" s="257" t="n"/>
+      <c r="I19" s="284" t="n"/>
       <c r="J19" s="130" t="n"/>
-      <c r="K19" s="257" t="n"/>
+      <c r="K19" s="284" t="n"/>
       <c r="L19" s="130" t="n"/>
-      <c r="M19" s="257" t="n"/>
+      <c r="M19" s="284" t="n"/>
       <c r="N19" s="130" t="n"/>
     </row>
     <row r="20">
-      <c r="A20" s="260" t="inlineStr">
+      <c r="A20" s="287" t="inlineStr">
         <is>
           <t>#QU0U2Q99G</t>
         </is>
       </c>
-      <c r="B20" s="260" t="n">
+      <c r="B20" s="287" t="n">
         <v>895</v>
       </c>
-      <c r="C20" s="250" t="n">
+      <c r="C20" s="277" t="n">
         <v>17</v>
       </c>
       <c r="D20" s="133" t="inlineStr">
@@ -1921,39 +1954,39 @@
           <t>big coc</t>
         </is>
       </c>
-      <c r="E20" s="261" t="n">
+      <c r="E20" s="288" t="n">
         <v>5</v>
       </c>
       <c r="F20" s="139" t="n">
         <v>5150</v>
       </c>
-      <c r="G20" s="263" t="n">
+      <c r="G20" s="290" t="n">
         <v>0</v>
       </c>
       <c r="H20" s="136" t="n">
         <v>40</v>
       </c>
-      <c r="I20" s="261" t="n">
+      <c r="I20" s="288" t="n">
         <v>6</v>
       </c>
       <c r="J20" s="133" t="n">
         <v>9075</v>
       </c>
-      <c r="K20" s="260" t="n"/>
+      <c r="K20" s="287" t="n"/>
       <c r="L20" s="136" t="n"/>
-      <c r="M20" s="260" t="n"/>
+      <c r="M20" s="287" t="n"/>
       <c r="N20" s="136" t="n"/>
     </row>
     <row r="21">
-      <c r="A21" s="259" t="inlineStr">
+      <c r="A21" s="286" t="inlineStr">
         <is>
           <t>#Q8YP9P8UJ</t>
         </is>
       </c>
-      <c r="B21" s="257" t="n">
+      <c r="B21" s="284" t="n">
         <v>945</v>
       </c>
-      <c r="C21" s="254" t="n">
+      <c r="C21" s="281" t="n">
         <v>18</v>
       </c>
       <c r="D21" s="127" t="inlineStr">
@@ -1961,19 +1994,19 @@
           <t>Ranger</t>
         </is>
       </c>
-      <c r="E21" s="258" t="n">
+      <c r="E21" s="285" t="n">
         <v>5</v>
       </c>
       <c r="F21" s="131" t="n">
         <v>4680</v>
       </c>
-      <c r="G21" s="257" t="n"/>
+      <c r="G21" s="284" t="n"/>
       <c r="H21" s="130" t="n"/>
-      <c r="I21" s="257" t="n"/>
+      <c r="I21" s="284" t="n"/>
       <c r="J21" s="130" t="n"/>
-      <c r="K21" s="257" t="n"/>
+      <c r="K21" s="284" t="n"/>
       <c r="L21" s="130" t="n"/>
-      <c r="M21" s="257" t="n"/>
+      <c r="M21" s="284" t="n"/>
       <c r="N21" s="130" t="n"/>
     </row>
     <row r="22">
@@ -2025,15 +2058,15 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="257" t="inlineStr">
+      <c r="A23" s="284" t="inlineStr">
         <is>
           <t>#QJC8LQU9U</t>
         </is>
       </c>
-      <c r="B23" s="257" t="n">
+      <c r="B23" s="284" t="n">
         <v>1032</v>
       </c>
-      <c r="C23" s="254" t="n">
+      <c r="C23" s="281" t="n">
         <v>20</v>
       </c>
       <c r="D23" s="137" t="inlineStr">
@@ -2041,31 +2074,31 @@
           <t>Master01</t>
         </is>
       </c>
-      <c r="E23" s="259" t="n">
+      <c r="E23" s="286" t="n">
         <v>0</v>
       </c>
       <c r="F23" s="137" t="n">
         <v>0</v>
       </c>
-      <c r="G23" s="259" t="n">
+      <c r="G23" s="286" t="n">
         <v>0</v>
       </c>
       <c r="H23" s="130" t="n">
         <v>0</v>
       </c>
-      <c r="I23" s="258" t="n">
+      <c r="I23" s="285" t="n">
         <v>6</v>
       </c>
       <c r="J23" s="131" t="n">
         <v>5415</v>
       </c>
-      <c r="K23" s="258" t="n">
+      <c r="K23" s="285" t="n">
         <v>6</v>
       </c>
       <c r="L23" s="131" t="n">
         <v>4835</v>
       </c>
-      <c r="M23" s="258" t="n">
+      <c r="M23" s="285" t="n">
         <v>5</v>
       </c>
       <c r="N23" s="131" t="n">
@@ -2073,15 +2106,15 @@
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="260" t="inlineStr">
+      <c r="A24" s="287" t="inlineStr">
         <is>
           <t>#QV8JJ0URU</t>
         </is>
       </c>
-      <c r="B24" s="260" t="n">
+      <c r="B24" s="287" t="n">
         <v>756</v>
       </c>
-      <c r="C24" s="250" t="n">
+      <c r="C24" s="277" t="n">
         <v>21</v>
       </c>
       <c r="D24" s="148" t="inlineStr">
@@ -2089,31 +2122,31 @@
           <t>✨Jacob</t>
         </is>
       </c>
-      <c r="E24" s="263" t="n">
+      <c r="E24" s="290" t="n">
         <v>0</v>
       </c>
       <c r="F24" s="148" t="n">
         <v>0</v>
       </c>
-      <c r="G24" s="263" t="n">
+      <c r="G24" s="290" t="n">
         <v>0</v>
       </c>
       <c r="H24" s="136" t="n">
         <v>0</v>
       </c>
-      <c r="I24" s="263" t="n">
+      <c r="I24" s="290" t="n">
         <v>0</v>
       </c>
       <c r="J24" s="148" t="n">
         <v>0</v>
       </c>
-      <c r="K24" s="261" t="n">
+      <c r="K24" s="288" t="n">
         <v>6</v>
       </c>
       <c r="L24" s="133" t="n">
         <v>7385</v>
       </c>
-      <c r="M24" s="261" t="n">
+      <c r="M24" s="288" t="n">
         <v>6</v>
       </c>
       <c r="N24" s="133" t="n">
@@ -2121,15 +2154,15 @@
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="257" t="inlineStr">
+      <c r="A25" s="284" t="inlineStr">
         <is>
           <t>#QY8L2GLUR</t>
         </is>
       </c>
-      <c r="B25" s="257" t="n">
+      <c r="B25" s="284" t="n">
         <v>907</v>
       </c>
-      <c r="C25" s="254" t="n">
+      <c r="C25" s="281" t="n">
         <v>22</v>
       </c>
       <c r="D25" s="137" t="inlineStr">
@@ -2137,31 +2170,31 @@
           <t>Huy</t>
         </is>
       </c>
-      <c r="E25" s="259" t="n">
+      <c r="E25" s="286" t="n">
         <v>0</v>
       </c>
       <c r="F25" s="137" t="n">
         <v>0</v>
       </c>
-      <c r="G25" s="259" t="n">
+      <c r="G25" s="286" t="n">
         <v>0</v>
       </c>
       <c r="H25" s="130" t="n">
         <v>0</v>
       </c>
-      <c r="I25" s="259" t="n">
+      <c r="I25" s="286" t="n">
         <v>0</v>
       </c>
       <c r="J25" s="137" t="n">
         <v>0</v>
       </c>
-      <c r="K25" s="258" t="n">
+      <c r="K25" s="285" t="n">
         <v>6</v>
       </c>
       <c r="L25" s="127" t="n">
         <v>6995</v>
       </c>
-      <c r="M25" s="258" t="n">
+      <c r="M25" s="285" t="n">
         <v>6</v>
       </c>
       <c r="N25" s="127" t="n">
@@ -2169,15 +2202,15 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="260" t="inlineStr">
+      <c r="A26" s="287" t="inlineStr">
         <is>
           <t>#L2QQL9QVJ</t>
         </is>
       </c>
-      <c r="B26" s="260" t="n">
+      <c r="B26" s="287" t="n">
         <v>1450</v>
       </c>
-      <c r="C26" s="250" t="n">
+      <c r="C26" s="277" t="n">
         <v>23</v>
       </c>
       <c r="D26" s="148" t="inlineStr">
@@ -2185,31 +2218,31 @@
           <t>JustPre10d</t>
         </is>
       </c>
-      <c r="E26" s="263" t="n">
+      <c r="E26" s="290" t="n">
         <v>0</v>
       </c>
       <c r="F26" s="148" t="n">
         <v>0</v>
       </c>
-      <c r="G26" s="263" t="n">
+      <c r="G26" s="290" t="n">
         <v>0</v>
       </c>
       <c r="H26" s="136" t="n">
         <v>0</v>
       </c>
-      <c r="I26" s="263" t="n">
+      <c r="I26" s="290" t="n">
         <v>0</v>
       </c>
       <c r="J26" s="148" t="n">
         <v>0</v>
       </c>
-      <c r="K26" s="261" t="n">
+      <c r="K26" s="288" t="n">
         <v>6</v>
       </c>
       <c r="L26" s="133" t="n">
         <v>6655</v>
       </c>
-      <c r="M26" s="261" t="n">
+      <c r="M26" s="288" t="n">
         <v>6</v>
       </c>
       <c r="N26" s="133" t="n">
@@ -2217,15 +2250,15 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="257" t="inlineStr">
+      <c r="A27" s="284" t="inlineStr">
         <is>
           <t>#LPR9RPCY9</t>
         </is>
       </c>
-      <c r="B27" s="257" t="n">
+      <c r="B27" s="284" t="n">
         <v>990</v>
       </c>
-      <c r="C27" s="254" t="n">
+      <c r="C27" s="281" t="n">
         <v>24</v>
       </c>
       <c r="D27" s="137" t="inlineStr">
@@ -2233,43 +2266,43 @@
           <t>sayhuss17</t>
         </is>
       </c>
-      <c r="E27" s="259" t="n">
+      <c r="E27" s="286" t="n">
         <v>0</v>
       </c>
       <c r="F27" s="137" t="n">
         <v>0</v>
       </c>
-      <c r="G27" s="259" t="n">
+      <c r="G27" s="286" t="n">
         <v>0</v>
       </c>
       <c r="H27" s="130" t="n">
         <v>0</v>
       </c>
-      <c r="I27" s="259" t="n">
+      <c r="I27" s="286" t="n">
         <v>0</v>
       </c>
       <c r="J27" s="137" t="n">
         <v>0</v>
       </c>
-      <c r="K27" s="264" t="n">
+      <c r="K27" s="291" t="n">
         <v>4</v>
       </c>
       <c r="L27" s="131" t="n">
         <v>4240</v>
       </c>
-      <c r="M27" s="257" t="n"/>
+      <c r="M27" s="284" t="n"/>
       <c r="N27" s="130" t="n"/>
     </row>
     <row r="28">
-      <c r="A28" s="260" t="inlineStr">
+      <c r="A28" s="287" t="inlineStr">
         <is>
           <t>#QQL8C29CY</t>
         </is>
       </c>
-      <c r="B28" s="260" t="n">
+      <c r="B28" s="287" t="n">
         <v>918</v>
       </c>
-      <c r="C28" s="250" t="n">
+      <c r="C28" s="277" t="n">
         <v>25</v>
       </c>
       <c r="D28" s="148" t="inlineStr">
@@ -2277,31 +2310,31 @@
           <t>TypicalTeague#2</t>
         </is>
       </c>
-      <c r="E28" s="263" t="n">
+      <c r="E28" s="290" t="n">
         <v>0</v>
       </c>
       <c r="F28" s="148" t="n">
         <v>0</v>
       </c>
-      <c r="G28" s="263" t="n">
+      <c r="G28" s="290" t="n">
         <v>0</v>
       </c>
       <c r="H28" s="136" t="n">
         <v>0</v>
       </c>
-      <c r="I28" s="263" t="n">
+      <c r="I28" s="290" t="n">
         <v>0</v>
       </c>
       <c r="J28" s="148" t="n">
         <v>0</v>
       </c>
-      <c r="K28" s="261" t="n">
+      <c r="K28" s="288" t="n">
         <v>5</v>
       </c>
       <c r="L28" s="139" t="n">
         <v>4070</v>
       </c>
-      <c r="M28" s="261" t="n">
+      <c r="M28" s="288" t="n">
         <v>6</v>
       </c>
       <c r="N28" s="133" t="n">
@@ -2309,15 +2342,15 @@
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="257" t="inlineStr">
+      <c r="A29" s="284" t="inlineStr">
         <is>
           <t>#L9JJQY992</t>
         </is>
       </c>
-      <c r="B29" s="257" t="n">
+      <c r="B29" s="284" t="n">
         <v>773</v>
       </c>
-      <c r="C29" s="254" t="n">
+      <c r="C29" s="281" t="n">
         <v>26</v>
       </c>
       <c r="D29" s="137" t="inlineStr">
@@ -2325,43 +2358,43 @@
           <t>Fisted_Waffle</t>
         </is>
       </c>
-      <c r="E29" s="259" t="n">
+      <c r="E29" s="286" t="n">
         <v>0</v>
       </c>
       <c r="F29" s="137" t="n">
         <v>0</v>
       </c>
-      <c r="G29" s="259" t="n">
+      <c r="G29" s="286" t="n">
         <v>0</v>
       </c>
       <c r="H29" s="130" t="n">
         <v>0</v>
       </c>
-      <c r="I29" s="259" t="n">
+      <c r="I29" s="286" t="n">
         <v>0</v>
       </c>
       <c r="J29" s="137" t="n">
         <v>0</v>
       </c>
-      <c r="K29" s="259" t="n">
+      <c r="K29" s="286" t="n">
         <v>0</v>
       </c>
       <c r="L29" s="137" t="n">
         <v>0</v>
       </c>
-      <c r="M29" s="257" t="n"/>
+      <c r="M29" s="284" t="n"/>
       <c r="N29" s="130" t="n"/>
     </row>
     <row r="30">
-      <c r="A30" s="260" t="inlineStr">
+      <c r="A30" s="287" t="inlineStr">
         <is>
           <t>#L9QL9YQQY</t>
         </is>
       </c>
-      <c r="B30" s="260" t="n">
+      <c r="B30" s="287" t="n">
         <v>975</v>
       </c>
-      <c r="C30" s="250" t="n">
+      <c r="C30" s="277" t="n">
         <v>27</v>
       </c>
       <c r="D30" s="148" t="inlineStr">
@@ -2369,31 +2402,31 @@
           <t>Ima Chad</t>
         </is>
       </c>
-      <c r="E30" s="263" t="n">
+      <c r="E30" s="290" t="n">
         <v>0</v>
       </c>
       <c r="F30" s="148" t="n">
         <v>0</v>
       </c>
-      <c r="G30" s="263" t="n">
+      <c r="G30" s="290" t="n">
         <v>0</v>
       </c>
       <c r="H30" s="136" t="n">
         <v>0</v>
       </c>
-      <c r="I30" s="263" t="n">
+      <c r="I30" s="290" t="n">
         <v>0</v>
       </c>
       <c r="J30" s="148" t="n">
         <v>0</v>
       </c>
-      <c r="K30" s="263" t="n">
+      <c r="K30" s="290" t="n">
         <v>0</v>
       </c>
       <c r="L30" s="148" t="n">
         <v>0</v>
       </c>
-      <c r="M30" s="261" t="n">
+      <c r="M30" s="288" t="n">
         <v>5</v>
       </c>
       <c r="N30" s="148" t="n">
@@ -2401,15 +2434,15 @@
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="257" t="inlineStr">
+      <c r="A31" s="284" t="inlineStr">
         <is>
           <t>#PJYVV989R</t>
         </is>
       </c>
-      <c r="B31" s="257" t="n">
+      <c r="B31" s="284" t="n">
         <v>1584</v>
       </c>
-      <c r="C31" s="254" t="n">
+      <c r="C31" s="281" t="n">
         <v>28</v>
       </c>
       <c r="D31" s="137" t="inlineStr">
@@ -2417,43 +2450,43 @@
           <t>nx</t>
         </is>
       </c>
-      <c r="E31" s="259" t="n">
+      <c r="E31" s="286" t="n">
         <v>0</v>
       </c>
       <c r="F31" s="137" t="n">
         <v>0</v>
       </c>
-      <c r="G31" s="259" t="n">
+      <c r="G31" s="286" t="n">
         <v>0</v>
       </c>
       <c r="H31" s="130" t="n">
         <v>0</v>
       </c>
-      <c r="I31" s="259" t="n">
+      <c r="I31" s="286" t="n">
         <v>0</v>
       </c>
       <c r="J31" s="137" t="n">
         <v>0</v>
       </c>
-      <c r="K31" s="259" t="n">
+      <c r="K31" s="286" t="n">
         <v>0</v>
       </c>
       <c r="L31" s="137" t="n">
         <v>0</v>
       </c>
-      <c r="M31" s="257" t="n"/>
+      <c r="M31" s="284" t="n"/>
       <c r="N31" s="130" t="n"/>
     </row>
     <row r="32">
-      <c r="A32" s="260" t="inlineStr">
+      <c r="A32" s="287" t="inlineStr">
         <is>
           <t>#LC9GUPJJG</t>
         </is>
       </c>
-      <c r="B32" s="260" t="n">
+      <c r="B32" s="287" t="n">
         <v>966</v>
       </c>
-      <c r="C32" s="250" t="n">
+      <c r="C32" s="277" t="n">
         <v>29</v>
       </c>
       <c r="D32" s="148" t="inlineStr">
@@ -2461,23 +2494,23 @@
           <t>raptor2222a</t>
         </is>
       </c>
-      <c r="E32" s="263" t="n">
+      <c r="E32" s="290" t="n">
         <v>0</v>
       </c>
       <c r="F32" s="148" t="n">
         <v>0</v>
       </c>
-      <c r="G32" s="263" t="n">
+      <c r="G32" s="290" t="n">
         <v>0</v>
       </c>
       <c r="H32" s="136" t="n">
         <v>0</v>
       </c>
-      <c r="I32" s="260" t="n"/>
+      <c r="I32" s="287" t="n"/>
       <c r="J32" s="136" t="n"/>
-      <c r="K32" s="260" t="n"/>
+      <c r="K32" s="287" t="n"/>
       <c r="L32" s="136" t="n"/>
-      <c r="M32" s="260" t="n"/>
+      <c r="M32" s="287" t="n"/>
       <c r="N32" s="136" t="n"/>
     </row>
     <row r="33">
@@ -2513,15 +2546,15 @@
       <c r="N33" s="235" t="n"/>
     </row>
     <row r="34">
-      <c r="A34" s="263" t="inlineStr">
+      <c r="A34" s="290" t="inlineStr">
         <is>
           <t>#UVCCQC02</t>
         </is>
       </c>
-      <c r="B34" s="260" t="n">
+      <c r="B34" s="287" t="n">
         <v>1806</v>
       </c>
-      <c r="C34" s="250" t="n">
+      <c r="C34" s="277" t="n">
         <v>31</v>
       </c>
       <c r="D34" s="136" t="inlineStr">
@@ -2529,23 +2562,23 @@
           <t>lordshisha</t>
         </is>
       </c>
-      <c r="E34" s="260" t="n"/>
+      <c r="E34" s="287" t="n"/>
       <c r="F34" s="136" t="n"/>
-      <c r="G34" s="260" t="n"/>
+      <c r="G34" s="287" t="n"/>
       <c r="H34" s="136" t="n"/>
-      <c r="I34" s="261" t="n">
+      <c r="I34" s="288" t="n">
         <v>6</v>
       </c>
       <c r="J34" s="133" t="n">
         <v>8496</v>
       </c>
-      <c r="K34" s="261" t="n">
+      <c r="K34" s="288" t="n">
         <v>6</v>
       </c>
       <c r="L34" s="133" t="n">
         <v>6310</v>
       </c>
-      <c r="M34" s="261" t="n">
+      <c r="M34" s="288" t="n">
         <v>6</v>
       </c>
       <c r="N34" s="133" t="n">
@@ -2553,15 +2586,15 @@
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="259" t="inlineStr">
+      <c r="A35" s="286" t="inlineStr">
         <is>
           <t>#P2CPRPQU</t>
         </is>
       </c>
-      <c r="B35" s="257" t="n">
+      <c r="B35" s="284" t="n">
         <v>2232</v>
       </c>
-      <c r="C35" s="254" t="n">
+      <c r="C35" s="281" t="n">
         <v>32</v>
       </c>
       <c r="D35" s="130" t="inlineStr">
@@ -2569,23 +2602,23 @@
           <t>The Drift King</t>
         </is>
       </c>
-      <c r="E35" s="257" t="n"/>
+      <c r="E35" s="284" t="n"/>
       <c r="F35" s="130" t="n"/>
-      <c r="G35" s="257" t="n"/>
+      <c r="G35" s="284" t="n"/>
       <c r="H35" s="130" t="n"/>
-      <c r="I35" s="258" t="n">
+      <c r="I35" s="285" t="n">
         <v>6</v>
       </c>
       <c r="J35" s="127" t="n">
         <v>8023</v>
       </c>
-      <c r="K35" s="258" t="n">
+      <c r="K35" s="285" t="n">
         <v>6</v>
       </c>
       <c r="L35" s="127" t="n">
         <v>7625</v>
       </c>
-      <c r="M35" s="258" t="n">
+      <c r="M35" s="285" t="n">
         <v>6</v>
       </c>
       <c r="N35" s="127" t="n">
@@ -2593,15 +2626,15 @@
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="263" t="inlineStr">
+      <c r="A36" s="290" t="inlineStr">
         <is>
           <t>#QJVL0LYQQ</t>
         </is>
       </c>
-      <c r="B36" s="260" t="n">
+      <c r="B36" s="287" t="n">
         <v>921</v>
       </c>
-      <c r="C36" s="250" t="n">
+      <c r="C36" s="277" t="n">
         <v>33</v>
       </c>
       <c r="D36" s="136" t="inlineStr">
@@ -2609,23 +2642,23 @@
           <t>mobbb341</t>
         </is>
       </c>
-      <c r="E36" s="260" t="n"/>
+      <c r="E36" s="287" t="n"/>
       <c r="F36" s="136" t="n"/>
-      <c r="G36" s="260" t="n"/>
+      <c r="G36" s="287" t="n"/>
       <c r="H36" s="136" t="n"/>
-      <c r="I36" s="261" t="n">
+      <c r="I36" s="288" t="n">
         <v>6</v>
       </c>
       <c r="J36" s="133" t="n">
         <v>7710</v>
       </c>
-      <c r="K36" s="261" t="n">
+      <c r="K36" s="288" t="n">
         <v>6</v>
       </c>
       <c r="L36" s="133" t="n">
         <v>8810</v>
       </c>
-      <c r="M36" s="261" t="n">
+      <c r="M36" s="288" t="n">
         <v>6</v>
       </c>
       <c r="N36" s="139" t="n">
@@ -2633,15 +2666,15 @@
       </c>
     </row>
     <row r="37">
-      <c r="A37" s="259" t="inlineStr">
+      <c r="A37" s="286" t="inlineStr">
         <is>
           <t>#L8R82C8VC</t>
         </is>
       </c>
-      <c r="B37" s="257" t="n">
+      <c r="B37" s="284" t="n">
         <v>1162</v>
       </c>
-      <c r="C37" s="254" t="n">
+      <c r="C37" s="281" t="n">
         <v>34</v>
       </c>
       <c r="D37" s="130" t="inlineStr">
@@ -2649,23 +2682,23 @@
           <t>caden asue</t>
         </is>
       </c>
-      <c r="E37" s="257" t="n"/>
+      <c r="E37" s="284" t="n"/>
       <c r="F37" s="130" t="n"/>
-      <c r="G37" s="257" t="n"/>
+      <c r="G37" s="284" t="n"/>
       <c r="H37" s="130" t="n"/>
-      <c r="I37" s="258" t="n">
+      <c r="I37" s="285" t="n">
         <v>6</v>
       </c>
       <c r="J37" s="131" t="n">
         <v>5112</v>
       </c>
-      <c r="K37" s="258" t="n">
+      <c r="K37" s="285" t="n">
         <v>6</v>
       </c>
       <c r="L37" s="131" t="n">
         <v>4283</v>
       </c>
-      <c r="M37" s="258" t="n">
+      <c r="M37" s="285" t="n">
         <v>6</v>
       </c>
       <c r="N37" s="131" t="n">
@@ -2673,15 +2706,15 @@
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="263" t="inlineStr">
+      <c r="A38" s="290" t="inlineStr">
         <is>
           <t>#L9Q8VLLQG</t>
         </is>
       </c>
-      <c r="B38" s="260" t="n">
+      <c r="B38" s="287" t="n">
         <v>1130</v>
       </c>
-      <c r="C38" s="250" t="n">
+      <c r="C38" s="277" t="n">
         <v>35</v>
       </c>
       <c r="D38" s="136" t="inlineStr">
@@ -2689,15 +2722,15 @@
           <t>cat</t>
         </is>
       </c>
-      <c r="E38" s="260" t="n"/>
+      <c r="E38" s="287" t="n"/>
       <c r="F38" s="136" t="n"/>
-      <c r="G38" s="260" t="n"/>
+      <c r="G38" s="287" t="n"/>
       <c r="H38" s="136" t="n"/>
-      <c r="I38" s="260" t="n"/>
+      <c r="I38" s="287" t="n"/>
       <c r="J38" s="136" t="n"/>
-      <c r="K38" s="260" t="n"/>
+      <c r="K38" s="287" t="n"/>
       <c r="L38" s="136" t="n"/>
-      <c r="M38" s="261" t="n">
+      <c r="M38" s="288" t="n">
         <v>6</v>
       </c>
       <c r="N38" s="139" t="n">
@@ -2705,15 +2738,15 @@
       </c>
     </row>
     <row r="39">
-      <c r="A39" s="259" t="inlineStr">
+      <c r="A39" s="286" t="inlineStr">
         <is>
           <t>#QV0PQC9JU</t>
         </is>
       </c>
-      <c r="B39" s="257" t="n">
+      <c r="B39" s="284" t="n">
         <v>539</v>
       </c>
-      <c r="C39" s="254" t="n">
+      <c r="C39" s="281" t="n">
         <v>36</v>
       </c>
       <c r="D39" s="130" t="inlineStr">
@@ -2721,15 +2754,15 @@
           <t>Superman</t>
         </is>
       </c>
-      <c r="E39" s="257" t="n"/>
+      <c r="E39" s="284" t="n"/>
       <c r="F39" s="130" t="n"/>
-      <c r="G39" s="257" t="n"/>
+      <c r="G39" s="284" t="n"/>
       <c r="H39" s="130" t="n"/>
-      <c r="I39" s="257" t="n"/>
+      <c r="I39" s="284" t="n"/>
       <c r="J39" s="130" t="n"/>
-      <c r="K39" s="257" t="n"/>
+      <c r="K39" s="284" t="n"/>
       <c r="L39" s="130" t="n"/>
-      <c r="M39" s="258" t="n">
+      <c r="M39" s="285" t="n">
         <v>6</v>
       </c>
       <c r="N39" s="131" t="n">
@@ -2737,15 +2770,15 @@
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="263" t="inlineStr">
+      <c r="A40" s="290" t="inlineStr">
         <is>
           <t>#LU0CRP09L</t>
         </is>
       </c>
-      <c r="B40" s="260" t="n">
+      <c r="B40" s="287" t="n">
         <v>809</v>
       </c>
-      <c r="C40" s="250" t="n">
+      <c r="C40" s="277" t="n">
         <v>37</v>
       </c>
       <c r="D40" s="136" t="inlineStr">
@@ -2753,15 +2786,15 @@
           <t>I Dont Know</t>
         </is>
       </c>
-      <c r="E40" s="260" t="n"/>
+      <c r="E40" s="287" t="n"/>
       <c r="F40" s="136" t="n"/>
-      <c r="G40" s="260" t="n"/>
+      <c r="G40" s="287" t="n"/>
       <c r="H40" s="136" t="n"/>
-      <c r="I40" s="260" t="n"/>
+      <c r="I40" s="287" t="n"/>
       <c r="J40" s="136" t="n"/>
-      <c r="K40" s="260" t="n"/>
+      <c r="K40" s="287" t="n"/>
       <c r="L40" s="136" t="n"/>
-      <c r="M40" s="262" t="n">
+      <c r="M40" s="289" t="n">
         <v>3</v>
       </c>
       <c r="N40" s="148" t="n">
@@ -2769,15 +2802,15 @@
       </c>
     </row>
     <row r="41">
-      <c r="A41" s="259" t="inlineStr">
+      <c r="A41" s="286" t="inlineStr">
         <is>
           <t>#YCPP0QPP8</t>
         </is>
       </c>
-      <c r="B41" s="257" t="n">
+      <c r="B41" s="284" t="n">
         <v>3327</v>
       </c>
-      <c r="C41" s="254" t="n">
+      <c r="C41" s="281" t="n">
         <v>38</v>
       </c>
       <c r="D41" s="130" t="inlineStr">
@@ -2785,15 +2818,15 @@
           <t>Coach</t>
         </is>
       </c>
-      <c r="E41" s="257" t="n"/>
+      <c r="E41" s="284" t="n"/>
       <c r="F41" s="130" t="n"/>
-      <c r="G41" s="257" t="n"/>
+      <c r="G41" s="284" t="n"/>
       <c r="H41" s="130" t="n"/>
-      <c r="I41" s="257" t="n"/>
+      <c r="I41" s="284" t="n"/>
       <c r="J41" s="130" t="n"/>
-      <c r="K41" s="257" t="n"/>
+      <c r="K41" s="284" t="n"/>
       <c r="L41" s="130" t="n"/>
-      <c r="M41" s="259" t="n">
+      <c r="M41" s="286" t="n">
         <v>0</v>
       </c>
       <c r="N41" s="137" t="n">
@@ -3660,12 +3693,12 @@
       </c>
     </row>
     <row r="4">
-      <c r="B4" s="238" t="inlineStr">
+      <c r="B4" s="265" t="inlineStr">
         <is>
           <t>#98JG2UJQL</t>
         </is>
       </c>
-      <c r="C4" s="239" t="inlineStr">
+      <c r="C4" s="266" t="inlineStr">
         <is>
           <t>Dragonux</t>
         </is>
@@ -3682,12 +3715,12 @@
       </c>
     </row>
     <row r="5">
-      <c r="B5" s="240" t="inlineStr">
+      <c r="B5" s="267" t="inlineStr">
         <is>
           <t>#82QLQCJRJ</t>
         </is>
       </c>
-      <c r="C5" s="240" t="inlineStr">
+      <c r="C5" s="267" t="inlineStr">
         <is>
           <t>Raging Fury</t>
         </is>
@@ -3696,12 +3729,12 @@
       <c r="E5" s="93" t="n"/>
     </row>
     <row r="6">
-      <c r="B6" s="241" t="inlineStr">
+      <c r="B6" s="268" t="inlineStr">
         <is>
           <t>#90U0VPU9U</t>
         </is>
       </c>
-      <c r="C6" s="242" t="inlineStr">
+      <c r="C6" s="269" t="inlineStr">
         <is>
           <t>KYANI7E</t>
         </is>
@@ -3718,12 +3751,12 @@
       </c>
     </row>
     <row r="7">
-      <c r="B7" s="240" t="inlineStr">
+      <c r="B7" s="267" t="inlineStr">
         <is>
           <t>#PJYVV989R</t>
         </is>
       </c>
-      <c r="C7" s="240" t="inlineStr">
+      <c r="C7" s="267" t="inlineStr">
         <is>
           <t>nx</t>
         </is>
@@ -3732,12 +3765,12 @@
       <c r="E7" s="93" t="n"/>
     </row>
     <row r="8">
-      <c r="B8" s="241" t="inlineStr">
+      <c r="B8" s="268" t="inlineStr">
         <is>
           <t>#QLJ2U20Y2</t>
         </is>
       </c>
-      <c r="C8" s="242" t="inlineStr">
+      <c r="C8" s="269" t="inlineStr">
         <is>
           <t>DeadLeaf</t>
         </is>
@@ -3754,12 +3787,12 @@
       </c>
     </row>
     <row r="9">
-      <c r="B9" s="240" t="inlineStr">
+      <c r="B9" s="267" t="inlineStr">
         <is>
           <t>#L2QQL9QVJ</t>
         </is>
       </c>
-      <c r="C9" s="240" t="inlineStr">
+      <c r="C9" s="267" t="inlineStr">
         <is>
           <t>JustPre10d</t>
         </is>
@@ -3768,12 +3801,12 @@
       <c r="E9" s="112" t="n"/>
     </row>
     <row r="10">
-      <c r="B10" s="241" t="inlineStr">
+      <c r="B10" s="268" t="inlineStr">
         <is>
           <t>#YJ20CRJYQ</t>
         </is>
       </c>
-      <c r="C10" s="242" t="inlineStr">
+      <c r="C10" s="269" t="inlineStr">
         <is>
           <t>UnluckGod</t>
         </is>
@@ -3790,12 +3823,12 @@
       </c>
     </row>
     <row r="11">
-      <c r="B11" s="243" t="inlineStr">
+      <c r="B11" s="270" t="inlineStr">
         <is>
           <t>#YRGRRJQCY</t>
         </is>
       </c>
-      <c r="C11" s="244" t="inlineStr">
+      <c r="C11" s="271" t="inlineStr">
         <is>
           <t>DoubleSpice</t>
         </is>
@@ -3812,12 +3845,12 @@
       </c>
     </row>
     <row r="12">
-      <c r="B12" s="241" t="inlineStr">
+      <c r="B12" s="268" t="inlineStr">
         <is>
           <t>#Q8CLCUCC2</t>
         </is>
       </c>
-      <c r="C12" s="242" t="inlineStr">
+      <c r="C12" s="269" t="inlineStr">
         <is>
           <t>Moxxi</t>
         </is>
@@ -3834,12 +3867,12 @@
       </c>
     </row>
     <row r="13">
-      <c r="B13" s="240" t="inlineStr">
+      <c r="B13" s="267" t="inlineStr">
         <is>
           <t>#G0JPUQGYR</t>
         </is>
       </c>
-      <c r="C13" s="245" t="inlineStr">
+      <c r="C13" s="272" t="inlineStr">
         <is>
           <t>Collin</t>
         </is>
@@ -3856,12 +3889,12 @@
       </c>
     </row>
     <row r="14">
-      <c r="B14" s="238" t="inlineStr">
+      <c r="B14" s="265" t="inlineStr">
         <is>
           <t>#QLG0VJG2J</t>
         </is>
       </c>
-      <c r="C14" s="238" t="inlineStr">
+      <c r="C14" s="265" t="inlineStr">
         <is>
           <t>PocketRocket</t>
         </is>
@@ -3870,12 +3903,12 @@
       <c r="E14" s="107" t="n"/>
     </row>
     <row r="15">
-      <c r="B15" s="240" t="inlineStr">
+      <c r="B15" s="267" t="inlineStr">
         <is>
           <t>#QJC8LQU9U</t>
         </is>
       </c>
-      <c r="C15" s="240" t="inlineStr">
+      <c r="C15" s="267" t="inlineStr">
         <is>
           <t>Master01</t>
         </is>
@@ -3884,12 +3917,12 @@
       <c r="E15" s="93" t="n"/>
     </row>
     <row r="16">
-      <c r="B16" s="238" t="inlineStr">
+      <c r="B16" s="265" t="inlineStr">
         <is>
           <t>#QRPRYR8LL</t>
         </is>
       </c>
-      <c r="C16" s="238" t="inlineStr">
+      <c r="C16" s="265" t="inlineStr">
         <is>
           <t>FidelCashflow</t>
         </is>
@@ -3898,12 +3931,12 @@
       <c r="E16" s="97" t="n"/>
     </row>
     <row r="17">
-      <c r="B17" s="240" t="inlineStr">
+      <c r="B17" s="267" t="inlineStr">
         <is>
           <t>#LPR9RPCY9</t>
         </is>
       </c>
-      <c r="C17" s="246" t="inlineStr">
+      <c r="C17" s="273" t="inlineStr">
         <is>
           <t>sayhuss17</t>
         </is>
@@ -3920,12 +3953,12 @@
       </c>
     </row>
     <row r="18">
-      <c r="B18" s="238" t="inlineStr">
+      <c r="B18" s="265" t="inlineStr">
         <is>
           <t>#L9QL9YQQY</t>
         </is>
       </c>
-      <c r="C18" s="238" t="inlineStr">
+      <c r="C18" s="265" t="inlineStr">
         <is>
           <t>Ima Chad</t>
         </is>
@@ -3934,12 +3967,12 @@
       <c r="E18" s="107" t="n"/>
     </row>
     <row r="19">
-      <c r="B19" s="240" t="inlineStr">
+      <c r="B19" s="267" t="inlineStr">
         <is>
           <t>#LC9GUPJJG</t>
         </is>
       </c>
-      <c r="C19" s="240" t="inlineStr">
+      <c r="C19" s="267" t="inlineStr">
         <is>
           <t>raptor2222a</t>
         </is>
@@ -3948,12 +3981,12 @@
       <c r="E19" s="112" t="n"/>
     </row>
     <row r="20">
-      <c r="B20" s="241" t="inlineStr">
+      <c r="B20" s="268" t="inlineStr">
         <is>
           <t>#QUG8QQJ92</t>
         </is>
       </c>
-      <c r="C20" s="242" t="inlineStr">
+      <c r="C20" s="269" t="inlineStr">
         <is>
           <t>Karma</t>
         </is>
@@ -3970,12 +4003,12 @@
       </c>
     </row>
     <row r="21">
-      <c r="B21" s="243" t="inlineStr">
+      <c r="B21" s="270" t="inlineStr">
         <is>
           <t>#QUYG0PQC8</t>
         </is>
       </c>
-      <c r="C21" s="244" t="inlineStr">
+      <c r="C21" s="271" t="inlineStr">
         <is>
           <t>Luffy</t>
         </is>
@@ -3992,12 +4025,12 @@
       </c>
     </row>
     <row r="22">
-      <c r="B22" s="238" t="inlineStr">
+      <c r="B22" s="265" t="inlineStr">
         <is>
           <t>#QQL8C29CY</t>
         </is>
       </c>
-      <c r="C22" s="238" t="inlineStr">
+      <c r="C22" s="265" t="inlineStr">
         <is>
           <t>TypicalTeague#2</t>
         </is>
@@ -4006,12 +4039,12 @@
       <c r="E22" s="97" t="n"/>
     </row>
     <row r="23">
-      <c r="B23" s="240" t="inlineStr">
+      <c r="B23" s="267" t="inlineStr">
         <is>
           <t>#QY8L2GLUR</t>
         </is>
       </c>
-      <c r="C23" s="240" t="inlineStr">
+      <c r="C23" s="267" t="inlineStr">
         <is>
           <t>Huy</t>
         </is>
@@ -4020,12 +4053,12 @@
       <c r="E23" s="93" t="n"/>
     </row>
     <row r="24">
-      <c r="B24" s="238" t="inlineStr">
+      <c r="B24" s="265" t="inlineStr">
         <is>
           <t>#QU0U2Q99G</t>
         </is>
       </c>
-      <c r="C24" s="238" t="inlineStr">
+      <c r="C24" s="265" t="inlineStr">
         <is>
           <t>big coc</t>
         </is>
@@ -4034,12 +4067,12 @@
       <c r="E24" s="97" t="n"/>
     </row>
     <row r="25">
-      <c r="B25" s="240" t="inlineStr">
+      <c r="B25" s="267" t="inlineStr">
         <is>
           <t>#QL8LVLYG8</t>
         </is>
       </c>
-      <c r="C25" s="240" t="inlineStr">
+      <c r="C25" s="267" t="inlineStr">
         <is>
           <t>Some guy</t>
         </is>
@@ -4048,12 +4081,12 @@
       <c r="E25" s="93" t="n"/>
     </row>
     <row r="26">
-      <c r="B26" s="238" t="inlineStr">
+      <c r="B26" s="265" t="inlineStr">
         <is>
           <t>#L9JJQY992</t>
         </is>
       </c>
-      <c r="C26" s="238" t="inlineStr">
+      <c r="C26" s="265" t="inlineStr">
         <is>
           <t>Fisted_Waffle</t>
         </is>
@@ -4062,12 +4095,12 @@
       <c r="E26" s="97" t="n"/>
     </row>
     <row r="27">
-      <c r="B27" s="243" t="inlineStr">
+      <c r="B27" s="270" t="inlineStr">
         <is>
           <t>#G0QPVJY9L</t>
         </is>
       </c>
-      <c r="C27" s="244" t="inlineStr">
+      <c r="C27" s="271" t="inlineStr">
         <is>
           <t>Zoro</t>
         </is>
@@ -4084,12 +4117,12 @@
       </c>
     </row>
     <row r="28">
-      <c r="B28" s="238" t="inlineStr">
+      <c r="B28" s="265" t="inlineStr">
         <is>
           <t>#QV8JJ0URU</t>
         </is>
       </c>
-      <c r="C28" s="238" t="inlineStr">
+      <c r="C28" s="265" t="inlineStr">
         <is>
           <t>✨Jacob</t>
         </is>
@@ -4098,12 +4131,12 @@
       <c r="E28" s="97" t="n"/>
     </row>
     <row r="29">
-      <c r="B29" s="243" t="inlineStr">
+      <c r="B29" s="270" t="inlineStr">
         <is>
           <t>#QLR088LC9</t>
         </is>
       </c>
-      <c r="C29" s="244" t="inlineStr">
+      <c r="C29" s="271" t="inlineStr">
         <is>
           <t>Sanji</t>
         </is>
@@ -4120,12 +4153,12 @@
       </c>
     </row>
     <row r="30">
-      <c r="B30" s="241" t="inlineStr">
+      <c r="B30" s="268" t="inlineStr">
         <is>
           <t>#QCV22VP0G</t>
         </is>
       </c>
-      <c r="C30" s="242" t="inlineStr">
+      <c r="C30" s="269" t="inlineStr">
         <is>
           <t>Nami</t>
         </is>
@@ -4142,12 +4175,12 @@
       </c>
     </row>
     <row r="31">
-      <c r="B31" s="243" t="inlineStr">
+      <c r="B31" s="270" t="inlineStr">
         <is>
           <t>#QUV2GP88U</t>
         </is>
       </c>
-      <c r="C31" s="244" t="inlineStr">
+      <c r="C31" s="271" t="inlineStr">
         <is>
           <t>Nico Robin</t>
         </is>
@@ -4164,12 +4197,12 @@
       </c>
     </row>
     <row r="32">
-      <c r="B32" s="247" t="inlineStr">
+      <c r="B32" s="274" t="inlineStr">
         <is>
           <t>#Q0JG2RJQ8</t>
         </is>
       </c>
-      <c r="C32" s="248" t="inlineStr">
+      <c r="C32" s="275" t="inlineStr">
         <is>
           <t>bozo</t>
         </is>

</xml_diff>

<commit_message>
updating the clash file from bat
</commit_message>
<xml_diff>
--- a/Clash.xlsx
+++ b/Clash.xlsx
@@ -179,7 +179,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="39">
+  <borders count="41">
     <border>
       <left/>
       <right/>
@@ -290,11 +290,13 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6"/>
   </cellStyleXfs>
-  <cellXfs count="515">
+  <cellXfs count="542">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -928,6 +930,37 @@
     <xf numFmtId="164" fontId="5" fillId="25" borderId="38" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="5" fillId="24" borderId="38" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="5" fillId="23" borderId="38" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="6" fillId="18" borderId="39" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="6" fillId="19" borderId="39" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="6" fillId="21" borderId="39" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="6" fillId="22" borderId="39" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="5" fillId="21" borderId="39" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="5" fillId="18" borderId="39" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="5" fillId="20" borderId="39" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="5" fillId="24" borderId="39" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="5" fillId="22" borderId="39" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="5" fillId="25" borderId="39" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="5" fillId="19" borderId="39" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="6" fillId="18" borderId="40" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="18" borderId="40" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="19" borderId="40" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="6" fillId="24" borderId="40" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="6" fillId="21" borderId="40" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="21" borderId="40" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="22" borderId="40" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="6" fillId="25" borderId="40" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="5" fillId="18" borderId="40" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="5" fillId="19" borderId="40" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="5" fillId="20" borderId="40" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="5" fillId="21" borderId="40" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="5" fillId="22" borderId="40" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="5" fillId="25" borderId="40" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="5" fillId="24" borderId="40" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="5" fillId="23" borderId="40" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1476,15 +1509,15 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="499" t="inlineStr">
+      <c r="A4" s="526" t="inlineStr">
         <is>
           <t>#QLJ2U20Y2</t>
         </is>
       </c>
-      <c r="B4" s="499" t="n">
+      <c r="B4" s="526" t="n">
         <v>1486</v>
       </c>
-      <c r="C4" s="500" t="n">
+      <c r="C4" s="527" t="n">
         <v>1</v>
       </c>
       <c r="D4" s="116" t="inlineStr">
@@ -1492,37 +1525,37 @@
           <t>DeadLeaf</t>
         </is>
       </c>
-      <c r="E4" s="501" t="n">
+      <c r="E4" s="528" t="n">
         <v>6</v>
       </c>
       <c r="F4" s="116" t="n">
         <v>13763</v>
       </c>
-      <c r="G4" s="502" t="n">
+      <c r="G4" s="529" t="n">
         <v>0</v>
       </c>
       <c r="H4" s="119" t="n">
         <v>30</v>
       </c>
-      <c r="I4" s="501" t="n">
+      <c r="I4" s="528" t="n">
         <v>6</v>
       </c>
       <c r="J4" s="116" t="n">
         <v>11140</v>
       </c>
-      <c r="K4" s="501" t="n">
+      <c r="K4" s="528" t="n">
         <v>6</v>
       </c>
       <c r="L4" s="116" t="n">
         <v>15509</v>
       </c>
-      <c r="M4" s="501" t="n">
+      <c r="M4" s="528" t="n">
         <v>6</v>
       </c>
       <c r="N4" s="116" t="n">
         <v>8567</v>
       </c>
-      <c r="O4" s="501" t="n">
+      <c r="O4" s="528" t="n">
         <v>6</v>
       </c>
       <c r="P4" s="116" t="n">
@@ -1530,15 +1563,15 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="503" t="inlineStr">
+      <c r="A5" s="530" t="inlineStr">
         <is>
           <t>#G0QPVJY9L</t>
         </is>
       </c>
-      <c r="B5" s="503" t="n">
+      <c r="B5" s="530" t="n">
         <v>840</v>
       </c>
-      <c r="C5" s="504" t="n">
+      <c r="C5" s="531" t="n">
         <v>2</v>
       </c>
       <c r="D5" s="122" t="inlineStr">
@@ -1546,37 +1579,37 @@
           <t>Zoro</t>
         </is>
       </c>
-      <c r="E5" s="505" t="n">
+      <c r="E5" s="532" t="n">
         <v>6</v>
       </c>
       <c r="F5" s="122" t="n">
         <v>13432</v>
       </c>
-      <c r="G5" s="506" t="n">
+      <c r="G5" s="533" t="n">
         <v>0</v>
       </c>
       <c r="H5" s="125" t="n">
         <v>0</v>
       </c>
-      <c r="I5" s="505" t="n">
+      <c r="I5" s="532" t="n">
         <v>6</v>
       </c>
       <c r="J5" s="122" t="n">
         <v>8855</v>
       </c>
-      <c r="K5" s="505" t="n">
+      <c r="K5" s="532" t="n">
         <v>6</v>
       </c>
       <c r="L5" s="122" t="n">
         <v>10965</v>
       </c>
-      <c r="M5" s="505" t="n">
+      <c r="M5" s="532" t="n">
         <v>6</v>
       </c>
       <c r="N5" s="122" t="n">
         <v>7905</v>
       </c>
-      <c r="O5" s="505" t="n">
+      <c r="O5" s="532" t="n">
         <v>6</v>
       </c>
       <c r="P5" s="122" t="n">
@@ -1584,15 +1617,15 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="499" t="inlineStr">
+      <c r="A6" s="526" t="inlineStr">
         <is>
           <t>#90U0VPU9U</t>
         </is>
       </c>
-      <c r="B6" s="499" t="n">
+      <c r="B6" s="526" t="n">
         <v>2509</v>
       </c>
-      <c r="C6" s="500" t="n">
+      <c r="C6" s="527" t="n">
         <v>3</v>
       </c>
       <c r="D6" s="116" t="inlineStr">
@@ -1600,37 +1633,37 @@
           <t>KYANI7E</t>
         </is>
       </c>
-      <c r="E6" s="501" t="n">
+      <c r="E6" s="528" t="n">
         <v>6</v>
       </c>
       <c r="F6" s="116" t="n">
         <v>13260</v>
       </c>
-      <c r="G6" s="502" t="n">
+      <c r="G6" s="529" t="n">
         <v>61</v>
       </c>
       <c r="H6" s="119" t="n">
         <v>4</v>
       </c>
-      <c r="I6" s="501" t="n">
+      <c r="I6" s="528" t="n">
         <v>6</v>
       </c>
       <c r="J6" s="116" t="n">
         <v>12144</v>
       </c>
-      <c r="K6" s="501" t="n">
+      <c r="K6" s="528" t="n">
         <v>6</v>
       </c>
       <c r="L6" s="116" t="n">
         <v>12835</v>
       </c>
-      <c r="M6" s="501" t="n">
+      <c r="M6" s="528" t="n">
         <v>6</v>
       </c>
       <c r="N6" s="116" t="n">
         <v>7696</v>
       </c>
-      <c r="O6" s="501" t="n">
+      <c r="O6" s="528" t="n">
         <v>6</v>
       </c>
       <c r="P6" s="116" t="n">
@@ -1638,15 +1671,15 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="503" t="inlineStr">
+      <c r="A7" s="530" t="inlineStr">
         <is>
           <t>#YJ20CRJYQ</t>
         </is>
       </c>
-      <c r="B7" s="503" t="n">
+      <c r="B7" s="530" t="n">
         <v>1350</v>
       </c>
-      <c r="C7" s="504" t="n">
+      <c r="C7" s="531" t="n">
         <v>4</v>
       </c>
       <c r="D7" s="122" t="inlineStr">
@@ -1654,37 +1687,37 @@
           <t>UnluckGod</t>
         </is>
       </c>
-      <c r="E7" s="505" t="n">
+      <c r="E7" s="532" t="n">
         <v>6</v>
       </c>
       <c r="F7" s="122" t="n">
         <v>12824</v>
       </c>
-      <c r="G7" s="506" t="n">
+      <c r="G7" s="533" t="n">
         <v>0</v>
       </c>
       <c r="H7" s="125" t="n">
         <v>61</v>
       </c>
-      <c r="I7" s="505" t="n">
+      <c r="I7" s="532" t="n">
         <v>6</v>
       </c>
       <c r="J7" s="122" t="n">
         <v>11999</v>
       </c>
-      <c r="K7" s="505" t="n">
+      <c r="K7" s="532" t="n">
         <v>6</v>
       </c>
       <c r="L7" s="122" t="n">
         <v>12972</v>
       </c>
-      <c r="M7" s="505" t="n">
+      <c r="M7" s="532" t="n">
         <v>6</v>
       </c>
       <c r="N7" s="122" t="n">
         <v>8286</v>
       </c>
-      <c r="O7" s="505" t="n">
+      <c r="O7" s="532" t="n">
         <v>6</v>
       </c>
       <c r="P7" s="122" t="n">
@@ -1692,15 +1725,15 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="499" t="inlineStr">
+      <c r="A8" s="526" t="inlineStr">
         <is>
           <t>#QUV2GP88U</t>
         </is>
       </c>
-      <c r="B8" s="499" t="n">
+      <c r="B8" s="526" t="n">
         <v>729</v>
       </c>
-      <c r="C8" s="500" t="n">
+      <c r="C8" s="527" t="n">
         <v>5</v>
       </c>
       <c r="D8" s="116" t="inlineStr">
@@ -1708,37 +1741,37 @@
           <t>Nico Robin</t>
         </is>
       </c>
-      <c r="E8" s="501" t="n">
+      <c r="E8" s="528" t="n">
         <v>6</v>
       </c>
       <c r="F8" s="116" t="n">
         <v>12612</v>
       </c>
-      <c r="G8" s="502" t="n">
+      <c r="G8" s="529" t="n">
         <v>0</v>
       </c>
       <c r="H8" s="119" t="n">
         <v>0</v>
       </c>
-      <c r="I8" s="501" t="n">
+      <c r="I8" s="528" t="n">
         <v>6</v>
       </c>
       <c r="J8" s="116" t="n">
         <v>11338</v>
       </c>
-      <c r="K8" s="501" t="n">
+      <c r="K8" s="528" t="n">
         <v>6</v>
       </c>
       <c r="L8" s="116" t="n">
         <v>10997</v>
       </c>
-      <c r="M8" s="501" t="n">
+      <c r="M8" s="528" t="n">
         <v>6</v>
       </c>
       <c r="N8" s="116" t="n">
         <v>11087</v>
       </c>
-      <c r="O8" s="501" t="n">
+      <c r="O8" s="528" t="n">
         <v>6</v>
       </c>
       <c r="P8" s="116" t="n">
@@ -1746,15 +1779,15 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="503" t="inlineStr">
+      <c r="A9" s="530" t="inlineStr">
         <is>
           <t>#QCV22VP0G</t>
         </is>
       </c>
-      <c r="B9" s="503" t="n">
+      <c r="B9" s="530" t="n">
         <v>778</v>
       </c>
-      <c r="C9" s="504" t="n">
+      <c r="C9" s="531" t="n">
         <v>6</v>
       </c>
       <c r="D9" s="122" t="inlineStr">
@@ -1762,37 +1795,37 @@
           <t>Nami</t>
         </is>
       </c>
-      <c r="E9" s="505" t="n">
+      <c r="E9" s="532" t="n">
         <v>6</v>
       </c>
       <c r="F9" s="122" t="n">
         <v>11795</v>
       </c>
-      <c r="G9" s="506" t="n">
+      <c r="G9" s="533" t="n">
         <v>0</v>
       </c>
       <c r="H9" s="125" t="n">
         <v>0</v>
       </c>
-      <c r="I9" s="505" t="n">
+      <c r="I9" s="532" t="n">
         <v>6</v>
       </c>
       <c r="J9" s="122" t="n">
         <v>10769</v>
       </c>
-      <c r="K9" s="505" t="n">
+      <c r="K9" s="532" t="n">
         <v>6</v>
       </c>
       <c r="L9" s="122" t="n">
         <v>12486</v>
       </c>
-      <c r="M9" s="505" t="n">
+      <c r="M9" s="532" t="n">
         <v>6</v>
       </c>
       <c r="N9" s="122" t="n">
         <v>8472</v>
       </c>
-      <c r="O9" s="505" t="n">
+      <c r="O9" s="532" t="n">
         <v>6</v>
       </c>
       <c r="P9" s="122" t="n">
@@ -1800,15 +1833,15 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="499" t="inlineStr">
+      <c r="A10" s="526" t="inlineStr">
         <is>
           <t>#YRGRRJQCY</t>
         </is>
       </c>
-      <c r="B10" s="499" t="n">
+      <c r="B10" s="526" t="n">
         <v>1337</v>
       </c>
-      <c r="C10" s="500" t="n">
+      <c r="C10" s="527" t="n">
         <v>7</v>
       </c>
       <c r="D10" s="116" t="inlineStr">
@@ -1816,37 +1849,37 @@
           <t>DoubleSpice</t>
         </is>
       </c>
-      <c r="E10" s="501" t="n">
+      <c r="E10" s="528" t="n">
         <v>6</v>
       </c>
       <c r="F10" s="116" t="n">
         <v>11620</v>
       </c>
-      <c r="G10" s="502" t="n">
+      <c r="G10" s="529" t="n">
         <v>0</v>
       </c>
       <c r="H10" s="119" t="n">
         <v>60</v>
       </c>
-      <c r="I10" s="501" t="n">
+      <c r="I10" s="528" t="n">
         <v>6</v>
       </c>
       <c r="J10" s="116" t="n">
         <v>14095</v>
       </c>
-      <c r="K10" s="501" t="n">
+      <c r="K10" s="528" t="n">
         <v>6</v>
       </c>
       <c r="L10" s="116" t="n">
         <v>12379</v>
       </c>
-      <c r="M10" s="501" t="n">
+      <c r="M10" s="528" t="n">
         <v>6</v>
       </c>
       <c r="N10" s="116" t="n">
         <v>8256</v>
       </c>
-      <c r="O10" s="501" t="n">
+      <c r="O10" s="528" t="n">
         <v>6</v>
       </c>
       <c r="P10" s="116" t="n">
@@ -1854,15 +1887,15 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="503" t="inlineStr">
+      <c r="A11" s="530" t="inlineStr">
         <is>
           <t>#QUG8QQJ92</t>
         </is>
       </c>
-      <c r="B11" s="503" t="n">
+      <c r="B11" s="530" t="n">
         <v>920</v>
       </c>
-      <c r="C11" s="504" t="n">
+      <c r="C11" s="531" t="n">
         <v>8</v>
       </c>
       <c r="D11" s="122" t="inlineStr">
@@ -1870,37 +1903,37 @@
           <t>Karma</t>
         </is>
       </c>
-      <c r="E11" s="505" t="n">
+      <c r="E11" s="532" t="n">
         <v>6</v>
       </c>
       <c r="F11" s="122" t="n">
         <v>11355</v>
       </c>
-      <c r="G11" s="506" t="n">
+      <c r="G11" s="533" t="n">
         <v>0</v>
       </c>
       <c r="H11" s="125" t="n">
         <v>0</v>
       </c>
-      <c r="I11" s="505" t="n">
+      <c r="I11" s="532" t="n">
         <v>6</v>
       </c>
       <c r="J11" s="122" t="n">
         <v>10003</v>
       </c>
-      <c r="K11" s="505" t="n">
+      <c r="K11" s="532" t="n">
         <v>6</v>
       </c>
       <c r="L11" s="122" t="n">
         <v>10595</v>
       </c>
-      <c r="M11" s="505" t="n">
+      <c r="M11" s="532" t="n">
         <v>6</v>
       </c>
       <c r="N11" s="122" t="n">
         <v>9240</v>
       </c>
-      <c r="O11" s="505" t="n">
+      <c r="O11" s="532" t="n">
         <v>6</v>
       </c>
       <c r="P11" s="122" t="n">
@@ -1908,15 +1941,15 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="507" t="inlineStr">
+      <c r="A12" s="534" t="inlineStr">
         <is>
           <t>#98JG2UJQL</t>
         </is>
       </c>
-      <c r="B12" s="507" t="n">
+      <c r="B12" s="534" t="n">
         <v>2957</v>
       </c>
-      <c r="C12" s="500" t="n">
+      <c r="C12" s="527" t="n">
         <v>9</v>
       </c>
       <c r="D12" s="133" t="inlineStr">
@@ -1924,37 +1957,37 @@
           <t>Dragonux</t>
         </is>
       </c>
-      <c r="E12" s="508" t="n">
+      <c r="E12" s="535" t="n">
         <v>6</v>
       </c>
       <c r="F12" s="133" t="n">
         <v>10910</v>
       </c>
-      <c r="G12" s="509" t="n">
+      <c r="G12" s="536" t="n">
         <v>211</v>
       </c>
       <c r="H12" s="136" t="n">
         <v>0</v>
       </c>
-      <c r="I12" s="508" t="n">
+      <c r="I12" s="535" t="n">
         <v>6</v>
       </c>
       <c r="J12" s="133" t="n">
         <v>8750</v>
       </c>
-      <c r="K12" s="508" t="n">
+      <c r="K12" s="535" t="n">
         <v>6</v>
       </c>
       <c r="L12" s="133" t="n">
         <v>10865</v>
       </c>
-      <c r="M12" s="508" t="n">
+      <c r="M12" s="535" t="n">
         <v>6</v>
       </c>
       <c r="N12" s="133" t="n">
         <v>8025</v>
       </c>
-      <c r="O12" s="508" t="n">
+      <c r="O12" s="535" t="n">
         <v>6</v>
       </c>
       <c r="P12" s="133" t="n">
@@ -1962,15 +1995,15 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="503" t="inlineStr">
+      <c r="A13" s="530" t="inlineStr">
         <is>
           <t>#QLR088LC9</t>
         </is>
       </c>
-      <c r="B13" s="503" t="n">
+      <c r="B13" s="530" t="n">
         <v>857</v>
       </c>
-      <c r="C13" s="504" t="n">
+      <c r="C13" s="531" t="n">
         <v>10</v>
       </c>
       <c r="D13" s="122" t="inlineStr">
@@ -1978,37 +2011,37 @@
           <t>Sanji</t>
         </is>
       </c>
-      <c r="E13" s="505" t="n">
+      <c r="E13" s="532" t="n">
         <v>6</v>
       </c>
       <c r="F13" s="122" t="n">
         <v>10910</v>
       </c>
-      <c r="G13" s="506" t="n">
+      <c r="G13" s="533" t="n">
         <v>0</v>
       </c>
       <c r="H13" s="125" t="n">
         <v>0</v>
       </c>
-      <c r="I13" s="505" t="n">
+      <c r="I13" s="532" t="n">
         <v>6</v>
       </c>
       <c r="J13" s="122" t="n">
         <v>9550</v>
       </c>
-      <c r="K13" s="505" t="n">
+      <c r="K13" s="532" t="n">
         <v>6</v>
       </c>
       <c r="L13" s="122" t="n">
         <v>9138</v>
       </c>
-      <c r="M13" s="505" t="n">
+      <c r="M13" s="532" t="n">
         <v>6</v>
       </c>
       <c r="N13" s="122" t="n">
         <v>8897</v>
       </c>
-      <c r="O13" s="505" t="n">
+      <c r="O13" s="532" t="n">
         <v>6</v>
       </c>
       <c r="P13" s="122" t="n">
@@ -2016,15 +2049,15 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="499" t="inlineStr">
+      <c r="A14" s="526" t="inlineStr">
         <is>
           <t>#QUYG0PQC8</t>
         </is>
       </c>
-      <c r="B14" s="499" t="n">
+      <c r="B14" s="526" t="n">
         <v>940</v>
       </c>
-      <c r="C14" s="500" t="n">
+      <c r="C14" s="527" t="n">
         <v>11</v>
       </c>
       <c r="D14" s="116" t="inlineStr">
@@ -2032,37 +2065,37 @@
           <t>Luffy</t>
         </is>
       </c>
-      <c r="E14" s="501" t="n">
+      <c r="E14" s="528" t="n">
         <v>6</v>
       </c>
       <c r="F14" s="116" t="n">
         <v>10879</v>
       </c>
-      <c r="G14" s="502" t="n">
+      <c r="G14" s="529" t="n">
         <v>0</v>
       </c>
       <c r="H14" s="119" t="n">
         <v>0</v>
       </c>
-      <c r="I14" s="501" t="n">
+      <c r="I14" s="528" t="n">
         <v>6</v>
       </c>
       <c r="J14" s="116" t="n">
         <v>9114</v>
       </c>
-      <c r="K14" s="501" t="n">
+      <c r="K14" s="528" t="n">
         <v>6</v>
       </c>
       <c r="L14" s="116" t="n">
         <v>13385</v>
       </c>
-      <c r="M14" s="501" t="n">
+      <c r="M14" s="528" t="n">
         <v>6</v>
       </c>
       <c r="N14" s="116" t="n">
         <v>7877</v>
       </c>
-      <c r="O14" s="501" t="n">
+      <c r="O14" s="528" t="n">
         <v>6</v>
       </c>
       <c r="P14" s="116" t="n">
@@ -2070,15 +2103,15 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="510" t="inlineStr">
+      <c r="A15" s="537" t="inlineStr">
         <is>
           <t>#G0JPUQGYR</t>
         </is>
       </c>
-      <c r="B15" s="510" t="n">
+      <c r="B15" s="537" t="n">
         <v>1286</v>
       </c>
-      <c r="C15" s="504" t="n">
+      <c r="C15" s="531" t="n">
         <v>12</v>
       </c>
       <c r="D15" s="127" t="inlineStr">
@@ -2086,37 +2119,37 @@
           <t>Collin</t>
         </is>
       </c>
-      <c r="E15" s="511" t="n">
+      <c r="E15" s="538" t="n">
         <v>6</v>
       </c>
       <c r="F15" s="127" t="n">
         <v>8833</v>
       </c>
-      <c r="G15" s="512" t="n">
+      <c r="G15" s="539" t="n">
         <v>20</v>
       </c>
       <c r="H15" s="130" t="n">
         <v>0</v>
       </c>
-      <c r="I15" s="511" t="n">
+      <c r="I15" s="538" t="n">
         <v>6</v>
       </c>
       <c r="J15" s="127" t="n">
         <v>9238</v>
       </c>
-      <c r="K15" s="511" t="n">
+      <c r="K15" s="538" t="n">
         <v>6</v>
       </c>
       <c r="L15" s="127" t="n">
         <v>7756</v>
       </c>
-      <c r="M15" s="511" t="n">
+      <c r="M15" s="538" t="n">
         <v>6</v>
       </c>
       <c r="N15" s="131" t="n">
         <v>5943</v>
       </c>
-      <c r="O15" s="511" t="n">
+      <c r="O15" s="538" t="n">
         <v>6</v>
       </c>
       <c r="P15" s="127" t="n">
@@ -2124,15 +2157,15 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="507" t="inlineStr">
+      <c r="A16" s="534" t="inlineStr">
         <is>
           <t>#82QLQCJRJ</t>
         </is>
       </c>
-      <c r="B16" s="507" t="n">
+      <c r="B16" s="534" t="n">
         <v>2919</v>
       </c>
-      <c r="C16" s="500" t="n">
+      <c r="C16" s="527" t="n">
         <v>13</v>
       </c>
       <c r="D16" s="133" t="inlineStr">
@@ -2140,37 +2173,37 @@
           <t>Raging Fury</t>
         </is>
       </c>
-      <c r="E16" s="508" t="n">
+      <c r="E16" s="535" t="n">
         <v>6</v>
       </c>
       <c r="F16" s="133" t="n">
         <v>8055</v>
       </c>
-      <c r="G16" s="513" t="n">
+      <c r="G16" s="540" t="n">
         <v>0</v>
       </c>
       <c r="H16" s="136" t="n">
         <v>0</v>
       </c>
-      <c r="I16" s="508" t="n">
+      <c r="I16" s="535" t="n">
         <v>6</v>
       </c>
       <c r="J16" s="133" t="n">
         <v>7115</v>
       </c>
-      <c r="K16" s="513" t="n">
+      <c r="K16" s="540" t="n">
         <v>2</v>
       </c>
       <c r="L16" s="148" t="n">
         <v>2320</v>
       </c>
-      <c r="M16" s="508" t="n">
+      <c r="M16" s="535" t="n">
         <v>6</v>
       </c>
       <c r="N16" s="139" t="n">
         <v>4920</v>
       </c>
-      <c r="O16" s="508" t="n">
+      <c r="O16" s="535" t="n">
         <v>6</v>
       </c>
       <c r="P16" s="139" t="n">
@@ -2178,15 +2211,15 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="503" t="inlineStr">
+      <c r="A17" s="530" t="inlineStr">
         <is>
           <t>#Q8CLCUCC2</t>
         </is>
       </c>
-      <c r="B17" s="503" t="n">
+      <c r="B17" s="530" t="n">
         <v>1327</v>
       </c>
-      <c r="C17" s="504" t="n">
+      <c r="C17" s="531" t="n">
         <v>14</v>
       </c>
       <c r="D17" s="122" t="inlineStr">
@@ -2194,37 +2227,37 @@
           <t>Moxxi</t>
         </is>
       </c>
-      <c r="E17" s="505" t="n">
+      <c r="E17" s="532" t="n">
         <v>6</v>
       </c>
       <c r="F17" s="122" t="n">
         <v>8015</v>
       </c>
-      <c r="G17" s="506" t="n">
+      <c r="G17" s="533" t="n">
         <v>0</v>
       </c>
       <c r="H17" s="125" t="n">
         <v>60</v>
       </c>
-      <c r="I17" s="505" t="n">
+      <c r="I17" s="532" t="n">
         <v>6</v>
       </c>
       <c r="J17" s="122" t="n">
         <v>11010</v>
       </c>
-      <c r="K17" s="505" t="n">
+      <c r="K17" s="532" t="n">
         <v>6</v>
       </c>
       <c r="L17" s="122" t="n">
         <v>13857</v>
       </c>
-      <c r="M17" s="505" t="n">
+      <c r="M17" s="532" t="n">
         <v>6</v>
       </c>
       <c r="N17" s="122" t="n">
         <v>7905</v>
       </c>
-      <c r="O17" s="505" t="n">
+      <c r="O17" s="532" t="n">
         <v>6</v>
       </c>
       <c r="P17" s="122" t="n">
@@ -2232,15 +2265,15 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="507" t="inlineStr">
+      <c r="A18" s="534" t="inlineStr">
         <is>
           <t>#QU0U2Q99G</t>
         </is>
       </c>
-      <c r="B18" s="507" t="n">
+      <c r="B18" s="534" t="n">
         <v>913</v>
       </c>
-      <c r="C18" s="500" t="n">
+      <c r="C18" s="527" t="n">
         <v>15</v>
       </c>
       <c r="D18" s="133" t="inlineStr">
@@ -2248,45 +2281,45 @@
           <t>big coc</t>
         </is>
       </c>
-      <c r="E18" s="508" t="n">
+      <c r="E18" s="535" t="n">
         <v>6</v>
       </c>
       <c r="F18" s="133" t="n">
         <v>7420</v>
       </c>
-      <c r="G18" s="513" t="n">
+      <c r="G18" s="540" t="n">
         <v>0</v>
       </c>
       <c r="H18" s="136" t="n">
         <v>40</v>
       </c>
-      <c r="I18" s="508" t="n">
+      <c r="I18" s="535" t="n">
         <v>5</v>
       </c>
       <c r="J18" s="139" t="n">
         <v>5150</v>
       </c>
-      <c r="K18" s="508" t="n">
+      <c r="K18" s="535" t="n">
         <v>6</v>
       </c>
       <c r="L18" s="133" t="n">
         <v>9075</v>
       </c>
-      <c r="M18" s="507" t="n"/>
+      <c r="M18" s="534" t="n"/>
       <c r="N18" s="136" t="n"/>
-      <c r="O18" s="507" t="n"/>
+      <c r="O18" s="534" t="n"/>
       <c r="P18" s="136" t="n"/>
     </row>
     <row r="19">
-      <c r="A19" s="510" t="inlineStr">
+      <c r="A19" s="537" t="inlineStr">
         <is>
           <t>#QRPRYR8LL</t>
         </is>
       </c>
-      <c r="B19" s="510" t="n">
+      <c r="B19" s="537" t="n">
         <v>1086</v>
       </c>
-      <c r="C19" s="504" t="n">
+      <c r="C19" s="531" t="n">
         <v>16</v>
       </c>
       <c r="D19" s="127" t="inlineStr">
@@ -2294,37 +2327,37 @@
           <t>FidelCashflow</t>
         </is>
       </c>
-      <c r="E19" s="511" t="n">
+      <c r="E19" s="538" t="n">
         <v>6</v>
       </c>
       <c r="F19" s="127" t="n">
         <v>6415</v>
       </c>
-      <c r="G19" s="512" t="n">
+      <c r="G19" s="539" t="n">
         <v>4</v>
       </c>
       <c r="H19" s="130" t="n">
         <v>0</v>
       </c>
-      <c r="I19" s="511" t="n">
+      <c r="I19" s="538" t="n">
         <v>6</v>
       </c>
       <c r="J19" s="127" t="n">
         <v>6547</v>
       </c>
-      <c r="K19" s="511" t="n">
+      <c r="K19" s="538" t="n">
         <v>6</v>
       </c>
       <c r="L19" s="127" t="n">
         <v>6811</v>
       </c>
-      <c r="M19" s="511" t="n">
+      <c r="M19" s="538" t="n">
         <v>6</v>
       </c>
       <c r="N19" s="131" t="n">
         <v>4239</v>
       </c>
-      <c r="O19" s="511" t="n">
+      <c r="O19" s="538" t="n">
         <v>6</v>
       </c>
       <c r="P19" s="131" t="n">
@@ -2332,15 +2365,15 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="507" t="inlineStr">
+      <c r="A20" s="534" t="inlineStr">
         <is>
           <t>#QY0VGPQGQ</t>
         </is>
       </c>
-      <c r="B20" s="507" t="n">
+      <c r="B20" s="534" t="n">
         <v>570</v>
       </c>
-      <c r="C20" s="500" t="n">
+      <c r="C20" s="527" t="n">
         <v>17</v>
       </c>
       <c r="D20" s="133" t="inlineStr">
@@ -2348,37 +2381,37 @@
           <t>killerjones</t>
         </is>
       </c>
-      <c r="E20" s="508" t="n">
+      <c r="E20" s="535" t="n">
         <v>6</v>
       </c>
       <c r="F20" s="133" t="n">
         <v>6320</v>
       </c>
-      <c r="G20" s="513" t="n">
+      <c r="G20" s="540" t="n">
         <v>0</v>
       </c>
       <c r="H20" s="136" t="n">
         <v>15</v>
       </c>
-      <c r="I20" s="507" t="n"/>
+      <c r="I20" s="534" t="n"/>
       <c r="J20" s="136" t="n"/>
-      <c r="K20" s="507" t="n"/>
+      <c r="K20" s="534" t="n"/>
       <c r="L20" s="136" t="n"/>
-      <c r="M20" s="507" t="n"/>
+      <c r="M20" s="534" t="n"/>
       <c r="N20" s="136" t="n"/>
-      <c r="O20" s="507" t="n"/>
+      <c r="O20" s="534" t="n"/>
       <c r="P20" s="136" t="n"/>
     </row>
     <row r="21">
-      <c r="A21" s="510" t="inlineStr">
+      <c r="A21" s="537" t="inlineStr">
         <is>
           <t>#LC9GUPJJG</t>
         </is>
       </c>
-      <c r="B21" s="510" t="n">
+      <c r="B21" s="537" t="n">
         <v>953</v>
       </c>
-      <c r="C21" s="504" t="n">
+      <c r="C21" s="531" t="n">
         <v>18</v>
       </c>
       <c r="D21" s="127" t="inlineStr">
@@ -2386,41 +2419,41 @@
           <t>raptor2222a</t>
         </is>
       </c>
-      <c r="E21" s="511" t="n">
+      <c r="E21" s="538" t="n">
         <v>5</v>
       </c>
       <c r="F21" s="131" t="n">
         <v>4350</v>
       </c>
-      <c r="G21" s="512" t="n">
+      <c r="G21" s="539" t="n">
         <v>0</v>
       </c>
       <c r="H21" s="130" t="n">
         <v>0</v>
       </c>
-      <c r="I21" s="512" t="n">
+      <c r="I21" s="539" t="n">
         <v>0</v>
       </c>
       <c r="J21" s="137" t="n">
         <v>0</v>
       </c>
-      <c r="K21" s="510" t="n"/>
+      <c r="K21" s="537" t="n"/>
       <c r="L21" s="130" t="n"/>
-      <c r="M21" s="510" t="n"/>
+      <c r="M21" s="537" t="n"/>
       <c r="N21" s="130" t="n"/>
-      <c r="O21" s="510" t="n"/>
+      <c r="O21" s="537" t="n"/>
       <c r="P21" s="130" t="n"/>
     </row>
     <row r="22">
-      <c r="A22" s="507" t="inlineStr">
+      <c r="A22" s="534" t="inlineStr">
         <is>
           <t>#QLG0VJG2J</t>
         </is>
       </c>
-      <c r="B22" s="507" t="n">
+      <c r="B22" s="534" t="n">
         <v>1092</v>
       </c>
-      <c r="C22" s="500" t="n">
+      <c r="C22" s="527" t="n">
         <v>19</v>
       </c>
       <c r="D22" s="139" t="inlineStr">
@@ -2428,41 +2461,41 @@
           <t>PocketRocket</t>
         </is>
       </c>
-      <c r="E22" s="509" t="n">
+      <c r="E22" s="536" t="n">
         <v>4</v>
       </c>
       <c r="F22" s="139" t="n">
         <v>4327</v>
       </c>
-      <c r="G22" s="513" t="n">
+      <c r="G22" s="540" t="n">
         <v>20</v>
       </c>
       <c r="H22" s="136" t="n">
         <v>0</v>
       </c>
-      <c r="I22" s="509" t="n">
+      <c r="I22" s="536" t="n">
         <v>4</v>
       </c>
       <c r="J22" s="139" t="n">
         <v>5215</v>
       </c>
-      <c r="K22" s="507" t="n"/>
+      <c r="K22" s="534" t="n"/>
       <c r="L22" s="136" t="n"/>
-      <c r="M22" s="507" t="n"/>
+      <c r="M22" s="534" t="n"/>
       <c r="N22" s="136" t="n"/>
-      <c r="O22" s="507" t="n"/>
+      <c r="O22" s="534" t="n"/>
       <c r="P22" s="136" t="n"/>
     </row>
     <row r="23">
-      <c r="A23" s="510" t="inlineStr">
+      <c r="A23" s="537" t="inlineStr">
         <is>
           <t>#QL8LVLYG8</t>
         </is>
       </c>
-      <c r="B23" s="510" t="n">
+      <c r="B23" s="537" t="n">
         <v>876</v>
       </c>
-      <c r="C23" s="504" t="n">
+      <c r="C23" s="531" t="n">
         <v>20</v>
       </c>
       <c r="D23" s="137" t="inlineStr">
@@ -2470,37 +2503,37 @@
           <t>Some guy</t>
         </is>
       </c>
-      <c r="E23" s="512" t="n">
+      <c r="E23" s="539" t="n">
         <v>2</v>
       </c>
       <c r="F23" s="137" t="n">
         <v>2650</v>
       </c>
-      <c r="G23" s="512" t="n">
+      <c r="G23" s="539" t="n">
         <v>0</v>
       </c>
       <c r="H23" s="130" t="n">
         <v>20</v>
       </c>
-      <c r="I23" s="512" t="n">
+      <c r="I23" s="539" t="n">
         <v>0</v>
       </c>
       <c r="J23" s="137" t="n">
         <v>0</v>
       </c>
-      <c r="K23" s="511" t="n">
+      <c r="K23" s="538" t="n">
         <v>6</v>
       </c>
       <c r="L23" s="127" t="n">
         <v>6917</v>
       </c>
-      <c r="M23" s="512" t="n">
+      <c r="M23" s="539" t="n">
         <v>0</v>
       </c>
       <c r="N23" s="137" t="n">
         <v>0</v>
       </c>
-      <c r="O23" s="512" t="n">
+      <c r="O23" s="539" t="n">
         <v>2</v>
       </c>
       <c r="P23" s="137" t="n">
@@ -2562,15 +2595,15 @@
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="510" t="inlineStr">
+      <c r="A25" s="537" t="inlineStr">
         <is>
           <t>#QV8JJ0URU</t>
         </is>
       </c>
-      <c r="B25" s="510" t="n">
+      <c r="B25" s="537" t="n">
         <v>741</v>
       </c>
-      <c r="C25" s="504" t="n">
+      <c r="C25" s="531" t="n">
         <v>22</v>
       </c>
       <c r="D25" s="137" t="inlineStr">
@@ -2578,37 +2611,37 @@
           <t>✨Jacob</t>
         </is>
       </c>
-      <c r="E25" s="512" t="n">
+      <c r="E25" s="539" t="n">
         <v>0</v>
       </c>
       <c r="F25" s="137" t="n">
         <v>0</v>
       </c>
-      <c r="G25" s="512" t="n">
+      <c r="G25" s="539" t="n">
         <v>0</v>
       </c>
       <c r="H25" s="130" t="n">
         <v>0</v>
       </c>
-      <c r="I25" s="512" t="n">
+      <c r="I25" s="539" t="n">
         <v>0</v>
       </c>
       <c r="J25" s="137" t="n">
         <v>0</v>
       </c>
-      <c r="K25" s="512" t="n">
+      <c r="K25" s="539" t="n">
         <v>0</v>
       </c>
       <c r="L25" s="137" t="n">
         <v>0</v>
       </c>
-      <c r="M25" s="511" t="n">
+      <c r="M25" s="538" t="n">
         <v>6</v>
       </c>
       <c r="N25" s="127" t="n">
         <v>7385</v>
       </c>
-      <c r="O25" s="511" t="n">
+      <c r="O25" s="538" t="n">
         <v>6</v>
       </c>
       <c r="P25" s="127" t="n">
@@ -2616,15 +2649,15 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="507" t="inlineStr">
+      <c r="A26" s="534" t="inlineStr">
         <is>
           <t>#QY8L2GLUR</t>
         </is>
       </c>
-      <c r="B26" s="507" t="n">
+      <c r="B26" s="534" t="n">
         <v>907</v>
       </c>
-      <c r="C26" s="500" t="n">
+      <c r="C26" s="527" t="n">
         <v>23</v>
       </c>
       <c r="D26" s="148" t="inlineStr">
@@ -2632,37 +2665,37 @@
           <t>Huy</t>
         </is>
       </c>
-      <c r="E26" s="513" t="n">
+      <c r="E26" s="540" t="n">
         <v>0</v>
       </c>
       <c r="F26" s="148" t="n">
         <v>0</v>
       </c>
-      <c r="G26" s="513" t="n">
+      <c r="G26" s="540" t="n">
         <v>0</v>
       </c>
       <c r="H26" s="136" t="n">
         <v>0</v>
       </c>
-      <c r="I26" s="513" t="n">
+      <c r="I26" s="540" t="n">
         <v>0</v>
       </c>
       <c r="J26" s="148" t="n">
         <v>0</v>
       </c>
-      <c r="K26" s="513" t="n">
+      <c r="K26" s="540" t="n">
         <v>0</v>
       </c>
       <c r="L26" s="148" t="n">
         <v>0</v>
       </c>
-      <c r="M26" s="508" t="n">
+      <c r="M26" s="535" t="n">
         <v>6</v>
       </c>
       <c r="N26" s="133" t="n">
         <v>6995</v>
       </c>
-      <c r="O26" s="508" t="n">
+      <c r="O26" s="535" t="n">
         <v>6</v>
       </c>
       <c r="P26" s="133" t="n">
@@ -2670,15 +2703,15 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="510" t="inlineStr">
+      <c r="A27" s="537" t="inlineStr">
         <is>
           <t>#L2QQL9QVJ</t>
         </is>
       </c>
-      <c r="B27" s="510" t="n">
+      <c r="B27" s="537" t="n">
         <v>1450</v>
       </c>
-      <c r="C27" s="504" t="n">
+      <c r="C27" s="531" t="n">
         <v>24</v>
       </c>
       <c r="D27" s="137" t="inlineStr">
@@ -2686,37 +2719,37 @@
           <t>JustPre10d</t>
         </is>
       </c>
-      <c r="E27" s="512" t="n">
+      <c r="E27" s="539" t="n">
         <v>0</v>
       </c>
       <c r="F27" s="137" t="n">
         <v>0</v>
       </c>
-      <c r="G27" s="512" t="n">
+      <c r="G27" s="539" t="n">
         <v>0</v>
       </c>
       <c r="H27" s="130" t="n">
         <v>0</v>
       </c>
-      <c r="I27" s="512" t="n">
+      <c r="I27" s="539" t="n">
         <v>0</v>
       </c>
       <c r="J27" s="137" t="n">
         <v>0</v>
       </c>
-      <c r="K27" s="512" t="n">
+      <c r="K27" s="539" t="n">
         <v>0</v>
       </c>
       <c r="L27" s="137" t="n">
         <v>0</v>
       </c>
-      <c r="M27" s="511" t="n">
+      <c r="M27" s="538" t="n">
         <v>6</v>
       </c>
       <c r="N27" s="127" t="n">
         <v>6655</v>
       </c>
-      <c r="O27" s="511" t="n">
+      <c r="O27" s="538" t="n">
         <v>6</v>
       </c>
       <c r="P27" s="127" t="n">
@@ -2724,15 +2757,15 @@
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="507" t="inlineStr">
+      <c r="A28" s="534" t="inlineStr">
         <is>
           <t>#LPR9RPCY9</t>
         </is>
       </c>
-      <c r="B28" s="507" t="n">
+      <c r="B28" s="534" t="n">
         <v>990</v>
       </c>
-      <c r="C28" s="500" t="n">
+      <c r="C28" s="527" t="n">
         <v>25</v>
       </c>
       <c r="D28" s="148" t="inlineStr">
@@ -2740,49 +2773,49 @@
           <t>sayhuss17</t>
         </is>
       </c>
-      <c r="E28" s="513" t="n">
+      <c r="E28" s="540" t="n">
         <v>0</v>
       </c>
       <c r="F28" s="148" t="n">
         <v>0</v>
       </c>
-      <c r="G28" s="513" t="n">
+      <c r="G28" s="540" t="n">
         <v>0</v>
       </c>
       <c r="H28" s="136" t="n">
         <v>0</v>
       </c>
-      <c r="I28" s="513" t="n">
+      <c r="I28" s="540" t="n">
         <v>0</v>
       </c>
       <c r="J28" s="148" t="n">
         <v>0</v>
       </c>
-      <c r="K28" s="513" t="n">
+      <c r="K28" s="540" t="n">
         <v>0</v>
       </c>
       <c r="L28" s="148" t="n">
         <v>0</v>
       </c>
-      <c r="M28" s="509" t="n">
+      <c r="M28" s="536" t="n">
         <v>4</v>
       </c>
       <c r="N28" s="139" t="n">
         <v>4240</v>
       </c>
-      <c r="O28" s="507" t="n"/>
+      <c r="O28" s="534" t="n"/>
       <c r="P28" s="136" t="n"/>
     </row>
     <row r="29">
-      <c r="A29" s="510" t="inlineStr">
+      <c r="A29" s="537" t="inlineStr">
         <is>
           <t>#QQL8C29CY</t>
         </is>
       </c>
-      <c r="B29" s="510" t="n">
+      <c r="B29" s="537" t="n">
         <v>891</v>
       </c>
-      <c r="C29" s="504" t="n">
+      <c r="C29" s="531" t="n">
         <v>26</v>
       </c>
       <c r="D29" s="137" t="inlineStr">
@@ -2790,37 +2823,37 @@
           <t>TypicalTeague#2</t>
         </is>
       </c>
-      <c r="E29" s="512" t="n">
+      <c r="E29" s="539" t="n">
         <v>0</v>
       </c>
       <c r="F29" s="137" t="n">
         <v>0</v>
       </c>
-      <c r="G29" s="512" t="n">
+      <c r="G29" s="539" t="n">
         <v>0</v>
       </c>
       <c r="H29" s="130" t="n">
         <v>0</v>
       </c>
-      <c r="I29" s="512" t="n">
+      <c r="I29" s="539" t="n">
         <v>0</v>
       </c>
       <c r="J29" s="137" t="n">
         <v>0</v>
       </c>
-      <c r="K29" s="512" t="n">
+      <c r="K29" s="539" t="n">
         <v>0</v>
       </c>
       <c r="L29" s="137" t="n">
         <v>0</v>
       </c>
-      <c r="M29" s="511" t="n">
+      <c r="M29" s="538" t="n">
         <v>5</v>
       </c>
       <c r="N29" s="131" t="n">
         <v>4070</v>
       </c>
-      <c r="O29" s="511" t="n">
+      <c r="O29" s="538" t="n">
         <v>6</v>
       </c>
       <c r="P29" s="127" t="n">
@@ -2828,15 +2861,15 @@
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="507" t="inlineStr">
+      <c r="A30" s="534" t="inlineStr">
         <is>
           <t>#PJYVV989R</t>
         </is>
       </c>
-      <c r="B30" s="507" t="n">
+      <c r="B30" s="534" t="n">
         <v>1584</v>
       </c>
-      <c r="C30" s="500" t="n">
+      <c r="C30" s="527" t="n">
         <v>27</v>
       </c>
       <c r="D30" s="148" t="inlineStr">
@@ -2844,49 +2877,49 @@
           <t>nx</t>
         </is>
       </c>
-      <c r="E30" s="513" t="n">
+      <c r="E30" s="540" t="n">
         <v>0</v>
       </c>
       <c r="F30" s="148" t="n">
         <v>0</v>
       </c>
-      <c r="G30" s="513" t="n">
+      <c r="G30" s="540" t="n">
         <v>0</v>
       </c>
       <c r="H30" s="136" t="n">
         <v>0</v>
       </c>
-      <c r="I30" s="513" t="n">
+      <c r="I30" s="540" t="n">
         <v>0</v>
       </c>
       <c r="J30" s="148" t="n">
         <v>0</v>
       </c>
-      <c r="K30" s="513" t="n">
+      <c r="K30" s="540" t="n">
         <v>0</v>
       </c>
       <c r="L30" s="148" t="n">
         <v>0</v>
       </c>
-      <c r="M30" s="513" t="n">
+      <c r="M30" s="540" t="n">
         <v>0</v>
       </c>
       <c r="N30" s="148" t="n">
         <v>0</v>
       </c>
-      <c r="O30" s="507" t="n"/>
+      <c r="O30" s="534" t="n"/>
       <c r="P30" s="136" t="n"/>
     </row>
     <row r="31">
-      <c r="A31" s="510" t="inlineStr">
+      <c r="A31" s="537" t="inlineStr">
         <is>
           <t>#L9JJQY992</t>
         </is>
       </c>
-      <c r="B31" s="510" t="n">
+      <c r="B31" s="537" t="n">
         <v>773</v>
       </c>
-      <c r="C31" s="504" t="n">
+      <c r="C31" s="531" t="n">
         <v>28</v>
       </c>
       <c r="D31" s="137" t="inlineStr">
@@ -2894,49 +2927,49 @@
           <t>Fisted_Waffle</t>
         </is>
       </c>
-      <c r="E31" s="512" t="n">
+      <c r="E31" s="539" t="n">
         <v>0</v>
       </c>
       <c r="F31" s="137" t="n">
         <v>0</v>
       </c>
-      <c r="G31" s="512" t="n">
+      <c r="G31" s="539" t="n">
         <v>0</v>
       </c>
       <c r="H31" s="130" t="n">
         <v>0</v>
       </c>
-      <c r="I31" s="512" t="n">
+      <c r="I31" s="539" t="n">
         <v>0</v>
       </c>
       <c r="J31" s="137" t="n">
         <v>0</v>
       </c>
-      <c r="K31" s="512" t="n">
+      <c r="K31" s="539" t="n">
         <v>0</v>
       </c>
       <c r="L31" s="137" t="n">
         <v>0</v>
       </c>
-      <c r="M31" s="512" t="n">
+      <c r="M31" s="539" t="n">
         <v>0</v>
       </c>
       <c r="N31" s="137" t="n">
         <v>0</v>
       </c>
-      <c r="O31" s="510" t="n"/>
+      <c r="O31" s="537" t="n"/>
       <c r="P31" s="130" t="n"/>
     </row>
     <row r="32">
-      <c r="A32" s="507" t="inlineStr">
+      <c r="A32" s="534" t="inlineStr">
         <is>
           <t>#L9QL9YQQY</t>
         </is>
       </c>
-      <c r="B32" s="507" t="n">
+      <c r="B32" s="534" t="n">
         <v>975</v>
       </c>
-      <c r="C32" s="500" t="n">
+      <c r="C32" s="527" t="n">
         <v>29</v>
       </c>
       <c r="D32" s="148" t="inlineStr">
@@ -2944,37 +2977,37 @@
           <t>Ima Chad</t>
         </is>
       </c>
-      <c r="E32" s="513" t="n">
+      <c r="E32" s="540" t="n">
         <v>0</v>
       </c>
       <c r="F32" s="148" t="n">
         <v>0</v>
       </c>
-      <c r="G32" s="513" t="n">
+      <c r="G32" s="540" t="n">
         <v>0</v>
       </c>
       <c r="H32" s="136" t="n">
         <v>0</v>
       </c>
-      <c r="I32" s="513" t="n">
+      <c r="I32" s="540" t="n">
         <v>0</v>
       </c>
       <c r="J32" s="148" t="n">
         <v>0</v>
       </c>
-      <c r="K32" s="513" t="n">
+      <c r="K32" s="540" t="n">
         <v>0</v>
       </c>
       <c r="L32" s="148" t="n">
         <v>0</v>
       </c>
-      <c r="M32" s="513" t="n">
+      <c r="M32" s="540" t="n">
         <v>0</v>
       </c>
       <c r="N32" s="148" t="n">
         <v>0</v>
       </c>
-      <c r="O32" s="508" t="n">
+      <c r="O32" s="535" t="n">
         <v>5</v>
       </c>
       <c r="P32" s="148" t="n">
@@ -3016,15 +3049,15 @@
       <c r="P33" s="235" t="n"/>
     </row>
     <row r="34">
-      <c r="A34" s="513" t="inlineStr">
+      <c r="A34" s="540" t="inlineStr">
         <is>
           <t>#Q0JG2RJQ8</t>
         </is>
       </c>
-      <c r="B34" s="507" t="n">
+      <c r="B34" s="534" t="n">
         <v>997</v>
       </c>
-      <c r="C34" s="500" t="n">
+      <c r="C34" s="527" t="n">
         <v>31</v>
       </c>
       <c r="D34" s="136" t="inlineStr">
@@ -3032,33 +3065,33 @@
           <t>bozo</t>
         </is>
       </c>
-      <c r="E34" s="507" t="n"/>
+      <c r="E34" s="534" t="n"/>
       <c r="F34" s="136" t="n"/>
-      <c r="G34" s="507" t="n"/>
+      <c r="G34" s="534" t="n"/>
       <c r="H34" s="136" t="n"/>
-      <c r="I34" s="507" t="n"/>
+      <c r="I34" s="534" t="n"/>
       <c r="J34" s="136" t="n"/>
-      <c r="K34" s="508" t="n">
+      <c r="K34" s="535" t="n">
         <v>6</v>
       </c>
       <c r="L34" s="133" t="n">
         <v>6495</v>
       </c>
-      <c r="M34" s="507" t="n"/>
+      <c r="M34" s="534" t="n"/>
       <c r="N34" s="136" t="n"/>
-      <c r="O34" s="507" t="n"/>
+      <c r="O34" s="534" t="n"/>
       <c r="P34" s="136" t="n"/>
     </row>
     <row r="35">
-      <c r="A35" s="512" t="inlineStr">
+      <c r="A35" s="539" t="inlineStr">
         <is>
           <t>#UVCCQC02</t>
         </is>
       </c>
-      <c r="B35" s="510" t="n">
+      <c r="B35" s="537" t="n">
         <v>1806</v>
       </c>
-      <c r="C35" s="504" t="n">
+      <c r="C35" s="531" t="n">
         <v>32</v>
       </c>
       <c r="D35" s="130" t="inlineStr">
@@ -3066,25 +3099,25 @@
           <t>lordshisha</t>
         </is>
       </c>
-      <c r="E35" s="510" t="n"/>
+      <c r="E35" s="537" t="n"/>
       <c r="F35" s="130" t="n"/>
-      <c r="G35" s="510" t="n"/>
+      <c r="G35" s="537" t="n"/>
       <c r="H35" s="130" t="n"/>
-      <c r="I35" s="510" t="n"/>
+      <c r="I35" s="537" t="n"/>
       <c r="J35" s="130" t="n"/>
-      <c r="K35" s="511" t="n">
+      <c r="K35" s="538" t="n">
         <v>6</v>
       </c>
       <c r="L35" s="127" t="n">
         <v>8496</v>
       </c>
-      <c r="M35" s="511" t="n">
+      <c r="M35" s="538" t="n">
         <v>6</v>
       </c>
       <c r="N35" s="127" t="n">
         <v>6310</v>
       </c>
-      <c r="O35" s="511" t="n">
+      <c r="O35" s="538" t="n">
         <v>6</v>
       </c>
       <c r="P35" s="127" t="n">
@@ -3092,15 +3125,15 @@
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="513" t="inlineStr">
+      <c r="A36" s="540" t="inlineStr">
         <is>
           <t>#P2CPRPQU</t>
         </is>
       </c>
-      <c r="B36" s="507" t="n">
+      <c r="B36" s="534" t="n">
         <v>2232</v>
       </c>
-      <c r="C36" s="500" t="n">
+      <c r="C36" s="527" t="n">
         <v>33</v>
       </c>
       <c r="D36" s="136" t="inlineStr">
@@ -3108,25 +3141,25 @@
           <t>The Drift King</t>
         </is>
       </c>
-      <c r="E36" s="507" t="n"/>
+      <c r="E36" s="534" t="n"/>
       <c r="F36" s="136" t="n"/>
-      <c r="G36" s="507" t="n"/>
+      <c r="G36" s="534" t="n"/>
       <c r="H36" s="136" t="n"/>
-      <c r="I36" s="507" t="n"/>
+      <c r="I36" s="534" t="n"/>
       <c r="J36" s="136" t="n"/>
-      <c r="K36" s="508" t="n">
+      <c r="K36" s="535" t="n">
         <v>6</v>
       </c>
       <c r="L36" s="133" t="n">
         <v>8023</v>
       </c>
-      <c r="M36" s="508" t="n">
+      <c r="M36" s="535" t="n">
         <v>6</v>
       </c>
       <c r="N36" s="133" t="n">
         <v>7625</v>
       </c>
-      <c r="O36" s="508" t="n">
+      <c r="O36" s="535" t="n">
         <v>6</v>
       </c>
       <c r="P36" s="133" t="n">
@@ -3134,15 +3167,15 @@
       </c>
     </row>
     <row r="37">
-      <c r="A37" s="512" t="inlineStr">
+      <c r="A37" s="539" t="inlineStr">
         <is>
           <t>#QJVL0LYQQ</t>
         </is>
       </c>
-      <c r="B37" s="510" t="n">
+      <c r="B37" s="537" t="n">
         <v>921</v>
       </c>
-      <c r="C37" s="504" t="n">
+      <c r="C37" s="531" t="n">
         <v>34</v>
       </c>
       <c r="D37" s="130" t="inlineStr">
@@ -3150,25 +3183,25 @@
           <t>mobbb341</t>
         </is>
       </c>
-      <c r="E37" s="510" t="n"/>
+      <c r="E37" s="537" t="n"/>
       <c r="F37" s="130" t="n"/>
-      <c r="G37" s="510" t="n"/>
+      <c r="G37" s="537" t="n"/>
       <c r="H37" s="130" t="n"/>
-      <c r="I37" s="510" t="n"/>
+      <c r="I37" s="537" t="n"/>
       <c r="J37" s="130" t="n"/>
-      <c r="K37" s="511" t="n">
+      <c r="K37" s="538" t="n">
         <v>6</v>
       </c>
       <c r="L37" s="127" t="n">
         <v>7710</v>
       </c>
-      <c r="M37" s="511" t="n">
+      <c r="M37" s="538" t="n">
         <v>6</v>
       </c>
       <c r="N37" s="127" t="n">
         <v>8810</v>
       </c>
-      <c r="O37" s="511" t="n">
+      <c r="O37" s="538" t="n">
         <v>6</v>
       </c>
       <c r="P37" s="131" t="n">
@@ -3176,15 +3209,15 @@
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="513" t="inlineStr">
+      <c r="A38" s="540" t="inlineStr">
         <is>
           <t>#L8R82C8VC</t>
         </is>
       </c>
-      <c r="B38" s="507" t="n">
+      <c r="B38" s="534" t="n">
         <v>1162</v>
       </c>
-      <c r="C38" s="500" t="n">
+      <c r="C38" s="527" t="n">
         <v>35</v>
       </c>
       <c r="D38" s="136" t="inlineStr">
@@ -3192,25 +3225,25 @@
           <t>caden asue</t>
         </is>
       </c>
-      <c r="E38" s="507" t="n"/>
+      <c r="E38" s="534" t="n"/>
       <c r="F38" s="136" t="n"/>
-      <c r="G38" s="507" t="n"/>
+      <c r="G38" s="534" t="n"/>
       <c r="H38" s="136" t="n"/>
-      <c r="I38" s="507" t="n"/>
+      <c r="I38" s="534" t="n"/>
       <c r="J38" s="136" t="n"/>
-      <c r="K38" s="508" t="n">
+      <c r="K38" s="535" t="n">
         <v>6</v>
       </c>
       <c r="L38" s="139" t="n">
         <v>5112</v>
       </c>
-      <c r="M38" s="508" t="n">
+      <c r="M38" s="535" t="n">
         <v>6</v>
       </c>
       <c r="N38" s="139" t="n">
         <v>4283</v>
       </c>
-      <c r="O38" s="508" t="n">
+      <c r="O38" s="535" t="n">
         <v>6</v>
       </c>
       <c r="P38" s="139" t="n">
@@ -3218,15 +3251,15 @@
       </c>
     </row>
     <row r="39">
-      <c r="A39" s="512" t="inlineStr">
+      <c r="A39" s="539" t="inlineStr">
         <is>
           <t>#L9Q8VLLQG</t>
         </is>
       </c>
-      <c r="B39" s="510" t="n">
+      <c r="B39" s="537" t="n">
         <v>1130</v>
       </c>
-      <c r="C39" s="504" t="n">
+      <c r="C39" s="531" t="n">
         <v>36</v>
       </c>
       <c r="D39" s="130" t="inlineStr">
@@ -3234,17 +3267,17 @@
           <t>cat</t>
         </is>
       </c>
-      <c r="E39" s="510" t="n"/>
+      <c r="E39" s="537" t="n"/>
       <c r="F39" s="130" t="n"/>
-      <c r="G39" s="510" t="n"/>
+      <c r="G39" s="537" t="n"/>
       <c r="H39" s="130" t="n"/>
-      <c r="I39" s="510" t="n"/>
+      <c r="I39" s="537" t="n"/>
       <c r="J39" s="130" t="n"/>
-      <c r="K39" s="510" t="n"/>
+      <c r="K39" s="537" t="n"/>
       <c r="L39" s="130" t="n"/>
-      <c r="M39" s="510" t="n"/>
+      <c r="M39" s="537" t="n"/>
       <c r="N39" s="130" t="n"/>
-      <c r="O39" s="511" t="n">
+      <c r="O39" s="538" t="n">
         <v>6</v>
       </c>
       <c r="P39" s="131" t="n">
@@ -3252,15 +3285,15 @@
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="513" t="inlineStr">
+      <c r="A40" s="540" t="inlineStr">
         <is>
           <t>#QV0PQC9JU</t>
         </is>
       </c>
-      <c r="B40" s="507" t="n">
+      <c r="B40" s="534" t="n">
         <v>539</v>
       </c>
-      <c r="C40" s="500" t="n">
+      <c r="C40" s="527" t="n">
         <v>37</v>
       </c>
       <c r="D40" s="136" t="inlineStr">
@@ -3268,17 +3301,17 @@
           <t>Superman</t>
         </is>
       </c>
-      <c r="E40" s="507" t="n"/>
+      <c r="E40" s="534" t="n"/>
       <c r="F40" s="136" t="n"/>
-      <c r="G40" s="507" t="n"/>
+      <c r="G40" s="534" t="n"/>
       <c r="H40" s="136" t="n"/>
-      <c r="I40" s="507" t="n"/>
+      <c r="I40" s="534" t="n"/>
       <c r="J40" s="136" t="n"/>
-      <c r="K40" s="507" t="n"/>
+      <c r="K40" s="534" t="n"/>
       <c r="L40" s="136" t="n"/>
-      <c r="M40" s="507" t="n"/>
+      <c r="M40" s="534" t="n"/>
       <c r="N40" s="136" t="n"/>
-      <c r="O40" s="508" t="n">
+      <c r="O40" s="535" t="n">
         <v>6</v>
       </c>
       <c r="P40" s="139" t="n">
@@ -3286,15 +3319,15 @@
       </c>
     </row>
     <row r="41">
-      <c r="A41" s="512" t="inlineStr">
+      <c r="A41" s="539" t="inlineStr">
         <is>
           <t>#LU0CRP09L</t>
         </is>
       </c>
-      <c r="B41" s="510" t="n">
+      <c r="B41" s="537" t="n">
         <v>809</v>
       </c>
-      <c r="C41" s="504" t="n">
+      <c r="C41" s="531" t="n">
         <v>38</v>
       </c>
       <c r="D41" s="130" t="inlineStr">
@@ -3302,17 +3335,17 @@
           <t>I Dont Know</t>
         </is>
       </c>
-      <c r="E41" s="510" t="n"/>
+      <c r="E41" s="537" t="n"/>
       <c r="F41" s="130" t="n"/>
-      <c r="G41" s="510" t="n"/>
+      <c r="G41" s="537" t="n"/>
       <c r="H41" s="130" t="n"/>
-      <c r="I41" s="510" t="n"/>
+      <c r="I41" s="537" t="n"/>
       <c r="J41" s="130" t="n"/>
-      <c r="K41" s="510" t="n"/>
+      <c r="K41" s="537" t="n"/>
       <c r="L41" s="130" t="n"/>
-      <c r="M41" s="510" t="n"/>
+      <c r="M41" s="537" t="n"/>
       <c r="N41" s="130" t="n"/>
-      <c r="O41" s="514" t="n">
+      <c r="O41" s="541" t="n">
         <v>3</v>
       </c>
       <c r="P41" s="137" t="n">
@@ -3320,15 +3353,15 @@
       </c>
     </row>
     <row r="42">
-      <c r="A42" s="513" t="inlineStr">
+      <c r="A42" s="540" t="inlineStr">
         <is>
           <t>#YCPP0QPP8</t>
         </is>
       </c>
-      <c r="B42" s="507" t="n">
+      <c r="B42" s="534" t="n">
         <v>3327</v>
       </c>
-      <c r="C42" s="500" t="n">
+      <c r="C42" s="527" t="n">
         <v>39</v>
       </c>
       <c r="D42" s="136" t="inlineStr">
@@ -3336,17 +3369,17 @@
           <t>Coach</t>
         </is>
       </c>
-      <c r="E42" s="507" t="n"/>
+      <c r="E42" s="534" t="n"/>
       <c r="F42" s="136" t="n"/>
-      <c r="G42" s="507" t="n"/>
+      <c r="G42" s="534" t="n"/>
       <c r="H42" s="136" t="n"/>
-      <c r="I42" s="507" t="n"/>
+      <c r="I42" s="534" t="n"/>
       <c r="J42" s="136" t="n"/>
-      <c r="K42" s="507" t="n"/>
+      <c r="K42" s="534" t="n"/>
       <c r="L42" s="136" t="n"/>
-      <c r="M42" s="507" t="n"/>
+      <c r="M42" s="534" t="n"/>
       <c r="N42" s="136" t="n"/>
-      <c r="O42" s="513" t="n">
+      <c r="O42" s="540" t="n">
         <v>0</v>
       </c>
       <c r="P42" s="148" t="n">
@@ -3466,259 +3499,259 @@
       </c>
     </row>
     <row r="4">
-      <c r="B4" s="488" t="inlineStr">
+      <c r="B4" s="515" t="inlineStr">
         <is>
           <t>#QUYG0PQC8</t>
         </is>
       </c>
-      <c r="C4" s="488" t="n">
+      <c r="C4" s="515" t="n">
         <v>1</v>
       </c>
-      <c r="D4" s="489" t="inlineStr">
+      <c r="D4" s="516" t="inlineStr">
         <is>
           <t>Luffy</t>
         </is>
       </c>
-      <c r="E4" s="489" t="n">
+      <c r="E4" s="516" t="n">
         <v>2</v>
       </c>
       <c r="F4" s="116" t="n">
         <v>6</v>
       </c>
-      <c r="G4" s="488" t="n"/>
+      <c r="G4" s="515" t="n"/>
       <c r="H4" s="119" t="n"/>
-      <c r="I4" s="488" t="n"/>
+      <c r="I4" s="515" t="n"/>
       <c r="J4" s="119" t="n"/>
-      <c r="K4" s="488" t="n"/>
+      <c r="K4" s="515" t="n"/>
       <c r="L4" s="119" t="n"/>
     </row>
     <row r="5">
-      <c r="B5" s="490" t="inlineStr">
+      <c r="B5" s="517" t="inlineStr">
         <is>
           <t>#G0QPVJY9L</t>
         </is>
       </c>
-      <c r="C5" s="490" t="n">
+      <c r="C5" s="517" t="n">
         <v>2</v>
       </c>
-      <c r="D5" s="491" t="inlineStr">
+      <c r="D5" s="518" t="inlineStr">
         <is>
           <t>Zoro</t>
         </is>
       </c>
-      <c r="E5" s="491" t="n">
+      <c r="E5" s="518" t="n">
         <v>2</v>
       </c>
       <c r="F5" s="122" t="n">
         <v>6</v>
       </c>
-      <c r="G5" s="490" t="n"/>
+      <c r="G5" s="517" t="n"/>
       <c r="H5" s="125" t="n"/>
-      <c r="I5" s="490" t="n"/>
+      <c r="I5" s="517" t="n"/>
       <c r="J5" s="125" t="n"/>
-      <c r="K5" s="490" t="n"/>
+      <c r="K5" s="517" t="n"/>
       <c r="L5" s="125" t="n"/>
     </row>
     <row r="6">
-      <c r="B6" s="488" t="inlineStr">
+      <c r="B6" s="515" t="inlineStr">
         <is>
           <t>#QLR088LC9</t>
         </is>
       </c>
-      <c r="C6" s="488" t="n">
+      <c r="C6" s="515" t="n">
         <v>3</v>
       </c>
-      <c r="D6" s="489" t="inlineStr">
+      <c r="D6" s="516" t="inlineStr">
         <is>
           <t>Sanji</t>
         </is>
       </c>
-      <c r="E6" s="489" t="n">
+      <c r="E6" s="516" t="n">
         <v>2</v>
       </c>
       <c r="F6" s="116" t="n">
         <v>6</v>
       </c>
-      <c r="G6" s="488" t="n"/>
+      <c r="G6" s="515" t="n"/>
       <c r="H6" s="119" t="n"/>
-      <c r="I6" s="488" t="n"/>
+      <c r="I6" s="515" t="n"/>
       <c r="J6" s="119" t="n"/>
-      <c r="K6" s="488" t="n"/>
+      <c r="K6" s="515" t="n"/>
       <c r="L6" s="119" t="n"/>
     </row>
     <row r="7">
-      <c r="B7" s="490" t="inlineStr">
+      <c r="B7" s="517" t="inlineStr">
         <is>
           <t>#QCV22VP0G</t>
         </is>
       </c>
-      <c r="C7" s="490" t="n">
+      <c r="C7" s="517" t="n">
         <v>4</v>
       </c>
-      <c r="D7" s="491" t="inlineStr">
+      <c r="D7" s="518" t="inlineStr">
         <is>
           <t>Nami</t>
         </is>
       </c>
-      <c r="E7" s="491" t="n">
+      <c r="E7" s="518" t="n">
         <v>2</v>
       </c>
       <c r="F7" s="122" t="n">
         <v>6</v>
       </c>
-      <c r="G7" s="490" t="n"/>
+      <c r="G7" s="517" t="n"/>
       <c r="H7" s="125" t="n"/>
-      <c r="I7" s="490" t="n"/>
+      <c r="I7" s="517" t="n"/>
       <c r="J7" s="125" t="n"/>
-      <c r="K7" s="490" t="n"/>
+      <c r="K7" s="517" t="n"/>
       <c r="L7" s="125" t="n"/>
     </row>
     <row r="8">
-      <c r="B8" s="488" t="inlineStr">
+      <c r="B8" s="515" t="inlineStr">
         <is>
           <t>#QUV2GP88U</t>
         </is>
       </c>
-      <c r="C8" s="488" t="n">
+      <c r="C8" s="515" t="n">
         <v>5</v>
       </c>
-      <c r="D8" s="489" t="inlineStr">
+      <c r="D8" s="516" t="inlineStr">
         <is>
           <t>Nico Robin</t>
         </is>
       </c>
-      <c r="E8" s="489" t="n">
+      <c r="E8" s="516" t="n">
         <v>2</v>
       </c>
       <c r="F8" s="116" t="n">
         <v>6</v>
       </c>
-      <c r="G8" s="488" t="n"/>
+      <c r="G8" s="515" t="n"/>
       <c r="H8" s="119" t="n"/>
-      <c r="I8" s="488" t="n"/>
+      <c r="I8" s="515" t="n"/>
       <c r="J8" s="119" t="n"/>
-      <c r="K8" s="488" t="n"/>
+      <c r="K8" s="515" t="n"/>
       <c r="L8" s="119" t="n"/>
     </row>
     <row r="9">
-      <c r="B9" s="492" t="inlineStr">
+      <c r="B9" s="519" t="inlineStr">
         <is>
           <t>#98JG2UJQL</t>
         </is>
       </c>
-      <c r="C9" s="492" t="n"/>
-      <c r="D9" s="492" t="inlineStr">
+      <c r="C9" s="519" t="n"/>
+      <c r="D9" s="519" t="inlineStr">
         <is>
           <t>Dragonux</t>
         </is>
       </c>
-      <c r="E9" s="492" t="n"/>
+      <c r="E9" s="519" t="n"/>
       <c r="F9" s="130" t="n"/>
-      <c r="G9" s="492" t="n"/>
+      <c r="G9" s="519" t="n"/>
       <c r="H9" s="130" t="n"/>
-      <c r="I9" s="492" t="n"/>
+      <c r="I9" s="519" t="n"/>
       <c r="J9" s="130" t="n"/>
-      <c r="K9" s="492" t="n"/>
+      <c r="K9" s="519" t="n"/>
       <c r="L9" s="130" t="n"/>
     </row>
     <row r="10">
-      <c r="B10" s="493" t="inlineStr">
+      <c r="B10" s="520" t="inlineStr">
         <is>
           <t>#82QLQCJRJ</t>
         </is>
       </c>
-      <c r="C10" s="493" t="n"/>
-      <c r="D10" s="493" t="inlineStr">
+      <c r="C10" s="520" t="n"/>
+      <c r="D10" s="520" t="inlineStr">
         <is>
           <t>Raging Fury</t>
         </is>
       </c>
-      <c r="E10" s="493" t="n"/>
+      <c r="E10" s="520" t="n"/>
       <c r="F10" s="136" t="n"/>
-      <c r="G10" s="493" t="n"/>
+      <c r="G10" s="520" t="n"/>
       <c r="H10" s="136" t="n"/>
-      <c r="I10" s="493" t="n"/>
+      <c r="I10" s="520" t="n"/>
       <c r="J10" s="136" t="n"/>
-      <c r="K10" s="493" t="n"/>
+      <c r="K10" s="520" t="n"/>
       <c r="L10" s="136" t="n"/>
     </row>
     <row r="11">
-      <c r="B11" s="490" t="inlineStr">
+      <c r="B11" s="517" t="inlineStr">
         <is>
           <t>#90U0VPU9U</t>
         </is>
       </c>
-      <c r="C11" s="490" t="n"/>
-      <c r="D11" s="490" t="inlineStr">
+      <c r="C11" s="517" t="n"/>
+      <c r="D11" s="517" t="inlineStr">
         <is>
           <t>KYANI7E</t>
         </is>
       </c>
-      <c r="E11" s="490" t="n"/>
+      <c r="E11" s="517" t="n"/>
       <c r="F11" s="125" t="n"/>
-      <c r="G11" s="490" t="n"/>
+      <c r="G11" s="517" t="n"/>
       <c r="H11" s="125" t="n"/>
-      <c r="I11" s="490" t="n"/>
+      <c r="I11" s="517" t="n"/>
       <c r="J11" s="125" t="n"/>
-      <c r="K11" s="490" t="n"/>
+      <c r="K11" s="517" t="n"/>
       <c r="L11" s="125" t="n"/>
     </row>
     <row r="12">
-      <c r="B12" s="493" t="inlineStr">
+      <c r="B12" s="520" t="inlineStr">
         <is>
           <t>#PJYVV989R</t>
         </is>
       </c>
-      <c r="C12" s="493" t="n"/>
-      <c r="D12" s="493" t="inlineStr">
+      <c r="C12" s="520" t="n"/>
+      <c r="D12" s="520" t="inlineStr">
         <is>
           <t>nx</t>
         </is>
       </c>
-      <c r="E12" s="493" t="n"/>
+      <c r="E12" s="520" t="n"/>
       <c r="F12" s="136" t="n"/>
-      <c r="G12" s="494" t="n">
+      <c r="G12" s="521" t="n">
         <v>1</v>
       </c>
       <c r="H12" s="139" t="n">
         <v>3</v>
       </c>
-      <c r="I12" s="494" t="n">
+      <c r="I12" s="521" t="n">
         <v>1</v>
       </c>
       <c r="J12" s="139" t="n">
         <v>3</v>
       </c>
-      <c r="K12" s="493" t="n"/>
+      <c r="K12" s="520" t="n"/>
       <c r="L12" s="136" t="n"/>
     </row>
     <row r="13">
-      <c r="B13" s="490" t="inlineStr">
+      <c r="B13" s="517" t="inlineStr">
         <is>
           <t>#QLJ2U20Y2</t>
         </is>
       </c>
-      <c r="C13" s="490" t="n"/>
-      <c r="D13" s="490" t="inlineStr">
+      <c r="C13" s="517" t="n"/>
+      <c r="D13" s="517" t="inlineStr">
         <is>
           <t>DeadLeaf</t>
         </is>
       </c>
-      <c r="E13" s="490" t="n"/>
+      <c r="E13" s="517" t="n"/>
       <c r="F13" s="125" t="n"/>
-      <c r="G13" s="491" t="n">
+      <c r="G13" s="518" t="n">
         <v>2</v>
       </c>
       <c r="H13" s="122" t="n">
         <v>5</v>
       </c>
-      <c r="I13" s="491" t="n">
+      <c r="I13" s="518" t="n">
         <v>2</v>
       </c>
       <c r="J13" s="122" t="n">
         <v>5</v>
       </c>
-      <c r="K13" s="491" t="n">
+      <c r="K13" s="518" t="n">
         <v>2</v>
       </c>
       <c r="L13" s="122" t="n">
@@ -3726,28 +3759,28 @@
       </c>
     </row>
     <row r="14">
-      <c r="B14" s="493" t="inlineStr">
+      <c r="B14" s="520" t="inlineStr">
         <is>
           <t>#L2QQL9QVJ</t>
         </is>
       </c>
-      <c r="C14" s="493" t="n"/>
-      <c r="D14" s="493" t="inlineStr">
+      <c r="C14" s="520" t="n"/>
+      <c r="D14" s="520" t="inlineStr">
         <is>
           <t>JustPre10d</t>
         </is>
       </c>
-      <c r="E14" s="493" t="n"/>
+      <c r="E14" s="520" t="n"/>
       <c r="F14" s="136" t="n"/>
-      <c r="G14" s="493" t="n"/>
+      <c r="G14" s="520" t="n"/>
       <c r="H14" s="136" t="n"/>
-      <c r="I14" s="495" t="n">
+      <c r="I14" s="522" t="n">
         <v>0</v>
       </c>
       <c r="J14" s="148" t="n">
         <v>0</v>
       </c>
-      <c r="K14" s="494" t="n">
+      <c r="K14" s="521" t="n">
         <v>1</v>
       </c>
       <c r="L14" s="148" t="n">
@@ -3755,32 +3788,32 @@
       </c>
     </row>
     <row r="15">
-      <c r="B15" s="490" t="inlineStr">
+      <c r="B15" s="517" t="inlineStr">
         <is>
           <t>#YJ20CRJYQ</t>
         </is>
       </c>
-      <c r="C15" s="490" t="n"/>
-      <c r="D15" s="490" t="inlineStr">
+      <c r="C15" s="517" t="n"/>
+      <c r="D15" s="517" t="inlineStr">
         <is>
           <t>UnluckGod</t>
         </is>
       </c>
-      <c r="E15" s="490" t="n"/>
+      <c r="E15" s="517" t="n"/>
       <c r="F15" s="125" t="n"/>
-      <c r="G15" s="491" t="n">
+      <c r="G15" s="518" t="n">
         <v>2</v>
       </c>
       <c r="H15" s="122" t="n">
         <v>6</v>
       </c>
-      <c r="I15" s="491" t="n">
+      <c r="I15" s="518" t="n">
         <v>2</v>
       </c>
       <c r="J15" s="122" t="n">
         <v>4</v>
       </c>
-      <c r="K15" s="491" t="n">
+      <c r="K15" s="518" t="n">
         <v>2</v>
       </c>
       <c r="L15" s="122" t="n">
@@ -3788,61 +3821,61 @@
       </c>
     </row>
     <row r="16">
-      <c r="B16" s="488" t="inlineStr">
+      <c r="B16" s="515" t="inlineStr">
         <is>
           <t>#YRGRRJQCY</t>
         </is>
       </c>
-      <c r="C16" s="488" t="n"/>
-      <c r="D16" s="488" t="inlineStr">
+      <c r="C16" s="515" t="n"/>
+      <c r="D16" s="515" t="inlineStr">
         <is>
           <t>DoubleSpice</t>
         </is>
       </c>
-      <c r="E16" s="488" t="n"/>
+      <c r="E16" s="515" t="n"/>
       <c r="F16" s="119" t="n"/>
-      <c r="G16" s="489" t="n">
+      <c r="G16" s="516" t="n">
         <v>2</v>
       </c>
       <c r="H16" s="116" t="n">
         <v>5</v>
       </c>
-      <c r="I16" s="489" t="n">
+      <c r="I16" s="516" t="n">
         <v>2</v>
       </c>
       <c r="J16" s="116" t="n">
         <v>6</v>
       </c>
-      <c r="K16" s="488" t="n"/>
+      <c r="K16" s="515" t="n"/>
       <c r="L16" s="119" t="n"/>
     </row>
     <row r="17">
-      <c r="B17" s="490" t="inlineStr">
+      <c r="B17" s="517" t="inlineStr">
         <is>
           <t>#Q8CLCUCC2</t>
         </is>
       </c>
-      <c r="C17" s="490" t="n"/>
-      <c r="D17" s="490" t="inlineStr">
+      <c r="C17" s="517" t="n"/>
+      <c r="D17" s="517" t="inlineStr">
         <is>
           <t>Moxxi</t>
         </is>
       </c>
-      <c r="E17" s="490" t="n"/>
+      <c r="E17" s="517" t="n"/>
       <c r="F17" s="125" t="n"/>
-      <c r="G17" s="491" t="n">
+      <c r="G17" s="518" t="n">
         <v>2</v>
       </c>
       <c r="H17" s="122" t="n">
         <v>6</v>
       </c>
-      <c r="I17" s="491" t="n">
+      <c r="I17" s="518" t="n">
         <v>2</v>
       </c>
       <c r="J17" s="122" t="n">
         <v>5</v>
       </c>
-      <c r="K17" s="491" t="n">
+      <c r="K17" s="518" t="n">
         <v>2</v>
       </c>
       <c r="L17" s="122" t="n">
@@ -3850,396 +3883,396 @@
       </c>
     </row>
     <row r="18">
-      <c r="B18" s="493" t="inlineStr">
+      <c r="B18" s="520" t="inlineStr">
         <is>
           <t>#G0JPUQGYR</t>
         </is>
       </c>
-      <c r="C18" s="493" t="n"/>
-      <c r="D18" s="493" t="inlineStr">
+      <c r="C18" s="520" t="n"/>
+      <c r="D18" s="520" t="inlineStr">
         <is>
           <t>Collin</t>
         </is>
       </c>
-      <c r="E18" s="493" t="n"/>
+      <c r="E18" s="520" t="n"/>
       <c r="F18" s="136" t="n"/>
-      <c r="G18" s="493" t="n"/>
+      <c r="G18" s="520" t="n"/>
       <c r="H18" s="136" t="n"/>
-      <c r="I18" s="493" t="n"/>
+      <c r="I18" s="520" t="n"/>
       <c r="J18" s="136" t="n"/>
-      <c r="K18" s="493" t="n"/>
+      <c r="K18" s="520" t="n"/>
       <c r="L18" s="136" t="n"/>
     </row>
     <row r="19">
-      <c r="B19" s="492" t="inlineStr">
+      <c r="B19" s="519" t="inlineStr">
         <is>
           <t>#QLG0VJG2J</t>
         </is>
       </c>
-      <c r="C19" s="492" t="n"/>
-      <c r="D19" s="492" t="inlineStr">
+      <c r="C19" s="519" t="n"/>
+      <c r="D19" s="519" t="inlineStr">
         <is>
           <t>PocketRocket</t>
         </is>
       </c>
-      <c r="E19" s="492" t="n"/>
+      <c r="E19" s="519" t="n"/>
       <c r="F19" s="130" t="n"/>
-      <c r="G19" s="492" t="n"/>
+      <c r="G19" s="519" t="n"/>
       <c r="H19" s="130" t="n"/>
-      <c r="I19" s="492" t="n"/>
+      <c r="I19" s="519" t="n"/>
       <c r="J19" s="130" t="n"/>
-      <c r="K19" s="492" t="n"/>
+      <c r="K19" s="519" t="n"/>
       <c r="L19" s="130" t="n"/>
     </row>
     <row r="20">
-      <c r="B20" s="493" t="inlineStr">
+      <c r="B20" s="520" t="inlineStr">
         <is>
           <t>#QRPRYR8LL</t>
         </is>
       </c>
-      <c r="C20" s="493" t="n"/>
-      <c r="D20" s="493" t="inlineStr">
+      <c r="C20" s="520" t="n"/>
+      <c r="D20" s="520" t="inlineStr">
         <is>
           <t>FidelCashflow</t>
         </is>
       </c>
-      <c r="E20" s="493" t="n"/>
+      <c r="E20" s="520" t="n"/>
       <c r="F20" s="136" t="n"/>
-      <c r="G20" s="493" t="n"/>
+      <c r="G20" s="520" t="n"/>
       <c r="H20" s="136" t="n"/>
-      <c r="I20" s="493" t="n"/>
+      <c r="I20" s="520" t="n"/>
       <c r="J20" s="136" t="n"/>
-      <c r="K20" s="493" t="n"/>
+      <c r="K20" s="520" t="n"/>
       <c r="L20" s="136" t="n"/>
     </row>
     <row r="21">
-      <c r="B21" s="492" t="inlineStr">
+      <c r="B21" s="519" t="inlineStr">
         <is>
           <t>#QJC8LQU9U</t>
         </is>
       </c>
-      <c r="C21" s="492" t="n"/>
-      <c r="D21" s="492" t="inlineStr">
+      <c r="C21" s="519" t="n"/>
+      <c r="D21" s="519" t="inlineStr">
         <is>
           <t>Master01</t>
         </is>
       </c>
-      <c r="E21" s="492" t="n"/>
+      <c r="E21" s="519" t="n"/>
       <c r="F21" s="130" t="n"/>
-      <c r="G21" s="496" t="n">
+      <c r="G21" s="523" t="n">
         <v>2</v>
       </c>
       <c r="H21" s="127" t="n">
         <v>4</v>
       </c>
-      <c r="I21" s="492" t="n"/>
+      <c r="I21" s="519" t="n"/>
       <c r="J21" s="130" t="n"/>
-      <c r="K21" s="492" t="n"/>
+      <c r="K21" s="519" t="n"/>
       <c r="L21" s="130" t="n"/>
     </row>
     <row r="22">
-      <c r="B22" s="493" t="inlineStr">
+      <c r="B22" s="520" t="inlineStr">
         <is>
           <t>#LPR9RPCY9</t>
         </is>
       </c>
-      <c r="C22" s="493" t="n"/>
-      <c r="D22" s="493" t="inlineStr">
+      <c r="C22" s="520" t="n"/>
+      <c r="D22" s="520" t="inlineStr">
         <is>
           <t>sayhuss17</t>
         </is>
       </c>
-      <c r="E22" s="493" t="n"/>
+      <c r="E22" s="520" t="n"/>
       <c r="F22" s="136" t="n"/>
-      <c r="G22" s="495" t="n">
+      <c r="G22" s="522" t="n">
         <v>0</v>
       </c>
       <c r="H22" s="148" t="n">
         <v>0</v>
       </c>
-      <c r="I22" s="495" t="n">
+      <c r="I22" s="522" t="n">
         <v>0</v>
       </c>
       <c r="J22" s="148" t="n">
         <v>0</v>
       </c>
-      <c r="K22" s="493" t="n"/>
+      <c r="K22" s="520" t="n"/>
       <c r="L22" s="136" t="n"/>
     </row>
     <row r="23">
-      <c r="B23" s="492" t="inlineStr">
+      <c r="B23" s="519" t="inlineStr">
         <is>
           <t>#L9QL9YQQY</t>
         </is>
       </c>
-      <c r="C23" s="492" t="n"/>
-      <c r="D23" s="492" t="inlineStr">
+      <c r="C23" s="519" t="n"/>
+      <c r="D23" s="519" t="inlineStr">
         <is>
           <t>Ima Chad</t>
         </is>
       </c>
-      <c r="E23" s="492" t="n"/>
+      <c r="E23" s="519" t="n"/>
       <c r="F23" s="130" t="n"/>
-      <c r="G23" s="492" t="n"/>
+      <c r="G23" s="519" t="n"/>
       <c r="H23" s="130" t="n"/>
-      <c r="I23" s="492" t="n"/>
+      <c r="I23" s="519" t="n"/>
       <c r="J23" s="130" t="n"/>
-      <c r="K23" s="492" t="n"/>
+      <c r="K23" s="519" t="n"/>
       <c r="L23" s="130" t="n"/>
     </row>
     <row r="24">
-      <c r="B24" s="493" t="inlineStr">
+      <c r="B24" s="520" t="inlineStr">
         <is>
           <t>#LC9GUPJJG</t>
         </is>
       </c>
-      <c r="C24" s="493" t="n"/>
-      <c r="D24" s="493" t="inlineStr">
+      <c r="C24" s="520" t="n"/>
+      <c r="D24" s="520" t="inlineStr">
         <is>
           <t>raptor2222a</t>
         </is>
       </c>
-      <c r="E24" s="493" t="n"/>
+      <c r="E24" s="520" t="n"/>
       <c r="F24" s="136" t="n"/>
-      <c r="G24" s="493" t="n"/>
+      <c r="G24" s="520" t="n"/>
       <c r="H24" s="136" t="n"/>
-      <c r="I24" s="493" t="n"/>
+      <c r="I24" s="520" t="n"/>
       <c r="J24" s="136" t="n"/>
-      <c r="K24" s="493" t="n"/>
+      <c r="K24" s="520" t="n"/>
       <c r="L24" s="136" t="n"/>
     </row>
     <row r="25">
-      <c r="B25" s="490" t="inlineStr">
+      <c r="B25" s="517" t="inlineStr">
         <is>
           <t>#QUG8QQJ92</t>
         </is>
       </c>
-      <c r="C25" s="490" t="n"/>
-      <c r="D25" s="490" t="inlineStr">
+      <c r="C25" s="517" t="n"/>
+      <c r="D25" s="517" t="inlineStr">
         <is>
           <t>Karma</t>
         </is>
       </c>
-      <c r="E25" s="490" t="n"/>
+      <c r="E25" s="517" t="n"/>
       <c r="F25" s="125" t="n"/>
-      <c r="G25" s="490" t="n"/>
+      <c r="G25" s="517" t="n"/>
       <c r="H25" s="125" t="n"/>
-      <c r="I25" s="490" t="n"/>
+      <c r="I25" s="517" t="n"/>
       <c r="J25" s="125" t="n"/>
-      <c r="K25" s="490" t="n"/>
+      <c r="K25" s="517" t="n"/>
       <c r="L25" s="125" t="n"/>
     </row>
     <row r="26">
-      <c r="B26" s="493" t="inlineStr">
+      <c r="B26" s="520" t="inlineStr">
         <is>
           <t>#QU0U2Q99G</t>
         </is>
       </c>
-      <c r="C26" s="493" t="n"/>
-      <c r="D26" s="493" t="inlineStr">
+      <c r="C26" s="520" t="n"/>
+      <c r="D26" s="520" t="inlineStr">
         <is>
           <t>big coc</t>
         </is>
       </c>
-      <c r="E26" s="493" t="n"/>
+      <c r="E26" s="520" t="n"/>
       <c r="F26" s="136" t="n"/>
-      <c r="G26" s="493" t="n"/>
+      <c r="G26" s="520" t="n"/>
       <c r="H26" s="136" t="n"/>
-      <c r="I26" s="493" t="n"/>
+      <c r="I26" s="520" t="n"/>
       <c r="J26" s="136" t="n"/>
-      <c r="K26" s="493" t="n"/>
+      <c r="K26" s="520" t="n"/>
       <c r="L26" s="136" t="n"/>
     </row>
     <row r="27">
-      <c r="B27" s="492" t="inlineStr">
+      <c r="B27" s="519" t="inlineStr">
         <is>
           <t>#QY8L2GLUR</t>
         </is>
       </c>
-      <c r="C27" s="492" t="n"/>
-      <c r="D27" s="492" t="inlineStr">
+      <c r="C27" s="519" t="n"/>
+      <c r="D27" s="519" t="inlineStr">
         <is>
           <t>Huy</t>
         </is>
       </c>
-      <c r="E27" s="492" t="n"/>
+      <c r="E27" s="519" t="n"/>
       <c r="F27" s="130" t="n"/>
-      <c r="G27" s="497" t="n">
+      <c r="G27" s="524" t="n">
         <v>0</v>
       </c>
       <c r="H27" s="137" t="n">
         <v>0</v>
       </c>
-      <c r="I27" s="492" t="n"/>
+      <c r="I27" s="519" t="n"/>
       <c r="J27" s="130" t="n"/>
-      <c r="K27" s="492" t="n"/>
+      <c r="K27" s="519" t="n"/>
       <c r="L27" s="130" t="n"/>
     </row>
     <row r="28">
-      <c r="B28" s="493" t="inlineStr">
+      <c r="B28" s="520" t="inlineStr">
         <is>
           <t>#QQL8C29CY</t>
         </is>
       </c>
-      <c r="C28" s="493" t="n"/>
-      <c r="D28" s="493" t="inlineStr">
+      <c r="C28" s="520" t="n"/>
+      <c r="D28" s="520" t="inlineStr">
         <is>
           <t>TypicalTeague#2</t>
         </is>
       </c>
-      <c r="E28" s="493" t="n"/>
+      <c r="E28" s="520" t="n"/>
       <c r="F28" s="136" t="n"/>
-      <c r="G28" s="493" t="n"/>
+      <c r="G28" s="520" t="n"/>
       <c r="H28" s="136" t="n"/>
-      <c r="I28" s="493" t="n"/>
+      <c r="I28" s="520" t="n"/>
       <c r="J28" s="136" t="n"/>
-      <c r="K28" s="493" t="n"/>
+      <c r="K28" s="520" t="n"/>
       <c r="L28" s="136" t="n"/>
     </row>
     <row r="29">
-      <c r="B29" s="492" t="inlineStr">
+      <c r="B29" s="519" t="inlineStr">
         <is>
           <t>#QL8LVLYG8</t>
         </is>
       </c>
-      <c r="C29" s="492" t="n"/>
-      <c r="D29" s="492" t="inlineStr">
+      <c r="C29" s="519" t="n"/>
+      <c r="D29" s="519" t="inlineStr">
         <is>
           <t>Some guy</t>
         </is>
       </c>
-      <c r="E29" s="492" t="n"/>
+      <c r="E29" s="519" t="n"/>
       <c r="F29" s="130" t="n"/>
-      <c r="G29" s="492" t="n"/>
+      <c r="G29" s="519" t="n"/>
       <c r="H29" s="130" t="n"/>
-      <c r="I29" s="492" t="n"/>
+      <c r="I29" s="519" t="n"/>
       <c r="J29" s="130" t="n"/>
-      <c r="K29" s="492" t="n"/>
+      <c r="K29" s="519" t="n"/>
       <c r="L29" s="130" t="n"/>
     </row>
     <row r="30">
-      <c r="B30" s="493" t="inlineStr">
+      <c r="B30" s="520" t="inlineStr">
         <is>
           <t>#L9JJQY992</t>
         </is>
       </c>
-      <c r="C30" s="493" t="n"/>
-      <c r="D30" s="493" t="inlineStr">
+      <c r="C30" s="520" t="n"/>
+      <c r="D30" s="520" t="inlineStr">
         <is>
           <t>Fisted_Waffle</t>
         </is>
       </c>
-      <c r="E30" s="493" t="n"/>
+      <c r="E30" s="520" t="n"/>
       <c r="F30" s="136" t="n"/>
-      <c r="G30" s="493" t="n"/>
+      <c r="G30" s="520" t="n"/>
       <c r="H30" s="136" t="n"/>
-      <c r="I30" s="493" t="n"/>
+      <c r="I30" s="520" t="n"/>
       <c r="J30" s="136" t="n"/>
-      <c r="K30" s="493" t="n"/>
+      <c r="K30" s="520" t="n"/>
       <c r="L30" s="136" t="n"/>
     </row>
     <row r="31">
-      <c r="B31" s="492" t="inlineStr">
+      <c r="B31" s="519" t="inlineStr">
         <is>
           <t>#QV8JJ0URU</t>
         </is>
       </c>
-      <c r="C31" s="492" t="n"/>
-      <c r="D31" s="492" t="inlineStr">
+      <c r="C31" s="519" t="n"/>
+      <c r="D31" s="519" t="inlineStr">
         <is>
           <t>✨Jacob</t>
         </is>
       </c>
-      <c r="E31" s="492" t="n"/>
+      <c r="E31" s="519" t="n"/>
       <c r="F31" s="130" t="n"/>
-      <c r="G31" s="492" t="n"/>
+      <c r="G31" s="519" t="n"/>
       <c r="H31" s="130" t="n"/>
-      <c r="I31" s="497" t="n">
+      <c r="I31" s="524" t="n">
         <v>0</v>
       </c>
       <c r="J31" s="137" t="n">
         <v>0</v>
       </c>
-      <c r="K31" s="492" t="n"/>
+      <c r="K31" s="519" t="n"/>
       <c r="L31" s="130" t="n"/>
     </row>
     <row r="32">
-      <c r="B32" s="493" t="inlineStr">
+      <c r="B32" s="520" t="inlineStr">
         <is>
           <t>#QY0VGPQGQ</t>
         </is>
       </c>
-      <c r="C32" s="493" t="n"/>
-      <c r="D32" s="493" t="inlineStr">
+      <c r="C32" s="520" t="n"/>
+      <c r="D32" s="520" t="inlineStr">
         <is>
           <t>killerjones</t>
         </is>
       </c>
-      <c r="E32" s="493" t="n"/>
+      <c r="E32" s="520" t="n"/>
       <c r="F32" s="136" t="n"/>
-      <c r="G32" s="493" t="n"/>
+      <c r="G32" s="520" t="n"/>
       <c r="H32" s="136" t="n"/>
-      <c r="I32" s="493" t="n"/>
+      <c r="I32" s="520" t="n"/>
       <c r="J32" s="136" t="n"/>
-      <c r="K32" s="493" t="n"/>
+      <c r="K32" s="520" t="n"/>
       <c r="L32" s="136" t="n"/>
     </row>
     <row r="33">
-      <c r="B33" s="497" t="inlineStr">
+      <c r="B33" s="524" t="inlineStr">
         <is>
           <t>#P2CPRPQU</t>
         </is>
       </c>
-      <c r="C33" s="492" t="n"/>
-      <c r="D33" s="492" t="inlineStr">
+      <c r="C33" s="519" t="n"/>
+      <c r="D33" s="519" t="inlineStr">
         <is>
           <t>The Drift King</t>
         </is>
       </c>
-      <c r="E33" s="492" t="n"/>
+      <c r="E33" s="519" t="n"/>
       <c r="F33" s="130" t="n"/>
-      <c r="G33" s="496" t="n">
+      <c r="G33" s="523" t="n">
         <v>2</v>
       </c>
       <c r="H33" s="127" t="n">
         <v>6</v>
       </c>
-      <c r="I33" s="496" t="n">
+      <c r="I33" s="523" t="n">
         <v>2</v>
       </c>
       <c r="J33" s="127" t="n">
         <v>6</v>
       </c>
-      <c r="K33" s="492" t="n"/>
+      <c r="K33" s="519" t="n"/>
       <c r="L33" s="130" t="n"/>
     </row>
     <row r="34">
-      <c r="B34" s="495" t="inlineStr">
+      <c r="B34" s="522" t="inlineStr">
         <is>
           <t>#UVCCQC02</t>
         </is>
       </c>
-      <c r="C34" s="493" t="n"/>
-      <c r="D34" s="493" t="inlineStr">
+      <c r="C34" s="520" t="n"/>
+      <c r="D34" s="520" t="inlineStr">
         <is>
           <t>lordshisha</t>
         </is>
       </c>
-      <c r="E34" s="493" t="n"/>
+      <c r="E34" s="520" t="n"/>
       <c r="F34" s="136" t="n"/>
-      <c r="G34" s="498" t="n">
+      <c r="G34" s="525" t="n">
         <v>2</v>
       </c>
       <c r="H34" s="133" t="n">
         <v>6</v>
       </c>
-      <c r="I34" s="498" t="n">
+      <c r="I34" s="525" t="n">
         <v>2</v>
       </c>
       <c r="J34" s="139" t="n">
         <v>3</v>
       </c>
-      <c r="K34" s="498" t="n">
+      <c r="K34" s="525" t="n">
         <v>2</v>
       </c>
       <c r="L34" s="148" t="n">
@@ -4247,66 +4280,66 @@
       </c>
     </row>
     <row r="35">
-      <c r="B35" s="497" t="inlineStr">
+      <c r="B35" s="524" t="inlineStr">
         <is>
           <t>#Q0JG2RJQ8</t>
         </is>
       </c>
-      <c r="C35" s="492" t="n"/>
-      <c r="D35" s="492" t="inlineStr">
+      <c r="C35" s="519" t="n"/>
+      <c r="D35" s="519" t="inlineStr">
         <is>
           <t>bozo</t>
         </is>
       </c>
-      <c r="E35" s="492" t="n"/>
+      <c r="E35" s="519" t="n"/>
       <c r="F35" s="130" t="n"/>
-      <c r="G35" s="492" t="n"/>
+      <c r="G35" s="519" t="n"/>
       <c r="H35" s="130" t="n"/>
-      <c r="I35" s="492" t="n"/>
+      <c r="I35" s="519" t="n"/>
       <c r="J35" s="130" t="n"/>
-      <c r="K35" s="492" t="n"/>
+      <c r="K35" s="519" t="n"/>
       <c r="L35" s="130" t="n"/>
     </row>
     <row r="36">
-      <c r="B36" s="495" t="inlineStr">
+      <c r="B36" s="522" t="inlineStr">
         <is>
           <t>#QJVL0LYQQ</t>
         </is>
       </c>
-      <c r="C36" s="493" t="n"/>
-      <c r="D36" s="493" t="inlineStr">
+      <c r="C36" s="520" t="n"/>
+      <c r="D36" s="520" t="inlineStr">
         <is>
           <t>mobbb341</t>
         </is>
       </c>
-      <c r="E36" s="493" t="n"/>
+      <c r="E36" s="520" t="n"/>
       <c r="F36" s="136" t="n"/>
-      <c r="G36" s="493" t="n"/>
+      <c r="G36" s="520" t="n"/>
       <c r="H36" s="136" t="n"/>
-      <c r="I36" s="493" t="n"/>
+      <c r="I36" s="520" t="n"/>
       <c r="J36" s="136" t="n"/>
-      <c r="K36" s="493" t="n"/>
+      <c r="K36" s="520" t="n"/>
       <c r="L36" s="136" t="n"/>
     </row>
     <row r="37">
-      <c r="B37" s="497" t="inlineStr">
+      <c r="B37" s="524" t="inlineStr">
         <is>
           <t>#L8R82C8VC</t>
         </is>
       </c>
-      <c r="C37" s="492" t="n"/>
-      <c r="D37" s="492" t="inlineStr">
+      <c r="C37" s="519" t="n"/>
+      <c r="D37" s="519" t="inlineStr">
         <is>
           <t>caden asue</t>
         </is>
       </c>
-      <c r="E37" s="492" t="n"/>
+      <c r="E37" s="519" t="n"/>
       <c r="F37" s="130" t="n"/>
-      <c r="G37" s="492" t="n"/>
+      <c r="G37" s="519" t="n"/>
       <c r="H37" s="130" t="n"/>
-      <c r="I37" s="492" t="n"/>
+      <c r="I37" s="519" t="n"/>
       <c r="J37" s="130" t="n"/>
-      <c r="K37" s="492" t="n"/>
+      <c r="K37" s="519" t="n"/>
       <c r="L37" s="130" t="n"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
sorting now prioritizes none instead of zero
</commit_message>
<xml_diff>
--- a/Clash.xlsx
+++ b/Clash.xlsx
@@ -223,7 +223,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="28">
     <border>
       <left/>
       <right/>
@@ -321,11 +321,21 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9"/>
   </cellStyleXfs>
-  <cellXfs count="202">
+  <cellXfs count="372">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -586,6 +596,216 @@
     <xf numFmtId="164" fontId="8" fillId="27" borderId="17" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="8" fillId="31" borderId="17" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="8" fillId="32" borderId="17" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="7" fillId="25" borderId="18" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="25" borderId="18" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="26" borderId="18" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="7" fillId="27" borderId="18" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="7" fillId="28" borderId="18" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="28" borderId="18" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="29" borderId="18" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="7" fillId="30" borderId="18" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="7" fillId="31" borderId="18" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="8" fillId="28" borderId="18" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="8" fillId="29" borderId="18" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="8" fillId="30" borderId="18" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="8" fillId="25" borderId="18" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="8" fillId="26" borderId="18" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="8" fillId="27" borderId="18" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="8" fillId="31" borderId="18" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="8" fillId="32" borderId="18" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="7" fillId="25" borderId="19" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="25" borderId="19" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="26" borderId="19" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="7" fillId="27" borderId="19" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="7" fillId="28" borderId="19" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="28" borderId="19" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="29" borderId="19" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="7" fillId="30" borderId="19" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="7" fillId="31" borderId="19" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="8" fillId="28" borderId="19" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="8" fillId="29" borderId="19" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="8" fillId="30" borderId="19" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="8" fillId="25" borderId="19" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="8" fillId="26" borderId="19" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="8" fillId="27" borderId="19" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="8" fillId="31" borderId="19" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="8" fillId="32" borderId="19" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="7" fillId="25" borderId="20" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="25" borderId="20" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="26" borderId="20" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="7" fillId="27" borderId="20" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="7" fillId="28" borderId="20" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="28" borderId="20" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="29" borderId="20" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="7" fillId="30" borderId="20" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="7" fillId="31" borderId="20" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="8" fillId="28" borderId="20" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="8" fillId="29" borderId="20" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="8" fillId="30" borderId="20" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="8" fillId="25" borderId="20" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="8" fillId="26" borderId="20" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="8" fillId="27" borderId="20" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="8" fillId="31" borderId="20" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="8" fillId="32" borderId="20" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="7" fillId="25" borderId="21" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="25" borderId="21" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="26" borderId="21" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="7" fillId="27" borderId="21" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="7" fillId="28" borderId="21" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="28" borderId="21" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="29" borderId="21" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="7" fillId="30" borderId="21" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="7" fillId="31" borderId="21" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="8" fillId="28" borderId="21" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="8" fillId="29" borderId="21" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="8" fillId="30" borderId="21" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="8" fillId="25" borderId="21" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="8" fillId="26" borderId="21" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="8" fillId="27" borderId="21" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="8" fillId="31" borderId="21" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="8" fillId="32" borderId="21" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="7" fillId="25" borderId="22" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="25" borderId="22" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="26" borderId="22" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="7" fillId="27" borderId="22" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="7" fillId="28" borderId="22" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="28" borderId="22" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="29" borderId="22" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="7" fillId="30" borderId="22" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="7" fillId="31" borderId="22" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="8" fillId="28" borderId="22" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="8" fillId="29" borderId="22" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="8" fillId="30" borderId="22" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="8" fillId="25" borderId="22" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="8" fillId="26" borderId="22" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="8" fillId="27" borderId="22" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="8" fillId="31" borderId="22" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="8" fillId="32" borderId="22" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="7" fillId="25" borderId="23" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="25" borderId="23" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="26" borderId="23" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="7" fillId="27" borderId="23" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="7" fillId="28" borderId="23" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="28" borderId="23" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="29" borderId="23" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="7" fillId="30" borderId="23" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="7" fillId="31" borderId="23" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="8" fillId="28" borderId="23" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="8" fillId="29" borderId="23" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="8" fillId="30" borderId="23" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="8" fillId="25" borderId="23" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="8" fillId="26" borderId="23" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="8" fillId="27" borderId="23" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="8" fillId="31" borderId="23" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="8" fillId="32" borderId="23" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="7" fillId="25" borderId="24" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="25" borderId="24" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="26" borderId="24" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="7" fillId="27" borderId="24" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="7" fillId="28" borderId="24" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="28" borderId="24" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="29" borderId="24" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="7" fillId="30" borderId="24" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="7" fillId="31" borderId="24" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="8" fillId="28" borderId="24" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="8" fillId="29" borderId="24" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="8" fillId="30" borderId="24" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="8" fillId="25" borderId="24" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="8" fillId="26" borderId="24" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="8" fillId="27" borderId="24" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="8" fillId="31" borderId="24" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="8" fillId="32" borderId="24" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="7" fillId="25" borderId="25" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="25" borderId="25" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="26" borderId="25" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="7" fillId="27" borderId="25" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="7" fillId="28" borderId="25" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="28" borderId="25" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="29" borderId="25" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="7" fillId="30" borderId="25" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="7" fillId="31" borderId="25" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="8" fillId="28" borderId="25" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="8" fillId="29" borderId="25" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="8" fillId="30" borderId="25" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="8" fillId="25" borderId="25" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="8" fillId="26" borderId="25" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="8" fillId="27" borderId="25" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="8" fillId="31" borderId="25" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="8" fillId="32" borderId="25" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="7" fillId="25" borderId="26" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="25" borderId="26" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="26" borderId="26" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="7" fillId="27" borderId="26" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="7" fillId="28" borderId="26" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="28" borderId="26" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="29" borderId="26" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="7" fillId="30" borderId="26" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="7" fillId="31" borderId="26" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="8" fillId="28" borderId="26" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="8" fillId="29" borderId="26" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="8" fillId="30" borderId="26" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="8" fillId="25" borderId="26" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="8" fillId="26" borderId="26" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="8" fillId="27" borderId="26" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="8" fillId="31" borderId="26" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="8" fillId="32" borderId="26" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="7" fillId="25" borderId="27" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="25" borderId="27" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="26" borderId="27" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="7" fillId="27" borderId="27" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="7" fillId="28" borderId="27" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="28" borderId="27" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="29" borderId="27" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="7" fillId="30" borderId="27" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="7" fillId="31" borderId="27" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="8" fillId="28" borderId="27" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="8" fillId="29" borderId="27" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="8" fillId="30" borderId="27" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="8" fillId="25" borderId="27" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="8" fillId="26" borderId="27" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="8" fillId="27" borderId="27" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="8" fillId="32" borderId="27" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="8" fillId="31" borderId="27" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1184,15 +1404,15 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="185" t="inlineStr">
+      <c r="A4" s="355" t="inlineStr">
         <is>
           <t>#G0QPVJY9L</t>
         </is>
       </c>
-      <c r="B4" s="185" t="n">
+      <c r="B4" s="355" t="n">
         <v>779</v>
       </c>
-      <c r="C4" s="186" t="n">
+      <c r="C4" s="356" t="n">
         <v>1</v>
       </c>
       <c r="D4" s="95" t="inlineStr">
@@ -1200,49 +1420,49 @@
           <t>Zoro</t>
         </is>
       </c>
-      <c r="E4" s="187" t="n">
+      <c r="E4" s="357" t="n">
         <v>6</v>
       </c>
       <c r="F4" s="95" t="n">
         <v>13801</v>
       </c>
-      <c r="G4" s="188" t="n">
+      <c r="G4" s="358" t="n">
         <v>0</v>
       </c>
       <c r="H4" s="98" t="n">
         <v>0</v>
       </c>
-      <c r="I4" s="187" t="n">
+      <c r="I4" s="357" t="n">
         <v>6</v>
       </c>
       <c r="J4" s="95" t="n">
         <v>12116</v>
       </c>
-      <c r="K4" s="187" t="n">
+      <c r="K4" s="357" t="n">
         <v>6</v>
       </c>
       <c r="L4" s="95" t="n">
         <v>13432</v>
       </c>
-      <c r="M4" s="187" t="n">
+      <c r="M4" s="357" t="n">
         <v>6</v>
       </c>
       <c r="N4" s="95" t="n">
         <v>8855</v>
       </c>
-      <c r="O4" s="187" t="n">
+      <c r="O4" s="357" t="n">
         <v>6</v>
       </c>
       <c r="P4" s="95" t="n">
         <v>10965</v>
       </c>
-      <c r="Q4" s="187" t="n">
+      <c r="Q4" s="357" t="n">
         <v>6</v>
       </c>
       <c r="R4" s="95" t="n">
         <v>7905</v>
       </c>
-      <c r="S4" s="187" t="n">
+      <c r="S4" s="357" t="n">
         <v>6</v>
       </c>
       <c r="T4" s="95" t="n">
@@ -1250,15 +1470,15 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="189" t="inlineStr">
+      <c r="A5" s="359" t="inlineStr">
         <is>
           <t>#YRGRRJQCY</t>
         </is>
       </c>
-      <c r="B5" s="189" t="n">
+      <c r="B5" s="359" t="n">
         <v>1306</v>
       </c>
-      <c r="C5" s="190" t="n">
+      <c r="C5" s="360" t="n">
         <v>2</v>
       </c>
       <c r="D5" s="101" t="inlineStr">
@@ -1266,49 +1486,49 @@
           <t>DoubleSpice</t>
         </is>
       </c>
-      <c r="E5" s="191" t="n">
+      <c r="E5" s="361" t="n">
         <v>6</v>
       </c>
       <c r="F5" s="101" t="n">
         <v>13656</v>
       </c>
-      <c r="G5" s="192" t="n">
+      <c r="G5" s="362" t="n">
         <v>0</v>
       </c>
       <c r="H5" s="104" t="n">
         <v>0</v>
       </c>
-      <c r="I5" s="191" t="n">
+      <c r="I5" s="361" t="n">
         <v>6</v>
       </c>
       <c r="J5" s="101" t="n">
         <v>10016</v>
       </c>
-      <c r="K5" s="191" t="n">
+      <c r="K5" s="361" t="n">
         <v>6</v>
       </c>
       <c r="L5" s="101" t="n">
         <v>11620</v>
       </c>
-      <c r="M5" s="191" t="n">
+      <c r="M5" s="361" t="n">
         <v>6</v>
       </c>
       <c r="N5" s="101" t="n">
         <v>14095</v>
       </c>
-      <c r="O5" s="191" t="n">
+      <c r="O5" s="361" t="n">
         <v>6</v>
       </c>
       <c r="P5" s="101" t="n">
         <v>12379</v>
       </c>
-      <c r="Q5" s="191" t="n">
+      <c r="Q5" s="361" t="n">
         <v>6</v>
       </c>
       <c r="R5" s="101" t="n">
         <v>8256</v>
       </c>
-      <c r="S5" s="191" t="n">
+      <c r="S5" s="361" t="n">
         <v>6</v>
       </c>
       <c r="T5" s="101" t="n">
@@ -1316,15 +1536,15 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="185" t="inlineStr">
+      <c r="A6" s="355" t="inlineStr">
         <is>
           <t>#90U0VPU9U</t>
         </is>
       </c>
-      <c r="B6" s="185" t="n">
+      <c r="B6" s="355" t="n">
         <v>2597</v>
       </c>
-      <c r="C6" s="186" t="n">
+      <c r="C6" s="356" t="n">
         <v>3</v>
       </c>
       <c r="D6" s="95" t="inlineStr">
@@ -1332,49 +1552,49 @@
           <t>KYANI7E</t>
         </is>
       </c>
-      <c r="E6" s="187" t="n">
+      <c r="E6" s="357" t="n">
         <v>6</v>
       </c>
       <c r="F6" s="95" t="n">
         <v>13278</v>
       </c>
-      <c r="G6" s="193" t="n">
+      <c r="G6" s="363" t="n">
         <v>141</v>
       </c>
       <c r="H6" s="98" t="n">
         <v>0</v>
       </c>
-      <c r="I6" s="187" t="n">
+      <c r="I6" s="357" t="n">
         <v>6</v>
       </c>
       <c r="J6" s="95" t="n">
         <v>12477</v>
       </c>
-      <c r="K6" s="187" t="n">
+      <c r="K6" s="357" t="n">
         <v>6</v>
       </c>
       <c r="L6" s="95" t="n">
         <v>13260</v>
       </c>
-      <c r="M6" s="187" t="n">
+      <c r="M6" s="357" t="n">
         <v>6</v>
       </c>
       <c r="N6" s="95" t="n">
         <v>12144</v>
       </c>
-      <c r="O6" s="187" t="n">
+      <c r="O6" s="357" t="n">
         <v>6</v>
       </c>
       <c r="P6" s="95" t="n">
         <v>12835</v>
       </c>
-      <c r="Q6" s="187" t="n">
+      <c r="Q6" s="357" t="n">
         <v>6</v>
       </c>
       <c r="R6" s="95" t="n">
         <v>7696</v>
       </c>
-      <c r="S6" s="187" t="n">
+      <c r="S6" s="357" t="n">
         <v>6</v>
       </c>
       <c r="T6" s="95" t="n">
@@ -1382,15 +1602,15 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="189" t="inlineStr">
+      <c r="A7" s="359" t="inlineStr">
         <is>
           <t>#YJ20CRJYQ</t>
         </is>
       </c>
-      <c r="B7" s="189" t="n">
+      <c r="B7" s="359" t="n">
         <v>1255</v>
       </c>
-      <c r="C7" s="190" t="n">
+      <c r="C7" s="360" t="n">
         <v>4</v>
       </c>
       <c r="D7" s="101" t="inlineStr">
@@ -1398,49 +1618,49 @@
           <t>UnluckGod</t>
         </is>
       </c>
-      <c r="E7" s="191" t="n">
+      <c r="E7" s="361" t="n">
         <v>6</v>
       </c>
       <c r="F7" s="101" t="n">
         <v>13062</v>
       </c>
-      <c r="G7" s="192" t="n">
+      <c r="G7" s="362" t="n">
         <v>0</v>
       </c>
       <c r="H7" s="104" t="n">
         <v>0</v>
       </c>
-      <c r="I7" s="191" t="n">
+      <c r="I7" s="361" t="n">
         <v>6</v>
       </c>
       <c r="J7" s="101" t="n">
         <v>8886</v>
       </c>
-      <c r="K7" s="191" t="n">
+      <c r="K7" s="361" t="n">
         <v>6</v>
       </c>
       <c r="L7" s="101" t="n">
         <v>12824</v>
       </c>
-      <c r="M7" s="191" t="n">
+      <c r="M7" s="361" t="n">
         <v>6</v>
       </c>
       <c r="N7" s="101" t="n">
         <v>11999</v>
       </c>
-      <c r="O7" s="191" t="n">
+      <c r="O7" s="361" t="n">
         <v>6</v>
       </c>
       <c r="P7" s="101" t="n">
         <v>12972</v>
       </c>
-      <c r="Q7" s="191" t="n">
+      <c r="Q7" s="361" t="n">
         <v>6</v>
       </c>
       <c r="R7" s="101" t="n">
         <v>8286</v>
       </c>
-      <c r="S7" s="191" t="n">
+      <c r="S7" s="361" t="n">
         <v>6</v>
       </c>
       <c r="T7" s="101" t="n">
@@ -1448,15 +1668,15 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="185" t="inlineStr">
+      <c r="A8" s="355" t="inlineStr">
         <is>
           <t>#QUYG0PQC8</t>
         </is>
       </c>
-      <c r="B8" s="185" t="n">
+      <c r="B8" s="355" t="n">
         <v>854</v>
       </c>
-      <c r="C8" s="186" t="n">
+      <c r="C8" s="356" t="n">
         <v>5</v>
       </c>
       <c r="D8" s="95" t="inlineStr">
@@ -1464,49 +1684,49 @@
           <t>Luffy</t>
         </is>
       </c>
-      <c r="E8" s="187" t="n">
+      <c r="E8" s="357" t="n">
         <v>6</v>
       </c>
       <c r="F8" s="95" t="n">
         <v>12820</v>
       </c>
-      <c r="G8" s="188" t="n">
+      <c r="G8" s="358" t="n">
         <v>0</v>
       </c>
       <c r="H8" s="98" t="n">
         <v>0</v>
       </c>
-      <c r="I8" s="187" t="n">
+      <c r="I8" s="357" t="n">
         <v>6</v>
       </c>
       <c r="J8" s="95" t="n">
         <v>11357</v>
       </c>
-      <c r="K8" s="187" t="n">
+      <c r="K8" s="357" t="n">
         <v>6</v>
       </c>
       <c r="L8" s="95" t="n">
         <v>10879</v>
       </c>
-      <c r="M8" s="187" t="n">
+      <c r="M8" s="357" t="n">
         <v>6</v>
       </c>
       <c r="N8" s="95" t="n">
         <v>9114</v>
       </c>
-      <c r="O8" s="187" t="n">
+      <c r="O8" s="357" t="n">
         <v>6</v>
       </c>
       <c r="P8" s="95" t="n">
         <v>13385</v>
       </c>
-      <c r="Q8" s="187" t="n">
+      <c r="Q8" s="357" t="n">
         <v>6</v>
       </c>
       <c r="R8" s="95" t="n">
         <v>7877</v>
       </c>
-      <c r="S8" s="187" t="n">
+      <c r="S8" s="357" t="n">
         <v>6</v>
       </c>
       <c r="T8" s="95" t="n">
@@ -1514,15 +1734,15 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="194" t="inlineStr">
+      <c r="A9" s="364" t="inlineStr">
         <is>
           <t>#LPCLQUCCY</t>
         </is>
       </c>
-      <c r="B9" s="194" t="n">
+      <c r="B9" s="364" t="n">
         <v>1024</v>
       </c>
-      <c r="C9" s="190" t="n">
+      <c r="C9" s="360" t="n">
         <v>6</v>
       </c>
       <c r="D9" s="106" t="inlineStr">
@@ -1530,49 +1750,49 @@
           <t>Zodiac</t>
         </is>
       </c>
-      <c r="E9" s="195" t="n">
+      <c r="E9" s="365" t="n">
         <v>6</v>
       </c>
       <c r="F9" s="106" t="n">
         <v>12035</v>
       </c>
-      <c r="G9" s="196" t="n">
+      <c r="G9" s="366" t="n">
         <v>0</v>
       </c>
       <c r="H9" s="109" t="n">
         <v>0</v>
       </c>
-      <c r="I9" s="195" t="n">
+      <c r="I9" s="365" t="n">
         <v>6</v>
       </c>
       <c r="J9" s="106" t="n">
         <v>7463</v>
       </c>
-      <c r="K9" s="196" t="n">
+      <c r="K9" s="366" t="n">
         <v>0</v>
       </c>
       <c r="L9" s="110" t="n">
         <v>0</v>
       </c>
-      <c r="M9" s="194" t="n"/>
+      <c r="M9" s="364" t="n"/>
       <c r="N9" s="109" t="n"/>
-      <c r="O9" s="194" t="n"/>
+      <c r="O9" s="364" t="n"/>
       <c r="P9" s="109" t="n"/>
-      <c r="Q9" s="194" t="n"/>
+      <c r="Q9" s="364" t="n"/>
       <c r="R9" s="109" t="n"/>
-      <c r="S9" s="194" t="n"/>
+      <c r="S9" s="364" t="n"/>
       <c r="T9" s="109" t="n"/>
     </row>
     <row r="10">
-      <c r="A10" s="185" t="inlineStr">
+      <c r="A10" s="355" t="inlineStr">
         <is>
           <t>#QUV2GP88U</t>
         </is>
       </c>
-      <c r="B10" s="185" t="n">
+      <c r="B10" s="355" t="n">
         <v>777</v>
       </c>
-      <c r="C10" s="186" t="n">
+      <c r="C10" s="356" t="n">
         <v>7</v>
       </c>
       <c r="D10" s="95" t="inlineStr">
@@ -1580,49 +1800,49 @@
           <t>Nico Robin</t>
         </is>
       </c>
-      <c r="E10" s="187" t="n">
+      <c r="E10" s="357" t="n">
         <v>6</v>
       </c>
       <c r="F10" s="95" t="n">
         <v>11670</v>
       </c>
-      <c r="G10" s="188" t="n">
+      <c r="G10" s="358" t="n">
         <v>0</v>
       </c>
       <c r="H10" s="98" t="n">
         <v>0</v>
       </c>
-      <c r="I10" s="187" t="n">
+      <c r="I10" s="357" t="n">
         <v>6</v>
       </c>
       <c r="J10" s="95" t="n">
         <v>10389</v>
       </c>
-      <c r="K10" s="187" t="n">
+      <c r="K10" s="357" t="n">
         <v>6</v>
       </c>
       <c r="L10" s="95" t="n">
         <v>12612</v>
       </c>
-      <c r="M10" s="187" t="n">
+      <c r="M10" s="357" t="n">
         <v>6</v>
       </c>
       <c r="N10" s="95" t="n">
         <v>11338</v>
       </c>
-      <c r="O10" s="187" t="n">
+      <c r="O10" s="357" t="n">
         <v>6</v>
       </c>
       <c r="P10" s="95" t="n">
         <v>10997</v>
       </c>
-      <c r="Q10" s="187" t="n">
+      <c r="Q10" s="357" t="n">
         <v>6</v>
       </c>
       <c r="R10" s="95" t="n">
         <v>11087</v>
       </c>
-      <c r="S10" s="187" t="n">
+      <c r="S10" s="357" t="n">
         <v>6</v>
       </c>
       <c r="T10" s="95" t="n">
@@ -1630,15 +1850,15 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="189" t="inlineStr">
+      <c r="A11" s="359" t="inlineStr">
         <is>
           <t>#QCV22VP0G</t>
         </is>
       </c>
-      <c r="B11" s="189" t="n">
+      <c r="B11" s="359" t="n">
         <v>774</v>
       </c>
-      <c r="C11" s="190" t="n">
+      <c r="C11" s="360" t="n">
         <v>8</v>
       </c>
       <c r="D11" s="101" t="inlineStr">
@@ -1646,49 +1866,49 @@
           <t>Nami</t>
         </is>
       </c>
-      <c r="E11" s="191" t="n">
+      <c r="E11" s="361" t="n">
         <v>6</v>
       </c>
       <c r="F11" s="101" t="n">
         <v>11484</v>
       </c>
-      <c r="G11" s="192" t="n">
+      <c r="G11" s="362" t="n">
         <v>0</v>
       </c>
       <c r="H11" s="104" t="n">
         <v>0</v>
       </c>
-      <c r="I11" s="191" t="n">
+      <c r="I11" s="361" t="n">
         <v>6</v>
       </c>
       <c r="J11" s="101" t="n">
         <v>11657</v>
       </c>
-      <c r="K11" s="191" t="n">
+      <c r="K11" s="361" t="n">
         <v>6</v>
       </c>
       <c r="L11" s="101" t="n">
         <v>11795</v>
       </c>
-      <c r="M11" s="191" t="n">
+      <c r="M11" s="361" t="n">
         <v>6</v>
       </c>
       <c r="N11" s="101" t="n">
         <v>10769</v>
       </c>
-      <c r="O11" s="191" t="n">
+      <c r="O11" s="361" t="n">
         <v>6</v>
       </c>
       <c r="P11" s="101" t="n">
         <v>12486</v>
       </c>
-      <c r="Q11" s="191" t="n">
+      <c r="Q11" s="361" t="n">
         <v>6</v>
       </c>
       <c r="R11" s="101" t="n">
         <v>8472</v>
       </c>
-      <c r="S11" s="191" t="n">
+      <c r="S11" s="361" t="n">
         <v>6</v>
       </c>
       <c r="T11" s="101" t="n">
@@ -1696,15 +1916,15 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="185" t="inlineStr">
+      <c r="A12" s="355" t="inlineStr">
         <is>
           <t>#QLR088LC9</t>
         </is>
       </c>
-      <c r="B12" s="185" t="n">
+      <c r="B12" s="355" t="n">
         <v>814</v>
       </c>
-      <c r="C12" s="186" t="n">
+      <c r="C12" s="356" t="n">
         <v>9</v>
       </c>
       <c r="D12" s="95" t="inlineStr">
@@ -1712,49 +1932,49 @@
           <t>Sanji</t>
         </is>
       </c>
-      <c r="E12" s="187" t="n">
+      <c r="E12" s="357" t="n">
         <v>6</v>
       </c>
       <c r="F12" s="95" t="n">
         <v>11473</v>
       </c>
-      <c r="G12" s="188" t="n">
+      <c r="G12" s="358" t="n">
         <v>0</v>
       </c>
       <c r="H12" s="98" t="n">
         <v>0</v>
       </c>
-      <c r="I12" s="187" t="n">
+      <c r="I12" s="357" t="n">
         <v>6</v>
       </c>
       <c r="J12" s="95" t="n">
         <v>11960</v>
       </c>
-      <c r="K12" s="187" t="n">
+      <c r="K12" s="357" t="n">
         <v>6</v>
       </c>
       <c r="L12" s="95" t="n">
         <v>10910</v>
       </c>
-      <c r="M12" s="187" t="n">
+      <c r="M12" s="357" t="n">
         <v>6</v>
       </c>
       <c r="N12" s="95" t="n">
         <v>9550</v>
       </c>
-      <c r="O12" s="187" t="n">
+      <c r="O12" s="357" t="n">
         <v>6</v>
       </c>
       <c r="P12" s="95" t="n">
         <v>9138</v>
       </c>
-      <c r="Q12" s="187" t="n">
+      <c r="Q12" s="357" t="n">
         <v>6</v>
       </c>
       <c r="R12" s="95" t="n">
         <v>8897</v>
       </c>
-      <c r="S12" s="187" t="n">
+      <c r="S12" s="357" t="n">
         <v>6</v>
       </c>
       <c r="T12" s="95" t="n">
@@ -1762,15 +1982,15 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="189" t="inlineStr">
+      <c r="A13" s="359" t="inlineStr">
         <is>
           <t>#QLJ2U20Y2</t>
         </is>
       </c>
-      <c r="B13" s="189" t="n">
+      <c r="B13" s="359" t="n">
         <v>1484</v>
       </c>
-      <c r="C13" s="190" t="n">
+      <c r="C13" s="360" t="n">
         <v>10</v>
       </c>
       <c r="D13" s="101" t="inlineStr">
@@ -1778,49 +1998,49 @@
           <t>DeadLeaf</t>
         </is>
       </c>
-      <c r="E13" s="191" t="n">
+      <c r="E13" s="361" t="n">
         <v>6</v>
       </c>
       <c r="F13" s="101" t="n">
         <v>11433</v>
       </c>
-      <c r="G13" s="192" t="n">
+      <c r="G13" s="362" t="n">
         <v>0</v>
       </c>
       <c r="H13" s="104" t="n">
         <v>0</v>
       </c>
-      <c r="I13" s="191" t="n">
+      <c r="I13" s="361" t="n">
         <v>6</v>
       </c>
       <c r="J13" s="101" t="n">
         <v>12676</v>
       </c>
-      <c r="K13" s="191" t="n">
+      <c r="K13" s="361" t="n">
         <v>6</v>
       </c>
       <c r="L13" s="101" t="n">
         <v>13763</v>
       </c>
-      <c r="M13" s="191" t="n">
+      <c r="M13" s="361" t="n">
         <v>6</v>
       </c>
       <c r="N13" s="101" t="n">
         <v>11140</v>
       </c>
-      <c r="O13" s="191" t="n">
+      <c r="O13" s="361" t="n">
         <v>6</v>
       </c>
       <c r="P13" s="101" t="n">
         <v>15509</v>
       </c>
-      <c r="Q13" s="191" t="n">
+      <c r="Q13" s="361" t="n">
         <v>6</v>
       </c>
       <c r="R13" s="101" t="n">
         <v>8567</v>
       </c>
-      <c r="S13" s="191" t="n">
+      <c r="S13" s="361" t="n">
         <v>6</v>
       </c>
       <c r="T13" s="101" t="n">
@@ -1828,15 +2048,15 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="185" t="inlineStr">
+      <c r="A14" s="355" t="inlineStr">
         <is>
           <t>#Q8CLCUCC2</t>
         </is>
       </c>
-      <c r="B14" s="185" t="n">
+      <c r="B14" s="355" t="n">
         <v>1409</v>
       </c>
-      <c r="C14" s="186" t="n">
+      <c r="C14" s="356" t="n">
         <v>11</v>
       </c>
       <c r="D14" s="95" t="inlineStr">
@@ -1844,49 +2064,49 @@
           <t>Moxxi</t>
         </is>
       </c>
-      <c r="E14" s="187" t="n">
+      <c r="E14" s="357" t="n">
         <v>6</v>
       </c>
       <c r="F14" s="95" t="n">
         <v>10777</v>
       </c>
-      <c r="G14" s="188" t="n">
+      <c r="G14" s="358" t="n">
         <v>0</v>
       </c>
       <c r="H14" s="98" t="n">
         <v>0</v>
       </c>
-      <c r="I14" s="187" t="n">
+      <c r="I14" s="357" t="n">
         <v>6</v>
       </c>
       <c r="J14" s="95" t="n">
         <v>12912</v>
       </c>
-      <c r="K14" s="187" t="n">
+      <c r="K14" s="357" t="n">
         <v>6</v>
       </c>
       <c r="L14" s="95" t="n">
         <v>8015</v>
       </c>
-      <c r="M14" s="187" t="n">
+      <c r="M14" s="357" t="n">
         <v>6</v>
       </c>
       <c r="N14" s="95" t="n">
         <v>11010</v>
       </c>
-      <c r="O14" s="187" t="n">
+      <c r="O14" s="357" t="n">
         <v>6</v>
       </c>
       <c r="P14" s="95" t="n">
         <v>13857</v>
       </c>
-      <c r="Q14" s="187" t="n">
+      <c r="Q14" s="357" t="n">
         <v>6</v>
       </c>
       <c r="R14" s="95" t="n">
         <v>7905</v>
       </c>
-      <c r="S14" s="187" t="n">
+      <c r="S14" s="357" t="n">
         <v>6</v>
       </c>
       <c r="T14" s="95" t="n">
@@ -1894,15 +2114,15 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="189" t="inlineStr">
+      <c r="A15" s="359" t="inlineStr">
         <is>
           <t>#QUG8QQJ92</t>
         </is>
       </c>
-      <c r="B15" s="189" t="n">
+      <c r="B15" s="359" t="n">
         <v>894</v>
       </c>
-      <c r="C15" s="190" t="n">
+      <c r="C15" s="360" t="n">
         <v>12</v>
       </c>
       <c r="D15" s="101" t="inlineStr">
@@ -1910,49 +2130,49 @@
           <t>Karma</t>
         </is>
       </c>
-      <c r="E15" s="191" t="n">
+      <c r="E15" s="361" t="n">
         <v>6</v>
       </c>
       <c r="F15" s="101" t="n">
         <v>10105</v>
       </c>
-      <c r="G15" s="192" t="n">
+      <c r="G15" s="362" t="n">
         <v>0</v>
       </c>
       <c r="H15" s="104" t="n">
         <v>0</v>
       </c>
-      <c r="I15" s="191" t="n">
+      <c r="I15" s="361" t="n">
         <v>6</v>
       </c>
       <c r="J15" s="101" t="n">
         <v>12204</v>
       </c>
-      <c r="K15" s="191" t="n">
+      <c r="K15" s="361" t="n">
         <v>6</v>
       </c>
       <c r="L15" s="101" t="n">
         <v>11355</v>
       </c>
-      <c r="M15" s="191" t="n">
+      <c r="M15" s="361" t="n">
         <v>6</v>
       </c>
       <c r="N15" s="101" t="n">
         <v>10003</v>
       </c>
-      <c r="O15" s="191" t="n">
+      <c r="O15" s="361" t="n">
         <v>6</v>
       </c>
       <c r="P15" s="101" t="n">
         <v>10595</v>
       </c>
-      <c r="Q15" s="191" t="n">
+      <c r="Q15" s="361" t="n">
         <v>6</v>
       </c>
       <c r="R15" s="101" t="n">
         <v>9240</v>
       </c>
-      <c r="S15" s="191" t="n">
+      <c r="S15" s="361" t="n">
         <v>6</v>
       </c>
       <c r="T15" s="101" t="n">
@@ -1960,15 +2180,15 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="197" t="inlineStr">
+      <c r="A16" s="367" t="inlineStr">
         <is>
           <t>#QUGYGY88C</t>
         </is>
       </c>
-      <c r="B16" s="197" t="n">
+      <c r="B16" s="367" t="n">
         <v>971</v>
       </c>
-      <c r="C16" s="186" t="n">
+      <c r="C16" s="356" t="n">
         <v>13</v>
       </c>
       <c r="D16" s="112" t="inlineStr">
@@ -1976,49 +2196,49 @@
           <t>Kingsman</t>
         </is>
       </c>
-      <c r="E16" s="198" t="n">
+      <c r="E16" s="368" t="n">
         <v>6</v>
       </c>
       <c r="F16" s="112" t="n">
         <v>9948</v>
       </c>
-      <c r="G16" s="199" t="n">
+      <c r="G16" s="369" t="n">
         <v>0</v>
       </c>
       <c r="H16" s="115" t="n">
         <v>0</v>
       </c>
-      <c r="I16" s="199" t="n">
+      <c r="I16" s="369" t="n">
         <v>0</v>
       </c>
       <c r="J16" s="116" t="n">
         <v>0</v>
       </c>
-      <c r="K16" s="199" t="n">
+      <c r="K16" s="369" t="n">
         <v>0</v>
       </c>
       <c r="L16" s="116" t="n">
         <v>0</v>
       </c>
-      <c r="M16" s="197" t="n"/>
+      <c r="M16" s="367" t="n"/>
       <c r="N16" s="115" t="n"/>
-      <c r="O16" s="197" t="n"/>
+      <c r="O16" s="367" t="n"/>
       <c r="P16" s="115" t="n"/>
-      <c r="Q16" s="197" t="n"/>
+      <c r="Q16" s="367" t="n"/>
       <c r="R16" s="115" t="n"/>
-      <c r="S16" s="197" t="n"/>
+      <c r="S16" s="367" t="n"/>
       <c r="T16" s="115" t="n"/>
     </row>
     <row r="17">
-      <c r="A17" s="194" t="inlineStr">
+      <c r="A17" s="364" t="inlineStr">
         <is>
           <t>#98JG2UJQL</t>
         </is>
       </c>
-      <c r="B17" s="194" t="n">
+      <c r="B17" s="364" t="n">
         <v>3030</v>
       </c>
-      <c r="C17" s="190" t="n">
+      <c r="C17" s="360" t="n">
         <v>14</v>
       </c>
       <c r="D17" s="106" t="inlineStr">
@@ -2026,49 +2246,49 @@
           <t>Dragonux</t>
         </is>
       </c>
-      <c r="E17" s="195" t="n">
+      <c r="E17" s="365" t="n">
         <v>6</v>
       </c>
       <c r="F17" s="106" t="n">
         <v>8745</v>
       </c>
-      <c r="G17" s="196" t="n">
+      <c r="G17" s="366" t="n">
         <v>0</v>
       </c>
       <c r="H17" s="109" t="n">
         <v>0</v>
       </c>
-      <c r="I17" s="195" t="n">
+      <c r="I17" s="365" t="n">
         <v>6</v>
       </c>
       <c r="J17" s="106" t="n">
         <v>10385</v>
       </c>
-      <c r="K17" s="195" t="n">
+      <c r="K17" s="365" t="n">
         <v>6</v>
       </c>
       <c r="L17" s="106" t="n">
         <v>10910</v>
       </c>
-      <c r="M17" s="195" t="n">
+      <c r="M17" s="365" t="n">
         <v>6</v>
       </c>
       <c r="N17" s="106" t="n">
         <v>8750</v>
       </c>
-      <c r="O17" s="195" t="n">
+      <c r="O17" s="365" t="n">
         <v>6</v>
       </c>
       <c r="P17" s="106" t="n">
         <v>10865</v>
       </c>
-      <c r="Q17" s="195" t="n">
+      <c r="Q17" s="365" t="n">
         <v>6</v>
       </c>
       <c r="R17" s="106" t="n">
         <v>8025</v>
       </c>
-      <c r="S17" s="195" t="n">
+      <c r="S17" s="365" t="n">
         <v>6</v>
       </c>
       <c r="T17" s="106" t="n">
@@ -2076,15 +2296,15 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="197" t="inlineStr">
+      <c r="A18" s="367" t="inlineStr">
         <is>
           <t>#G0JPUQGYR</t>
         </is>
       </c>
-      <c r="B18" s="197" t="n">
+      <c r="B18" s="367" t="n">
         <v>1540</v>
       </c>
-      <c r="C18" s="186" t="n">
+      <c r="C18" s="356" t="n">
         <v>15</v>
       </c>
       <c r="D18" s="112" t="inlineStr">
@@ -2092,49 +2312,49 @@
           <t>Collin</t>
         </is>
       </c>
-      <c r="E18" s="198" t="n">
+      <c r="E18" s="368" t="n">
         <v>6</v>
       </c>
       <c r="F18" s="112" t="n">
         <v>8725</v>
       </c>
-      <c r="G18" s="199" t="n">
+      <c r="G18" s="369" t="n">
         <v>0</v>
       </c>
       <c r="H18" s="115" t="n">
         <v>0</v>
       </c>
-      <c r="I18" s="198" t="n">
+      <c r="I18" s="368" t="n">
         <v>6</v>
       </c>
       <c r="J18" s="112" t="n">
         <v>10299</v>
       </c>
-      <c r="K18" s="198" t="n">
+      <c r="K18" s="368" t="n">
         <v>6</v>
       </c>
       <c r="L18" s="112" t="n">
         <v>8833</v>
       </c>
-      <c r="M18" s="198" t="n">
+      <c r="M18" s="368" t="n">
         <v>6</v>
       </c>
       <c r="N18" s="112" t="n">
         <v>9238</v>
       </c>
-      <c r="O18" s="198" t="n">
+      <c r="O18" s="368" t="n">
         <v>6</v>
       </c>
       <c r="P18" s="112" t="n">
         <v>7756</v>
       </c>
-      <c r="Q18" s="198" t="n">
+      <c r="Q18" s="368" t="n">
         <v>6</v>
       </c>
       <c r="R18" s="117" t="n">
         <v>5943</v>
       </c>
-      <c r="S18" s="198" t="n">
+      <c r="S18" s="368" t="n">
         <v>6</v>
       </c>
       <c r="T18" s="112" t="n">
@@ -2142,15 +2362,15 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="194" t="inlineStr">
+      <c r="A19" s="364" t="inlineStr">
         <is>
           <t>#8U9CRC8G</t>
         </is>
       </c>
-      <c r="B19" s="194" t="n">
-        <v>1785</v>
-      </c>
-      <c r="C19" s="190" t="n">
+      <c r="B19" s="364" t="n">
+        <v>1773</v>
+      </c>
+      <c r="C19" s="360" t="n">
         <v>16</v>
       </c>
       <c r="D19" s="106" t="inlineStr">
@@ -2158,49 +2378,49 @@
           <t>CEO JACK</t>
         </is>
       </c>
-      <c r="E19" s="195" t="n">
+      <c r="E19" s="365" t="n">
         <v>6</v>
       </c>
       <c r="F19" s="106" t="n">
         <v>8657</v>
       </c>
-      <c r="G19" s="196" t="n">
+      <c r="G19" s="370" t="n">
         <v>16</v>
       </c>
       <c r="H19" s="109" t="n">
         <v>132</v>
       </c>
-      <c r="I19" s="195" t="n">
+      <c r="I19" s="365" t="n">
         <v>6</v>
       </c>
       <c r="J19" s="106" t="n">
         <v>6980</v>
       </c>
-      <c r="K19" s="196" t="n">
+      <c r="K19" s="366" t="n">
         <v>0</v>
       </c>
       <c r="L19" s="110" t="n">
         <v>0</v>
       </c>
-      <c r="M19" s="194" t="n"/>
+      <c r="M19" s="364" t="n"/>
       <c r="N19" s="109" t="n"/>
-      <c r="O19" s="194" t="n"/>
+      <c r="O19" s="364" t="n"/>
       <c r="P19" s="109" t="n"/>
-      <c r="Q19" s="194" t="n"/>
+      <c r="Q19" s="364" t="n"/>
       <c r="R19" s="109" t="n"/>
-      <c r="S19" s="194" t="n"/>
+      <c r="S19" s="364" t="n"/>
       <c r="T19" s="109" t="n"/>
     </row>
     <row r="20">
-      <c r="A20" s="197" t="inlineStr">
+      <c r="A20" s="367" t="inlineStr">
         <is>
           <t>#LLQQ8CGPV</t>
         </is>
       </c>
-      <c r="B20" s="197" t="n">
+      <c r="B20" s="367" t="n">
         <v>1405</v>
       </c>
-      <c r="C20" s="186" t="n">
+      <c r="C20" s="356" t="n">
         <v>17</v>
       </c>
       <c r="D20" s="112" t="inlineStr">
@@ -2208,41 +2428,41 @@
           <t>jojomoonky</t>
         </is>
       </c>
-      <c r="E20" s="198" t="n">
+      <c r="E20" s="368" t="n">
         <v>6</v>
       </c>
       <c r="F20" s="112" t="n">
         <v>8465</v>
       </c>
-      <c r="G20" s="199" t="n">
+      <c r="G20" s="369" t="n">
         <v>0</v>
       </c>
       <c r="H20" s="115" t="n">
         <v>0</v>
       </c>
-      <c r="I20" s="197" t="n"/>
+      <c r="I20" s="367" t="n"/>
       <c r="J20" s="115" t="n"/>
-      <c r="K20" s="197" t="n"/>
+      <c r="K20" s="367" t="n"/>
       <c r="L20" s="115" t="n"/>
-      <c r="M20" s="197" t="n"/>
+      <c r="M20" s="367" t="n"/>
       <c r="N20" s="115" t="n"/>
-      <c r="O20" s="197" t="n"/>
+      <c r="O20" s="367" t="n"/>
       <c r="P20" s="115" t="n"/>
-      <c r="Q20" s="197" t="n"/>
+      <c r="Q20" s="367" t="n"/>
       <c r="R20" s="115" t="n"/>
-      <c r="S20" s="197" t="n"/>
+      <c r="S20" s="367" t="n"/>
       <c r="T20" s="115" t="n"/>
     </row>
     <row r="21">
-      <c r="A21" s="194" t="inlineStr">
+      <c r="A21" s="364" t="inlineStr">
         <is>
           <t>#QRPRYR8LL</t>
         </is>
       </c>
-      <c r="B21" s="194" t="n">
+      <c r="B21" s="364" t="n">
         <v>1216</v>
       </c>
-      <c r="C21" s="190" t="n">
+      <c r="C21" s="360" t="n">
         <v>18</v>
       </c>
       <c r="D21" s="106" t="inlineStr">
@@ -2250,49 +2470,49 @@
           <t>FidelCashflow</t>
         </is>
       </c>
-      <c r="E21" s="195" t="n">
+      <c r="E21" s="365" t="n">
         <v>6</v>
       </c>
       <c r="F21" s="106" t="n">
         <v>8263</v>
       </c>
-      <c r="G21" s="196" t="n">
+      <c r="G21" s="366" t="n">
         <v>0</v>
       </c>
       <c r="H21" s="109" t="n">
         <v>0</v>
       </c>
-      <c r="I21" s="195" t="n">
+      <c r="I21" s="365" t="n">
         <v>6</v>
       </c>
       <c r="J21" s="106" t="n">
         <v>8298</v>
       </c>
-      <c r="K21" s="195" t="n">
+      <c r="K21" s="365" t="n">
         <v>6</v>
       </c>
       <c r="L21" s="106" t="n">
         <v>6415</v>
       </c>
-      <c r="M21" s="195" t="n">
+      <c r="M21" s="365" t="n">
         <v>6</v>
       </c>
       <c r="N21" s="106" t="n">
         <v>6547</v>
       </c>
-      <c r="O21" s="195" t="n">
+      <c r="O21" s="365" t="n">
         <v>6</v>
       </c>
       <c r="P21" s="106" t="n">
         <v>6811</v>
       </c>
-      <c r="Q21" s="195" t="n">
+      <c r="Q21" s="365" t="n">
         <v>6</v>
       </c>
       <c r="R21" s="118" t="n">
         <v>4239</v>
       </c>
-      <c r="S21" s="195" t="n">
+      <c r="S21" s="365" t="n">
         <v>6</v>
       </c>
       <c r="T21" s="118" t="n">
@@ -2300,15 +2520,15 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="197" t="inlineStr">
+      <c r="A22" s="367" t="inlineStr">
         <is>
           <t>#QLGUYQPL0</t>
         </is>
       </c>
-      <c r="B22" s="197" t="n">
+      <c r="B22" s="367" t="n">
         <v>1529</v>
       </c>
-      <c r="C22" s="186" t="n">
+      <c r="C22" s="356" t="n">
         <v>19</v>
       </c>
       <c r="D22" s="112" t="inlineStr">
@@ -2316,45 +2536,45 @@
           <t>i got time</t>
         </is>
       </c>
-      <c r="E22" s="198" t="n">
+      <c r="E22" s="368" t="n">
         <v>6</v>
       </c>
       <c r="F22" s="112" t="n">
         <v>8087</v>
       </c>
-      <c r="G22" s="199" t="n">
+      <c r="G22" s="369" t="n">
         <v>0</v>
       </c>
       <c r="H22" s="115" t="n">
         <v>0</v>
       </c>
-      <c r="I22" s="199" t="n">
+      <c r="I22" s="369" t="n">
         <v>1</v>
       </c>
       <c r="J22" s="116" t="n">
         <v>1435</v>
       </c>
-      <c r="K22" s="197" t="n"/>
+      <c r="K22" s="367" t="n"/>
       <c r="L22" s="115" t="n"/>
-      <c r="M22" s="197" t="n"/>
+      <c r="M22" s="367" t="n"/>
       <c r="N22" s="115" t="n"/>
-      <c r="O22" s="197" t="n"/>
+      <c r="O22" s="367" t="n"/>
       <c r="P22" s="115" t="n"/>
-      <c r="Q22" s="197" t="n"/>
+      <c r="Q22" s="367" t="n"/>
       <c r="R22" s="115" t="n"/>
-      <c r="S22" s="197" t="n"/>
+      <c r="S22" s="367" t="n"/>
       <c r="T22" s="115" t="n"/>
     </row>
     <row r="23">
-      <c r="A23" s="194" t="inlineStr">
+      <c r="A23" s="364" t="inlineStr">
         <is>
           <t>#G0LJCVR2P</t>
         </is>
       </c>
-      <c r="B23" s="194" t="n">
+      <c r="B23" s="364" t="n">
         <v>1188</v>
       </c>
-      <c r="C23" s="190" t="n">
+      <c r="C23" s="360" t="n">
         <v>20</v>
       </c>
       <c r="D23" s="106" t="inlineStr">
@@ -2362,45 +2582,45 @@
           <t>DaddyChill</t>
         </is>
       </c>
-      <c r="E23" s="195" t="n">
+      <c r="E23" s="365" t="n">
         <v>6</v>
       </c>
       <c r="F23" s="106" t="n">
         <v>7874</v>
       </c>
-      <c r="G23" s="196" t="n">
+      <c r="G23" s="366" t="n">
         <v>0</v>
       </c>
       <c r="H23" s="109" t="n">
         <v>0</v>
       </c>
-      <c r="I23" s="196" t="n">
+      <c r="I23" s="366" t="n">
         <v>0</v>
       </c>
       <c r="J23" s="110" t="n">
         <v>0</v>
       </c>
-      <c r="K23" s="194" t="n"/>
+      <c r="K23" s="364" t="n"/>
       <c r="L23" s="109" t="n"/>
-      <c r="M23" s="194" t="n"/>
+      <c r="M23" s="364" t="n"/>
       <c r="N23" s="109" t="n"/>
-      <c r="O23" s="194" t="n"/>
+      <c r="O23" s="364" t="n"/>
       <c r="P23" s="109" t="n"/>
-      <c r="Q23" s="194" t="n"/>
+      <c r="Q23" s="364" t="n"/>
       <c r="R23" s="109" t="n"/>
-      <c r="S23" s="194" t="n"/>
+      <c r="S23" s="364" t="n"/>
       <c r="T23" s="109" t="n"/>
     </row>
     <row r="24">
-      <c r="A24" s="197" t="inlineStr">
+      <c r="A24" s="367" t="inlineStr">
         <is>
           <t>#QU0U2Q99G</t>
         </is>
       </c>
-      <c r="B24" s="197" t="n">
+      <c r="B24" s="367" t="n">
         <v>1010</v>
       </c>
-      <c r="C24" s="186" t="n">
+      <c r="C24" s="356" t="n">
         <v>21</v>
       </c>
       <c r="D24" s="112" t="inlineStr">
@@ -2408,57 +2628,57 @@
           <t>big coc</t>
         </is>
       </c>
-      <c r="E24" s="198" t="n">
+      <c r="E24" s="368" t="n">
         <v>6</v>
       </c>
       <c r="F24" s="112" t="n">
         <v>7550</v>
       </c>
-      <c r="G24" s="199" t="n">
+      <c r="G24" s="369" t="n">
         <v>0</v>
       </c>
       <c r="H24" s="115" t="n">
         <v>0</v>
       </c>
-      <c r="I24" s="198" t="n">
+      <c r="I24" s="368" t="n">
         <v>6</v>
       </c>
       <c r="J24" s="112" t="n">
         <v>7115</v>
       </c>
-      <c r="K24" s="198" t="n">
+      <c r="K24" s="368" t="n">
         <v>6</v>
       </c>
       <c r="L24" s="112" t="n">
         <v>7420</v>
       </c>
-      <c r="M24" s="198" t="n">
+      <c r="M24" s="368" t="n">
         <v>5</v>
       </c>
       <c r="N24" s="117" t="n">
         <v>5150</v>
       </c>
-      <c r="O24" s="198" t="n">
+      <c r="O24" s="368" t="n">
         <v>6</v>
       </c>
       <c r="P24" s="112" t="n">
         <v>9075</v>
       </c>
-      <c r="Q24" s="197" t="n"/>
+      <c r="Q24" s="367" t="n"/>
       <c r="R24" s="115" t="n"/>
-      <c r="S24" s="197" t="n"/>
+      <c r="S24" s="367" t="n"/>
       <c r="T24" s="115" t="n"/>
     </row>
     <row r="25">
-      <c r="A25" s="194" t="inlineStr">
+      <c r="A25" s="364" t="inlineStr">
         <is>
           <t>#QUVJGC0VQ</t>
         </is>
       </c>
-      <c r="B25" s="194" t="n">
+      <c r="B25" s="364" t="n">
         <v>1413</v>
       </c>
-      <c r="C25" s="190" t="n">
+      <c r="C25" s="360" t="n">
         <v>22</v>
       </c>
       <c r="D25" s="106" t="inlineStr">
@@ -2466,49 +2686,49 @@
           <t>Cam</t>
         </is>
       </c>
-      <c r="E25" s="195" t="n">
+      <c r="E25" s="365" t="n">
         <v>6</v>
       </c>
       <c r="F25" s="118" t="n">
         <v>5361</v>
       </c>
-      <c r="G25" s="196" t="n">
+      <c r="G25" s="366" t="n">
         <v>0</v>
       </c>
       <c r="H25" s="109" t="n">
         <v>0</v>
       </c>
-      <c r="I25" s="195" t="n">
+      <c r="I25" s="365" t="n">
         <v>6</v>
       </c>
       <c r="J25" s="106" t="n">
         <v>8080</v>
       </c>
-      <c r="K25" s="196" t="n">
+      <c r="K25" s="366" t="n">
         <v>0</v>
       </c>
       <c r="L25" s="110" t="n">
         <v>0</v>
       </c>
-      <c r="M25" s="194" t="n"/>
+      <c r="M25" s="364" t="n"/>
       <c r="N25" s="109" t="n"/>
-      <c r="O25" s="194" t="n"/>
+      <c r="O25" s="364" t="n"/>
       <c r="P25" s="109" t="n"/>
-      <c r="Q25" s="194" t="n"/>
+      <c r="Q25" s="364" t="n"/>
       <c r="R25" s="109" t="n"/>
-      <c r="S25" s="194" t="n"/>
+      <c r="S25" s="364" t="n"/>
       <c r="T25" s="109" t="n"/>
     </row>
     <row r="26">
-      <c r="A26" s="197" t="inlineStr">
+      <c r="A26" s="367" t="inlineStr">
         <is>
           <t>#QJQV82JG0</t>
         </is>
       </c>
-      <c r="B26" s="197" t="n">
+      <c r="B26" s="367" t="n">
         <v>1036</v>
       </c>
-      <c r="C26" s="186" t="n">
+      <c r="C26" s="356" t="n">
         <v>23</v>
       </c>
       <c r="D26" s="112" t="inlineStr">
@@ -2516,45 +2736,45 @@
           <t>The UnknownYT</t>
         </is>
       </c>
-      <c r="E26" s="198" t="n">
+      <c r="E26" s="368" t="n">
         <v>6</v>
       </c>
       <c r="F26" s="117" t="n">
         <v>5005</v>
       </c>
-      <c r="G26" s="199" t="n">
+      <c r="G26" s="369" t="n">
         <v>0</v>
       </c>
       <c r="H26" s="115" t="n">
         <v>0</v>
       </c>
-      <c r="I26" s="199" t="n">
+      <c r="I26" s="369" t="n">
         <v>0</v>
       </c>
       <c r="J26" s="116" t="n">
         <v>0</v>
       </c>
-      <c r="K26" s="197" t="n"/>
+      <c r="K26" s="367" t="n"/>
       <c r="L26" s="115" t="n"/>
-      <c r="M26" s="197" t="n"/>
+      <c r="M26" s="367" t="n"/>
       <c r="N26" s="115" t="n"/>
-      <c r="O26" s="197" t="n"/>
+      <c r="O26" s="367" t="n"/>
       <c r="P26" s="115" t="n"/>
-      <c r="Q26" s="197" t="n"/>
+      <c r="Q26" s="367" t="n"/>
       <c r="R26" s="115" t="n"/>
-      <c r="S26" s="197" t="n"/>
+      <c r="S26" s="367" t="n"/>
       <c r="T26" s="115" t="n"/>
     </row>
     <row r="27">
-      <c r="A27" s="194" t="inlineStr">
+      <c r="A27" s="364" t="inlineStr">
         <is>
           <t>#LC9GUPJJG</t>
         </is>
       </c>
-      <c r="B27" s="194" t="n">
+      <c r="B27" s="364" t="n">
         <v>1054</v>
       </c>
-      <c r="C27" s="190" t="n">
+      <c r="C27" s="360" t="n">
         <v>24</v>
       </c>
       <c r="D27" s="106" t="inlineStr">
@@ -2562,53 +2782,53 @@
           <t>raptor2222a</t>
         </is>
       </c>
-      <c r="E27" s="195" t="n">
+      <c r="E27" s="365" t="n">
         <v>5</v>
       </c>
       <c r="F27" s="118" t="n">
         <v>4940</v>
       </c>
-      <c r="G27" s="196" t="n">
+      <c r="G27" s="366" t="n">
         <v>0</v>
       </c>
       <c r="H27" s="109" t="n">
         <v>0</v>
       </c>
-      <c r="I27" s="195" t="n">
+      <c r="I27" s="365" t="n">
         <v>6</v>
       </c>
       <c r="J27" s="106" t="n">
         <v>6971</v>
       </c>
-      <c r="K27" s="195" t="n">
+      <c r="K27" s="365" t="n">
         <v>5</v>
       </c>
       <c r="L27" s="118" t="n">
         <v>4350</v>
       </c>
-      <c r="M27" s="196" t="n">
+      <c r="M27" s="366" t="n">
         <v>0</v>
       </c>
       <c r="N27" s="110" t="n">
         <v>0</v>
       </c>
-      <c r="O27" s="194" t="n"/>
+      <c r="O27" s="364" t="n"/>
       <c r="P27" s="109" t="n"/>
-      <c r="Q27" s="194" t="n"/>
+      <c r="Q27" s="364" t="n"/>
       <c r="R27" s="109" t="n"/>
-      <c r="S27" s="194" t="n"/>
+      <c r="S27" s="364" t="n"/>
       <c r="T27" s="109" t="n"/>
     </row>
     <row r="28">
-      <c r="A28" s="197" t="inlineStr">
+      <c r="A28" s="367" t="inlineStr">
         <is>
           <t>#82QLQCJRJ</t>
         </is>
       </c>
-      <c r="B28" s="197" t="n">
+      <c r="B28" s="367" t="n">
         <v>3004</v>
       </c>
-      <c r="C28" s="186" t="n">
+      <c r="C28" s="356" t="n">
         <v>25</v>
       </c>
       <c r="D28" s="117" t="inlineStr">
@@ -2616,49 +2836,49 @@
           <t>Raging Fury</t>
         </is>
       </c>
-      <c r="E28" s="200" t="n">
+      <c r="E28" s="371" t="n">
         <v>4</v>
       </c>
       <c r="F28" s="117" t="n">
         <v>4850</v>
       </c>
-      <c r="G28" s="199" t="n">
+      <c r="G28" s="369" t="n">
         <v>0</v>
       </c>
       <c r="H28" s="115" t="n">
         <v>0</v>
       </c>
-      <c r="I28" s="198" t="n">
+      <c r="I28" s="368" t="n">
         <v>6</v>
       </c>
       <c r="J28" s="112" t="n">
         <v>6145</v>
       </c>
-      <c r="K28" s="198" t="n">
+      <c r="K28" s="368" t="n">
         <v>6</v>
       </c>
       <c r="L28" s="112" t="n">
         <v>8055</v>
       </c>
-      <c r="M28" s="198" t="n">
+      <c r="M28" s="368" t="n">
         <v>6</v>
       </c>
       <c r="N28" s="112" t="n">
         <v>7115</v>
       </c>
-      <c r="O28" s="199" t="n">
+      <c r="O28" s="369" t="n">
         <v>2</v>
       </c>
       <c r="P28" s="116" t="n">
         <v>2320</v>
       </c>
-      <c r="Q28" s="198" t="n">
+      <c r="Q28" s="368" t="n">
         <v>6</v>
       </c>
       <c r="R28" s="117" t="n">
         <v>4920</v>
       </c>
-      <c r="S28" s="198" t="n">
+      <c r="S28" s="368" t="n">
         <v>6</v>
       </c>
       <c r="T28" s="117" t="n">
@@ -2668,18 +2888,18 @@
     <row r="29">
       <c r="A29" s="120" t="inlineStr">
         <is>
-          <t>#LGCVY0L9P</t>
+          <t>#QPCLYCPV9</t>
         </is>
       </c>
       <c r="B29" s="120" t="n">
-        <v>873</v>
+        <v>977</v>
       </c>
       <c r="C29" s="121" t="n">
         <v>26</v>
       </c>
       <c r="D29" s="122" t="inlineStr">
         <is>
-          <t>Death1wolf</t>
+          <t>aadhirajr</t>
         </is>
       </c>
       <c r="E29" s="123" t="n">
@@ -2694,12 +2914,8 @@
       <c r="H29" s="124" t="n">
         <v>0</v>
       </c>
-      <c r="I29" s="125" t="n">
-        <v>6</v>
-      </c>
-      <c r="J29" s="126" t="n">
-        <v>7998</v>
-      </c>
+      <c r="I29" s="120" t="n"/>
+      <c r="J29" s="124" t="n"/>
       <c r="K29" s="120" t="n"/>
       <c r="L29" s="124" t="n"/>
       <c r="M29" s="120" t="n"/>
@@ -2712,883 +2928,851 @@
       <c r="T29" s="124" t="n"/>
     </row>
     <row r="30">
-      <c r="A30" s="197" t="inlineStr">
+      <c r="A30" s="367" t="inlineStr">
+        <is>
+          <t>#G288QGVQ2</t>
+        </is>
+      </c>
+      <c r="B30" s="367" t="n">
+        <v>909</v>
+      </c>
+      <c r="C30" s="356" t="n">
+        <v>27</v>
+      </c>
+      <c r="D30" s="116" t="inlineStr">
+        <is>
+          <t>Sehaj123</t>
+        </is>
+      </c>
+      <c r="E30" s="369" t="n">
+        <v>0</v>
+      </c>
+      <c r="F30" s="116" t="n">
+        <v>0</v>
+      </c>
+      <c r="G30" s="371" t="n">
+        <v>21</v>
+      </c>
+      <c r="H30" s="115" t="n">
+        <v>0</v>
+      </c>
+      <c r="I30" s="367" t="n"/>
+      <c r="J30" s="115" t="n"/>
+      <c r="K30" s="367" t="n"/>
+      <c r="L30" s="115" t="n"/>
+      <c r="M30" s="367" t="n"/>
+      <c r="N30" s="115" t="n"/>
+      <c r="O30" s="367" t="n"/>
+      <c r="P30" s="115" t="n"/>
+      <c r="Q30" s="367" t="n"/>
+      <c r="R30" s="115" t="n"/>
+      <c r="S30" s="367" t="n"/>
+      <c r="T30" s="115" t="n"/>
+    </row>
+    <row r="31">
+      <c r="A31" s="364" t="inlineStr">
+        <is>
+          <t>#QRUQQUPLV</t>
+        </is>
+      </c>
+      <c r="B31" s="364" t="n">
+        <v>906</v>
+      </c>
+      <c r="C31" s="360" t="n">
+        <v>28</v>
+      </c>
+      <c r="D31" s="110" t="inlineStr">
+        <is>
+          <t>datka/56</t>
+        </is>
+      </c>
+      <c r="E31" s="366" t="n">
+        <v>0</v>
+      </c>
+      <c r="F31" s="110" t="n">
+        <v>0</v>
+      </c>
+      <c r="G31" s="366" t="n">
+        <v>0</v>
+      </c>
+      <c r="H31" s="109" t="n">
+        <v>0</v>
+      </c>
+      <c r="I31" s="364" t="n"/>
+      <c r="J31" s="109" t="n"/>
+      <c r="K31" s="364" t="n"/>
+      <c r="L31" s="109" t="n"/>
+      <c r="M31" s="364" t="n"/>
+      <c r="N31" s="109" t="n"/>
+      <c r="O31" s="364" t="n"/>
+      <c r="P31" s="109" t="n"/>
+      <c r="Q31" s="364" t="n"/>
+      <c r="R31" s="109" t="n"/>
+      <c r="S31" s="364" t="n"/>
+      <c r="T31" s="109" t="n"/>
+    </row>
+    <row r="32">
+      <c r="A32" s="367" t="inlineStr">
+        <is>
+          <t>#LGCVY0L9P</t>
+        </is>
+      </c>
+      <c r="B32" s="367" t="n">
+        <v>873</v>
+      </c>
+      <c r="C32" s="356" t="n">
+        <v>29</v>
+      </c>
+      <c r="D32" s="116" t="inlineStr">
+        <is>
+          <t>Death1wolf</t>
+        </is>
+      </c>
+      <c r="E32" s="369" t="n">
+        <v>0</v>
+      </c>
+      <c r="F32" s="116" t="n">
+        <v>0</v>
+      </c>
+      <c r="G32" s="369" t="n">
+        <v>0</v>
+      </c>
+      <c r="H32" s="115" t="n">
+        <v>0</v>
+      </c>
+      <c r="I32" s="368" t="n">
+        <v>6</v>
+      </c>
+      <c r="J32" s="112" t="n">
+        <v>7998</v>
+      </c>
+      <c r="K32" s="367" t="n"/>
+      <c r="L32" s="115" t="n"/>
+      <c r="M32" s="367" t="n"/>
+      <c r="N32" s="115" t="n"/>
+      <c r="O32" s="367" t="n"/>
+      <c r="P32" s="115" t="n"/>
+      <c r="Q32" s="367" t="n"/>
+      <c r="R32" s="115" t="n"/>
+      <c r="S32" s="367" t="n"/>
+      <c r="T32" s="115" t="n"/>
+    </row>
+    <row r="33">
+      <c r="A33" s="364" t="inlineStr">
         <is>
           <t>#Q9QUUVQ02</t>
         </is>
       </c>
-      <c r="B30" s="197" t="n">
+      <c r="B33" s="364" t="n">
         <v>1438</v>
       </c>
-      <c r="C30" s="186" t="n">
-        <v>27</v>
-      </c>
-      <c r="D30" s="116" t="inlineStr">
+      <c r="C33" s="360" t="n">
+        <v>30</v>
+      </c>
+      <c r="D33" s="110" t="inlineStr">
         <is>
           <t>zach</t>
         </is>
       </c>
-      <c r="E30" s="199" t="n">
-        <v>0</v>
-      </c>
-      <c r="F30" s="116" t="n">
-        <v>0</v>
-      </c>
-      <c r="G30" s="199" t="n">
-        <v>0</v>
-      </c>
-      <c r="H30" s="115" t="n">
-        <v>0</v>
-      </c>
-      <c r="I30" s="198" t="n">
-        <v>6</v>
-      </c>
-      <c r="J30" s="112" t="n">
+      <c r="E33" s="366" t="n">
+        <v>0</v>
+      </c>
+      <c r="F33" s="110" t="n">
+        <v>0</v>
+      </c>
+      <c r="G33" s="366" t="n">
+        <v>0</v>
+      </c>
+      <c r="H33" s="109" t="n">
+        <v>0</v>
+      </c>
+      <c r="I33" s="365" t="n">
+        <v>6</v>
+      </c>
+      <c r="J33" s="106" t="n">
         <v>6106</v>
       </c>
-      <c r="K30" s="197" t="n"/>
-      <c r="L30" s="115" t="n"/>
-      <c r="M30" s="197" t="n"/>
-      <c r="N30" s="115" t="n"/>
-      <c r="O30" s="197" t="n"/>
-      <c r="P30" s="115" t="n"/>
-      <c r="Q30" s="197" t="n"/>
-      <c r="R30" s="115" t="n"/>
-      <c r="S30" s="197" t="n"/>
-      <c r="T30" s="115" t="n"/>
-    </row>
-    <row r="31">
-      <c r="A31" s="194" t="inlineStr">
+      <c r="K33" s="364" t="n"/>
+      <c r="L33" s="109" t="n"/>
+      <c r="M33" s="364" t="n"/>
+      <c r="N33" s="109" t="n"/>
+      <c r="O33" s="364" t="n"/>
+      <c r="P33" s="109" t="n"/>
+      <c r="Q33" s="364" t="n"/>
+      <c r="R33" s="109" t="n"/>
+      <c r="S33" s="364" t="n"/>
+      <c r="T33" s="109" t="n"/>
+    </row>
+    <row r="34">
+      <c r="A34" s="367" t="inlineStr">
         <is>
           <t>#VGG9LYL0</t>
         </is>
       </c>
-      <c r="B31" s="194" t="n">
+      <c r="B34" s="367" t="n">
         <v>1035</v>
       </c>
-      <c r="C31" s="190" t="n">
-        <v>28</v>
-      </c>
-      <c r="D31" s="110" t="inlineStr">
+      <c r="C34" s="356" t="n">
+        <v>31</v>
+      </c>
+      <c r="D34" s="116" t="inlineStr">
         <is>
           <t>ptripp1048</t>
         </is>
       </c>
-      <c r="E31" s="196" t="n">
-        <v>0</v>
-      </c>
-      <c r="F31" s="110" t="n">
-        <v>0</v>
-      </c>
-      <c r="G31" s="196" t="n">
-        <v>0</v>
-      </c>
-      <c r="H31" s="109" t="n">
-        <v>0</v>
-      </c>
-      <c r="I31" s="195" t="n">
-        <v>6</v>
-      </c>
-      <c r="J31" s="106" t="n">
+      <c r="E34" s="369" t="n">
+        <v>0</v>
+      </c>
+      <c r="F34" s="116" t="n">
+        <v>0</v>
+      </c>
+      <c r="G34" s="369" t="n">
+        <v>0</v>
+      </c>
+      <c r="H34" s="115" t="n">
+        <v>0</v>
+      </c>
+      <c r="I34" s="368" t="n">
+        <v>6</v>
+      </c>
+      <c r="J34" s="112" t="n">
         <v>6023</v>
       </c>
-      <c r="K31" s="196" t="n">
-        <v>0</v>
-      </c>
-      <c r="L31" s="110" t="n">
-        <v>0</v>
-      </c>
-      <c r="M31" s="194" t="n"/>
-      <c r="N31" s="109" t="n"/>
-      <c r="O31" s="194" t="n"/>
-      <c r="P31" s="109" t="n"/>
-      <c r="Q31" s="194" t="n"/>
-      <c r="R31" s="109" t="n"/>
-      <c r="S31" s="194" t="n"/>
-      <c r="T31" s="109" t="n"/>
-    </row>
-    <row r="32">
-      <c r="A32" s="197" t="inlineStr">
+      <c r="K34" s="369" t="n">
+        <v>0</v>
+      </c>
+      <c r="L34" s="116" t="n">
+        <v>0</v>
+      </c>
+      <c r="M34" s="367" t="n"/>
+      <c r="N34" s="115" t="n"/>
+      <c r="O34" s="367" t="n"/>
+      <c r="P34" s="115" t="n"/>
+      <c r="Q34" s="367" t="n"/>
+      <c r="R34" s="115" t="n"/>
+      <c r="S34" s="367" t="n"/>
+      <c r="T34" s="115" t="n"/>
+    </row>
+    <row r="35">
+      <c r="A35" s="364" t="inlineStr">
         <is>
           <t>#QLG0VJG2J</t>
         </is>
       </c>
-      <c r="B32" s="197" t="n">
-        <v>1407</v>
-      </c>
-      <c r="C32" s="186" t="n">
-        <v>29</v>
-      </c>
-      <c r="D32" s="116" t="inlineStr">
+      <c r="B35" s="364" t="n">
+        <v>1463</v>
+      </c>
+      <c r="C35" s="360" t="n">
+        <v>32</v>
+      </c>
+      <c r="D35" s="110" t="inlineStr">
         <is>
           <t>PocketRocket</t>
         </is>
       </c>
-      <c r="E32" s="199" t="n">
-        <v>0</v>
-      </c>
-      <c r="F32" s="116" t="n">
-        <v>0</v>
-      </c>
-      <c r="G32" s="199" t="n">
-        <v>0</v>
-      </c>
-      <c r="H32" s="115" t="n">
-        <v>0</v>
-      </c>
-      <c r="I32" s="198" t="n">
-        <v>6</v>
-      </c>
-      <c r="J32" s="117" t="n">
+      <c r="E35" s="366" t="n">
+        <v>0</v>
+      </c>
+      <c r="F35" s="110" t="n">
+        <v>0</v>
+      </c>
+      <c r="G35" s="366" t="n">
+        <v>0</v>
+      </c>
+      <c r="H35" s="109" t="n">
+        <v>0</v>
+      </c>
+      <c r="I35" s="365" t="n">
+        <v>6</v>
+      </c>
+      <c r="J35" s="118" t="n">
         <v>5660</v>
       </c>
-      <c r="K32" s="200" t="n">
+      <c r="K35" s="370" t="n">
         <v>4</v>
       </c>
-      <c r="L32" s="117" t="n">
+      <c r="L35" s="118" t="n">
         <v>4327</v>
       </c>
-      <c r="M32" s="200" t="n">
+      <c r="M35" s="370" t="n">
         <v>4</v>
       </c>
-      <c r="N32" s="117" t="n">
+      <c r="N35" s="118" t="n">
         <v>5215</v>
       </c>
-      <c r="O32" s="197" t="n"/>
-      <c r="P32" s="115" t="n"/>
-      <c r="Q32" s="197" t="n"/>
-      <c r="R32" s="115" t="n"/>
-      <c r="S32" s="197" t="n"/>
-      <c r="T32" s="115" t="n"/>
-    </row>
-    <row r="33">
-      <c r="A33" s="194" t="inlineStr">
+      <c r="O35" s="364" t="n"/>
+      <c r="P35" s="109" t="n"/>
+      <c r="Q35" s="364" t="n"/>
+      <c r="R35" s="109" t="n"/>
+      <c r="S35" s="364" t="n"/>
+      <c r="T35" s="109" t="n"/>
+    </row>
+    <row r="36">
+      <c r="A36" s="367" t="inlineStr">
+        <is>
+          <t>#QLUV29GGJ</t>
+        </is>
+      </c>
+      <c r="B36" s="367" t="n">
+        <v>1040</v>
+      </c>
+      <c r="C36" s="356" t="n">
+        <v>33</v>
+      </c>
+      <c r="D36" s="116" t="inlineStr">
+        <is>
+          <t>Kukoshibo</t>
+        </is>
+      </c>
+      <c r="E36" s="369" t="n">
+        <v>0</v>
+      </c>
+      <c r="F36" s="116" t="n">
+        <v>0</v>
+      </c>
+      <c r="G36" s="369" t="n">
+        <v>0</v>
+      </c>
+      <c r="H36" s="115" t="n">
+        <v>0</v>
+      </c>
+      <c r="I36" s="369" t="n">
+        <v>0</v>
+      </c>
+      <c r="J36" s="116" t="n">
+        <v>0</v>
+      </c>
+      <c r="K36" s="367" t="n"/>
+      <c r="L36" s="115" t="n"/>
+      <c r="M36" s="367" t="n"/>
+      <c r="N36" s="115" t="n"/>
+      <c r="O36" s="367" t="n"/>
+      <c r="P36" s="115" t="n"/>
+      <c r="Q36" s="367" t="n"/>
+      <c r="R36" s="115" t="n"/>
+      <c r="S36" s="367" t="n"/>
+      <c r="T36" s="115" t="n"/>
+    </row>
+    <row r="37">
+      <c r="A37" s="364" t="inlineStr">
+        <is>
+          <t>#Q0U0CRCGJ</t>
+        </is>
+      </c>
+      <c r="B37" s="364" t="n">
+        <v>691</v>
+      </c>
+      <c r="C37" s="360" t="n">
+        <v>34</v>
+      </c>
+      <c r="D37" s="110" t="inlineStr">
+        <is>
+          <t>Sn0wc0ne</t>
+        </is>
+      </c>
+      <c r="E37" s="366" t="n">
+        <v>0</v>
+      </c>
+      <c r="F37" s="110" t="n">
+        <v>0</v>
+      </c>
+      <c r="G37" s="366" t="n">
+        <v>0</v>
+      </c>
+      <c r="H37" s="109" t="n">
+        <v>0</v>
+      </c>
+      <c r="I37" s="366" t="n">
+        <v>0</v>
+      </c>
+      <c r="J37" s="110" t="n">
+        <v>0</v>
+      </c>
+      <c r="K37" s="364" t="n"/>
+      <c r="L37" s="109" t="n"/>
+      <c r="M37" s="364" t="n"/>
+      <c r="N37" s="109" t="n"/>
+      <c r="O37" s="364" t="n"/>
+      <c r="P37" s="109" t="n"/>
+      <c r="Q37" s="364" t="n"/>
+      <c r="R37" s="109" t="n"/>
+      <c r="S37" s="364" t="n"/>
+      <c r="T37" s="109" t="n"/>
+    </row>
+    <row r="38">
+      <c r="A38" s="367" t="inlineStr">
         <is>
           <t>#QY0VGPQGQ</t>
         </is>
       </c>
-      <c r="B33" s="194" t="n">
+      <c r="B38" s="367" t="n">
         <v>613</v>
       </c>
-      <c r="C33" s="190" t="n">
-        <v>30</v>
-      </c>
-      <c r="D33" s="110" t="inlineStr">
+      <c r="C38" s="356" t="n">
+        <v>35</v>
+      </c>
+      <c r="D38" s="116" t="inlineStr">
         <is>
           <t>killerjones</t>
         </is>
       </c>
-      <c r="E33" s="196" t="n">
-        <v>0</v>
-      </c>
-      <c r="F33" s="110" t="n">
-        <v>0</v>
-      </c>
-      <c r="G33" s="196" t="n">
-        <v>0</v>
-      </c>
-      <c r="H33" s="109" t="n">
-        <v>0</v>
-      </c>
-      <c r="I33" s="196" t="n">
-        <v>0</v>
-      </c>
-      <c r="J33" s="110" t="n">
-        <v>0</v>
-      </c>
-      <c r="K33" s="195" t="n">
-        <v>6</v>
-      </c>
-      <c r="L33" s="106" t="n">
+      <c r="E38" s="369" t="n">
+        <v>0</v>
+      </c>
+      <c r="F38" s="116" t="n">
+        <v>0</v>
+      </c>
+      <c r="G38" s="369" t="n">
+        <v>0</v>
+      </c>
+      <c r="H38" s="115" t="n">
+        <v>0</v>
+      </c>
+      <c r="I38" s="369" t="n">
+        <v>0</v>
+      </c>
+      <c r="J38" s="116" t="n">
+        <v>0</v>
+      </c>
+      <c r="K38" s="368" t="n">
+        <v>6</v>
+      </c>
+      <c r="L38" s="112" t="n">
         <v>6320</v>
       </c>
-      <c r="M33" s="194" t="n"/>
-      <c r="N33" s="109" t="n"/>
-      <c r="O33" s="194" t="n"/>
-      <c r="P33" s="109" t="n"/>
-      <c r="Q33" s="194" t="n"/>
-      <c r="R33" s="109" t="n"/>
-      <c r="S33" s="194" t="n"/>
-      <c r="T33" s="109" t="n"/>
-    </row>
-    <row r="34">
-      <c r="A34" s="197" t="inlineStr">
+      <c r="M38" s="367" t="n"/>
+      <c r="N38" s="115" t="n"/>
+      <c r="O38" s="367" t="n"/>
+      <c r="P38" s="115" t="n"/>
+      <c r="Q38" s="367" t="n"/>
+      <c r="R38" s="115" t="n"/>
+      <c r="S38" s="367" t="n"/>
+      <c r="T38" s="115" t="n"/>
+    </row>
+    <row r="39">
+      <c r="A39" s="364" t="inlineStr">
         <is>
           <t>#QL8LVLYG8</t>
         </is>
       </c>
-      <c r="B34" s="197" t="n">
+      <c r="B39" s="364" t="n">
         <v>971</v>
       </c>
-      <c r="C34" s="186" t="n">
+      <c r="C39" s="360" t="n">
+        <v>36</v>
+      </c>
+      <c r="D39" s="110" t="inlineStr">
+        <is>
+          <t>Some guy</t>
+        </is>
+      </c>
+      <c r="E39" s="366" t="n">
+        <v>0</v>
+      </c>
+      <c r="F39" s="110" t="n">
+        <v>0</v>
+      </c>
+      <c r="G39" s="366" t="n">
+        <v>0</v>
+      </c>
+      <c r="H39" s="109" t="n">
+        <v>0</v>
+      </c>
+      <c r="I39" s="366" t="n">
+        <v>0</v>
+      </c>
+      <c r="J39" s="110" t="n">
+        <v>0</v>
+      </c>
+      <c r="K39" s="366" t="n">
+        <v>2</v>
+      </c>
+      <c r="L39" s="110" t="n">
+        <v>2650</v>
+      </c>
+      <c r="M39" s="366" t="n">
+        <v>0</v>
+      </c>
+      <c r="N39" s="110" t="n">
+        <v>0</v>
+      </c>
+      <c r="O39" s="365" t="n">
+        <v>6</v>
+      </c>
+      <c r="P39" s="106" t="n">
+        <v>6917</v>
+      </c>
+      <c r="Q39" s="366" t="n">
+        <v>0</v>
+      </c>
+      <c r="R39" s="110" t="n">
+        <v>0</v>
+      </c>
+      <c r="S39" s="366" t="n">
+        <v>2</v>
+      </c>
+      <c r="T39" s="110" t="n">
+        <v>1965</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="367" t="inlineStr">
+        <is>
+          <t>#QQL28Y2UL</t>
+        </is>
+      </c>
+      <c r="B40" s="367" t="n">
+        <v>1085</v>
+      </c>
+      <c r="C40" s="356" t="n">
+        <v>37</v>
+      </c>
+      <c r="D40" s="116" t="inlineStr">
+        <is>
+          <t>SUPoT</t>
+        </is>
+      </c>
+      <c r="E40" s="369" t="n">
+        <v>0</v>
+      </c>
+      <c r="F40" s="116" t="n">
+        <v>0</v>
+      </c>
+      <c r="G40" s="369" t="n">
+        <v>0</v>
+      </c>
+      <c r="H40" s="115" t="n">
         <v>31</v>
       </c>
-      <c r="D34" s="116" t="inlineStr">
-        <is>
-          <t>Some guy</t>
-        </is>
-      </c>
-      <c r="E34" s="199" t="n">
-        <v>0</v>
-      </c>
-      <c r="F34" s="116" t="n">
-        <v>0</v>
-      </c>
-      <c r="G34" s="199" t="n">
-        <v>0</v>
-      </c>
-      <c r="H34" s="115" t="n">
-        <v>0</v>
-      </c>
-      <c r="I34" s="199" t="n">
-        <v>0</v>
-      </c>
-      <c r="J34" s="116" t="n">
-        <v>0</v>
-      </c>
-      <c r="K34" s="199" t="n">
-        <v>2</v>
-      </c>
-      <c r="L34" s="116" t="n">
-        <v>2650</v>
-      </c>
-      <c r="M34" s="199" t="n">
-        <v>0</v>
-      </c>
-      <c r="N34" s="116" t="n">
-        <v>0</v>
-      </c>
-      <c r="O34" s="198" t="n">
-        <v>6</v>
-      </c>
-      <c r="P34" s="112" t="n">
-        <v>6917</v>
-      </c>
-      <c r="Q34" s="199" t="n">
-        <v>0</v>
-      </c>
-      <c r="R34" s="116" t="n">
-        <v>0</v>
-      </c>
-      <c r="S34" s="199" t="n">
-        <v>2</v>
-      </c>
-      <c r="T34" s="116" t="n">
-        <v>1965</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" s="194" t="inlineStr">
+      <c r="I40" s="369" t="n">
+        <v>0</v>
+      </c>
+      <c r="J40" s="116" t="n">
+        <v>0</v>
+      </c>
+      <c r="K40" s="369" t="n">
+        <v>0</v>
+      </c>
+      <c r="L40" s="116" t="n">
+        <v>0</v>
+      </c>
+      <c r="M40" s="367" t="n"/>
+      <c r="N40" s="115" t="n"/>
+      <c r="O40" s="367" t="n"/>
+      <c r="P40" s="115" t="n"/>
+      <c r="Q40" s="367" t="n"/>
+      <c r="R40" s="115" t="n"/>
+      <c r="S40" s="367" t="n"/>
+      <c r="T40" s="115" t="n"/>
+    </row>
+    <row r="41">
+      <c r="A41" s="364" t="inlineStr">
+        <is>
+          <t>#QV8RY9UC8</t>
+        </is>
+      </c>
+      <c r="B41" s="364" t="n">
+        <v>747</v>
+      </c>
+      <c r="C41" s="360" t="n">
+        <v>38</v>
+      </c>
+      <c r="D41" s="110" t="inlineStr">
+        <is>
+          <t>Apollo</t>
+        </is>
+      </c>
+      <c r="E41" s="366" t="n">
+        <v>0</v>
+      </c>
+      <c r="F41" s="110" t="n">
+        <v>0</v>
+      </c>
+      <c r="G41" s="366" t="n">
+        <v>0</v>
+      </c>
+      <c r="H41" s="109" t="n">
+        <v>0</v>
+      </c>
+      <c r="I41" s="366" t="n">
+        <v>0</v>
+      </c>
+      <c r="J41" s="110" t="n">
+        <v>0</v>
+      </c>
+      <c r="K41" s="366" t="n">
+        <v>0</v>
+      </c>
+      <c r="L41" s="110" t="n">
+        <v>0</v>
+      </c>
+      <c r="M41" s="364" t="n"/>
+      <c r="N41" s="109" t="n"/>
+      <c r="O41" s="364" t="n"/>
+      <c r="P41" s="109" t="n"/>
+      <c r="Q41" s="364" t="n"/>
+      <c r="R41" s="109" t="n"/>
+      <c r="S41" s="364" t="n"/>
+      <c r="T41" s="109" t="n"/>
+    </row>
+    <row r="42">
+      <c r="A42" s="367" t="inlineStr">
         <is>
           <t>#QLGYRVPU0</t>
         </is>
       </c>
-      <c r="B35" s="194" t="n">
+      <c r="B42" s="367" t="n">
         <v>1198</v>
       </c>
-      <c r="C35" s="190" t="n">
-        <v>32</v>
-      </c>
-      <c r="D35" s="110" t="inlineStr">
+      <c r="C42" s="356" t="n">
+        <v>39</v>
+      </c>
+      <c r="D42" s="116" t="inlineStr">
         <is>
           <t>Black.Boy.</t>
         </is>
       </c>
-      <c r="E35" s="196" t="n">
-        <v>0</v>
-      </c>
-      <c r="F35" s="110" t="n">
-        <v>0</v>
-      </c>
-      <c r="G35" s="196" t="n">
-        <v>0</v>
-      </c>
-      <c r="H35" s="109" t="n">
+      <c r="E42" s="369" t="n">
+        <v>0</v>
+      </c>
+      <c r="F42" s="116" t="n">
+        <v>0</v>
+      </c>
+      <c r="G42" s="369" t="n">
+        <v>0</v>
+      </c>
+      <c r="H42" s="115" t="n">
         <v>15</v>
       </c>
-      <c r="I35" s="196" t="n">
-        <v>0</v>
-      </c>
-      <c r="J35" s="110" t="n">
-        <v>0</v>
-      </c>
-      <c r="K35" s="196" t="n">
-        <v>0</v>
-      </c>
-      <c r="L35" s="110" t="n">
-        <v>0</v>
-      </c>
-      <c r="M35" s="194" t="n"/>
-      <c r="N35" s="109" t="n"/>
-      <c r="O35" s="194" t="n"/>
-      <c r="P35" s="109" t="n"/>
-      <c r="Q35" s="194" t="n"/>
-      <c r="R35" s="109" t="n"/>
-      <c r="S35" s="194" t="n"/>
-      <c r="T35" s="109" t="n"/>
-    </row>
-    <row r="36">
-      <c r="A36" s="197" t="inlineStr">
-        <is>
-          <t>#G288QGVQ2</t>
-        </is>
-      </c>
-      <c r="B36" s="197" t="n">
-        <v>909</v>
-      </c>
-      <c r="C36" s="186" t="n">
-        <v>33</v>
-      </c>
-      <c r="D36" s="116" t="inlineStr">
-        <is>
-          <t>Sehaj123</t>
-        </is>
-      </c>
-      <c r="E36" s="199" t="n">
-        <v>0</v>
-      </c>
-      <c r="F36" s="116" t="n">
-        <v>0</v>
-      </c>
-      <c r="G36" s="199" t="n">
-        <v>21</v>
-      </c>
-      <c r="H36" s="115" t="n">
-        <v>0</v>
-      </c>
-      <c r="I36" s="197" t="n"/>
-      <c r="J36" s="115" t="n"/>
-      <c r="K36" s="197" t="n"/>
-      <c r="L36" s="115" t="n"/>
-      <c r="M36" s="197" t="n"/>
-      <c r="N36" s="115" t="n"/>
-      <c r="O36" s="197" t="n"/>
-      <c r="P36" s="115" t="n"/>
-      <c r="Q36" s="197" t="n"/>
-      <c r="R36" s="115" t="n"/>
-      <c r="S36" s="197" t="n"/>
-      <c r="T36" s="115" t="n"/>
-    </row>
-    <row r="37">
-      <c r="A37" s="194" t="inlineStr">
+      <c r="I42" s="369" t="n">
+        <v>0</v>
+      </c>
+      <c r="J42" s="116" t="n">
+        <v>0</v>
+      </c>
+      <c r="K42" s="369" t="n">
+        <v>0</v>
+      </c>
+      <c r="L42" s="116" t="n">
+        <v>0</v>
+      </c>
+      <c r="M42" s="367" t="n"/>
+      <c r="N42" s="115" t="n"/>
+      <c r="O42" s="367" t="n"/>
+      <c r="P42" s="115" t="n"/>
+      <c r="Q42" s="367" t="n"/>
+      <c r="R42" s="115" t="n"/>
+      <c r="S42" s="367" t="n"/>
+      <c r="T42" s="115" t="n"/>
+    </row>
+    <row r="43">
+      <c r="A43" s="364" t="inlineStr">
+        <is>
+          <t>#QJC8LQU9U</t>
+        </is>
+      </c>
+      <c r="B43" s="364" t="n">
+        <v>998</v>
+      </c>
+      <c r="C43" s="360" t="n">
+        <v>40</v>
+      </c>
+      <c r="D43" s="110" t="inlineStr">
+        <is>
+          <t>Master01</t>
+        </is>
+      </c>
+      <c r="E43" s="366" t="n">
+        <v>0</v>
+      </c>
+      <c r="F43" s="110" t="n">
+        <v>0</v>
+      </c>
+      <c r="G43" s="366" t="n">
+        <v>0</v>
+      </c>
+      <c r="H43" s="109" t="n">
+        <v>0</v>
+      </c>
+      <c r="I43" s="366" t="n">
+        <v>0</v>
+      </c>
+      <c r="J43" s="110" t="n">
+        <v>0</v>
+      </c>
+      <c r="K43" s="366" t="n">
+        <v>0</v>
+      </c>
+      <c r="L43" s="110" t="n">
+        <v>0</v>
+      </c>
+      <c r="M43" s="366" t="n">
+        <v>0</v>
+      </c>
+      <c r="N43" s="110" t="n">
+        <v>0</v>
+      </c>
+      <c r="O43" s="365" t="n">
+        <v>6</v>
+      </c>
+      <c r="P43" s="118" t="n">
+        <v>5415</v>
+      </c>
+      <c r="Q43" s="365" t="n">
+        <v>6</v>
+      </c>
+      <c r="R43" s="118" t="n">
+        <v>4835</v>
+      </c>
+      <c r="S43" s="365" t="n">
+        <v>5</v>
+      </c>
+      <c r="T43" s="118" t="n">
+        <v>4055</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="367" t="inlineStr">
+        <is>
+          <t>#QV8JJ0URU</t>
+        </is>
+      </c>
+      <c r="B44" s="367" t="n">
+        <v>741</v>
+      </c>
+      <c r="C44" s="356" t="n">
+        <v>41</v>
+      </c>
+      <c r="D44" s="116" t="inlineStr">
+        <is>
+          <t>✨Jacob</t>
+        </is>
+      </c>
+      <c r="E44" s="369" t="n">
+        <v>0</v>
+      </c>
+      <c r="F44" s="116" t="n">
+        <v>0</v>
+      </c>
+      <c r="G44" s="369" t="n">
+        <v>0</v>
+      </c>
+      <c r="H44" s="115" t="n">
+        <v>0</v>
+      </c>
+      <c r="I44" s="369" t="n">
+        <v>0</v>
+      </c>
+      <c r="J44" s="116" t="n">
+        <v>0</v>
+      </c>
+      <c r="K44" s="369" t="n">
+        <v>0</v>
+      </c>
+      <c r="L44" s="116" t="n">
+        <v>0</v>
+      </c>
+      <c r="M44" s="369" t="n">
+        <v>0</v>
+      </c>
+      <c r="N44" s="116" t="n">
+        <v>0</v>
+      </c>
+      <c r="O44" s="369" t="n">
+        <v>0</v>
+      </c>
+      <c r="P44" s="116" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q44" s="368" t="n">
+        <v>6</v>
+      </c>
+      <c r="R44" s="112" t="n">
+        <v>7385</v>
+      </c>
+      <c r="S44" s="368" t="n">
+        <v>6</v>
+      </c>
+      <c r="T44" s="112" t="n">
+        <v>9155</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="364" t="inlineStr">
         <is>
           <t>#QY8L2GLUR</t>
         </is>
       </c>
-      <c r="B37" s="194" t="n">
+      <c r="B45" s="364" t="n">
         <v>907</v>
       </c>
-      <c r="C37" s="190" t="n">
-        <v>34</v>
-      </c>
-      <c r="D37" s="110" t="inlineStr">
+      <c r="C45" s="360" t="n">
+        <v>42</v>
+      </c>
+      <c r="D45" s="110" t="inlineStr">
         <is>
           <t>Huy</t>
         </is>
       </c>
-      <c r="E37" s="196" t="n">
-        <v>0</v>
-      </c>
-      <c r="F37" s="110" t="n">
-        <v>0</v>
-      </c>
-      <c r="G37" s="196" t="n">
-        <v>0</v>
-      </c>
-      <c r="H37" s="109" t="n">
-        <v>0</v>
-      </c>
-      <c r="I37" s="196" t="n">
-        <v>0</v>
-      </c>
-      <c r="J37" s="110" t="n">
-        <v>0</v>
-      </c>
-      <c r="K37" s="196" t="n">
-        <v>0</v>
-      </c>
-      <c r="L37" s="110" t="n">
-        <v>0</v>
-      </c>
-      <c r="M37" s="196" t="n">
-        <v>0</v>
-      </c>
-      <c r="N37" s="110" t="n">
-        <v>0</v>
-      </c>
-      <c r="O37" s="196" t="n">
-        <v>0</v>
-      </c>
-      <c r="P37" s="110" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q37" s="195" t="n">
-        <v>6</v>
-      </c>
-      <c r="R37" s="106" t="n">
+      <c r="E45" s="366" t="n">
+        <v>0</v>
+      </c>
+      <c r="F45" s="110" t="n">
+        <v>0</v>
+      </c>
+      <c r="G45" s="366" t="n">
+        <v>0</v>
+      </c>
+      <c r="H45" s="109" t="n">
+        <v>0</v>
+      </c>
+      <c r="I45" s="366" t="n">
+        <v>0</v>
+      </c>
+      <c r="J45" s="110" t="n">
+        <v>0</v>
+      </c>
+      <c r="K45" s="366" t="n">
+        <v>0</v>
+      </c>
+      <c r="L45" s="110" t="n">
+        <v>0</v>
+      </c>
+      <c r="M45" s="366" t="n">
+        <v>0</v>
+      </c>
+      <c r="N45" s="110" t="n">
+        <v>0</v>
+      </c>
+      <c r="O45" s="366" t="n">
+        <v>0</v>
+      </c>
+      <c r="P45" s="110" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q45" s="365" t="n">
+        <v>6</v>
+      </c>
+      <c r="R45" s="106" t="n">
         <v>6995</v>
       </c>
-      <c r="S37" s="195" t="n">
-        <v>6</v>
-      </c>
-      <c r="T37" s="106" t="n">
+      <c r="S45" s="365" t="n">
+        <v>6</v>
+      </c>
+      <c r="T45" s="106" t="n">
         <v>6055</v>
       </c>
     </row>
-    <row r="38">
-      <c r="A38" s="197" t="inlineStr">
-        <is>
-          <t>#QRUQQUPLV</t>
-        </is>
-      </c>
-      <c r="B38" s="197" t="n">
-        <v>906</v>
-      </c>
-      <c r="C38" s="186" t="n">
-        <v>35</v>
-      </c>
-      <c r="D38" s="116" t="inlineStr">
-        <is>
-          <t>datka/56</t>
-        </is>
-      </c>
-      <c r="E38" s="199" t="n">
-        <v>0</v>
-      </c>
-      <c r="F38" s="116" t="n">
-        <v>0</v>
-      </c>
-      <c r="G38" s="199" t="n">
-        <v>0</v>
-      </c>
-      <c r="H38" s="115" t="n">
-        <v>0</v>
-      </c>
-      <c r="I38" s="197" t="n"/>
-      <c r="J38" s="115" t="n"/>
-      <c r="K38" s="197" t="n"/>
-      <c r="L38" s="115" t="n"/>
-      <c r="M38" s="197" t="n"/>
-      <c r="N38" s="115" t="n"/>
-      <c r="O38" s="197" t="n"/>
-      <c r="P38" s="115" t="n"/>
-      <c r="Q38" s="197" t="n"/>
-      <c r="R38" s="115" t="n"/>
-      <c r="S38" s="197" t="n"/>
-      <c r="T38" s="115" t="n"/>
-    </row>
-    <row r="39">
-      <c r="A39" s="194" t="inlineStr">
-        <is>
-          <t>#L9QL9YQQY</t>
-        </is>
-      </c>
-      <c r="B39" s="194" t="n">
-        <v>975</v>
-      </c>
-      <c r="C39" s="190" t="n">
-        <v>36</v>
-      </c>
-      <c r="D39" s="110" t="inlineStr">
-        <is>
-          <t>Ima Chad</t>
-        </is>
-      </c>
-      <c r="E39" s="196" t="n">
-        <v>0</v>
-      </c>
-      <c r="F39" s="110" t="n">
-        <v>0</v>
-      </c>
-      <c r="G39" s="196" t="n">
-        <v>0</v>
-      </c>
-      <c r="H39" s="109" t="n">
-        <v>0</v>
-      </c>
-      <c r="I39" s="196" t="n">
-        <v>0</v>
-      </c>
-      <c r="J39" s="110" t="n">
-        <v>0</v>
-      </c>
-      <c r="K39" s="196" t="n">
-        <v>0</v>
-      </c>
-      <c r="L39" s="110" t="n">
-        <v>0</v>
-      </c>
-      <c r="M39" s="196" t="n">
-        <v>0</v>
-      </c>
-      <c r="N39" s="110" t="n">
-        <v>0</v>
-      </c>
-      <c r="O39" s="196" t="n">
-        <v>0</v>
-      </c>
-      <c r="P39" s="110" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q39" s="196" t="n">
-        <v>0</v>
-      </c>
-      <c r="R39" s="110" t="n">
-        <v>0</v>
-      </c>
-      <c r="S39" s="195" t="n">
-        <v>5</v>
-      </c>
-      <c r="T39" s="110" t="n">
-        <v>3360</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" s="197" t="inlineStr">
-        <is>
-          <t>#QJC8LQU9U</t>
-        </is>
-      </c>
-      <c r="B40" s="197" t="n">
-        <v>998</v>
-      </c>
-      <c r="C40" s="186" t="n">
-        <v>37</v>
-      </c>
-      <c r="D40" s="116" t="inlineStr">
-        <is>
-          <t>Master01</t>
-        </is>
-      </c>
-      <c r="E40" s="199" t="n">
-        <v>0</v>
-      </c>
-      <c r="F40" s="116" t="n">
-        <v>0</v>
-      </c>
-      <c r="G40" s="199" t="n">
-        <v>0</v>
-      </c>
-      <c r="H40" s="115" t="n">
-        <v>0</v>
-      </c>
-      <c r="I40" s="199" t="n">
-        <v>0</v>
-      </c>
-      <c r="J40" s="116" t="n">
-        <v>0</v>
-      </c>
-      <c r="K40" s="199" t="n">
-        <v>0</v>
-      </c>
-      <c r="L40" s="116" t="n">
-        <v>0</v>
-      </c>
-      <c r="M40" s="199" t="n">
-        <v>0</v>
-      </c>
-      <c r="N40" s="116" t="n">
-        <v>0</v>
-      </c>
-      <c r="O40" s="198" t="n">
-        <v>6</v>
-      </c>
-      <c r="P40" s="117" t="n">
-        <v>5415</v>
-      </c>
-      <c r="Q40" s="198" t="n">
-        <v>6</v>
-      </c>
-      <c r="R40" s="117" t="n">
-        <v>4835</v>
-      </c>
-      <c r="S40" s="198" t="n">
-        <v>5</v>
-      </c>
-      <c r="T40" s="117" t="n">
-        <v>4055</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" s="194" t="inlineStr">
-        <is>
-          <t>#QQL8C29CY</t>
-        </is>
-      </c>
-      <c r="B41" s="194" t="n">
-        <v>864</v>
-      </c>
-      <c r="C41" s="190" t="n">
-        <v>38</v>
-      </c>
-      <c r="D41" s="110" t="inlineStr">
-        <is>
-          <t>TypicalTeague#2</t>
-        </is>
-      </c>
-      <c r="E41" s="196" t="n">
-        <v>0</v>
-      </c>
-      <c r="F41" s="110" t="n">
-        <v>0</v>
-      </c>
-      <c r="G41" s="196" t="n">
-        <v>0</v>
-      </c>
-      <c r="H41" s="109" t="n">
-        <v>0</v>
-      </c>
-      <c r="I41" s="196" t="n">
-        <v>0</v>
-      </c>
-      <c r="J41" s="110" t="n">
-        <v>0</v>
-      </c>
-      <c r="K41" s="196" t="n">
-        <v>0</v>
-      </c>
-      <c r="L41" s="110" t="n">
-        <v>0</v>
-      </c>
-      <c r="M41" s="196" t="n">
-        <v>0</v>
-      </c>
-      <c r="N41" s="110" t="n">
-        <v>0</v>
-      </c>
-      <c r="O41" s="196" t="n">
-        <v>0</v>
-      </c>
-      <c r="P41" s="110" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q41" s="195" t="n">
-        <v>5</v>
-      </c>
-      <c r="R41" s="118" t="n">
-        <v>4070</v>
-      </c>
-      <c r="S41" s="195" t="n">
-        <v>6</v>
-      </c>
-      <c r="T41" s="106" t="n">
-        <v>6410</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" s="197" t="inlineStr">
-        <is>
-          <t>#QQL28Y2UL</t>
-        </is>
-      </c>
-      <c r="B42" s="197" t="n">
-        <v>1085</v>
-      </c>
-      <c r="C42" s="186" t="n">
-        <v>39</v>
-      </c>
-      <c r="D42" s="116" t="inlineStr">
-        <is>
-          <t>SUPoT</t>
-        </is>
-      </c>
-      <c r="E42" s="199" t="n">
-        <v>0</v>
-      </c>
-      <c r="F42" s="116" t="n">
-        <v>0</v>
-      </c>
-      <c r="G42" s="199" t="n">
-        <v>0</v>
-      </c>
-      <c r="H42" s="115" t="n">
-        <v>31</v>
-      </c>
-      <c r="I42" s="199" t="n">
-        <v>0</v>
-      </c>
-      <c r="J42" s="116" t="n">
-        <v>0</v>
-      </c>
-      <c r="K42" s="199" t="n">
-        <v>0</v>
-      </c>
-      <c r="L42" s="116" t="n">
-        <v>0</v>
-      </c>
-      <c r="M42" s="197" t="n"/>
-      <c r="N42" s="115" t="n"/>
-      <c r="O42" s="197" t="n"/>
-      <c r="P42" s="115" t="n"/>
-      <c r="Q42" s="197" t="n"/>
-      <c r="R42" s="115" t="n"/>
-      <c r="S42" s="197" t="n"/>
-      <c r="T42" s="115" t="n"/>
-    </row>
-    <row r="43">
-      <c r="A43" s="194" t="inlineStr">
-        <is>
-          <t>#LPR9RPCY9</t>
-        </is>
-      </c>
-      <c r="B43" s="194" t="n">
-        <v>980</v>
-      </c>
-      <c r="C43" s="190" t="n">
-        <v>40</v>
-      </c>
-      <c r="D43" s="110" t="inlineStr">
-        <is>
-          <t>sayhuss17</t>
-        </is>
-      </c>
-      <c r="E43" s="196" t="n">
-        <v>0</v>
-      </c>
-      <c r="F43" s="110" t="n">
-        <v>0</v>
-      </c>
-      <c r="G43" s="196" t="n">
-        <v>0</v>
-      </c>
-      <c r="H43" s="109" t="n">
-        <v>0</v>
-      </c>
-      <c r="I43" s="196" t="n">
-        <v>0</v>
-      </c>
-      <c r="J43" s="110" t="n">
-        <v>0</v>
-      </c>
-      <c r="K43" s="196" t="n">
-        <v>0</v>
-      </c>
-      <c r="L43" s="110" t="n">
-        <v>0</v>
-      </c>
-      <c r="M43" s="196" t="n">
-        <v>0</v>
-      </c>
-      <c r="N43" s="110" t="n">
-        <v>0</v>
-      </c>
-      <c r="O43" s="196" t="n">
-        <v>0</v>
-      </c>
-      <c r="P43" s="110" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q43" s="201" t="n">
-        <v>4</v>
-      </c>
-      <c r="R43" s="118" t="n">
-        <v>4240</v>
-      </c>
-      <c r="S43" s="194" t="n"/>
-      <c r="T43" s="109" t="n"/>
-    </row>
-    <row r="44">
-      <c r="A44" s="197" t="inlineStr">
-        <is>
-          <t>#Q0U0CRCGJ</t>
-        </is>
-      </c>
-      <c r="B44" s="197" t="n">
-        <v>691</v>
-      </c>
-      <c r="C44" s="186" t="n">
-        <v>41</v>
-      </c>
-      <c r="D44" s="116" t="inlineStr">
-        <is>
-          <t>Sn0wc0ne</t>
-        </is>
-      </c>
-      <c r="E44" s="199" t="n">
-        <v>0</v>
-      </c>
-      <c r="F44" s="116" t="n">
-        <v>0</v>
-      </c>
-      <c r="G44" s="199" t="n">
-        <v>0</v>
-      </c>
-      <c r="H44" s="115" t="n">
-        <v>0</v>
-      </c>
-      <c r="I44" s="199" t="n">
-        <v>0</v>
-      </c>
-      <c r="J44" s="116" t="n">
-        <v>0</v>
-      </c>
-      <c r="K44" s="197" t="n"/>
-      <c r="L44" s="115" t="n"/>
-      <c r="M44" s="197" t="n"/>
-      <c r="N44" s="115" t="n"/>
-      <c r="O44" s="197" t="n"/>
-      <c r="P44" s="115" t="n"/>
-      <c r="Q44" s="197" t="n"/>
-      <c r="R44" s="115" t="n"/>
-      <c r="S44" s="197" t="n"/>
-      <c r="T44" s="115" t="n"/>
-    </row>
-    <row r="45">
-      <c r="A45" s="194" t="inlineStr">
-        <is>
-          <t>#QLUV29GGJ</t>
-        </is>
-      </c>
-      <c r="B45" s="194" t="n">
-        <v>1040</v>
-      </c>
-      <c r="C45" s="190" t="n">
-        <v>42</v>
-      </c>
-      <c r="D45" s="110" t="inlineStr">
-        <is>
-          <t>Kukoshibo</t>
-        </is>
-      </c>
-      <c r="E45" s="196" t="n">
-        <v>0</v>
-      </c>
-      <c r="F45" s="110" t="n">
-        <v>0</v>
-      </c>
-      <c r="G45" s="196" t="n">
-        <v>0</v>
-      </c>
-      <c r="H45" s="109" t="n">
-        <v>0</v>
-      </c>
-      <c r="I45" s="196" t="n">
-        <v>0</v>
-      </c>
-      <c r="J45" s="110" t="n">
-        <v>0</v>
-      </c>
-      <c r="K45" s="194" t="n"/>
-      <c r="L45" s="109" t="n"/>
-      <c r="M45" s="194" t="n"/>
-      <c r="N45" s="109" t="n"/>
-      <c r="O45" s="194" t="n"/>
-      <c r="P45" s="109" t="n"/>
-      <c r="Q45" s="194" t="n"/>
-      <c r="R45" s="109" t="n"/>
-      <c r="S45" s="194" t="n"/>
-      <c r="T45" s="109" t="n"/>
-    </row>
     <row r="46">
-      <c r="A46" s="197" t="inlineStr">
+      <c r="A46" s="367" t="inlineStr">
         <is>
           <t>#L2QQL9QVJ</t>
         </is>
       </c>
-      <c r="B46" s="197" t="n">
+      <c r="B46" s="367" t="n">
         <v>1450</v>
       </c>
-      <c r="C46" s="186" t="n">
+      <c r="C46" s="356" t="n">
         <v>43</v>
       </c>
       <c r="D46" s="116" t="inlineStr">
@@ -3596,49 +3780,49 @@
           <t>JustPre10d</t>
         </is>
       </c>
-      <c r="E46" s="199" t="n">
+      <c r="E46" s="369" t="n">
         <v>0</v>
       </c>
       <c r="F46" s="116" t="n">
         <v>0</v>
       </c>
-      <c r="G46" s="199" t="n">
+      <c r="G46" s="369" t="n">
         <v>0</v>
       </c>
       <c r="H46" s="115" t="n">
         <v>0</v>
       </c>
-      <c r="I46" s="199" t="n">
+      <c r="I46" s="369" t="n">
         <v>0</v>
       </c>
       <c r="J46" s="116" t="n">
         <v>0</v>
       </c>
-      <c r="K46" s="199" t="n">
+      <c r="K46" s="369" t="n">
         <v>0</v>
       </c>
       <c r="L46" s="116" t="n">
         <v>0</v>
       </c>
-      <c r="M46" s="199" t="n">
+      <c r="M46" s="369" t="n">
         <v>0</v>
       </c>
       <c r="N46" s="116" t="n">
         <v>0</v>
       </c>
-      <c r="O46" s="199" t="n">
+      <c r="O46" s="369" t="n">
         <v>0</v>
       </c>
       <c r="P46" s="116" t="n">
         <v>0</v>
       </c>
-      <c r="Q46" s="198" t="n">
+      <c r="Q46" s="368" t="n">
         <v>6</v>
       </c>
       <c r="R46" s="112" t="n">
         <v>6655</v>
       </c>
-      <c r="S46" s="198" t="n">
+      <c r="S46" s="368" t="n">
         <v>6</v>
       </c>
       <c r="T46" s="112" t="n">
@@ -3646,162 +3830,198 @@
       </c>
     </row>
     <row r="47">
-      <c r="A47" s="194" t="inlineStr">
-        <is>
-          <t>#QV8RY9UC8</t>
-        </is>
-      </c>
-      <c r="B47" s="194" t="n">
-        <v>747</v>
-      </c>
-      <c r="C47" s="190" t="n">
+      <c r="A47" s="364" t="inlineStr">
+        <is>
+          <t>#LPR9RPCY9</t>
+        </is>
+      </c>
+      <c r="B47" s="364" t="n">
+        <v>980</v>
+      </c>
+      <c r="C47" s="360" t="n">
         <v>44</v>
       </c>
       <c r="D47" s="110" t="inlineStr">
         <is>
-          <t>Apollo</t>
-        </is>
-      </c>
-      <c r="E47" s="196" t="n">
+          <t>sayhuss17</t>
+        </is>
+      </c>
+      <c r="E47" s="366" t="n">
         <v>0</v>
       </c>
       <c r="F47" s="110" t="n">
         <v>0</v>
       </c>
-      <c r="G47" s="196" t="n">
+      <c r="G47" s="366" t="n">
         <v>0</v>
       </c>
       <c r="H47" s="109" t="n">
         <v>0</v>
       </c>
-      <c r="I47" s="196" t="n">
+      <c r="I47" s="366" t="n">
         <v>0</v>
       </c>
       <c r="J47" s="110" t="n">
         <v>0</v>
       </c>
-      <c r="K47" s="196" t="n">
+      <c r="K47" s="366" t="n">
         <v>0</v>
       </c>
       <c r="L47" s="110" t="n">
         <v>0</v>
       </c>
-      <c r="M47" s="194" t="n"/>
-      <c r="N47" s="109" t="n"/>
-      <c r="O47" s="194" t="n"/>
-      <c r="P47" s="109" t="n"/>
-      <c r="Q47" s="194" t="n"/>
-      <c r="R47" s="109" t="n"/>
-      <c r="S47" s="194" t="n"/>
+      <c r="M47" s="366" t="n">
+        <v>0</v>
+      </c>
+      <c r="N47" s="110" t="n">
+        <v>0</v>
+      </c>
+      <c r="O47" s="366" t="n">
+        <v>0</v>
+      </c>
+      <c r="P47" s="110" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q47" s="370" t="n">
+        <v>4</v>
+      </c>
+      <c r="R47" s="118" t="n">
+        <v>4240</v>
+      </c>
+      <c r="S47" s="364" t="n"/>
       <c r="T47" s="109" t="n"/>
     </row>
     <row r="48">
-      <c r="A48" s="197" t="inlineStr">
-        <is>
-          <t>#QV8JJ0URU</t>
-        </is>
-      </c>
-      <c r="B48" s="197" t="n">
-        <v>741</v>
-      </c>
-      <c r="C48" s="186" t="n">
+      <c r="A48" s="367" t="inlineStr">
+        <is>
+          <t>#QQL8C29CY</t>
+        </is>
+      </c>
+      <c r="B48" s="367" t="n">
+        <v>864</v>
+      </c>
+      <c r="C48" s="356" t="n">
         <v>45</v>
       </c>
       <c r="D48" s="116" t="inlineStr">
         <is>
-          <t>✨Jacob</t>
-        </is>
-      </c>
-      <c r="E48" s="199" t="n">
+          <t>TypicalTeague#2</t>
+        </is>
+      </c>
+      <c r="E48" s="369" t="n">
         <v>0</v>
       </c>
       <c r="F48" s="116" t="n">
         <v>0</v>
       </c>
-      <c r="G48" s="199" t="n">
+      <c r="G48" s="369" t="n">
         <v>0</v>
       </c>
       <c r="H48" s="115" t="n">
         <v>0</v>
       </c>
-      <c r="I48" s="199" t="n">
+      <c r="I48" s="369" t="n">
         <v>0</v>
       </c>
       <c r="J48" s="116" t="n">
         <v>0</v>
       </c>
-      <c r="K48" s="199" t="n">
+      <c r="K48" s="369" t="n">
         <v>0</v>
       </c>
       <c r="L48" s="116" t="n">
         <v>0</v>
       </c>
-      <c r="M48" s="199" t="n">
+      <c r="M48" s="369" t="n">
         <v>0</v>
       </c>
       <c r="N48" s="116" t="n">
         <v>0</v>
       </c>
-      <c r="O48" s="199" t="n">
+      <c r="O48" s="369" t="n">
         <v>0</v>
       </c>
       <c r="P48" s="116" t="n">
         <v>0</v>
       </c>
-      <c r="Q48" s="198" t="n">
-        <v>6</v>
-      </c>
-      <c r="R48" s="112" t="n">
-        <v>7385</v>
-      </c>
-      <c r="S48" s="198" t="n">
+      <c r="Q48" s="368" t="n">
+        <v>5</v>
+      </c>
+      <c r="R48" s="117" t="n">
+        <v>4070</v>
+      </c>
+      <c r="S48" s="368" t="n">
         <v>6</v>
       </c>
       <c r="T48" s="112" t="n">
-        <v>9155</v>
+        <v>6410</v>
       </c>
     </row>
     <row r="49">
-      <c r="A49" s="194" t="inlineStr">
-        <is>
-          <t>#QPCLYCPV9</t>
-        </is>
-      </c>
-      <c r="B49" s="194" t="n">
-        <v>977</v>
-      </c>
-      <c r="C49" s="190" t="n">
+      <c r="A49" s="364" t="inlineStr">
+        <is>
+          <t>#L9QL9YQQY</t>
+        </is>
+      </c>
+      <c r="B49" s="364" t="n">
+        <v>975</v>
+      </c>
+      <c r="C49" s="360" t="n">
         <v>46</v>
       </c>
       <c r="D49" s="110" t="inlineStr">
         <is>
-          <t>aadhirajr</t>
-        </is>
-      </c>
-      <c r="E49" s="196" t="n">
+          <t>Ima Chad</t>
+        </is>
+      </c>
+      <c r="E49" s="366" t="n">
         <v>0</v>
       </c>
       <c r="F49" s="110" t="n">
         <v>0</v>
       </c>
-      <c r="G49" s="196" t="n">
+      <c r="G49" s="366" t="n">
         <v>0</v>
       </c>
       <c r="H49" s="109" t="n">
         <v>0</v>
       </c>
-      <c r="I49" s="194" t="n"/>
-      <c r="J49" s="109" t="n"/>
-      <c r="K49" s="194" t="n"/>
-      <c r="L49" s="109" t="n"/>
-      <c r="M49" s="194" t="n"/>
-      <c r="N49" s="109" t="n"/>
-      <c r="O49" s="194" t="n"/>
-      <c r="P49" s="109" t="n"/>
-      <c r="Q49" s="194" t="n"/>
-      <c r="R49" s="109" t="n"/>
-      <c r="S49" s="194" t="n"/>
-      <c r="T49" s="109" t="n"/>
+      <c r="I49" s="366" t="n">
+        <v>0</v>
+      </c>
+      <c r="J49" s="110" t="n">
+        <v>0</v>
+      </c>
+      <c r="K49" s="366" t="n">
+        <v>0</v>
+      </c>
+      <c r="L49" s="110" t="n">
+        <v>0</v>
+      </c>
+      <c r="M49" s="366" t="n">
+        <v>0</v>
+      </c>
+      <c r="N49" s="110" t="n">
+        <v>0</v>
+      </c>
+      <c r="O49" s="366" t="n">
+        <v>0</v>
+      </c>
+      <c r="P49" s="110" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q49" s="366" t="n">
+        <v>0</v>
+      </c>
+      <c r="R49" s="110" t="n">
+        <v>0</v>
+      </c>
+      <c r="S49" s="365" t="n">
+        <v>5</v>
+      </c>
+      <c r="T49" s="110" t="n">
+        <v>3360</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" s="128" t="inlineStr">
@@ -3858,15 +4078,15 @@
       <c r="T50" s="131" t="n"/>
     </row>
     <row r="51">
-      <c r="A51" s="196" t="inlineStr">
+      <c r="A51" s="366" t="inlineStr">
         <is>
           <t>#L9JJQY992</t>
         </is>
       </c>
-      <c r="B51" s="194" t="n">
+      <c r="B51" s="364" t="n">
         <v>773</v>
       </c>
-      <c r="C51" s="190" t="n">
+      <c r="C51" s="360" t="n">
         <v>48</v>
       </c>
       <c r="D51" s="109" t="inlineStr">
@@ -3874,53 +4094,53 @@
           <t>Fisted_Waffle</t>
         </is>
       </c>
-      <c r="E51" s="194" t="n"/>
+      <c r="E51" s="364" t="n"/>
       <c r="F51" s="109" t="n"/>
-      <c r="G51" s="194" t="n"/>
+      <c r="G51" s="364" t="n"/>
       <c r="H51" s="109" t="n"/>
-      <c r="I51" s="196" t="n">
+      <c r="I51" s="366" t="n">
         <v>0</v>
       </c>
       <c r="J51" s="110" t="n">
         <v>0</v>
       </c>
-      <c r="K51" s="196" t="n">
+      <c r="K51" s="366" t="n">
         <v>0</v>
       </c>
       <c r="L51" s="110" t="n">
         <v>0</v>
       </c>
-      <c r="M51" s="196" t="n">
+      <c r="M51" s="366" t="n">
         <v>0</v>
       </c>
       <c r="N51" s="110" t="n">
         <v>0</v>
       </c>
-      <c r="O51" s="196" t="n">
+      <c r="O51" s="366" t="n">
         <v>0</v>
       </c>
       <c r="P51" s="110" t="n">
         <v>0</v>
       </c>
-      <c r="Q51" s="196" t="n">
+      <c r="Q51" s="366" t="n">
         <v>0</v>
       </c>
       <c r="R51" s="110" t="n">
         <v>0</v>
       </c>
-      <c r="S51" s="194" t="n"/>
+      <c r="S51" s="364" t="n"/>
       <c r="T51" s="109" t="n"/>
     </row>
     <row r="52">
-      <c r="A52" s="199" t="inlineStr">
+      <c r="A52" s="369" t="inlineStr">
         <is>
           <t>#9JUR0JQV2</t>
         </is>
       </c>
-      <c r="B52" s="197" t="n">
+      <c r="B52" s="367" t="n">
         <v>1134</v>
       </c>
-      <c r="C52" s="186" t="n">
+      <c r="C52" s="356" t="n">
         <v>49</v>
       </c>
       <c r="D52" s="115" t="inlineStr">
@@ -3928,37 +4148,37 @@
           <t>atley</t>
         </is>
       </c>
-      <c r="E52" s="197" t="n"/>
+      <c r="E52" s="367" t="n"/>
       <c r="F52" s="115" t="n"/>
-      <c r="G52" s="197" t="n"/>
+      <c r="G52" s="367" t="n"/>
       <c r="H52" s="115" t="n"/>
-      <c r="I52" s="200" t="n">
+      <c r="I52" s="371" t="n">
         <v>3</v>
       </c>
       <c r="J52" s="117" t="n">
         <v>5277</v>
       </c>
-      <c r="K52" s="197" t="n"/>
+      <c r="K52" s="367" t="n"/>
       <c r="L52" s="115" t="n"/>
-      <c r="M52" s="197" t="n"/>
+      <c r="M52" s="367" t="n"/>
       <c r="N52" s="115" t="n"/>
-      <c r="O52" s="197" t="n"/>
+      <c r="O52" s="367" t="n"/>
       <c r="P52" s="115" t="n"/>
-      <c r="Q52" s="197" t="n"/>
+      <c r="Q52" s="367" t="n"/>
       <c r="R52" s="115" t="n"/>
-      <c r="S52" s="197" t="n"/>
+      <c r="S52" s="367" t="n"/>
       <c r="T52" s="115" t="n"/>
     </row>
     <row r="53">
-      <c r="A53" s="196" t="inlineStr">
+      <c r="A53" s="366" t="inlineStr">
         <is>
           <t>#QUCCVCCJ0</t>
         </is>
       </c>
-      <c r="B53" s="194" t="n">
+      <c r="B53" s="364" t="n">
         <v>783</v>
       </c>
-      <c r="C53" s="190" t="n">
+      <c r="C53" s="360" t="n">
         <v>50</v>
       </c>
       <c r="D53" s="109" t="inlineStr">
@@ -3966,33 +4186,33 @@
           <t>koi</t>
         </is>
       </c>
-      <c r="E53" s="194" t="n"/>
+      <c r="E53" s="364" t="n"/>
       <c r="F53" s="109" t="n"/>
-      <c r="G53" s="194" t="n"/>
+      <c r="G53" s="364" t="n"/>
       <c r="H53" s="109" t="n"/>
-      <c r="I53" s="194" t="n"/>
+      <c r="I53" s="364" t="n"/>
       <c r="J53" s="109" t="n"/>
-      <c r="K53" s="194" t="n"/>
+      <c r="K53" s="364" t="n"/>
       <c r="L53" s="109" t="n"/>
-      <c r="M53" s="194" t="n"/>
+      <c r="M53" s="364" t="n"/>
       <c r="N53" s="109" t="n"/>
-      <c r="O53" s="194" t="n"/>
+      <c r="O53" s="364" t="n"/>
       <c r="P53" s="109" t="n"/>
-      <c r="Q53" s="194" t="n"/>
+      <c r="Q53" s="364" t="n"/>
       <c r="R53" s="109" t="n"/>
-      <c r="S53" s="194" t="n"/>
+      <c r="S53" s="364" t="n"/>
       <c r="T53" s="109" t="n"/>
     </row>
     <row r="54">
-      <c r="A54" s="199" t="inlineStr">
+      <c r="A54" s="369" t="inlineStr">
         <is>
           <t>#QPRYCJVJL</t>
         </is>
       </c>
-      <c r="B54" s="197" t="n">
+      <c r="B54" s="367" t="n">
         <v>693</v>
       </c>
-      <c r="C54" s="186" t="n">
+      <c r="C54" s="356" t="n">
         <v>51</v>
       </c>
       <c r="D54" s="115" t="inlineStr">
@@ -4000,33 +4220,33 @@
           <t>cris</t>
         </is>
       </c>
-      <c r="E54" s="197" t="n"/>
+      <c r="E54" s="367" t="n"/>
       <c r="F54" s="115" t="n"/>
-      <c r="G54" s="197" t="n"/>
+      <c r="G54" s="367" t="n"/>
       <c r="H54" s="115" t="n"/>
-      <c r="I54" s="197" t="n"/>
+      <c r="I54" s="367" t="n"/>
       <c r="J54" s="115" t="n"/>
-      <c r="K54" s="197" t="n"/>
+      <c r="K54" s="367" t="n"/>
       <c r="L54" s="115" t="n"/>
-      <c r="M54" s="197" t="n"/>
+      <c r="M54" s="367" t="n"/>
       <c r="N54" s="115" t="n"/>
-      <c r="O54" s="197" t="n"/>
+      <c r="O54" s="367" t="n"/>
       <c r="P54" s="115" t="n"/>
-      <c r="Q54" s="197" t="n"/>
+      <c r="Q54" s="367" t="n"/>
       <c r="R54" s="115" t="n"/>
-      <c r="S54" s="197" t="n"/>
+      <c r="S54" s="367" t="n"/>
       <c r="T54" s="115" t="n"/>
     </row>
     <row r="55">
-      <c r="A55" s="196" t="inlineStr">
+      <c r="A55" s="366" t="inlineStr">
         <is>
           <t>#QQLVRJCGQ</t>
         </is>
       </c>
-      <c r="B55" s="194" t="n">
+      <c r="B55" s="364" t="n">
         <v>1240</v>
       </c>
-      <c r="C55" s="190" t="n">
+      <c r="C55" s="360" t="n">
         <v>52</v>
       </c>
       <c r="D55" s="109" t="inlineStr">
@@ -4034,33 +4254,33 @@
           <t>khant</t>
         </is>
       </c>
-      <c r="E55" s="194" t="n"/>
+      <c r="E55" s="364" t="n"/>
       <c r="F55" s="109" t="n"/>
-      <c r="G55" s="194" t="n"/>
+      <c r="G55" s="364" t="n"/>
       <c r="H55" s="109" t="n"/>
-      <c r="I55" s="194" t="n"/>
+      <c r="I55" s="364" t="n"/>
       <c r="J55" s="109" t="n"/>
-      <c r="K55" s="194" t="n"/>
+      <c r="K55" s="364" t="n"/>
       <c r="L55" s="109" t="n"/>
-      <c r="M55" s="194" t="n"/>
+      <c r="M55" s="364" t="n"/>
       <c r="N55" s="109" t="n"/>
-      <c r="O55" s="194" t="n"/>
+      <c r="O55" s="364" t="n"/>
       <c r="P55" s="109" t="n"/>
-      <c r="Q55" s="194" t="n"/>
+      <c r="Q55" s="364" t="n"/>
       <c r="R55" s="109" t="n"/>
-      <c r="S55" s="194" t="n"/>
+      <c r="S55" s="364" t="n"/>
       <c r="T55" s="109" t="n"/>
     </row>
     <row r="56">
-      <c r="A56" s="199" t="inlineStr">
+      <c r="A56" s="369" t="inlineStr">
         <is>
           <t>#QLL0PVCRV</t>
         </is>
       </c>
-      <c r="B56" s="197" t="n">
+      <c r="B56" s="367" t="n">
         <v>1704</v>
       </c>
-      <c r="C56" s="186" t="n">
+      <c r="C56" s="356" t="n">
         <v>53</v>
       </c>
       <c r="D56" s="115" t="inlineStr">
@@ -4068,33 +4288,33 @@
           <t>Harsh chhillar</t>
         </is>
       </c>
-      <c r="E56" s="197" t="n"/>
+      <c r="E56" s="367" t="n"/>
       <c r="F56" s="115" t="n"/>
-      <c r="G56" s="197" t="n"/>
+      <c r="G56" s="367" t="n"/>
       <c r="H56" s="115" t="n"/>
-      <c r="I56" s="197" t="n"/>
+      <c r="I56" s="367" t="n"/>
       <c r="J56" s="115" t="n"/>
-      <c r="K56" s="197" t="n"/>
+      <c r="K56" s="367" t="n"/>
       <c r="L56" s="115" t="n"/>
-      <c r="M56" s="197" t="n"/>
+      <c r="M56" s="367" t="n"/>
       <c r="N56" s="115" t="n"/>
-      <c r="O56" s="197" t="n"/>
+      <c r="O56" s="367" t="n"/>
       <c r="P56" s="115" t="n"/>
-      <c r="Q56" s="197" t="n"/>
+      <c r="Q56" s="367" t="n"/>
       <c r="R56" s="115" t="n"/>
-      <c r="S56" s="197" t="n"/>
+      <c r="S56" s="367" t="n"/>
       <c r="T56" s="115" t="n"/>
     </row>
     <row r="57">
-      <c r="A57" s="196" t="inlineStr">
+      <c r="A57" s="366" t="inlineStr">
         <is>
           <t>#Q8YP9P8UJ</t>
         </is>
       </c>
-      <c r="B57" s="194" t="n">
+      <c r="B57" s="364" t="n">
         <v>945</v>
       </c>
-      <c r="C57" s="190" t="n">
+      <c r="C57" s="360" t="n">
         <v>54</v>
       </c>
       <c r="D57" s="109" t="inlineStr">
@@ -4102,37 +4322,37 @@
           <t>Ranger</t>
         </is>
       </c>
-      <c r="E57" s="194" t="n"/>
+      <c r="E57" s="364" t="n"/>
       <c r="F57" s="109" t="n"/>
-      <c r="G57" s="194" t="n"/>
+      <c r="G57" s="364" t="n"/>
       <c r="H57" s="109" t="n"/>
-      <c r="I57" s="194" t="n"/>
+      <c r="I57" s="364" t="n"/>
       <c r="J57" s="109" t="n"/>
-      <c r="K57" s="194" t="n"/>
+      <c r="K57" s="364" t="n"/>
       <c r="L57" s="109" t="n"/>
-      <c r="M57" s="195" t="n">
+      <c r="M57" s="365" t="n">
         <v>5</v>
       </c>
       <c r="N57" s="118" t="n">
         <v>4680</v>
       </c>
-      <c r="O57" s="194" t="n"/>
+      <c r="O57" s="364" t="n"/>
       <c r="P57" s="109" t="n"/>
-      <c r="Q57" s="194" t="n"/>
+      <c r="Q57" s="364" t="n"/>
       <c r="R57" s="109" t="n"/>
-      <c r="S57" s="194" t="n"/>
+      <c r="S57" s="364" t="n"/>
       <c r="T57" s="109" t="n"/>
     </row>
     <row r="58">
-      <c r="A58" s="199" t="inlineStr">
+      <c r="A58" s="369" t="inlineStr">
         <is>
           <t>#Q0JG2RJQ8</t>
         </is>
       </c>
-      <c r="B58" s="197" t="n">
+      <c r="B58" s="367" t="n">
         <v>997</v>
       </c>
-      <c r="C58" s="186" t="n">
+      <c r="C58" s="356" t="n">
         <v>55</v>
       </c>
       <c r="D58" s="115" t="inlineStr">
@@ -4140,37 +4360,37 @@
           <t>bozo</t>
         </is>
       </c>
-      <c r="E58" s="197" t="n"/>
+      <c r="E58" s="367" t="n"/>
       <c r="F58" s="115" t="n"/>
-      <c r="G58" s="197" t="n"/>
+      <c r="G58" s="367" t="n"/>
       <c r="H58" s="115" t="n"/>
-      <c r="I58" s="197" t="n"/>
+      <c r="I58" s="367" t="n"/>
       <c r="J58" s="115" t="n"/>
-      <c r="K58" s="197" t="n"/>
+      <c r="K58" s="367" t="n"/>
       <c r="L58" s="115" t="n"/>
-      <c r="M58" s="197" t="n"/>
+      <c r="M58" s="367" t="n"/>
       <c r="N58" s="115" t="n"/>
-      <c r="O58" s="198" t="n">
+      <c r="O58" s="368" t="n">
         <v>6</v>
       </c>
       <c r="P58" s="112" t="n">
         <v>6495</v>
       </c>
-      <c r="Q58" s="197" t="n"/>
+      <c r="Q58" s="367" t="n"/>
       <c r="R58" s="115" t="n"/>
-      <c r="S58" s="197" t="n"/>
+      <c r="S58" s="367" t="n"/>
       <c r="T58" s="115" t="n"/>
     </row>
     <row r="59">
-      <c r="A59" s="196" t="inlineStr">
+      <c r="A59" s="366" t="inlineStr">
         <is>
           <t>#UVCCQC02</t>
         </is>
       </c>
-      <c r="B59" s="194" t="n">
+      <c r="B59" s="364" t="n">
         <v>1806</v>
       </c>
-      <c r="C59" s="190" t="n">
+      <c r="C59" s="360" t="n">
         <v>56</v>
       </c>
       <c r="D59" s="109" t="inlineStr">
@@ -4178,29 +4398,29 @@
           <t>lordshisha</t>
         </is>
       </c>
-      <c r="E59" s="194" t="n"/>
+      <c r="E59" s="364" t="n"/>
       <c r="F59" s="109" t="n"/>
-      <c r="G59" s="194" t="n"/>
+      <c r="G59" s="364" t="n"/>
       <c r="H59" s="109" t="n"/>
-      <c r="I59" s="194" t="n"/>
+      <c r="I59" s="364" t="n"/>
       <c r="J59" s="109" t="n"/>
-      <c r="K59" s="194" t="n"/>
+      <c r="K59" s="364" t="n"/>
       <c r="L59" s="109" t="n"/>
-      <c r="M59" s="194" t="n"/>
+      <c r="M59" s="364" t="n"/>
       <c r="N59" s="109" t="n"/>
-      <c r="O59" s="195" t="n">
+      <c r="O59" s="365" t="n">
         <v>6</v>
       </c>
       <c r="P59" s="106" t="n">
         <v>8496</v>
       </c>
-      <c r="Q59" s="195" t="n">
+      <c r="Q59" s="365" t="n">
         <v>6</v>
       </c>
       <c r="R59" s="106" t="n">
         <v>6310</v>
       </c>
-      <c r="S59" s="195" t="n">
+      <c r="S59" s="365" t="n">
         <v>6</v>
       </c>
       <c r="T59" s="106" t="n">
@@ -4208,15 +4428,15 @@
       </c>
     </row>
     <row r="60">
-      <c r="A60" s="199" t="inlineStr">
+      <c r="A60" s="369" t="inlineStr">
         <is>
           <t>#P2CPRPQU</t>
         </is>
       </c>
-      <c r="B60" s="197" t="n">
+      <c r="B60" s="367" t="n">
         <v>2232</v>
       </c>
-      <c r="C60" s="186" t="n">
+      <c r="C60" s="356" t="n">
         <v>57</v>
       </c>
       <c r="D60" s="115" t="inlineStr">
@@ -4224,29 +4444,29 @@
           <t>The Drift King</t>
         </is>
       </c>
-      <c r="E60" s="197" t="n"/>
+      <c r="E60" s="367" t="n"/>
       <c r="F60" s="115" t="n"/>
-      <c r="G60" s="197" t="n"/>
+      <c r="G60" s="367" t="n"/>
       <c r="H60" s="115" t="n"/>
-      <c r="I60" s="197" t="n"/>
+      <c r="I60" s="367" t="n"/>
       <c r="J60" s="115" t="n"/>
-      <c r="K60" s="197" t="n"/>
+      <c r="K60" s="367" t="n"/>
       <c r="L60" s="115" t="n"/>
-      <c r="M60" s="197" t="n"/>
+      <c r="M60" s="367" t="n"/>
       <c r="N60" s="115" t="n"/>
-      <c r="O60" s="198" t="n">
+      <c r="O60" s="368" t="n">
         <v>6</v>
       </c>
       <c r="P60" s="112" t="n">
         <v>8023</v>
       </c>
-      <c r="Q60" s="198" t="n">
+      <c r="Q60" s="368" t="n">
         <v>6</v>
       </c>
       <c r="R60" s="112" t="n">
         <v>7625</v>
       </c>
-      <c r="S60" s="198" t="n">
+      <c r="S60" s="368" t="n">
         <v>6</v>
       </c>
       <c r="T60" s="112" t="n">
@@ -4254,15 +4474,15 @@
       </c>
     </row>
     <row r="61">
-      <c r="A61" s="196" t="inlineStr">
+      <c r="A61" s="366" t="inlineStr">
         <is>
           <t>#QJVL0LYQQ</t>
         </is>
       </c>
-      <c r="B61" s="194" t="n">
+      <c r="B61" s="364" t="n">
         <v>921</v>
       </c>
-      <c r="C61" s="190" t="n">
+      <c r="C61" s="360" t="n">
         <v>58</v>
       </c>
       <c r="D61" s="109" t="inlineStr">
@@ -4270,29 +4490,29 @@
           <t>mobbb341</t>
         </is>
       </c>
-      <c r="E61" s="194" t="n"/>
+      <c r="E61" s="364" t="n"/>
       <c r="F61" s="109" t="n"/>
-      <c r="G61" s="194" t="n"/>
+      <c r="G61" s="364" t="n"/>
       <c r="H61" s="109" t="n"/>
-      <c r="I61" s="194" t="n"/>
+      <c r="I61" s="364" t="n"/>
       <c r="J61" s="109" t="n"/>
-      <c r="K61" s="194" t="n"/>
+      <c r="K61" s="364" t="n"/>
       <c r="L61" s="109" t="n"/>
-      <c r="M61" s="194" t="n"/>
+      <c r="M61" s="364" t="n"/>
       <c r="N61" s="109" t="n"/>
-      <c r="O61" s="195" t="n">
+      <c r="O61" s="365" t="n">
         <v>6</v>
       </c>
       <c r="P61" s="106" t="n">
         <v>7710</v>
       </c>
-      <c r="Q61" s="195" t="n">
+      <c r="Q61" s="365" t="n">
         <v>6</v>
       </c>
       <c r="R61" s="106" t="n">
         <v>8810</v>
       </c>
-      <c r="S61" s="195" t="n">
+      <c r="S61" s="365" t="n">
         <v>6</v>
       </c>
       <c r="T61" s="118" t="n">
@@ -4300,15 +4520,15 @@
       </c>
     </row>
     <row r="62">
-      <c r="A62" s="199" t="inlineStr">
+      <c r="A62" s="369" t="inlineStr">
         <is>
           <t>#L8R82C8VC</t>
         </is>
       </c>
-      <c r="B62" s="197" t="n">
+      <c r="B62" s="367" t="n">
         <v>1162</v>
       </c>
-      <c r="C62" s="186" t="n">
+      <c r="C62" s="356" t="n">
         <v>59</v>
       </c>
       <c r="D62" s="115" t="inlineStr">
@@ -4316,29 +4536,29 @@
           <t>caden asue</t>
         </is>
       </c>
-      <c r="E62" s="197" t="n"/>
+      <c r="E62" s="367" t="n"/>
       <c r="F62" s="115" t="n"/>
-      <c r="G62" s="197" t="n"/>
+      <c r="G62" s="367" t="n"/>
       <c r="H62" s="115" t="n"/>
-      <c r="I62" s="197" t="n"/>
+      <c r="I62" s="367" t="n"/>
       <c r="J62" s="115" t="n"/>
-      <c r="K62" s="197" t="n"/>
+      <c r="K62" s="367" t="n"/>
       <c r="L62" s="115" t="n"/>
-      <c r="M62" s="197" t="n"/>
+      <c r="M62" s="367" t="n"/>
       <c r="N62" s="115" t="n"/>
-      <c r="O62" s="198" t="n">
+      <c r="O62" s="368" t="n">
         <v>6</v>
       </c>
       <c r="P62" s="117" t="n">
         <v>5112</v>
       </c>
-      <c r="Q62" s="198" t="n">
+      <c r="Q62" s="368" t="n">
         <v>6</v>
       </c>
       <c r="R62" s="117" t="n">
         <v>4283</v>
       </c>
-      <c r="S62" s="198" t="n">
+      <c r="S62" s="368" t="n">
         <v>6</v>
       </c>
       <c r="T62" s="117" t="n">
@@ -4346,15 +4566,15 @@
       </c>
     </row>
     <row r="63">
-      <c r="A63" s="196" t="inlineStr">
+      <c r="A63" s="366" t="inlineStr">
         <is>
           <t>#L9Q8VLLQG</t>
         </is>
       </c>
-      <c r="B63" s="194" t="n">
+      <c r="B63" s="364" t="n">
         <v>1130</v>
       </c>
-      <c r="C63" s="190" t="n">
+      <c r="C63" s="360" t="n">
         <v>60</v>
       </c>
       <c r="D63" s="109" t="inlineStr">
@@ -4362,21 +4582,21 @@
           <t>cat</t>
         </is>
       </c>
-      <c r="E63" s="194" t="n"/>
+      <c r="E63" s="364" t="n"/>
       <c r="F63" s="109" t="n"/>
-      <c r="G63" s="194" t="n"/>
+      <c r="G63" s="364" t="n"/>
       <c r="H63" s="109" t="n"/>
-      <c r="I63" s="194" t="n"/>
+      <c r="I63" s="364" t="n"/>
       <c r="J63" s="109" t="n"/>
-      <c r="K63" s="194" t="n"/>
+      <c r="K63" s="364" t="n"/>
       <c r="L63" s="109" t="n"/>
-      <c r="M63" s="194" t="n"/>
+      <c r="M63" s="364" t="n"/>
       <c r="N63" s="109" t="n"/>
-      <c r="O63" s="194" t="n"/>
+      <c r="O63" s="364" t="n"/>
       <c r="P63" s="109" t="n"/>
-      <c r="Q63" s="194" t="n"/>
+      <c r="Q63" s="364" t="n"/>
       <c r="R63" s="109" t="n"/>
-      <c r="S63" s="195" t="n">
+      <c r="S63" s="365" t="n">
         <v>6</v>
       </c>
       <c r="T63" s="118" t="n">
@@ -4384,15 +4604,15 @@
       </c>
     </row>
     <row r="64">
-      <c r="A64" s="199" t="inlineStr">
+      <c r="A64" s="369" t="inlineStr">
         <is>
           <t>#QV0PQC9JU</t>
         </is>
       </c>
-      <c r="B64" s="197" t="n">
+      <c r="B64" s="367" t="n">
         <v>539</v>
       </c>
-      <c r="C64" s="186" t="n">
+      <c r="C64" s="356" t="n">
         <v>61</v>
       </c>
       <c r="D64" s="115" t="inlineStr">
@@ -4400,21 +4620,21 @@
           <t>Superman</t>
         </is>
       </c>
-      <c r="E64" s="197" t="n"/>
+      <c r="E64" s="367" t="n"/>
       <c r="F64" s="115" t="n"/>
-      <c r="G64" s="197" t="n"/>
+      <c r="G64" s="367" t="n"/>
       <c r="H64" s="115" t="n"/>
-      <c r="I64" s="197" t="n"/>
+      <c r="I64" s="367" t="n"/>
       <c r="J64" s="115" t="n"/>
-      <c r="K64" s="197" t="n"/>
+      <c r="K64" s="367" t="n"/>
       <c r="L64" s="115" t="n"/>
-      <c r="M64" s="197" t="n"/>
+      <c r="M64" s="367" t="n"/>
       <c r="N64" s="115" t="n"/>
-      <c r="O64" s="197" t="n"/>
+      <c r="O64" s="367" t="n"/>
       <c r="P64" s="115" t="n"/>
-      <c r="Q64" s="197" t="n"/>
+      <c r="Q64" s="367" t="n"/>
       <c r="R64" s="115" t="n"/>
-      <c r="S64" s="198" t="n">
+      <c r="S64" s="368" t="n">
         <v>6</v>
       </c>
       <c r="T64" s="117" t="n">
@@ -4422,15 +4642,15 @@
       </c>
     </row>
     <row r="65">
-      <c r="A65" s="196" t="inlineStr">
+      <c r="A65" s="366" t="inlineStr">
         <is>
           <t>#LU0CRP09L</t>
         </is>
       </c>
-      <c r="B65" s="194" t="n">
+      <c r="B65" s="364" t="n">
         <v>809</v>
       </c>
-      <c r="C65" s="190" t="n">
+      <c r="C65" s="360" t="n">
         <v>62</v>
       </c>
       <c r="D65" s="109" t="inlineStr">
@@ -4438,21 +4658,21 @@
           <t>I Dont Know</t>
         </is>
       </c>
-      <c r="E65" s="194" t="n"/>
+      <c r="E65" s="364" t="n"/>
       <c r="F65" s="109" t="n"/>
-      <c r="G65" s="194" t="n"/>
+      <c r="G65" s="364" t="n"/>
       <c r="H65" s="109" t="n"/>
-      <c r="I65" s="194" t="n"/>
+      <c r="I65" s="364" t="n"/>
       <c r="J65" s="109" t="n"/>
-      <c r="K65" s="194" t="n"/>
+      <c r="K65" s="364" t="n"/>
       <c r="L65" s="109" t="n"/>
-      <c r="M65" s="194" t="n"/>
+      <c r="M65" s="364" t="n"/>
       <c r="N65" s="109" t="n"/>
-      <c r="O65" s="194" t="n"/>
+      <c r="O65" s="364" t="n"/>
       <c r="P65" s="109" t="n"/>
-      <c r="Q65" s="194" t="n"/>
+      <c r="Q65" s="364" t="n"/>
       <c r="R65" s="109" t="n"/>
-      <c r="S65" s="201" t="n">
+      <c r="S65" s="370" t="n">
         <v>3</v>
       </c>
       <c r="T65" s="110" t="n">
@@ -4460,15 +4680,15 @@
       </c>
     </row>
     <row r="66">
-      <c r="A66" s="199" t="inlineStr">
+      <c r="A66" s="369" t="inlineStr">
         <is>
           <t>#YCPP0QPP8</t>
         </is>
       </c>
-      <c r="B66" s="197" t="n">
+      <c r="B66" s="367" t="n">
         <v>3327</v>
       </c>
-      <c r="C66" s="186" t="n">
+      <c r="C66" s="356" t="n">
         <v>63</v>
       </c>
       <c r="D66" s="115" t="inlineStr">
@@ -4476,21 +4696,21 @@
           <t>Coach</t>
         </is>
       </c>
-      <c r="E66" s="197" t="n"/>
+      <c r="E66" s="367" t="n"/>
       <c r="F66" s="115" t="n"/>
-      <c r="G66" s="197" t="n"/>
+      <c r="G66" s="367" t="n"/>
       <c r="H66" s="115" t="n"/>
-      <c r="I66" s="197" t="n"/>
+      <c r="I66" s="367" t="n"/>
       <c r="J66" s="115" t="n"/>
-      <c r="K66" s="197" t="n"/>
+      <c r="K66" s="367" t="n"/>
       <c r="L66" s="115" t="n"/>
-      <c r="M66" s="197" t="n"/>
+      <c r="M66" s="367" t="n"/>
       <c r="N66" s="115" t="n"/>
-      <c r="O66" s="197" t="n"/>
+      <c r="O66" s="367" t="n"/>
       <c r="P66" s="115" t="n"/>
-      <c r="Q66" s="197" t="n"/>
+      <c r="Q66" s="367" t="n"/>
       <c r="R66" s="115" t="n"/>
-      <c r="S66" s="199" t="n">
+      <c r="S66" s="369" t="n">
         <v>0</v>
       </c>
       <c r="T66" s="116" t="n">

</xml_diff>

<commit_message>
updating the clash file from bat manual run
</commit_message>
<xml_diff>
--- a/Clash.xlsx
+++ b/Clash.xlsx
@@ -223,7 +223,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="28">
+  <borders count="29">
     <border>
       <left/>
       <right/>
@@ -331,11 +331,12 @@
     <border/>
     <border/>
     <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9"/>
   </cellStyleXfs>
-  <cellXfs count="372">
+  <cellXfs count="391">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -806,6 +807,29 @@
     <xf numFmtId="164" fontId="8" fillId="27" borderId="27" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="8" fillId="32" borderId="27" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="8" fillId="31" borderId="27" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="7" fillId="25" borderId="28" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="25" borderId="28" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="26" borderId="28" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="7" fillId="27" borderId="28" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="7" fillId="28" borderId="28" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="28" borderId="28" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="29" borderId="28" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="7" fillId="30" borderId="28" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="7" fillId="31" borderId="28" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="8" fillId="28" borderId="28" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="8" fillId="29" borderId="28" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="8" fillId="30" borderId="28" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="8" fillId="25" borderId="28" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="8" fillId="26" borderId="28" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="8" fillId="27" borderId="28" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="8" fillId="32" borderId="28" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="8" fillId="31" borderId="28" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="8" fillId="26" borderId="12" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="8" fillId="26" borderId="13" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1404,15 +1428,15 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="355" t="inlineStr">
+      <c r="A4" s="372" t="inlineStr">
         <is>
           <t>#G0QPVJY9L</t>
         </is>
       </c>
-      <c r="B4" s="355" t="n">
+      <c r="B4" s="372" t="n">
         <v>779</v>
       </c>
-      <c r="C4" s="356" t="n">
+      <c r="C4" s="373" t="n">
         <v>1</v>
       </c>
       <c r="D4" s="95" t="inlineStr">
@@ -1420,49 +1444,49 @@
           <t>Zoro</t>
         </is>
       </c>
-      <c r="E4" s="357" t="n">
+      <c r="E4" s="374" t="n">
         <v>6</v>
       </c>
       <c r="F4" s="95" t="n">
         <v>13801</v>
       </c>
-      <c r="G4" s="358" t="n">
+      <c r="G4" s="375" t="n">
         <v>0</v>
       </c>
       <c r="H4" s="98" t="n">
         <v>0</v>
       </c>
-      <c r="I4" s="357" t="n">
+      <c r="I4" s="374" t="n">
         <v>6</v>
       </c>
       <c r="J4" s="95" t="n">
         <v>12116</v>
       </c>
-      <c r="K4" s="357" t="n">
+      <c r="K4" s="374" t="n">
         <v>6</v>
       </c>
       <c r="L4" s="95" t="n">
         <v>13432</v>
       </c>
-      <c r="M4" s="357" t="n">
+      <c r="M4" s="374" t="n">
         <v>6</v>
       </c>
       <c r="N4" s="95" t="n">
         <v>8855</v>
       </c>
-      <c r="O4" s="357" t="n">
+      <c r="O4" s="374" t="n">
         <v>6</v>
       </c>
       <c r="P4" s="95" t="n">
         <v>10965</v>
       </c>
-      <c r="Q4" s="357" t="n">
+      <c r="Q4" s="374" t="n">
         <v>6</v>
       </c>
       <c r="R4" s="95" t="n">
         <v>7905</v>
       </c>
-      <c r="S4" s="357" t="n">
+      <c r="S4" s="374" t="n">
         <v>6</v>
       </c>
       <c r="T4" s="95" t="n">
@@ -1470,15 +1494,15 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="359" t="inlineStr">
+      <c r="A5" s="376" t="inlineStr">
         <is>
           <t>#YRGRRJQCY</t>
         </is>
       </c>
-      <c r="B5" s="359" t="n">
+      <c r="B5" s="376" t="n">
         <v>1306</v>
       </c>
-      <c r="C5" s="360" t="n">
+      <c r="C5" s="377" t="n">
         <v>2</v>
       </c>
       <c r="D5" s="101" t="inlineStr">
@@ -1486,49 +1510,49 @@
           <t>DoubleSpice</t>
         </is>
       </c>
-      <c r="E5" s="361" t="n">
+      <c r="E5" s="378" t="n">
         <v>6</v>
       </c>
       <c r="F5" s="101" t="n">
         <v>13656</v>
       </c>
-      <c r="G5" s="362" t="n">
+      <c r="G5" s="379" t="n">
         <v>0</v>
       </c>
       <c r="H5" s="104" t="n">
         <v>0</v>
       </c>
-      <c r="I5" s="361" t="n">
+      <c r="I5" s="378" t="n">
         <v>6</v>
       </c>
       <c r="J5" s="101" t="n">
         <v>10016</v>
       </c>
-      <c r="K5" s="361" t="n">
+      <c r="K5" s="378" t="n">
         <v>6</v>
       </c>
       <c r="L5" s="101" t="n">
         <v>11620</v>
       </c>
-      <c r="M5" s="361" t="n">
+      <c r="M5" s="378" t="n">
         <v>6</v>
       </c>
       <c r="N5" s="101" t="n">
         <v>14095</v>
       </c>
-      <c r="O5" s="361" t="n">
+      <c r="O5" s="378" t="n">
         <v>6</v>
       </c>
       <c r="P5" s="101" t="n">
         <v>12379</v>
       </c>
-      <c r="Q5" s="361" t="n">
+      <c r="Q5" s="378" t="n">
         <v>6</v>
       </c>
       <c r="R5" s="101" t="n">
         <v>8256</v>
       </c>
-      <c r="S5" s="361" t="n">
+      <c r="S5" s="378" t="n">
         <v>6</v>
       </c>
       <c r="T5" s="101" t="n">
@@ -1536,15 +1560,15 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="355" t="inlineStr">
+      <c r="A6" s="372" t="inlineStr">
         <is>
           <t>#90U0VPU9U</t>
         </is>
       </c>
-      <c r="B6" s="355" t="n">
+      <c r="B6" s="372" t="n">
         <v>2597</v>
       </c>
-      <c r="C6" s="356" t="n">
+      <c r="C6" s="373" t="n">
         <v>3</v>
       </c>
       <c r="D6" s="95" t="inlineStr">
@@ -1552,49 +1576,49 @@
           <t>KYANI7E</t>
         </is>
       </c>
-      <c r="E6" s="357" t="n">
+      <c r="E6" s="374" t="n">
         <v>6</v>
       </c>
       <c r="F6" s="95" t="n">
         <v>13278</v>
       </c>
-      <c r="G6" s="363" t="n">
+      <c r="G6" s="380" t="n">
         <v>141</v>
       </c>
       <c r="H6" s="98" t="n">
         <v>0</v>
       </c>
-      <c r="I6" s="357" t="n">
+      <c r="I6" s="374" t="n">
         <v>6</v>
       </c>
       <c r="J6" s="95" t="n">
         <v>12477</v>
       </c>
-      <c r="K6" s="357" t="n">
+      <c r="K6" s="374" t="n">
         <v>6</v>
       </c>
       <c r="L6" s="95" t="n">
         <v>13260</v>
       </c>
-      <c r="M6" s="357" t="n">
+      <c r="M6" s="374" t="n">
         <v>6</v>
       </c>
       <c r="N6" s="95" t="n">
         <v>12144</v>
       </c>
-      <c r="O6" s="357" t="n">
+      <c r="O6" s="374" t="n">
         <v>6</v>
       </c>
       <c r="P6" s="95" t="n">
         <v>12835</v>
       </c>
-      <c r="Q6" s="357" t="n">
+      <c r="Q6" s="374" t="n">
         <v>6</v>
       </c>
       <c r="R6" s="95" t="n">
         <v>7696</v>
       </c>
-      <c r="S6" s="357" t="n">
+      <c r="S6" s="374" t="n">
         <v>6</v>
       </c>
       <c r="T6" s="95" t="n">
@@ -1602,15 +1626,15 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="359" t="inlineStr">
+      <c r="A7" s="376" t="inlineStr">
         <is>
           <t>#YJ20CRJYQ</t>
         </is>
       </c>
-      <c r="B7" s="359" t="n">
+      <c r="B7" s="376" t="n">
         <v>1255</v>
       </c>
-      <c r="C7" s="360" t="n">
+      <c r="C7" s="377" t="n">
         <v>4</v>
       </c>
       <c r="D7" s="101" t="inlineStr">
@@ -1618,49 +1642,49 @@
           <t>UnluckGod</t>
         </is>
       </c>
-      <c r="E7" s="361" t="n">
+      <c r="E7" s="378" t="n">
         <v>6</v>
       </c>
       <c r="F7" s="101" t="n">
         <v>13062</v>
       </c>
-      <c r="G7" s="362" t="n">
+      <c r="G7" s="379" t="n">
         <v>0</v>
       </c>
       <c r="H7" s="104" t="n">
         <v>0</v>
       </c>
-      <c r="I7" s="361" t="n">
+      <c r="I7" s="378" t="n">
         <v>6</v>
       </c>
       <c r="J7" s="101" t="n">
         <v>8886</v>
       </c>
-      <c r="K7" s="361" t="n">
+      <c r="K7" s="378" t="n">
         <v>6</v>
       </c>
       <c r="L7" s="101" t="n">
         <v>12824</v>
       </c>
-      <c r="M7" s="361" t="n">
+      <c r="M7" s="378" t="n">
         <v>6</v>
       </c>
       <c r="N7" s="101" t="n">
         <v>11999</v>
       </c>
-      <c r="O7" s="361" t="n">
+      <c r="O7" s="378" t="n">
         <v>6</v>
       </c>
       <c r="P7" s="101" t="n">
         <v>12972</v>
       </c>
-      <c r="Q7" s="361" t="n">
+      <c r="Q7" s="378" t="n">
         <v>6</v>
       </c>
       <c r="R7" s="101" t="n">
         <v>8286</v>
       </c>
-      <c r="S7" s="361" t="n">
+      <c r="S7" s="378" t="n">
         <v>6</v>
       </c>
       <c r="T7" s="101" t="n">
@@ -1668,15 +1692,15 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="355" t="inlineStr">
+      <c r="A8" s="372" t="inlineStr">
         <is>
           <t>#QUYG0PQC8</t>
         </is>
       </c>
-      <c r="B8" s="355" t="n">
+      <c r="B8" s="372" t="n">
         <v>854</v>
       </c>
-      <c r="C8" s="356" t="n">
+      <c r="C8" s="373" t="n">
         <v>5</v>
       </c>
       <c r="D8" s="95" t="inlineStr">
@@ -1684,49 +1708,49 @@
           <t>Luffy</t>
         </is>
       </c>
-      <c r="E8" s="357" t="n">
+      <c r="E8" s="374" t="n">
         <v>6</v>
       </c>
       <c r="F8" s="95" t="n">
         <v>12820</v>
       </c>
-      <c r="G8" s="358" t="n">
+      <c r="G8" s="375" t="n">
         <v>0</v>
       </c>
       <c r="H8" s="98" t="n">
         <v>0</v>
       </c>
-      <c r="I8" s="357" t="n">
+      <c r="I8" s="374" t="n">
         <v>6</v>
       </c>
       <c r="J8" s="95" t="n">
         <v>11357</v>
       </c>
-      <c r="K8" s="357" t="n">
+      <c r="K8" s="374" t="n">
         <v>6</v>
       </c>
       <c r="L8" s="95" t="n">
         <v>10879</v>
       </c>
-      <c r="M8" s="357" t="n">
+      <c r="M8" s="374" t="n">
         <v>6</v>
       </c>
       <c r="N8" s="95" t="n">
         <v>9114</v>
       </c>
-      <c r="O8" s="357" t="n">
+      <c r="O8" s="374" t="n">
         <v>6</v>
       </c>
       <c r="P8" s="95" t="n">
         <v>13385</v>
       </c>
-      <c r="Q8" s="357" t="n">
+      <c r="Q8" s="374" t="n">
         <v>6</v>
       </c>
       <c r="R8" s="95" t="n">
         <v>7877</v>
       </c>
-      <c r="S8" s="357" t="n">
+      <c r="S8" s="374" t="n">
         <v>6</v>
       </c>
       <c r="T8" s="95" t="n">
@@ -1734,15 +1758,15 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="364" t="inlineStr">
+      <c r="A9" s="381" t="inlineStr">
         <is>
           <t>#LPCLQUCCY</t>
         </is>
       </c>
-      <c r="B9" s="364" t="n">
+      <c r="B9" s="381" t="n">
         <v>1024</v>
       </c>
-      <c r="C9" s="360" t="n">
+      <c r="C9" s="377" t="n">
         <v>6</v>
       </c>
       <c r="D9" s="106" t="inlineStr">
@@ -1750,49 +1774,49 @@
           <t>Zodiac</t>
         </is>
       </c>
-      <c r="E9" s="365" t="n">
+      <c r="E9" s="382" t="n">
         <v>6</v>
       </c>
       <c r="F9" s="106" t="n">
         <v>12035</v>
       </c>
-      <c r="G9" s="366" t="n">
+      <c r="G9" s="383" t="n">
         <v>0</v>
       </c>
       <c r="H9" s="109" t="n">
         <v>0</v>
       </c>
-      <c r="I9" s="365" t="n">
+      <c r="I9" s="382" t="n">
         <v>6</v>
       </c>
       <c r="J9" s="106" t="n">
         <v>7463</v>
       </c>
-      <c r="K9" s="366" t="n">
+      <c r="K9" s="383" t="n">
         <v>0</v>
       </c>
       <c r="L9" s="110" t="n">
         <v>0</v>
       </c>
-      <c r="M9" s="364" t="n"/>
+      <c r="M9" s="381" t="n"/>
       <c r="N9" s="109" t="n"/>
-      <c r="O9" s="364" t="n"/>
+      <c r="O9" s="381" t="n"/>
       <c r="P9" s="109" t="n"/>
-      <c r="Q9" s="364" t="n"/>
+      <c r="Q9" s="381" t="n"/>
       <c r="R9" s="109" t="n"/>
-      <c r="S9" s="364" t="n"/>
+      <c r="S9" s="381" t="n"/>
       <c r="T9" s="109" t="n"/>
     </row>
     <row r="10">
-      <c r="A10" s="355" t="inlineStr">
+      <c r="A10" s="372" t="inlineStr">
         <is>
           <t>#QUV2GP88U</t>
         </is>
       </c>
-      <c r="B10" s="355" t="n">
+      <c r="B10" s="372" t="n">
         <v>777</v>
       </c>
-      <c r="C10" s="356" t="n">
+      <c r="C10" s="373" t="n">
         <v>7</v>
       </c>
       <c r="D10" s="95" t="inlineStr">
@@ -1800,49 +1824,49 @@
           <t>Nico Robin</t>
         </is>
       </c>
-      <c r="E10" s="357" t="n">
+      <c r="E10" s="374" t="n">
         <v>6</v>
       </c>
       <c r="F10" s="95" t="n">
         <v>11670</v>
       </c>
-      <c r="G10" s="358" t="n">
+      <c r="G10" s="375" t="n">
         <v>0</v>
       </c>
       <c r="H10" s="98" t="n">
         <v>0</v>
       </c>
-      <c r="I10" s="357" t="n">
+      <c r="I10" s="374" t="n">
         <v>6</v>
       </c>
       <c r="J10" s="95" t="n">
         <v>10389</v>
       </c>
-      <c r="K10" s="357" t="n">
+      <c r="K10" s="374" t="n">
         <v>6</v>
       </c>
       <c r="L10" s="95" t="n">
         <v>12612</v>
       </c>
-      <c r="M10" s="357" t="n">
+      <c r="M10" s="374" t="n">
         <v>6</v>
       </c>
       <c r="N10" s="95" t="n">
         <v>11338</v>
       </c>
-      <c r="O10" s="357" t="n">
+      <c r="O10" s="374" t="n">
         <v>6</v>
       </c>
       <c r="P10" s="95" t="n">
         <v>10997</v>
       </c>
-      <c r="Q10" s="357" t="n">
+      <c r="Q10" s="374" t="n">
         <v>6</v>
       </c>
       <c r="R10" s="95" t="n">
         <v>11087</v>
       </c>
-      <c r="S10" s="357" t="n">
+      <c r="S10" s="374" t="n">
         <v>6</v>
       </c>
       <c r="T10" s="95" t="n">
@@ -1850,15 +1874,15 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="359" t="inlineStr">
+      <c r="A11" s="376" t="inlineStr">
         <is>
           <t>#QCV22VP0G</t>
         </is>
       </c>
-      <c r="B11" s="359" t="n">
+      <c r="B11" s="376" t="n">
         <v>774</v>
       </c>
-      <c r="C11" s="360" t="n">
+      <c r="C11" s="377" t="n">
         <v>8</v>
       </c>
       <c r="D11" s="101" t="inlineStr">
@@ -1866,49 +1890,49 @@
           <t>Nami</t>
         </is>
       </c>
-      <c r="E11" s="361" t="n">
+      <c r="E11" s="378" t="n">
         <v>6</v>
       </c>
       <c r="F11" s="101" t="n">
         <v>11484</v>
       </c>
-      <c r="G11" s="362" t="n">
+      <c r="G11" s="379" t="n">
         <v>0</v>
       </c>
       <c r="H11" s="104" t="n">
         <v>0</v>
       </c>
-      <c r="I11" s="361" t="n">
+      <c r="I11" s="378" t="n">
         <v>6</v>
       </c>
       <c r="J11" s="101" t="n">
         <v>11657</v>
       </c>
-      <c r="K11" s="361" t="n">
+      <c r="K11" s="378" t="n">
         <v>6</v>
       </c>
       <c r="L11" s="101" t="n">
         <v>11795</v>
       </c>
-      <c r="M11" s="361" t="n">
+      <c r="M11" s="378" t="n">
         <v>6</v>
       </c>
       <c r="N11" s="101" t="n">
         <v>10769</v>
       </c>
-      <c r="O11" s="361" t="n">
+      <c r="O11" s="378" t="n">
         <v>6</v>
       </c>
       <c r="P11" s="101" t="n">
         <v>12486</v>
       </c>
-      <c r="Q11" s="361" t="n">
+      <c r="Q11" s="378" t="n">
         <v>6</v>
       </c>
       <c r="R11" s="101" t="n">
         <v>8472</v>
       </c>
-      <c r="S11" s="361" t="n">
+      <c r="S11" s="378" t="n">
         <v>6</v>
       </c>
       <c r="T11" s="101" t="n">
@@ -1916,15 +1940,15 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="355" t="inlineStr">
+      <c r="A12" s="372" t="inlineStr">
         <is>
           <t>#QLR088LC9</t>
         </is>
       </c>
-      <c r="B12" s="355" t="n">
+      <c r="B12" s="372" t="n">
         <v>814</v>
       </c>
-      <c r="C12" s="356" t="n">
+      <c r="C12" s="373" t="n">
         <v>9</v>
       </c>
       <c r="D12" s="95" t="inlineStr">
@@ -1932,49 +1956,49 @@
           <t>Sanji</t>
         </is>
       </c>
-      <c r="E12" s="357" t="n">
+      <c r="E12" s="374" t="n">
         <v>6</v>
       </c>
       <c r="F12" s="95" t="n">
         <v>11473</v>
       </c>
-      <c r="G12" s="358" t="n">
+      <c r="G12" s="375" t="n">
         <v>0</v>
       </c>
       <c r="H12" s="98" t="n">
         <v>0</v>
       </c>
-      <c r="I12" s="357" t="n">
+      <c r="I12" s="374" t="n">
         <v>6</v>
       </c>
       <c r="J12" s="95" t="n">
         <v>11960</v>
       </c>
-      <c r="K12" s="357" t="n">
+      <c r="K12" s="374" t="n">
         <v>6</v>
       </c>
       <c r="L12" s="95" t="n">
         <v>10910</v>
       </c>
-      <c r="M12" s="357" t="n">
+      <c r="M12" s="374" t="n">
         <v>6</v>
       </c>
       <c r="N12" s="95" t="n">
         <v>9550</v>
       </c>
-      <c r="O12" s="357" t="n">
+      <c r="O12" s="374" t="n">
         <v>6</v>
       </c>
       <c r="P12" s="95" t="n">
         <v>9138</v>
       </c>
-      <c r="Q12" s="357" t="n">
+      <c r="Q12" s="374" t="n">
         <v>6</v>
       </c>
       <c r="R12" s="95" t="n">
         <v>8897</v>
       </c>
-      <c r="S12" s="357" t="n">
+      <c r="S12" s="374" t="n">
         <v>6</v>
       </c>
       <c r="T12" s="95" t="n">
@@ -1982,15 +2006,15 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="359" t="inlineStr">
+      <c r="A13" s="376" t="inlineStr">
         <is>
           <t>#QLJ2U20Y2</t>
         </is>
       </c>
-      <c r="B13" s="359" t="n">
+      <c r="B13" s="376" t="n">
         <v>1484</v>
       </c>
-      <c r="C13" s="360" t="n">
+      <c r="C13" s="377" t="n">
         <v>10</v>
       </c>
       <c r="D13" s="101" t="inlineStr">
@@ -1998,49 +2022,49 @@
           <t>DeadLeaf</t>
         </is>
       </c>
-      <c r="E13" s="361" t="n">
+      <c r="E13" s="378" t="n">
         <v>6</v>
       </c>
       <c r="F13" s="101" t="n">
         <v>11433</v>
       </c>
-      <c r="G13" s="362" t="n">
+      <c r="G13" s="379" t="n">
         <v>0</v>
       </c>
       <c r="H13" s="104" t="n">
         <v>0</v>
       </c>
-      <c r="I13" s="361" t="n">
+      <c r="I13" s="378" t="n">
         <v>6</v>
       </c>
       <c r="J13" s="101" t="n">
         <v>12676</v>
       </c>
-      <c r="K13" s="361" t="n">
+      <c r="K13" s="378" t="n">
         <v>6</v>
       </c>
       <c r="L13" s="101" t="n">
         <v>13763</v>
       </c>
-      <c r="M13" s="361" t="n">
+      <c r="M13" s="378" t="n">
         <v>6</v>
       </c>
       <c r="N13" s="101" t="n">
         <v>11140</v>
       </c>
-      <c r="O13" s="361" t="n">
+      <c r="O13" s="378" t="n">
         <v>6</v>
       </c>
       <c r="P13" s="101" t="n">
         <v>15509</v>
       </c>
-      <c r="Q13" s="361" t="n">
+      <c r="Q13" s="378" t="n">
         <v>6</v>
       </c>
       <c r="R13" s="101" t="n">
         <v>8567</v>
       </c>
-      <c r="S13" s="361" t="n">
+      <c r="S13" s="378" t="n">
         <v>6</v>
       </c>
       <c r="T13" s="101" t="n">
@@ -2048,15 +2072,15 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="355" t="inlineStr">
+      <c r="A14" s="372" t="inlineStr">
         <is>
           <t>#Q8CLCUCC2</t>
         </is>
       </c>
-      <c r="B14" s="355" t="n">
+      <c r="B14" s="372" t="n">
         <v>1409</v>
       </c>
-      <c r="C14" s="356" t="n">
+      <c r="C14" s="373" t="n">
         <v>11</v>
       </c>
       <c r="D14" s="95" t="inlineStr">
@@ -2064,49 +2088,49 @@
           <t>Moxxi</t>
         </is>
       </c>
-      <c r="E14" s="357" t="n">
+      <c r="E14" s="374" t="n">
         <v>6</v>
       </c>
       <c r="F14" s="95" t="n">
         <v>10777</v>
       </c>
-      <c r="G14" s="358" t="n">
+      <c r="G14" s="375" t="n">
         <v>0</v>
       </c>
       <c r="H14" s="98" t="n">
         <v>0</v>
       </c>
-      <c r="I14" s="357" t="n">
+      <c r="I14" s="374" t="n">
         <v>6</v>
       </c>
       <c r="J14" s="95" t="n">
         <v>12912</v>
       </c>
-      <c r="K14" s="357" t="n">
+      <c r="K14" s="374" t="n">
         <v>6</v>
       </c>
       <c r="L14" s="95" t="n">
         <v>8015</v>
       </c>
-      <c r="M14" s="357" t="n">
+      <c r="M14" s="374" t="n">
         <v>6</v>
       </c>
       <c r="N14" s="95" t="n">
         <v>11010</v>
       </c>
-      <c r="O14" s="357" t="n">
+      <c r="O14" s="374" t="n">
         <v>6</v>
       </c>
       <c r="P14" s="95" t="n">
         <v>13857</v>
       </c>
-      <c r="Q14" s="357" t="n">
+      <c r="Q14" s="374" t="n">
         <v>6</v>
       </c>
       <c r="R14" s="95" t="n">
         <v>7905</v>
       </c>
-      <c r="S14" s="357" t="n">
+      <c r="S14" s="374" t="n">
         <v>6</v>
       </c>
       <c r="T14" s="95" t="n">
@@ -2114,15 +2138,15 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="359" t="inlineStr">
+      <c r="A15" s="376" t="inlineStr">
         <is>
           <t>#QUG8QQJ92</t>
         </is>
       </c>
-      <c r="B15" s="359" t="n">
+      <c r="B15" s="376" t="n">
         <v>894</v>
       </c>
-      <c r="C15" s="360" t="n">
+      <c r="C15" s="377" t="n">
         <v>12</v>
       </c>
       <c r="D15" s="101" t="inlineStr">
@@ -2130,49 +2154,49 @@
           <t>Karma</t>
         </is>
       </c>
-      <c r="E15" s="361" t="n">
+      <c r="E15" s="378" t="n">
         <v>6</v>
       </c>
       <c r="F15" s="101" t="n">
         <v>10105</v>
       </c>
-      <c r="G15" s="362" t="n">
+      <c r="G15" s="379" t="n">
         <v>0</v>
       </c>
       <c r="H15" s="104" t="n">
         <v>0</v>
       </c>
-      <c r="I15" s="361" t="n">
+      <c r="I15" s="378" t="n">
         <v>6</v>
       </c>
       <c r="J15" s="101" t="n">
         <v>12204</v>
       </c>
-      <c r="K15" s="361" t="n">
+      <c r="K15" s="378" t="n">
         <v>6</v>
       </c>
       <c r="L15" s="101" t="n">
         <v>11355</v>
       </c>
-      <c r="M15" s="361" t="n">
+      <c r="M15" s="378" t="n">
         <v>6</v>
       </c>
       <c r="N15" s="101" t="n">
         <v>10003</v>
       </c>
-      <c r="O15" s="361" t="n">
+      <c r="O15" s="378" t="n">
         <v>6</v>
       </c>
       <c r="P15" s="101" t="n">
         <v>10595</v>
       </c>
-      <c r="Q15" s="361" t="n">
+      <c r="Q15" s="378" t="n">
         <v>6</v>
       </c>
       <c r="R15" s="101" t="n">
         <v>9240</v>
       </c>
-      <c r="S15" s="361" t="n">
+      <c r="S15" s="378" t="n">
         <v>6</v>
       </c>
       <c r="T15" s="101" t="n">
@@ -2180,15 +2204,15 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="367" t="inlineStr">
+      <c r="A16" s="384" t="inlineStr">
         <is>
           <t>#QUGYGY88C</t>
         </is>
       </c>
-      <c r="B16" s="367" t="n">
+      <c r="B16" s="384" t="n">
         <v>971</v>
       </c>
-      <c r="C16" s="356" t="n">
+      <c r="C16" s="373" t="n">
         <v>13</v>
       </c>
       <c r="D16" s="112" t="inlineStr">
@@ -2196,49 +2220,49 @@
           <t>Kingsman</t>
         </is>
       </c>
-      <c r="E16" s="368" t="n">
+      <c r="E16" s="385" t="n">
         <v>6</v>
       </c>
       <c r="F16" s="112" t="n">
         <v>9948</v>
       </c>
-      <c r="G16" s="369" t="n">
+      <c r="G16" s="386" t="n">
         <v>0</v>
       </c>
       <c r="H16" s="115" t="n">
         <v>0</v>
       </c>
-      <c r="I16" s="369" t="n">
+      <c r="I16" s="386" t="n">
         <v>0</v>
       </c>
       <c r="J16" s="116" t="n">
         <v>0</v>
       </c>
-      <c r="K16" s="369" t="n">
+      <c r="K16" s="386" t="n">
         <v>0</v>
       </c>
       <c r="L16" s="116" t="n">
         <v>0</v>
       </c>
-      <c r="M16" s="367" t="n"/>
+      <c r="M16" s="384" t="n"/>
       <c r="N16" s="115" t="n"/>
-      <c r="O16" s="367" t="n"/>
+      <c r="O16" s="384" t="n"/>
       <c r="P16" s="115" t="n"/>
-      <c r="Q16" s="367" t="n"/>
+      <c r="Q16" s="384" t="n"/>
       <c r="R16" s="115" t="n"/>
-      <c r="S16" s="367" t="n"/>
+      <c r="S16" s="384" t="n"/>
       <c r="T16" s="115" t="n"/>
     </row>
     <row r="17">
-      <c r="A17" s="364" t="inlineStr">
+      <c r="A17" s="381" t="inlineStr">
         <is>
           <t>#98JG2UJQL</t>
         </is>
       </c>
-      <c r="B17" s="364" t="n">
+      <c r="B17" s="381" t="n">
         <v>3030</v>
       </c>
-      <c r="C17" s="360" t="n">
+      <c r="C17" s="377" t="n">
         <v>14</v>
       </c>
       <c r="D17" s="106" t="inlineStr">
@@ -2246,49 +2270,49 @@
           <t>Dragonux</t>
         </is>
       </c>
-      <c r="E17" s="365" t="n">
+      <c r="E17" s="382" t="n">
         <v>6</v>
       </c>
       <c r="F17" s="106" t="n">
         <v>8745</v>
       </c>
-      <c r="G17" s="366" t="n">
+      <c r="G17" s="383" t="n">
         <v>0</v>
       </c>
       <c r="H17" s="109" t="n">
         <v>0</v>
       </c>
-      <c r="I17" s="365" t="n">
+      <c r="I17" s="382" t="n">
         <v>6</v>
       </c>
       <c r="J17" s="106" t="n">
         <v>10385</v>
       </c>
-      <c r="K17" s="365" t="n">
+      <c r="K17" s="382" t="n">
         <v>6</v>
       </c>
       <c r="L17" s="106" t="n">
         <v>10910</v>
       </c>
-      <c r="M17" s="365" t="n">
+      <c r="M17" s="382" t="n">
         <v>6</v>
       </c>
       <c r="N17" s="106" t="n">
         <v>8750</v>
       </c>
-      <c r="O17" s="365" t="n">
+      <c r="O17" s="382" t="n">
         <v>6</v>
       </c>
       <c r="P17" s="106" t="n">
         <v>10865</v>
       </c>
-      <c r="Q17" s="365" t="n">
+      <c r="Q17" s="382" t="n">
         <v>6</v>
       </c>
       <c r="R17" s="106" t="n">
         <v>8025</v>
       </c>
-      <c r="S17" s="365" t="n">
+      <c r="S17" s="382" t="n">
         <v>6</v>
       </c>
       <c r="T17" s="106" t="n">
@@ -2296,15 +2320,15 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="367" t="inlineStr">
+      <c r="A18" s="384" t="inlineStr">
         <is>
           <t>#G0JPUQGYR</t>
         </is>
       </c>
-      <c r="B18" s="367" t="n">
+      <c r="B18" s="384" t="n">
         <v>1540</v>
       </c>
-      <c r="C18" s="356" t="n">
+      <c r="C18" s="373" t="n">
         <v>15</v>
       </c>
       <c r="D18" s="112" t="inlineStr">
@@ -2312,49 +2336,49 @@
           <t>Collin</t>
         </is>
       </c>
-      <c r="E18" s="368" t="n">
+      <c r="E18" s="385" t="n">
         <v>6</v>
       </c>
       <c r="F18" s="112" t="n">
         <v>8725</v>
       </c>
-      <c r="G18" s="369" t="n">
+      <c r="G18" s="386" t="n">
         <v>0</v>
       </c>
       <c r="H18" s="115" t="n">
         <v>0</v>
       </c>
-      <c r="I18" s="368" t="n">
+      <c r="I18" s="385" t="n">
         <v>6</v>
       </c>
       <c r="J18" s="112" t="n">
         <v>10299</v>
       </c>
-      <c r="K18" s="368" t="n">
+      <c r="K18" s="385" t="n">
         <v>6</v>
       </c>
       <c r="L18" s="112" t="n">
         <v>8833</v>
       </c>
-      <c r="M18" s="368" t="n">
+      <c r="M18" s="385" t="n">
         <v>6</v>
       </c>
       <c r="N18" s="112" t="n">
         <v>9238</v>
       </c>
-      <c r="O18" s="368" t="n">
+      <c r="O18" s="385" t="n">
         <v>6</v>
       </c>
       <c r="P18" s="112" t="n">
         <v>7756</v>
       </c>
-      <c r="Q18" s="368" t="n">
+      <c r="Q18" s="385" t="n">
         <v>6</v>
       </c>
       <c r="R18" s="117" t="n">
         <v>5943</v>
       </c>
-      <c r="S18" s="368" t="n">
+      <c r="S18" s="385" t="n">
         <v>6</v>
       </c>
       <c r="T18" s="112" t="n">
@@ -2362,15 +2386,15 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="364" t="inlineStr">
+      <c r="A19" s="381" t="inlineStr">
         <is>
           <t>#8U9CRC8G</t>
         </is>
       </c>
-      <c r="B19" s="364" t="n">
+      <c r="B19" s="381" t="n">
         <v>1773</v>
       </c>
-      <c r="C19" s="360" t="n">
+      <c r="C19" s="377" t="n">
         <v>16</v>
       </c>
       <c r="D19" s="106" t="inlineStr">
@@ -2378,49 +2402,49 @@
           <t>CEO JACK</t>
         </is>
       </c>
-      <c r="E19" s="365" t="n">
+      <c r="E19" s="382" t="n">
         <v>6</v>
       </c>
       <c r="F19" s="106" t="n">
         <v>8657</v>
       </c>
-      <c r="G19" s="370" t="n">
+      <c r="G19" s="387" t="n">
         <v>16</v>
       </c>
       <c r="H19" s="109" t="n">
         <v>132</v>
       </c>
-      <c r="I19" s="365" t="n">
+      <c r="I19" s="382" t="n">
         <v>6</v>
       </c>
       <c r="J19" s="106" t="n">
         <v>6980</v>
       </c>
-      <c r="K19" s="366" t="n">
+      <c r="K19" s="383" t="n">
         <v>0</v>
       </c>
       <c r="L19" s="110" t="n">
         <v>0</v>
       </c>
-      <c r="M19" s="364" t="n"/>
+      <c r="M19" s="381" t="n"/>
       <c r="N19" s="109" t="n"/>
-      <c r="O19" s="364" t="n"/>
+      <c r="O19" s="381" t="n"/>
       <c r="P19" s="109" t="n"/>
-      <c r="Q19" s="364" t="n"/>
+      <c r="Q19" s="381" t="n"/>
       <c r="R19" s="109" t="n"/>
-      <c r="S19" s="364" t="n"/>
+      <c r="S19" s="381" t="n"/>
       <c r="T19" s="109" t="n"/>
     </row>
     <row r="20">
-      <c r="A20" s="367" t="inlineStr">
+      <c r="A20" s="384" t="inlineStr">
         <is>
           <t>#LLQQ8CGPV</t>
         </is>
       </c>
-      <c r="B20" s="367" t="n">
+      <c r="B20" s="384" t="n">
         <v>1405</v>
       </c>
-      <c r="C20" s="356" t="n">
+      <c r="C20" s="373" t="n">
         <v>17</v>
       </c>
       <c r="D20" s="112" t="inlineStr">
@@ -2428,41 +2452,41 @@
           <t>jojomoonky</t>
         </is>
       </c>
-      <c r="E20" s="368" t="n">
+      <c r="E20" s="385" t="n">
         <v>6</v>
       </c>
       <c r="F20" s="112" t="n">
         <v>8465</v>
       </c>
-      <c r="G20" s="369" t="n">
+      <c r="G20" s="386" t="n">
         <v>0</v>
       </c>
       <c r="H20" s="115" t="n">
         <v>0</v>
       </c>
-      <c r="I20" s="367" t="n"/>
+      <c r="I20" s="384" t="n"/>
       <c r="J20" s="115" t="n"/>
-      <c r="K20" s="367" t="n"/>
+      <c r="K20" s="384" t="n"/>
       <c r="L20" s="115" t="n"/>
-      <c r="M20" s="367" t="n"/>
+      <c r="M20" s="384" t="n"/>
       <c r="N20" s="115" t="n"/>
-      <c r="O20" s="367" t="n"/>
+      <c r="O20" s="384" t="n"/>
       <c r="P20" s="115" t="n"/>
-      <c r="Q20" s="367" t="n"/>
+      <c r="Q20" s="384" t="n"/>
       <c r="R20" s="115" t="n"/>
-      <c r="S20" s="367" t="n"/>
+      <c r="S20" s="384" t="n"/>
       <c r="T20" s="115" t="n"/>
     </row>
     <row r="21">
-      <c r="A21" s="364" t="inlineStr">
+      <c r="A21" s="381" t="inlineStr">
         <is>
           <t>#QRPRYR8LL</t>
         </is>
       </c>
-      <c r="B21" s="364" t="n">
+      <c r="B21" s="381" t="n">
         <v>1216</v>
       </c>
-      <c r="C21" s="360" t="n">
+      <c r="C21" s="377" t="n">
         <v>18</v>
       </c>
       <c r="D21" s="106" t="inlineStr">
@@ -2470,49 +2494,49 @@
           <t>FidelCashflow</t>
         </is>
       </c>
-      <c r="E21" s="365" t="n">
+      <c r="E21" s="382" t="n">
         <v>6</v>
       </c>
       <c r="F21" s="106" t="n">
         <v>8263</v>
       </c>
-      <c r="G21" s="366" t="n">
+      <c r="G21" s="383" t="n">
         <v>0</v>
       </c>
       <c r="H21" s="109" t="n">
         <v>0</v>
       </c>
-      <c r="I21" s="365" t="n">
+      <c r="I21" s="382" t="n">
         <v>6</v>
       </c>
       <c r="J21" s="106" t="n">
         <v>8298</v>
       </c>
-      <c r="K21" s="365" t="n">
+      <c r="K21" s="382" t="n">
         <v>6</v>
       </c>
       <c r="L21" s="106" t="n">
         <v>6415</v>
       </c>
-      <c r="M21" s="365" t="n">
+      <c r="M21" s="382" t="n">
         <v>6</v>
       </c>
       <c r="N21" s="106" t="n">
         <v>6547</v>
       </c>
-      <c r="O21" s="365" t="n">
+      <c r="O21" s="382" t="n">
         <v>6</v>
       </c>
       <c r="P21" s="106" t="n">
         <v>6811</v>
       </c>
-      <c r="Q21" s="365" t="n">
+      <c r="Q21" s="382" t="n">
         <v>6</v>
       </c>
       <c r="R21" s="118" t="n">
         <v>4239</v>
       </c>
-      <c r="S21" s="365" t="n">
+      <c r="S21" s="382" t="n">
         <v>6</v>
       </c>
       <c r="T21" s="118" t="n">
@@ -2520,15 +2544,15 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="367" t="inlineStr">
+      <c r="A22" s="384" t="inlineStr">
         <is>
           <t>#QLGUYQPL0</t>
         </is>
       </c>
-      <c r="B22" s="367" t="n">
+      <c r="B22" s="384" t="n">
         <v>1529</v>
       </c>
-      <c r="C22" s="356" t="n">
+      <c r="C22" s="373" t="n">
         <v>19</v>
       </c>
       <c r="D22" s="112" t="inlineStr">
@@ -2536,45 +2560,45 @@
           <t>i got time</t>
         </is>
       </c>
-      <c r="E22" s="368" t="n">
+      <c r="E22" s="385" t="n">
         <v>6</v>
       </c>
       <c r="F22" s="112" t="n">
         <v>8087</v>
       </c>
-      <c r="G22" s="369" t="n">
+      <c r="G22" s="386" t="n">
         <v>0</v>
       </c>
       <c r="H22" s="115" t="n">
         <v>0</v>
       </c>
-      <c r="I22" s="369" t="n">
+      <c r="I22" s="386" t="n">
         <v>1</v>
       </c>
       <c r="J22" s="116" t="n">
         <v>1435</v>
       </c>
-      <c r="K22" s="367" t="n"/>
+      <c r="K22" s="384" t="n"/>
       <c r="L22" s="115" t="n"/>
-      <c r="M22" s="367" t="n"/>
+      <c r="M22" s="384" t="n"/>
       <c r="N22" s="115" t="n"/>
-      <c r="O22" s="367" t="n"/>
+      <c r="O22" s="384" t="n"/>
       <c r="P22" s="115" t="n"/>
-      <c r="Q22" s="367" t="n"/>
+      <c r="Q22" s="384" t="n"/>
       <c r="R22" s="115" t="n"/>
-      <c r="S22" s="367" t="n"/>
+      <c r="S22" s="384" t="n"/>
       <c r="T22" s="115" t="n"/>
     </row>
     <row r="23">
-      <c r="A23" s="364" t="inlineStr">
+      <c r="A23" s="381" t="inlineStr">
         <is>
           <t>#G0LJCVR2P</t>
         </is>
       </c>
-      <c r="B23" s="364" t="n">
+      <c r="B23" s="381" t="n">
         <v>1188</v>
       </c>
-      <c r="C23" s="360" t="n">
+      <c r="C23" s="377" t="n">
         <v>20</v>
       </c>
       <c r="D23" s="106" t="inlineStr">
@@ -2582,45 +2606,45 @@
           <t>DaddyChill</t>
         </is>
       </c>
-      <c r="E23" s="365" t="n">
+      <c r="E23" s="382" t="n">
         <v>6</v>
       </c>
       <c r="F23" s="106" t="n">
         <v>7874</v>
       </c>
-      <c r="G23" s="366" t="n">
+      <c r="G23" s="383" t="n">
         <v>0</v>
       </c>
       <c r="H23" s="109" t="n">
         <v>0</v>
       </c>
-      <c r="I23" s="366" t="n">
+      <c r="I23" s="383" t="n">
         <v>0</v>
       </c>
       <c r="J23" s="110" t="n">
         <v>0</v>
       </c>
-      <c r="K23" s="364" t="n"/>
+      <c r="K23" s="381" t="n"/>
       <c r="L23" s="109" t="n"/>
-      <c r="M23" s="364" t="n"/>
+      <c r="M23" s="381" t="n"/>
       <c r="N23" s="109" t="n"/>
-      <c r="O23" s="364" t="n"/>
+      <c r="O23" s="381" t="n"/>
       <c r="P23" s="109" t="n"/>
-      <c r="Q23" s="364" t="n"/>
+      <c r="Q23" s="381" t="n"/>
       <c r="R23" s="109" t="n"/>
-      <c r="S23" s="364" t="n"/>
+      <c r="S23" s="381" t="n"/>
       <c r="T23" s="109" t="n"/>
     </row>
     <row r="24">
-      <c r="A24" s="367" t="inlineStr">
+      <c r="A24" s="384" t="inlineStr">
         <is>
           <t>#QU0U2Q99G</t>
         </is>
       </c>
-      <c r="B24" s="367" t="n">
+      <c r="B24" s="384" t="n">
         <v>1010</v>
       </c>
-      <c r="C24" s="356" t="n">
+      <c r="C24" s="373" t="n">
         <v>21</v>
       </c>
       <c r="D24" s="112" t="inlineStr">
@@ -2628,57 +2652,57 @@
           <t>big coc</t>
         </is>
       </c>
-      <c r="E24" s="368" t="n">
+      <c r="E24" s="385" t="n">
         <v>6</v>
       </c>
       <c r="F24" s="112" t="n">
         <v>7550</v>
       </c>
-      <c r="G24" s="369" t="n">
+      <c r="G24" s="386" t="n">
         <v>0</v>
       </c>
       <c r="H24" s="115" t="n">
         <v>0</v>
       </c>
-      <c r="I24" s="368" t="n">
+      <c r="I24" s="385" t="n">
         <v>6</v>
       </c>
       <c r="J24" s="112" t="n">
         <v>7115</v>
       </c>
-      <c r="K24" s="368" t="n">
+      <c r="K24" s="385" t="n">
         <v>6</v>
       </c>
       <c r="L24" s="112" t="n">
         <v>7420</v>
       </c>
-      <c r="M24" s="368" t="n">
+      <c r="M24" s="385" t="n">
         <v>5</v>
       </c>
       <c r="N24" s="117" t="n">
         <v>5150</v>
       </c>
-      <c r="O24" s="368" t="n">
+      <c r="O24" s="385" t="n">
         <v>6</v>
       </c>
       <c r="P24" s="112" t="n">
         <v>9075</v>
       </c>
-      <c r="Q24" s="367" t="n"/>
+      <c r="Q24" s="384" t="n"/>
       <c r="R24" s="115" t="n"/>
-      <c r="S24" s="367" t="n"/>
+      <c r="S24" s="384" t="n"/>
       <c r="T24" s="115" t="n"/>
     </row>
     <row r="25">
-      <c r="A25" s="364" t="inlineStr">
+      <c r="A25" s="381" t="inlineStr">
         <is>
           <t>#QUVJGC0VQ</t>
         </is>
       </c>
-      <c r="B25" s="364" t="n">
+      <c r="B25" s="381" t="n">
         <v>1413</v>
       </c>
-      <c r="C25" s="360" t="n">
+      <c r="C25" s="377" t="n">
         <v>22</v>
       </c>
       <c r="D25" s="106" t="inlineStr">
@@ -2686,49 +2710,49 @@
           <t>Cam</t>
         </is>
       </c>
-      <c r="E25" s="365" t="n">
+      <c r="E25" s="382" t="n">
         <v>6</v>
       </c>
       <c r="F25" s="118" t="n">
         <v>5361</v>
       </c>
-      <c r="G25" s="366" t="n">
+      <c r="G25" s="383" t="n">
         <v>0</v>
       </c>
       <c r="H25" s="109" t="n">
         <v>0</v>
       </c>
-      <c r="I25" s="365" t="n">
+      <c r="I25" s="382" t="n">
         <v>6</v>
       </c>
       <c r="J25" s="106" t="n">
         <v>8080</v>
       </c>
-      <c r="K25" s="366" t="n">
+      <c r="K25" s="383" t="n">
         <v>0</v>
       </c>
       <c r="L25" s="110" t="n">
         <v>0</v>
       </c>
-      <c r="M25" s="364" t="n"/>
+      <c r="M25" s="381" t="n"/>
       <c r="N25" s="109" t="n"/>
-      <c r="O25" s="364" t="n"/>
+      <c r="O25" s="381" t="n"/>
       <c r="P25" s="109" t="n"/>
-      <c r="Q25" s="364" t="n"/>
+      <c r="Q25" s="381" t="n"/>
       <c r="R25" s="109" t="n"/>
-      <c r="S25" s="364" t="n"/>
+      <c r="S25" s="381" t="n"/>
       <c r="T25" s="109" t="n"/>
     </row>
     <row r="26">
-      <c r="A26" s="367" t="inlineStr">
+      <c r="A26" s="384" t="inlineStr">
         <is>
           <t>#QJQV82JG0</t>
         </is>
       </c>
-      <c r="B26" s="367" t="n">
+      <c r="B26" s="384" t="n">
         <v>1036</v>
       </c>
-      <c r="C26" s="356" t="n">
+      <c r="C26" s="373" t="n">
         <v>23</v>
       </c>
       <c r="D26" s="112" t="inlineStr">
@@ -2736,45 +2760,45 @@
           <t>The UnknownYT</t>
         </is>
       </c>
-      <c r="E26" s="368" t="n">
+      <c r="E26" s="385" t="n">
         <v>6</v>
       </c>
       <c r="F26" s="117" t="n">
         <v>5005</v>
       </c>
-      <c r="G26" s="369" t="n">
+      <c r="G26" s="386" t="n">
         <v>0</v>
       </c>
       <c r="H26" s="115" t="n">
         <v>0</v>
       </c>
-      <c r="I26" s="369" t="n">
+      <c r="I26" s="386" t="n">
         <v>0</v>
       </c>
       <c r="J26" s="116" t="n">
         <v>0</v>
       </c>
-      <c r="K26" s="367" t="n"/>
+      <c r="K26" s="384" t="n"/>
       <c r="L26" s="115" t="n"/>
-      <c r="M26" s="367" t="n"/>
+      <c r="M26" s="384" t="n"/>
       <c r="N26" s="115" t="n"/>
-      <c r="O26" s="367" t="n"/>
+      <c r="O26" s="384" t="n"/>
       <c r="P26" s="115" t="n"/>
-      <c r="Q26" s="367" t="n"/>
+      <c r="Q26" s="384" t="n"/>
       <c r="R26" s="115" t="n"/>
-      <c r="S26" s="367" t="n"/>
+      <c r="S26" s="384" t="n"/>
       <c r="T26" s="115" t="n"/>
     </row>
     <row r="27">
-      <c r="A27" s="364" t="inlineStr">
+      <c r="A27" s="381" t="inlineStr">
         <is>
           <t>#LC9GUPJJG</t>
         </is>
       </c>
-      <c r="B27" s="364" t="n">
+      <c r="B27" s="381" t="n">
         <v>1054</v>
       </c>
-      <c r="C27" s="360" t="n">
+      <c r="C27" s="377" t="n">
         <v>24</v>
       </c>
       <c r="D27" s="106" t="inlineStr">
@@ -2782,53 +2806,53 @@
           <t>raptor2222a</t>
         </is>
       </c>
-      <c r="E27" s="365" t="n">
+      <c r="E27" s="382" t="n">
         <v>5</v>
       </c>
       <c r="F27" s="118" t="n">
         <v>4940</v>
       </c>
-      <c r="G27" s="366" t="n">
+      <c r="G27" s="383" t="n">
         <v>0</v>
       </c>
       <c r="H27" s="109" t="n">
         <v>0</v>
       </c>
-      <c r="I27" s="365" t="n">
+      <c r="I27" s="382" t="n">
         <v>6</v>
       </c>
       <c r="J27" s="106" t="n">
         <v>6971</v>
       </c>
-      <c r="K27" s="365" t="n">
+      <c r="K27" s="382" t="n">
         <v>5</v>
       </c>
       <c r="L27" s="118" t="n">
         <v>4350</v>
       </c>
-      <c r="M27" s="366" t="n">
+      <c r="M27" s="383" t="n">
         <v>0</v>
       </c>
       <c r="N27" s="110" t="n">
         <v>0</v>
       </c>
-      <c r="O27" s="364" t="n"/>
+      <c r="O27" s="381" t="n"/>
       <c r="P27" s="109" t="n"/>
-      <c r="Q27" s="364" t="n"/>
+      <c r="Q27" s="381" t="n"/>
       <c r="R27" s="109" t="n"/>
-      <c r="S27" s="364" t="n"/>
+      <c r="S27" s="381" t="n"/>
       <c r="T27" s="109" t="n"/>
     </row>
     <row r="28">
-      <c r="A28" s="367" t="inlineStr">
+      <c r="A28" s="384" t="inlineStr">
         <is>
           <t>#82QLQCJRJ</t>
         </is>
       </c>
-      <c r="B28" s="367" t="n">
+      <c r="B28" s="384" t="n">
         <v>3004</v>
       </c>
-      <c r="C28" s="356" t="n">
+      <c r="C28" s="373" t="n">
         <v>25</v>
       </c>
       <c r="D28" s="117" t="inlineStr">
@@ -2836,49 +2860,49 @@
           <t>Raging Fury</t>
         </is>
       </c>
-      <c r="E28" s="371" t="n">
+      <c r="E28" s="388" t="n">
         <v>4</v>
       </c>
       <c r="F28" s="117" t="n">
         <v>4850</v>
       </c>
-      <c r="G28" s="369" t="n">
+      <c r="G28" s="386" t="n">
         <v>0</v>
       </c>
       <c r="H28" s="115" t="n">
         <v>0</v>
       </c>
-      <c r="I28" s="368" t="n">
+      <c r="I28" s="385" t="n">
         <v>6</v>
       </c>
       <c r="J28" s="112" t="n">
         <v>6145</v>
       </c>
-      <c r="K28" s="368" t="n">
+      <c r="K28" s="385" t="n">
         <v>6</v>
       </c>
       <c r="L28" s="112" t="n">
         <v>8055</v>
       </c>
-      <c r="M28" s="368" t="n">
+      <c r="M28" s="385" t="n">
         <v>6</v>
       </c>
       <c r="N28" s="112" t="n">
         <v>7115</v>
       </c>
-      <c r="O28" s="369" t="n">
+      <c r="O28" s="386" t="n">
         <v>2</v>
       </c>
       <c r="P28" s="116" t="n">
         <v>2320</v>
       </c>
-      <c r="Q28" s="368" t="n">
+      <c r="Q28" s="385" t="n">
         <v>6</v>
       </c>
       <c r="R28" s="117" t="n">
         <v>4920</v>
       </c>
-      <c r="S28" s="368" t="n">
+      <c r="S28" s="385" t="n">
         <v>6</v>
       </c>
       <c r="T28" s="117" t="n">
@@ -2928,15 +2952,15 @@
       <c r="T29" s="124" t="n"/>
     </row>
     <row r="30">
-      <c r="A30" s="367" t="inlineStr">
+      <c r="A30" s="384" t="inlineStr">
         <is>
           <t>#G288QGVQ2</t>
         </is>
       </c>
-      <c r="B30" s="367" t="n">
+      <c r="B30" s="384" t="n">
         <v>909</v>
       </c>
-      <c r="C30" s="356" t="n">
+      <c r="C30" s="373" t="n">
         <v>27</v>
       </c>
       <c r="D30" s="116" t="inlineStr">
@@ -2944,41 +2968,41 @@
           <t>Sehaj123</t>
         </is>
       </c>
-      <c r="E30" s="369" t="n">
+      <c r="E30" s="386" t="n">
         <v>0</v>
       </c>
       <c r="F30" s="116" t="n">
         <v>0</v>
       </c>
-      <c r="G30" s="371" t="n">
+      <c r="G30" s="388" t="n">
         <v>21</v>
       </c>
       <c r="H30" s="115" t="n">
         <v>0</v>
       </c>
-      <c r="I30" s="367" t="n"/>
+      <c r="I30" s="384" t="n"/>
       <c r="J30" s="115" t="n"/>
-      <c r="K30" s="367" t="n"/>
+      <c r="K30" s="384" t="n"/>
       <c r="L30" s="115" t="n"/>
-      <c r="M30" s="367" t="n"/>
+      <c r="M30" s="384" t="n"/>
       <c r="N30" s="115" t="n"/>
-      <c r="O30" s="367" t="n"/>
+      <c r="O30" s="384" t="n"/>
       <c r="P30" s="115" t="n"/>
-      <c r="Q30" s="367" t="n"/>
+      <c r="Q30" s="384" t="n"/>
       <c r="R30" s="115" t="n"/>
-      <c r="S30" s="367" t="n"/>
+      <c r="S30" s="384" t="n"/>
       <c r="T30" s="115" t="n"/>
     </row>
     <row r="31">
-      <c r="A31" s="364" t="inlineStr">
+      <c r="A31" s="381" t="inlineStr">
         <is>
           <t>#QRUQQUPLV</t>
         </is>
       </c>
-      <c r="B31" s="364" t="n">
+      <c r="B31" s="381" t="n">
         <v>906</v>
       </c>
-      <c r="C31" s="360" t="n">
+      <c r="C31" s="377" t="n">
         <v>28</v>
       </c>
       <c r="D31" s="110" t="inlineStr">
@@ -2986,41 +3010,41 @@
           <t>datka/56</t>
         </is>
       </c>
-      <c r="E31" s="366" t="n">
+      <c r="E31" s="383" t="n">
         <v>0</v>
       </c>
       <c r="F31" s="110" t="n">
         <v>0</v>
       </c>
-      <c r="G31" s="366" t="n">
+      <c r="G31" s="383" t="n">
         <v>0</v>
       </c>
       <c r="H31" s="109" t="n">
         <v>0</v>
       </c>
-      <c r="I31" s="364" t="n"/>
+      <c r="I31" s="381" t="n"/>
       <c r="J31" s="109" t="n"/>
-      <c r="K31" s="364" t="n"/>
+      <c r="K31" s="381" t="n"/>
       <c r="L31" s="109" t="n"/>
-      <c r="M31" s="364" t="n"/>
+      <c r="M31" s="381" t="n"/>
       <c r="N31" s="109" t="n"/>
-      <c r="O31" s="364" t="n"/>
+      <c r="O31" s="381" t="n"/>
       <c r="P31" s="109" t="n"/>
-      <c r="Q31" s="364" t="n"/>
+      <c r="Q31" s="381" t="n"/>
       <c r="R31" s="109" t="n"/>
-      <c r="S31" s="364" t="n"/>
+      <c r="S31" s="381" t="n"/>
       <c r="T31" s="109" t="n"/>
     </row>
     <row r="32">
-      <c r="A32" s="367" t="inlineStr">
+      <c r="A32" s="384" t="inlineStr">
         <is>
           <t>#LGCVY0L9P</t>
         </is>
       </c>
-      <c r="B32" s="367" t="n">
+      <c r="B32" s="384" t="n">
         <v>873</v>
       </c>
-      <c r="C32" s="356" t="n">
+      <c r="C32" s="373" t="n">
         <v>29</v>
       </c>
       <c r="D32" s="116" t="inlineStr">
@@ -3028,45 +3052,45 @@
           <t>Death1wolf</t>
         </is>
       </c>
-      <c r="E32" s="369" t="n">
+      <c r="E32" s="386" t="n">
         <v>0</v>
       </c>
       <c r="F32" s="116" t="n">
         <v>0</v>
       </c>
-      <c r="G32" s="369" t="n">
+      <c r="G32" s="386" t="n">
         <v>0</v>
       </c>
       <c r="H32" s="115" t="n">
         <v>0</v>
       </c>
-      <c r="I32" s="368" t="n">
+      <c r="I32" s="385" t="n">
         <v>6</v>
       </c>
       <c r="J32" s="112" t="n">
         <v>7998</v>
       </c>
-      <c r="K32" s="367" t="n"/>
+      <c r="K32" s="384" t="n"/>
       <c r="L32" s="115" t="n"/>
-      <c r="M32" s="367" t="n"/>
+      <c r="M32" s="384" t="n"/>
       <c r="N32" s="115" t="n"/>
-      <c r="O32" s="367" t="n"/>
+      <c r="O32" s="384" t="n"/>
       <c r="P32" s="115" t="n"/>
-      <c r="Q32" s="367" t="n"/>
+      <c r="Q32" s="384" t="n"/>
       <c r="R32" s="115" t="n"/>
-      <c r="S32" s="367" t="n"/>
+      <c r="S32" s="384" t="n"/>
       <c r="T32" s="115" t="n"/>
     </row>
     <row r="33">
-      <c r="A33" s="364" t="inlineStr">
+      <c r="A33" s="381" t="inlineStr">
         <is>
           <t>#Q9QUUVQ02</t>
         </is>
       </c>
-      <c r="B33" s="364" t="n">
+      <c r="B33" s="381" t="n">
         <v>1438</v>
       </c>
-      <c r="C33" s="360" t="n">
+      <c r="C33" s="377" t="n">
         <v>30</v>
       </c>
       <c r="D33" s="110" t="inlineStr">
@@ -3074,45 +3098,45 @@
           <t>zach</t>
         </is>
       </c>
-      <c r="E33" s="366" t="n">
+      <c r="E33" s="383" t="n">
         <v>0</v>
       </c>
       <c r="F33" s="110" t="n">
         <v>0</v>
       </c>
-      <c r="G33" s="366" t="n">
+      <c r="G33" s="383" t="n">
         <v>0</v>
       </c>
       <c r="H33" s="109" t="n">
         <v>0</v>
       </c>
-      <c r="I33" s="365" t="n">
+      <c r="I33" s="382" t="n">
         <v>6</v>
       </c>
       <c r="J33" s="106" t="n">
         <v>6106</v>
       </c>
-      <c r="K33" s="364" t="n"/>
+      <c r="K33" s="381" t="n"/>
       <c r="L33" s="109" t="n"/>
-      <c r="M33" s="364" t="n"/>
+      <c r="M33" s="381" t="n"/>
       <c r="N33" s="109" t="n"/>
-      <c r="O33" s="364" t="n"/>
+      <c r="O33" s="381" t="n"/>
       <c r="P33" s="109" t="n"/>
-      <c r="Q33" s="364" t="n"/>
+      <c r="Q33" s="381" t="n"/>
       <c r="R33" s="109" t="n"/>
-      <c r="S33" s="364" t="n"/>
+      <c r="S33" s="381" t="n"/>
       <c r="T33" s="109" t="n"/>
     </row>
     <row r="34">
-      <c r="A34" s="367" t="inlineStr">
+      <c r="A34" s="384" t="inlineStr">
         <is>
           <t>#VGG9LYL0</t>
         </is>
       </c>
-      <c r="B34" s="367" t="n">
+      <c r="B34" s="384" t="n">
         <v>1035</v>
       </c>
-      <c r="C34" s="356" t="n">
+      <c r="C34" s="373" t="n">
         <v>31</v>
       </c>
       <c r="D34" s="116" t="inlineStr">
@@ -3120,49 +3144,49 @@
           <t>ptripp1048</t>
         </is>
       </c>
-      <c r="E34" s="369" t="n">
+      <c r="E34" s="386" t="n">
         <v>0</v>
       </c>
       <c r="F34" s="116" t="n">
         <v>0</v>
       </c>
-      <c r="G34" s="369" t="n">
+      <c r="G34" s="386" t="n">
         <v>0</v>
       </c>
       <c r="H34" s="115" t="n">
         <v>0</v>
       </c>
-      <c r="I34" s="368" t="n">
+      <c r="I34" s="385" t="n">
         <v>6</v>
       </c>
       <c r="J34" s="112" t="n">
         <v>6023</v>
       </c>
-      <c r="K34" s="369" t="n">
+      <c r="K34" s="386" t="n">
         <v>0</v>
       </c>
       <c r="L34" s="116" t="n">
         <v>0</v>
       </c>
-      <c r="M34" s="367" t="n"/>
+      <c r="M34" s="384" t="n"/>
       <c r="N34" s="115" t="n"/>
-      <c r="O34" s="367" t="n"/>
+      <c r="O34" s="384" t="n"/>
       <c r="P34" s="115" t="n"/>
-      <c r="Q34" s="367" t="n"/>
+      <c r="Q34" s="384" t="n"/>
       <c r="R34" s="115" t="n"/>
-      <c r="S34" s="367" t="n"/>
+      <c r="S34" s="384" t="n"/>
       <c r="T34" s="115" t="n"/>
     </row>
     <row r="35">
-      <c r="A35" s="364" t="inlineStr">
+      <c r="A35" s="381" t="inlineStr">
         <is>
           <t>#QLG0VJG2J</t>
         </is>
       </c>
-      <c r="B35" s="364" t="n">
+      <c r="B35" s="381" t="n">
         <v>1463</v>
       </c>
-      <c r="C35" s="360" t="n">
+      <c r="C35" s="377" t="n">
         <v>32</v>
       </c>
       <c r="D35" s="110" t="inlineStr">
@@ -3170,53 +3194,53 @@
           <t>PocketRocket</t>
         </is>
       </c>
-      <c r="E35" s="366" t="n">
+      <c r="E35" s="383" t="n">
         <v>0</v>
       </c>
       <c r="F35" s="110" t="n">
         <v>0</v>
       </c>
-      <c r="G35" s="366" t="n">
+      <c r="G35" s="383" t="n">
         <v>0</v>
       </c>
       <c r="H35" s="109" t="n">
         <v>0</v>
       </c>
-      <c r="I35" s="365" t="n">
+      <c r="I35" s="382" t="n">
         <v>6</v>
       </c>
       <c r="J35" s="118" t="n">
         <v>5660</v>
       </c>
-      <c r="K35" s="370" t="n">
+      <c r="K35" s="387" t="n">
         <v>4</v>
       </c>
       <c r="L35" s="118" t="n">
         <v>4327</v>
       </c>
-      <c r="M35" s="370" t="n">
+      <c r="M35" s="387" t="n">
         <v>4</v>
       </c>
       <c r="N35" s="118" t="n">
         <v>5215</v>
       </c>
-      <c r="O35" s="364" t="n"/>
+      <c r="O35" s="381" t="n"/>
       <c r="P35" s="109" t="n"/>
-      <c r="Q35" s="364" t="n"/>
+      <c r="Q35" s="381" t="n"/>
       <c r="R35" s="109" t="n"/>
-      <c r="S35" s="364" t="n"/>
+      <c r="S35" s="381" t="n"/>
       <c r="T35" s="109" t="n"/>
     </row>
     <row r="36">
-      <c r="A36" s="367" t="inlineStr">
+      <c r="A36" s="384" t="inlineStr">
         <is>
           <t>#QLUV29GGJ</t>
         </is>
       </c>
-      <c r="B36" s="367" t="n">
+      <c r="B36" s="384" t="n">
         <v>1040</v>
       </c>
-      <c r="C36" s="356" t="n">
+      <c r="C36" s="373" t="n">
         <v>33</v>
       </c>
       <c r="D36" s="116" t="inlineStr">
@@ -3224,45 +3248,45 @@
           <t>Kukoshibo</t>
         </is>
       </c>
-      <c r="E36" s="369" t="n">
+      <c r="E36" s="386" t="n">
         <v>0</v>
       </c>
       <c r="F36" s="116" t="n">
         <v>0</v>
       </c>
-      <c r="G36" s="369" t="n">
+      <c r="G36" s="386" t="n">
         <v>0</v>
       </c>
       <c r="H36" s="115" t="n">
         <v>0</v>
       </c>
-      <c r="I36" s="369" t="n">
+      <c r="I36" s="386" t="n">
         <v>0</v>
       </c>
       <c r="J36" s="116" t="n">
         <v>0</v>
       </c>
-      <c r="K36" s="367" t="n"/>
+      <c r="K36" s="384" t="n"/>
       <c r="L36" s="115" t="n"/>
-      <c r="M36" s="367" t="n"/>
+      <c r="M36" s="384" t="n"/>
       <c r="N36" s="115" t="n"/>
-      <c r="O36" s="367" t="n"/>
+      <c r="O36" s="384" t="n"/>
       <c r="P36" s="115" t="n"/>
-      <c r="Q36" s="367" t="n"/>
+      <c r="Q36" s="384" t="n"/>
       <c r="R36" s="115" t="n"/>
-      <c r="S36" s="367" t="n"/>
+      <c r="S36" s="384" t="n"/>
       <c r="T36" s="115" t="n"/>
     </row>
     <row r="37">
-      <c r="A37" s="364" t="inlineStr">
+      <c r="A37" s="381" t="inlineStr">
         <is>
           <t>#Q0U0CRCGJ</t>
         </is>
       </c>
-      <c r="B37" s="364" t="n">
+      <c r="B37" s="381" t="n">
         <v>691</v>
       </c>
-      <c r="C37" s="360" t="n">
+      <c r="C37" s="377" t="n">
         <v>34</v>
       </c>
       <c r="D37" s="110" t="inlineStr">
@@ -3270,45 +3294,45 @@
           <t>Sn0wc0ne</t>
         </is>
       </c>
-      <c r="E37" s="366" t="n">
+      <c r="E37" s="383" t="n">
         <v>0</v>
       </c>
       <c r="F37" s="110" t="n">
         <v>0</v>
       </c>
-      <c r="G37" s="366" t="n">
+      <c r="G37" s="383" t="n">
         <v>0</v>
       </c>
       <c r="H37" s="109" t="n">
         <v>0</v>
       </c>
-      <c r="I37" s="366" t="n">
+      <c r="I37" s="383" t="n">
         <v>0</v>
       </c>
       <c r="J37" s="110" t="n">
         <v>0</v>
       </c>
-      <c r="K37" s="364" t="n"/>
+      <c r="K37" s="381" t="n"/>
       <c r="L37" s="109" t="n"/>
-      <c r="M37" s="364" t="n"/>
+      <c r="M37" s="381" t="n"/>
       <c r="N37" s="109" t="n"/>
-      <c r="O37" s="364" t="n"/>
+      <c r="O37" s="381" t="n"/>
       <c r="P37" s="109" t="n"/>
-      <c r="Q37" s="364" t="n"/>
+      <c r="Q37" s="381" t="n"/>
       <c r="R37" s="109" t="n"/>
-      <c r="S37" s="364" t="n"/>
+      <c r="S37" s="381" t="n"/>
       <c r="T37" s="109" t="n"/>
     </row>
     <row r="38">
-      <c r="A38" s="367" t="inlineStr">
+      <c r="A38" s="384" t="inlineStr">
         <is>
           <t>#QY0VGPQGQ</t>
         </is>
       </c>
-      <c r="B38" s="367" t="n">
+      <c r="B38" s="384" t="n">
         <v>613</v>
       </c>
-      <c r="C38" s="356" t="n">
+      <c r="C38" s="373" t="n">
         <v>35</v>
       </c>
       <c r="D38" s="116" t="inlineStr">
@@ -3316,49 +3340,49 @@
           <t>killerjones</t>
         </is>
       </c>
-      <c r="E38" s="369" t="n">
+      <c r="E38" s="386" t="n">
         <v>0</v>
       </c>
       <c r="F38" s="116" t="n">
         <v>0</v>
       </c>
-      <c r="G38" s="369" t="n">
+      <c r="G38" s="386" t="n">
         <v>0</v>
       </c>
       <c r="H38" s="115" t="n">
         <v>0</v>
       </c>
-      <c r="I38" s="369" t="n">
+      <c r="I38" s="386" t="n">
         <v>0</v>
       </c>
       <c r="J38" s="116" t="n">
         <v>0</v>
       </c>
-      <c r="K38" s="368" t="n">
+      <c r="K38" s="385" t="n">
         <v>6</v>
       </c>
       <c r="L38" s="112" t="n">
         <v>6320</v>
       </c>
-      <c r="M38" s="367" t="n"/>
+      <c r="M38" s="384" t="n"/>
       <c r="N38" s="115" t="n"/>
-      <c r="O38" s="367" t="n"/>
+      <c r="O38" s="384" t="n"/>
       <c r="P38" s="115" t="n"/>
-      <c r="Q38" s="367" t="n"/>
+      <c r="Q38" s="384" t="n"/>
       <c r="R38" s="115" t="n"/>
-      <c r="S38" s="367" t="n"/>
+      <c r="S38" s="384" t="n"/>
       <c r="T38" s="115" t="n"/>
     </row>
     <row r="39">
-      <c r="A39" s="364" t="inlineStr">
+      <c r="A39" s="381" t="inlineStr">
         <is>
           <t>#QL8LVLYG8</t>
         </is>
       </c>
-      <c r="B39" s="364" t="n">
+      <c r="B39" s="381" t="n">
         <v>971</v>
       </c>
-      <c r="C39" s="360" t="n">
+      <c r="C39" s="377" t="n">
         <v>36</v>
       </c>
       <c r="D39" s="110" t="inlineStr">
@@ -3366,49 +3390,49 @@
           <t>Some guy</t>
         </is>
       </c>
-      <c r="E39" s="366" t="n">
+      <c r="E39" s="383" t="n">
         <v>0</v>
       </c>
       <c r="F39" s="110" t="n">
         <v>0</v>
       </c>
-      <c r="G39" s="366" t="n">
+      <c r="G39" s="383" t="n">
         <v>0</v>
       </c>
       <c r="H39" s="109" t="n">
         <v>0</v>
       </c>
-      <c r="I39" s="366" t="n">
+      <c r="I39" s="383" t="n">
         <v>0</v>
       </c>
       <c r="J39" s="110" t="n">
         <v>0</v>
       </c>
-      <c r="K39" s="366" t="n">
+      <c r="K39" s="383" t="n">
         <v>2</v>
       </c>
       <c r="L39" s="110" t="n">
         <v>2650</v>
       </c>
-      <c r="M39" s="366" t="n">
+      <c r="M39" s="383" t="n">
         <v>0</v>
       </c>
       <c r="N39" s="110" t="n">
         <v>0</v>
       </c>
-      <c r="O39" s="365" t="n">
+      <c r="O39" s="382" t="n">
         <v>6</v>
       </c>
       <c r="P39" s="106" t="n">
         <v>6917</v>
       </c>
-      <c r="Q39" s="366" t="n">
+      <c r="Q39" s="383" t="n">
         <v>0</v>
       </c>
       <c r="R39" s="110" t="n">
         <v>0</v>
       </c>
-      <c r="S39" s="366" t="n">
+      <c r="S39" s="383" t="n">
         <v>2</v>
       </c>
       <c r="T39" s="110" t="n">
@@ -3416,165 +3440,165 @@
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="367" t="inlineStr">
+      <c r="A40" s="384" t="inlineStr">
+        <is>
+          <t>#QLGYRVPU0</t>
+        </is>
+      </c>
+      <c r="B40" s="384" t="n">
+        <v>1198</v>
+      </c>
+      <c r="C40" s="373" t="n">
+        <v>37</v>
+      </c>
+      <c r="D40" s="116" t="inlineStr">
+        <is>
+          <t>Black.Boy.</t>
+        </is>
+      </c>
+      <c r="E40" s="386" t="n">
+        <v>0</v>
+      </c>
+      <c r="F40" s="116" t="n">
+        <v>0</v>
+      </c>
+      <c r="G40" s="386" t="n">
+        <v>0</v>
+      </c>
+      <c r="H40" s="115" t="n">
+        <v>15</v>
+      </c>
+      <c r="I40" s="386" t="n">
+        <v>0</v>
+      </c>
+      <c r="J40" s="116" t="n">
+        <v>0</v>
+      </c>
+      <c r="K40" s="386" t="n">
+        <v>0</v>
+      </c>
+      <c r="L40" s="116" t="n">
+        <v>0</v>
+      </c>
+      <c r="M40" s="384" t="n"/>
+      <c r="N40" s="115" t="n"/>
+      <c r="O40" s="384" t="n"/>
+      <c r="P40" s="115" t="n"/>
+      <c r="Q40" s="384" t="n"/>
+      <c r="R40" s="115" t="n"/>
+      <c r="S40" s="384" t="n"/>
+      <c r="T40" s="115" t="n"/>
+    </row>
+    <row r="41">
+      <c r="A41" s="381" t="inlineStr">
+        <is>
+          <t>#QV8RY9UC8</t>
+        </is>
+      </c>
+      <c r="B41" s="381" t="n">
+        <v>747</v>
+      </c>
+      <c r="C41" s="377" t="n">
+        <v>38</v>
+      </c>
+      <c r="D41" s="110" t="inlineStr">
+        <is>
+          <t>Apollo</t>
+        </is>
+      </c>
+      <c r="E41" s="383" t="n">
+        <v>0</v>
+      </c>
+      <c r="F41" s="110" t="n">
+        <v>0</v>
+      </c>
+      <c r="G41" s="383" t="n">
+        <v>0</v>
+      </c>
+      <c r="H41" s="109" t="n">
+        <v>0</v>
+      </c>
+      <c r="I41" s="383" t="n">
+        <v>0</v>
+      </c>
+      <c r="J41" s="110" t="n">
+        <v>0</v>
+      </c>
+      <c r="K41" s="383" t="n">
+        <v>0</v>
+      </c>
+      <c r="L41" s="110" t="n">
+        <v>0</v>
+      </c>
+      <c r="M41" s="381" t="n"/>
+      <c r="N41" s="109" t="n"/>
+      <c r="O41" s="381" t="n"/>
+      <c r="P41" s="109" t="n"/>
+      <c r="Q41" s="381" t="n"/>
+      <c r="R41" s="109" t="n"/>
+      <c r="S41" s="381" t="n"/>
+      <c r="T41" s="109" t="n"/>
+    </row>
+    <row r="42">
+      <c r="A42" s="384" t="inlineStr">
         <is>
           <t>#QQL28Y2UL</t>
         </is>
       </c>
-      <c r="B40" s="367" t="n">
+      <c r="B42" s="384" t="n">
         <v>1085</v>
       </c>
-      <c r="C40" s="356" t="n">
-        <v>37</v>
-      </c>
-      <c r="D40" s="116" t="inlineStr">
+      <c r="C42" s="373" t="n">
+        <v>39</v>
+      </c>
+      <c r="D42" s="116" t="inlineStr">
         <is>
           <t>SUPoT</t>
         </is>
       </c>
-      <c r="E40" s="369" t="n">
-        <v>0</v>
-      </c>
-      <c r="F40" s="116" t="n">
-        <v>0</v>
-      </c>
-      <c r="G40" s="369" t="n">
-        <v>0</v>
-      </c>
-      <c r="H40" s="115" t="n">
+      <c r="E42" s="386" t="n">
+        <v>0</v>
+      </c>
+      <c r="F42" s="116" t="n">
+        <v>0</v>
+      </c>
+      <c r="G42" s="386" t="n">
+        <v>0</v>
+      </c>
+      <c r="H42" s="115" t="n">
         <v>31</v>
       </c>
-      <c r="I40" s="369" t="n">
-        <v>0</v>
-      </c>
-      <c r="J40" s="116" t="n">
-        <v>0</v>
-      </c>
-      <c r="K40" s="369" t="n">
-        <v>0</v>
-      </c>
-      <c r="L40" s="116" t="n">
-        <v>0</v>
-      </c>
-      <c r="M40" s="367" t="n"/>
-      <c r="N40" s="115" t="n"/>
-      <c r="O40" s="367" t="n"/>
-      <c r="P40" s="115" t="n"/>
-      <c r="Q40" s="367" t="n"/>
-      <c r="R40" s="115" t="n"/>
-      <c r="S40" s="367" t="n"/>
-      <c r="T40" s="115" t="n"/>
-    </row>
-    <row r="41">
-      <c r="A41" s="364" t="inlineStr">
-        <is>
-          <t>#QV8RY9UC8</t>
-        </is>
-      </c>
-      <c r="B41" s="364" t="n">
-        <v>747</v>
-      </c>
-      <c r="C41" s="360" t="n">
-        <v>38</v>
-      </c>
-      <c r="D41" s="110" t="inlineStr">
-        <is>
-          <t>Apollo</t>
-        </is>
-      </c>
-      <c r="E41" s="366" t="n">
-        <v>0</v>
-      </c>
-      <c r="F41" s="110" t="n">
-        <v>0</v>
-      </c>
-      <c r="G41" s="366" t="n">
-        <v>0</v>
-      </c>
-      <c r="H41" s="109" t="n">
-        <v>0</v>
-      </c>
-      <c r="I41" s="366" t="n">
-        <v>0</v>
-      </c>
-      <c r="J41" s="110" t="n">
-        <v>0</v>
-      </c>
-      <c r="K41" s="366" t="n">
-        <v>0</v>
-      </c>
-      <c r="L41" s="110" t="n">
-        <v>0</v>
-      </c>
-      <c r="M41" s="364" t="n"/>
-      <c r="N41" s="109" t="n"/>
-      <c r="O41" s="364" t="n"/>
-      <c r="P41" s="109" t="n"/>
-      <c r="Q41" s="364" t="n"/>
-      <c r="R41" s="109" t="n"/>
-      <c r="S41" s="364" t="n"/>
-      <c r="T41" s="109" t="n"/>
-    </row>
-    <row r="42">
-      <c r="A42" s="367" t="inlineStr">
-        <is>
-          <t>#QLGYRVPU0</t>
-        </is>
-      </c>
-      <c r="B42" s="367" t="n">
-        <v>1198</v>
-      </c>
-      <c r="C42" s="356" t="n">
-        <v>39</v>
-      </c>
-      <c r="D42" s="116" t="inlineStr">
-        <is>
-          <t>Black.Boy.</t>
-        </is>
-      </c>
-      <c r="E42" s="369" t="n">
-        <v>0</v>
-      </c>
-      <c r="F42" s="116" t="n">
-        <v>0</v>
-      </c>
-      <c r="G42" s="369" t="n">
-        <v>0</v>
-      </c>
-      <c r="H42" s="115" t="n">
-        <v>15</v>
-      </c>
-      <c r="I42" s="369" t="n">
+      <c r="I42" s="386" t="n">
         <v>0</v>
       </c>
       <c r="J42" s="116" t="n">
         <v>0</v>
       </c>
-      <c r="K42" s="369" t="n">
+      <c r="K42" s="386" t="n">
         <v>0</v>
       </c>
       <c r="L42" s="116" t="n">
         <v>0</v>
       </c>
-      <c r="M42" s="367" t="n"/>
+      <c r="M42" s="384" t="n"/>
       <c r="N42" s="115" t="n"/>
-      <c r="O42" s="367" t="n"/>
+      <c r="O42" s="384" t="n"/>
       <c r="P42" s="115" t="n"/>
-      <c r="Q42" s="367" t="n"/>
+      <c r="Q42" s="384" t="n"/>
       <c r="R42" s="115" t="n"/>
-      <c r="S42" s="367" t="n"/>
+      <c r="S42" s="384" t="n"/>
       <c r="T42" s="115" t="n"/>
     </row>
     <row r="43">
-      <c r="A43" s="364" t="inlineStr">
+      <c r="A43" s="381" t="inlineStr">
         <is>
           <t>#QJC8LQU9U</t>
         </is>
       </c>
-      <c r="B43" s="364" t="n">
+      <c r="B43" s="381" t="n">
         <v>998</v>
       </c>
-      <c r="C43" s="360" t="n">
+      <c r="C43" s="377" t="n">
         <v>40</v>
       </c>
       <c r="D43" s="110" t="inlineStr">
@@ -3582,49 +3606,49 @@
           <t>Master01</t>
         </is>
       </c>
-      <c r="E43" s="366" t="n">
+      <c r="E43" s="383" t="n">
         <v>0</v>
       </c>
       <c r="F43" s="110" t="n">
         <v>0</v>
       </c>
-      <c r="G43" s="366" t="n">
+      <c r="G43" s="383" t="n">
         <v>0</v>
       </c>
       <c r="H43" s="109" t="n">
         <v>0</v>
       </c>
-      <c r="I43" s="366" t="n">
+      <c r="I43" s="383" t="n">
         <v>0</v>
       </c>
       <c r="J43" s="110" t="n">
         <v>0</v>
       </c>
-      <c r="K43" s="366" t="n">
+      <c r="K43" s="383" t="n">
         <v>0</v>
       </c>
       <c r="L43" s="110" t="n">
         <v>0</v>
       </c>
-      <c r="M43" s="366" t="n">
+      <c r="M43" s="383" t="n">
         <v>0</v>
       </c>
       <c r="N43" s="110" t="n">
         <v>0</v>
       </c>
-      <c r="O43" s="365" t="n">
+      <c r="O43" s="382" t="n">
         <v>6</v>
       </c>
       <c r="P43" s="118" t="n">
         <v>5415</v>
       </c>
-      <c r="Q43" s="365" t="n">
+      <c r="Q43" s="382" t="n">
         <v>6</v>
       </c>
       <c r="R43" s="118" t="n">
         <v>4835</v>
       </c>
-      <c r="S43" s="365" t="n">
+      <c r="S43" s="382" t="n">
         <v>5</v>
       </c>
       <c r="T43" s="118" t="n">
@@ -3632,15 +3656,15 @@
       </c>
     </row>
     <row r="44">
-      <c r="A44" s="367" t="inlineStr">
+      <c r="A44" s="384" t="inlineStr">
         <is>
           <t>#QV8JJ0URU</t>
         </is>
       </c>
-      <c r="B44" s="367" t="n">
+      <c r="B44" s="384" t="n">
         <v>741</v>
       </c>
-      <c r="C44" s="356" t="n">
+      <c r="C44" s="373" t="n">
         <v>41</v>
       </c>
       <c r="D44" s="116" t="inlineStr">
@@ -3648,49 +3672,49 @@
           <t>✨Jacob</t>
         </is>
       </c>
-      <c r="E44" s="369" t="n">
+      <c r="E44" s="386" t="n">
         <v>0</v>
       </c>
       <c r="F44" s="116" t="n">
         <v>0</v>
       </c>
-      <c r="G44" s="369" t="n">
+      <c r="G44" s="386" t="n">
         <v>0</v>
       </c>
       <c r="H44" s="115" t="n">
         <v>0</v>
       </c>
-      <c r="I44" s="369" t="n">
+      <c r="I44" s="386" t="n">
         <v>0</v>
       </c>
       <c r="J44" s="116" t="n">
         <v>0</v>
       </c>
-      <c r="K44" s="369" t="n">
+      <c r="K44" s="386" t="n">
         <v>0</v>
       </c>
       <c r="L44" s="116" t="n">
         <v>0</v>
       </c>
-      <c r="M44" s="369" t="n">
+      <c r="M44" s="386" t="n">
         <v>0</v>
       </c>
       <c r="N44" s="116" t="n">
         <v>0</v>
       </c>
-      <c r="O44" s="369" t="n">
+      <c r="O44" s="386" t="n">
         <v>0</v>
       </c>
       <c r="P44" s="116" t="n">
         <v>0</v>
       </c>
-      <c r="Q44" s="368" t="n">
+      <c r="Q44" s="385" t="n">
         <v>6</v>
       </c>
       <c r="R44" s="112" t="n">
         <v>7385</v>
       </c>
-      <c r="S44" s="368" t="n">
+      <c r="S44" s="385" t="n">
         <v>6</v>
       </c>
       <c r="T44" s="112" t="n">
@@ -3698,15 +3722,15 @@
       </c>
     </row>
     <row r="45">
-      <c r="A45" s="364" t="inlineStr">
+      <c r="A45" s="381" t="inlineStr">
         <is>
           <t>#QY8L2GLUR</t>
         </is>
       </c>
-      <c r="B45" s="364" t="n">
+      <c r="B45" s="381" t="n">
         <v>907</v>
       </c>
-      <c r="C45" s="360" t="n">
+      <c r="C45" s="377" t="n">
         <v>42</v>
       </c>
       <c r="D45" s="110" t="inlineStr">
@@ -3714,49 +3738,49 @@
           <t>Huy</t>
         </is>
       </c>
-      <c r="E45" s="366" t="n">
+      <c r="E45" s="383" t="n">
         <v>0</v>
       </c>
       <c r="F45" s="110" t="n">
         <v>0</v>
       </c>
-      <c r="G45" s="366" t="n">
+      <c r="G45" s="383" t="n">
         <v>0</v>
       </c>
       <c r="H45" s="109" t="n">
         <v>0</v>
       </c>
-      <c r="I45" s="366" t="n">
+      <c r="I45" s="383" t="n">
         <v>0</v>
       </c>
       <c r="J45" s="110" t="n">
         <v>0</v>
       </c>
-      <c r="K45" s="366" t="n">
+      <c r="K45" s="383" t="n">
         <v>0</v>
       </c>
       <c r="L45" s="110" t="n">
         <v>0</v>
       </c>
-      <c r="M45" s="366" t="n">
+      <c r="M45" s="383" t="n">
         <v>0</v>
       </c>
       <c r="N45" s="110" t="n">
         <v>0</v>
       </c>
-      <c r="O45" s="366" t="n">
+      <c r="O45" s="383" t="n">
         <v>0</v>
       </c>
       <c r="P45" s="110" t="n">
         <v>0</v>
       </c>
-      <c r="Q45" s="365" t="n">
+      <c r="Q45" s="382" t="n">
         <v>6</v>
       </c>
       <c r="R45" s="106" t="n">
         <v>6995</v>
       </c>
-      <c r="S45" s="365" t="n">
+      <c r="S45" s="382" t="n">
         <v>6</v>
       </c>
       <c r="T45" s="106" t="n">
@@ -3764,15 +3788,15 @@
       </c>
     </row>
     <row r="46">
-      <c r="A46" s="367" t="inlineStr">
+      <c r="A46" s="384" t="inlineStr">
         <is>
           <t>#L2QQL9QVJ</t>
         </is>
       </c>
-      <c r="B46" s="367" t="n">
+      <c r="B46" s="384" t="n">
         <v>1450</v>
       </c>
-      <c r="C46" s="356" t="n">
+      <c r="C46" s="373" t="n">
         <v>43</v>
       </c>
       <c r="D46" s="116" t="inlineStr">
@@ -3780,49 +3804,49 @@
           <t>JustPre10d</t>
         </is>
       </c>
-      <c r="E46" s="369" t="n">
+      <c r="E46" s="386" t="n">
         <v>0</v>
       </c>
       <c r="F46" s="116" t="n">
         <v>0</v>
       </c>
-      <c r="G46" s="369" t="n">
+      <c r="G46" s="386" t="n">
         <v>0</v>
       </c>
       <c r="H46" s="115" t="n">
         <v>0</v>
       </c>
-      <c r="I46" s="369" t="n">
+      <c r="I46" s="386" t="n">
         <v>0</v>
       </c>
       <c r="J46" s="116" t="n">
         <v>0</v>
       </c>
-      <c r="K46" s="369" t="n">
+      <c r="K46" s="386" t="n">
         <v>0</v>
       </c>
       <c r="L46" s="116" t="n">
         <v>0</v>
       </c>
-      <c r="M46" s="369" t="n">
+      <c r="M46" s="386" t="n">
         <v>0</v>
       </c>
       <c r="N46" s="116" t="n">
         <v>0</v>
       </c>
-      <c r="O46" s="369" t="n">
+      <c r="O46" s="386" t="n">
         <v>0</v>
       </c>
       <c r="P46" s="116" t="n">
         <v>0</v>
       </c>
-      <c r="Q46" s="368" t="n">
+      <c r="Q46" s="385" t="n">
         <v>6</v>
       </c>
       <c r="R46" s="112" t="n">
         <v>6655</v>
       </c>
-      <c r="S46" s="368" t="n">
+      <c r="S46" s="385" t="n">
         <v>6</v>
       </c>
       <c r="T46" s="112" t="n">
@@ -3830,15 +3854,15 @@
       </c>
     </row>
     <row r="47">
-      <c r="A47" s="364" t="inlineStr">
+      <c r="A47" s="381" t="inlineStr">
         <is>
           <t>#LPR9RPCY9</t>
         </is>
       </c>
-      <c r="B47" s="364" t="n">
+      <c r="B47" s="381" t="n">
         <v>980</v>
       </c>
-      <c r="C47" s="360" t="n">
+      <c r="C47" s="377" t="n">
         <v>44</v>
       </c>
       <c r="D47" s="110" t="inlineStr">
@@ -3846,177 +3870,161 @@
           <t>sayhuss17</t>
         </is>
       </c>
-      <c r="E47" s="366" t="n">
+      <c r="E47" s="383" t="n">
         <v>0</v>
       </c>
       <c r="F47" s="110" t="n">
         <v>0</v>
       </c>
-      <c r="G47" s="366" t="n">
+      <c r="G47" s="383" t="n">
         <v>0</v>
       </c>
       <c r="H47" s="109" t="n">
         <v>0</v>
       </c>
-      <c r="I47" s="366" t="n">
+      <c r="I47" s="383" t="n">
         <v>0</v>
       </c>
       <c r="J47" s="110" t="n">
         <v>0</v>
       </c>
-      <c r="K47" s="366" t="n">
+      <c r="K47" s="383" t="n">
         <v>0</v>
       </c>
       <c r="L47" s="110" t="n">
         <v>0</v>
       </c>
-      <c r="M47" s="366" t="n">
+      <c r="M47" s="383" t="n">
         <v>0</v>
       </c>
       <c r="N47" s="110" t="n">
         <v>0</v>
       </c>
-      <c r="O47" s="366" t="n">
+      <c r="O47" s="383" t="n">
         <v>0</v>
       </c>
       <c r="P47" s="110" t="n">
         <v>0</v>
       </c>
-      <c r="Q47" s="370" t="n">
+      <c r="Q47" s="387" t="n">
         <v>4</v>
       </c>
       <c r="R47" s="118" t="n">
         <v>4240</v>
       </c>
-      <c r="S47" s="364" t="n"/>
+      <c r="S47" s="381" t="n"/>
       <c r="T47" s="109" t="n"/>
     </row>
     <row r="48">
-      <c r="A48" s="367" t="inlineStr">
+      <c r="A48" s="128" t="inlineStr">
         <is>
           <t>#QQL8C29CY</t>
         </is>
       </c>
-      <c r="B48" s="367" t="n">
+      <c r="B48" s="129" t="n">
         <v>864</v>
       </c>
-      <c r="C48" s="356" t="n">
+      <c r="C48" s="130" t="n">
         <v>45</v>
       </c>
-      <c r="D48" s="116" t="inlineStr">
+      <c r="D48" s="131" t="inlineStr">
         <is>
           <t>TypicalTeague#2</t>
         </is>
       </c>
-      <c r="E48" s="369" t="n">
-        <v>0</v>
-      </c>
-      <c r="F48" s="116" t="n">
-        <v>0</v>
-      </c>
-      <c r="G48" s="369" t="n">
-        <v>0</v>
-      </c>
-      <c r="H48" s="115" t="n">
-        <v>0</v>
-      </c>
-      <c r="I48" s="369" t="n">
-        <v>0</v>
-      </c>
-      <c r="J48" s="116" t="n">
-        <v>0</v>
-      </c>
-      <c r="K48" s="369" t="n">
-        <v>0</v>
-      </c>
-      <c r="L48" s="116" t="n">
-        <v>0</v>
-      </c>
-      <c r="M48" s="369" t="n">
-        <v>0</v>
-      </c>
-      <c r="N48" s="116" t="n">
-        <v>0</v>
-      </c>
-      <c r="O48" s="369" t="n">
-        <v>0</v>
-      </c>
-      <c r="P48" s="116" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q48" s="368" t="n">
+      <c r="E48" s="129" t="n"/>
+      <c r="F48" s="131" t="n"/>
+      <c r="G48" s="129" t="n"/>
+      <c r="H48" s="131" t="n"/>
+      <c r="I48" s="128" t="n">
+        <v>0</v>
+      </c>
+      <c r="J48" s="167" t="n">
+        <v>0</v>
+      </c>
+      <c r="K48" s="128" t="n">
+        <v>0</v>
+      </c>
+      <c r="L48" s="167" t="n">
+        <v>0</v>
+      </c>
+      <c r="M48" s="128" t="n">
+        <v>0</v>
+      </c>
+      <c r="N48" s="167" t="n">
+        <v>0</v>
+      </c>
+      <c r="O48" s="128" t="n">
+        <v>0</v>
+      </c>
+      <c r="P48" s="167" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q48" s="389" t="n">
         <v>5</v>
       </c>
-      <c r="R48" s="117" t="n">
+      <c r="R48" s="133" t="n">
         <v>4070</v>
       </c>
-      <c r="S48" s="368" t="n">
-        <v>6</v>
-      </c>
-      <c r="T48" s="112" t="n">
+      <c r="S48" s="389" t="n">
+        <v>6</v>
+      </c>
+      <c r="T48" s="390" t="n">
         <v>6410</v>
       </c>
     </row>
     <row r="49">
-      <c r="A49" s="364" t="inlineStr">
+      <c r="A49" s="383" t="inlineStr">
         <is>
           <t>#L9QL9YQQY</t>
         </is>
       </c>
-      <c r="B49" s="364" t="n">
+      <c r="B49" s="381" t="n">
         <v>975</v>
       </c>
-      <c r="C49" s="360" t="n">
+      <c r="C49" s="377" t="n">
         <v>46</v>
       </c>
-      <c r="D49" s="110" t="inlineStr">
+      <c r="D49" s="109" t="inlineStr">
         <is>
           <t>Ima Chad</t>
         </is>
       </c>
-      <c r="E49" s="366" t="n">
-        <v>0</v>
-      </c>
-      <c r="F49" s="110" t="n">
-        <v>0</v>
-      </c>
-      <c r="G49" s="366" t="n">
-        <v>0</v>
-      </c>
-      <c r="H49" s="109" t="n">
-        <v>0</v>
-      </c>
-      <c r="I49" s="366" t="n">
+      <c r="E49" s="381" t="n"/>
+      <c r="F49" s="109" t="n"/>
+      <c r="G49" s="381" t="n"/>
+      <c r="H49" s="109" t="n"/>
+      <c r="I49" s="383" t="n">
         <v>0</v>
       </c>
       <c r="J49" s="110" t="n">
         <v>0</v>
       </c>
-      <c r="K49" s="366" t="n">
+      <c r="K49" s="383" t="n">
         <v>0</v>
       </c>
       <c r="L49" s="110" t="n">
         <v>0</v>
       </c>
-      <c r="M49" s="366" t="n">
+      <c r="M49" s="383" t="n">
         <v>0</v>
       </c>
       <c r="N49" s="110" t="n">
         <v>0</v>
       </c>
-      <c r="O49" s="366" t="n">
+      <c r="O49" s="383" t="n">
         <v>0</v>
       </c>
       <c r="P49" s="110" t="n">
         <v>0</v>
       </c>
-      <c r="Q49" s="366" t="n">
+      <c r="Q49" s="383" t="n">
         <v>0</v>
       </c>
       <c r="R49" s="110" t="n">
         <v>0</v>
       </c>
-      <c r="S49" s="365" t="n">
+      <c r="S49" s="382" t="n">
         <v>5</v>
       </c>
       <c r="T49" s="110" t="n">
@@ -4024,69 +4032,69 @@
       </c>
     </row>
     <row r="50">
-      <c r="A50" s="128" t="inlineStr">
+      <c r="A50" s="386" t="inlineStr">
         <is>
           <t>#PJYVV989R</t>
         </is>
       </c>
-      <c r="B50" s="129" t="n">
+      <c r="B50" s="384" t="n">
         <v>1574</v>
       </c>
-      <c r="C50" s="130" t="n">
+      <c r="C50" s="373" t="n">
         <v>47</v>
       </c>
-      <c r="D50" s="131" t="inlineStr">
+      <c r="D50" s="115" t="inlineStr">
         <is>
           <t>nx</t>
         </is>
       </c>
-      <c r="E50" s="129" t="n"/>
-      <c r="F50" s="131" t="n"/>
-      <c r="G50" s="129" t="n"/>
-      <c r="H50" s="131" t="n"/>
-      <c r="I50" s="128" t="n">
-        <v>0</v>
-      </c>
-      <c r="J50" s="167" t="n">
-        <v>0</v>
-      </c>
-      <c r="K50" s="128" t="n">
-        <v>0</v>
-      </c>
-      <c r="L50" s="167" t="n">
-        <v>0</v>
-      </c>
-      <c r="M50" s="128" t="n">
-        <v>0</v>
-      </c>
-      <c r="N50" s="167" t="n">
-        <v>0</v>
-      </c>
-      <c r="O50" s="128" t="n">
-        <v>0</v>
-      </c>
-      <c r="P50" s="167" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q50" s="128" t="n">
-        <v>0</v>
-      </c>
-      <c r="R50" s="167" t="n">
-        <v>0</v>
-      </c>
-      <c r="S50" s="129" t="n"/>
-      <c r="T50" s="131" t="n"/>
+      <c r="E50" s="384" t="n"/>
+      <c r="F50" s="115" t="n"/>
+      <c r="G50" s="384" t="n"/>
+      <c r="H50" s="115" t="n"/>
+      <c r="I50" s="386" t="n">
+        <v>0</v>
+      </c>
+      <c r="J50" s="116" t="n">
+        <v>0</v>
+      </c>
+      <c r="K50" s="386" t="n">
+        <v>0</v>
+      </c>
+      <c r="L50" s="116" t="n">
+        <v>0</v>
+      </c>
+      <c r="M50" s="386" t="n">
+        <v>0</v>
+      </c>
+      <c r="N50" s="116" t="n">
+        <v>0</v>
+      </c>
+      <c r="O50" s="386" t="n">
+        <v>0</v>
+      </c>
+      <c r="P50" s="116" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q50" s="386" t="n">
+        <v>0</v>
+      </c>
+      <c r="R50" s="116" t="n">
+        <v>0</v>
+      </c>
+      <c r="S50" s="384" t="n"/>
+      <c r="T50" s="115" t="n"/>
     </row>
     <row r="51">
-      <c r="A51" s="366" t="inlineStr">
+      <c r="A51" s="383" t="inlineStr">
         <is>
           <t>#L9JJQY992</t>
         </is>
       </c>
-      <c r="B51" s="364" t="n">
+      <c r="B51" s="381" t="n">
         <v>773</v>
       </c>
-      <c r="C51" s="360" t="n">
+      <c r="C51" s="377" t="n">
         <v>48</v>
       </c>
       <c r="D51" s="109" t="inlineStr">
@@ -4094,53 +4102,53 @@
           <t>Fisted_Waffle</t>
         </is>
       </c>
-      <c r="E51" s="364" t="n"/>
+      <c r="E51" s="381" t="n"/>
       <c r="F51" s="109" t="n"/>
-      <c r="G51" s="364" t="n"/>
+      <c r="G51" s="381" t="n"/>
       <c r="H51" s="109" t="n"/>
-      <c r="I51" s="366" t="n">
+      <c r="I51" s="383" t="n">
         <v>0</v>
       </c>
       <c r="J51" s="110" t="n">
         <v>0</v>
       </c>
-      <c r="K51" s="366" t="n">
+      <c r="K51" s="383" t="n">
         <v>0</v>
       </c>
       <c r="L51" s="110" t="n">
         <v>0</v>
       </c>
-      <c r="M51" s="366" t="n">
+      <c r="M51" s="383" t="n">
         <v>0</v>
       </c>
       <c r="N51" s="110" t="n">
         <v>0</v>
       </c>
-      <c r="O51" s="366" t="n">
+      <c r="O51" s="383" t="n">
         <v>0</v>
       </c>
       <c r="P51" s="110" t="n">
         <v>0</v>
       </c>
-      <c r="Q51" s="366" t="n">
+      <c r="Q51" s="383" t="n">
         <v>0</v>
       </c>
       <c r="R51" s="110" t="n">
         <v>0</v>
       </c>
-      <c r="S51" s="364" t="n"/>
+      <c r="S51" s="381" t="n"/>
       <c r="T51" s="109" t="n"/>
     </row>
     <row r="52">
-      <c r="A52" s="369" t="inlineStr">
+      <c r="A52" s="386" t="inlineStr">
         <is>
           <t>#9JUR0JQV2</t>
         </is>
       </c>
-      <c r="B52" s="367" t="n">
+      <c r="B52" s="384" t="n">
         <v>1134</v>
       </c>
-      <c r="C52" s="356" t="n">
+      <c r="C52" s="373" t="n">
         <v>49</v>
       </c>
       <c r="D52" s="115" t="inlineStr">
@@ -4148,37 +4156,37 @@
           <t>atley</t>
         </is>
       </c>
-      <c r="E52" s="367" t="n"/>
+      <c r="E52" s="384" t="n"/>
       <c r="F52" s="115" t="n"/>
-      <c r="G52" s="367" t="n"/>
+      <c r="G52" s="384" t="n"/>
       <c r="H52" s="115" t="n"/>
-      <c r="I52" s="371" t="n">
+      <c r="I52" s="388" t="n">
         <v>3</v>
       </c>
       <c r="J52" s="117" t="n">
         <v>5277</v>
       </c>
-      <c r="K52" s="367" t="n"/>
+      <c r="K52" s="384" t="n"/>
       <c r="L52" s="115" t="n"/>
-      <c r="M52" s="367" t="n"/>
+      <c r="M52" s="384" t="n"/>
       <c r="N52" s="115" t="n"/>
-      <c r="O52" s="367" t="n"/>
+      <c r="O52" s="384" t="n"/>
       <c r="P52" s="115" t="n"/>
-      <c r="Q52" s="367" t="n"/>
+      <c r="Q52" s="384" t="n"/>
       <c r="R52" s="115" t="n"/>
-      <c r="S52" s="367" t="n"/>
+      <c r="S52" s="384" t="n"/>
       <c r="T52" s="115" t="n"/>
     </row>
     <row r="53">
-      <c r="A53" s="366" t="inlineStr">
+      <c r="A53" s="383" t="inlineStr">
         <is>
           <t>#QUCCVCCJ0</t>
         </is>
       </c>
-      <c r="B53" s="364" t="n">
+      <c r="B53" s="381" t="n">
         <v>783</v>
       </c>
-      <c r="C53" s="360" t="n">
+      <c r="C53" s="377" t="n">
         <v>50</v>
       </c>
       <c r="D53" s="109" t="inlineStr">
@@ -4186,33 +4194,33 @@
           <t>koi</t>
         </is>
       </c>
-      <c r="E53" s="364" t="n"/>
+      <c r="E53" s="381" t="n"/>
       <c r="F53" s="109" t="n"/>
-      <c r="G53" s="364" t="n"/>
+      <c r="G53" s="381" t="n"/>
       <c r="H53" s="109" t="n"/>
-      <c r="I53" s="364" t="n"/>
+      <c r="I53" s="381" t="n"/>
       <c r="J53" s="109" t="n"/>
-      <c r="K53" s="364" t="n"/>
+      <c r="K53" s="381" t="n"/>
       <c r="L53" s="109" t="n"/>
-      <c r="M53" s="364" t="n"/>
+      <c r="M53" s="381" t="n"/>
       <c r="N53" s="109" t="n"/>
-      <c r="O53" s="364" t="n"/>
+      <c r="O53" s="381" t="n"/>
       <c r="P53" s="109" t="n"/>
-      <c r="Q53" s="364" t="n"/>
+      <c r="Q53" s="381" t="n"/>
       <c r="R53" s="109" t="n"/>
-      <c r="S53" s="364" t="n"/>
+      <c r="S53" s="381" t="n"/>
       <c r="T53" s="109" t="n"/>
     </row>
     <row r="54">
-      <c r="A54" s="369" t="inlineStr">
+      <c r="A54" s="386" t="inlineStr">
         <is>
           <t>#QPRYCJVJL</t>
         </is>
       </c>
-      <c r="B54" s="367" t="n">
+      <c r="B54" s="384" t="n">
         <v>693</v>
       </c>
-      <c r="C54" s="356" t="n">
+      <c r="C54" s="373" t="n">
         <v>51</v>
       </c>
       <c r="D54" s="115" t="inlineStr">
@@ -4220,33 +4228,33 @@
           <t>cris</t>
         </is>
       </c>
-      <c r="E54" s="367" t="n"/>
+      <c r="E54" s="384" t="n"/>
       <c r="F54" s="115" t="n"/>
-      <c r="G54" s="367" t="n"/>
+      <c r="G54" s="384" t="n"/>
       <c r="H54" s="115" t="n"/>
-      <c r="I54" s="367" t="n"/>
+      <c r="I54" s="384" t="n"/>
       <c r="J54" s="115" t="n"/>
-      <c r="K54" s="367" t="n"/>
+      <c r="K54" s="384" t="n"/>
       <c r="L54" s="115" t="n"/>
-      <c r="M54" s="367" t="n"/>
+      <c r="M54" s="384" t="n"/>
       <c r="N54" s="115" t="n"/>
-      <c r="O54" s="367" t="n"/>
+      <c r="O54" s="384" t="n"/>
       <c r="P54" s="115" t="n"/>
-      <c r="Q54" s="367" t="n"/>
+      <c r="Q54" s="384" t="n"/>
       <c r="R54" s="115" t="n"/>
-      <c r="S54" s="367" t="n"/>
+      <c r="S54" s="384" t="n"/>
       <c r="T54" s="115" t="n"/>
     </row>
     <row r="55">
-      <c r="A55" s="366" t="inlineStr">
+      <c r="A55" s="383" t="inlineStr">
         <is>
           <t>#QQLVRJCGQ</t>
         </is>
       </c>
-      <c r="B55" s="364" t="n">
+      <c r="B55" s="381" t="n">
         <v>1240</v>
       </c>
-      <c r="C55" s="360" t="n">
+      <c r="C55" s="377" t="n">
         <v>52</v>
       </c>
       <c r="D55" s="109" t="inlineStr">
@@ -4254,33 +4262,33 @@
           <t>khant</t>
         </is>
       </c>
-      <c r="E55" s="364" t="n"/>
+      <c r="E55" s="381" t="n"/>
       <c r="F55" s="109" t="n"/>
-      <c r="G55" s="364" t="n"/>
+      <c r="G55" s="381" t="n"/>
       <c r="H55" s="109" t="n"/>
-      <c r="I55" s="364" t="n"/>
+      <c r="I55" s="381" t="n"/>
       <c r="J55" s="109" t="n"/>
-      <c r="K55" s="364" t="n"/>
+      <c r="K55" s="381" t="n"/>
       <c r="L55" s="109" t="n"/>
-      <c r="M55" s="364" t="n"/>
+      <c r="M55" s="381" t="n"/>
       <c r="N55" s="109" t="n"/>
-      <c r="O55" s="364" t="n"/>
+      <c r="O55" s="381" t="n"/>
       <c r="P55" s="109" t="n"/>
-      <c r="Q55" s="364" t="n"/>
+      <c r="Q55" s="381" t="n"/>
       <c r="R55" s="109" t="n"/>
-      <c r="S55" s="364" t="n"/>
+      <c r="S55" s="381" t="n"/>
       <c r="T55" s="109" t="n"/>
     </row>
     <row r="56">
-      <c r="A56" s="369" t="inlineStr">
+      <c r="A56" s="386" t="inlineStr">
         <is>
           <t>#QLL0PVCRV</t>
         </is>
       </c>
-      <c r="B56" s="367" t="n">
+      <c r="B56" s="384" t="n">
         <v>1704</v>
       </c>
-      <c r="C56" s="356" t="n">
+      <c r="C56" s="373" t="n">
         <v>53</v>
       </c>
       <c r="D56" s="115" t="inlineStr">
@@ -4288,33 +4296,33 @@
           <t>Harsh chhillar</t>
         </is>
       </c>
-      <c r="E56" s="367" t="n"/>
+      <c r="E56" s="384" t="n"/>
       <c r="F56" s="115" t="n"/>
-      <c r="G56" s="367" t="n"/>
+      <c r="G56" s="384" t="n"/>
       <c r="H56" s="115" t="n"/>
-      <c r="I56" s="367" t="n"/>
+      <c r="I56" s="384" t="n"/>
       <c r="J56" s="115" t="n"/>
-      <c r="K56" s="367" t="n"/>
+      <c r="K56" s="384" t="n"/>
       <c r="L56" s="115" t="n"/>
-      <c r="M56" s="367" t="n"/>
+      <c r="M56" s="384" t="n"/>
       <c r="N56" s="115" t="n"/>
-      <c r="O56" s="367" t="n"/>
+      <c r="O56" s="384" t="n"/>
       <c r="P56" s="115" t="n"/>
-      <c r="Q56" s="367" t="n"/>
+      <c r="Q56" s="384" t="n"/>
       <c r="R56" s="115" t="n"/>
-      <c r="S56" s="367" t="n"/>
+      <c r="S56" s="384" t="n"/>
       <c r="T56" s="115" t="n"/>
     </row>
     <row r="57">
-      <c r="A57" s="366" t="inlineStr">
+      <c r="A57" s="383" t="inlineStr">
         <is>
           <t>#Q8YP9P8UJ</t>
         </is>
       </c>
-      <c r="B57" s="364" t="n">
+      <c r="B57" s="381" t="n">
         <v>945</v>
       </c>
-      <c r="C57" s="360" t="n">
+      <c r="C57" s="377" t="n">
         <v>54</v>
       </c>
       <c r="D57" s="109" t="inlineStr">
@@ -4322,37 +4330,37 @@
           <t>Ranger</t>
         </is>
       </c>
-      <c r="E57" s="364" t="n"/>
+      <c r="E57" s="381" t="n"/>
       <c r="F57" s="109" t="n"/>
-      <c r="G57" s="364" t="n"/>
+      <c r="G57" s="381" t="n"/>
       <c r="H57" s="109" t="n"/>
-      <c r="I57" s="364" t="n"/>
+      <c r="I57" s="381" t="n"/>
       <c r="J57" s="109" t="n"/>
-      <c r="K57" s="364" t="n"/>
+      <c r="K57" s="381" t="n"/>
       <c r="L57" s="109" t="n"/>
-      <c r="M57" s="365" t="n">
+      <c r="M57" s="382" t="n">
         <v>5</v>
       </c>
       <c r="N57" s="118" t="n">
         <v>4680</v>
       </c>
-      <c r="O57" s="364" t="n"/>
+      <c r="O57" s="381" t="n"/>
       <c r="P57" s="109" t="n"/>
-      <c r="Q57" s="364" t="n"/>
+      <c r="Q57" s="381" t="n"/>
       <c r="R57" s="109" t="n"/>
-      <c r="S57" s="364" t="n"/>
+      <c r="S57" s="381" t="n"/>
       <c r="T57" s="109" t="n"/>
     </row>
     <row r="58">
-      <c r="A58" s="369" t="inlineStr">
+      <c r="A58" s="386" t="inlineStr">
         <is>
           <t>#Q0JG2RJQ8</t>
         </is>
       </c>
-      <c r="B58" s="367" t="n">
+      <c r="B58" s="384" t="n">
         <v>997</v>
       </c>
-      <c r="C58" s="356" t="n">
+      <c r="C58" s="373" t="n">
         <v>55</v>
       </c>
       <c r="D58" s="115" t="inlineStr">
@@ -4360,37 +4368,37 @@
           <t>bozo</t>
         </is>
       </c>
-      <c r="E58" s="367" t="n"/>
+      <c r="E58" s="384" t="n"/>
       <c r="F58" s="115" t="n"/>
-      <c r="G58" s="367" t="n"/>
+      <c r="G58" s="384" t="n"/>
       <c r="H58" s="115" t="n"/>
-      <c r="I58" s="367" t="n"/>
+      <c r="I58" s="384" t="n"/>
       <c r="J58" s="115" t="n"/>
-      <c r="K58" s="367" t="n"/>
+      <c r="K58" s="384" t="n"/>
       <c r="L58" s="115" t="n"/>
-      <c r="M58" s="367" t="n"/>
+      <c r="M58" s="384" t="n"/>
       <c r="N58" s="115" t="n"/>
-      <c r="O58" s="368" t="n">
+      <c r="O58" s="385" t="n">
         <v>6</v>
       </c>
       <c r="P58" s="112" t="n">
         <v>6495</v>
       </c>
-      <c r="Q58" s="367" t="n"/>
+      <c r="Q58" s="384" t="n"/>
       <c r="R58" s="115" t="n"/>
-      <c r="S58" s="367" t="n"/>
+      <c r="S58" s="384" t="n"/>
       <c r="T58" s="115" t="n"/>
     </row>
     <row r="59">
-      <c r="A59" s="366" t="inlineStr">
+      <c r="A59" s="383" t="inlineStr">
         <is>
           <t>#UVCCQC02</t>
         </is>
       </c>
-      <c r="B59" s="364" t="n">
+      <c r="B59" s="381" t="n">
         <v>1806</v>
       </c>
-      <c r="C59" s="360" t="n">
+      <c r="C59" s="377" t="n">
         <v>56</v>
       </c>
       <c r="D59" s="109" t="inlineStr">
@@ -4398,29 +4406,29 @@
           <t>lordshisha</t>
         </is>
       </c>
-      <c r="E59" s="364" t="n"/>
+      <c r="E59" s="381" t="n"/>
       <c r="F59" s="109" t="n"/>
-      <c r="G59" s="364" t="n"/>
+      <c r="G59" s="381" t="n"/>
       <c r="H59" s="109" t="n"/>
-      <c r="I59" s="364" t="n"/>
+      <c r="I59" s="381" t="n"/>
       <c r="J59" s="109" t="n"/>
-      <c r="K59" s="364" t="n"/>
+      <c r="K59" s="381" t="n"/>
       <c r="L59" s="109" t="n"/>
-      <c r="M59" s="364" t="n"/>
+      <c r="M59" s="381" t="n"/>
       <c r="N59" s="109" t="n"/>
-      <c r="O59" s="365" t="n">
+      <c r="O59" s="382" t="n">
         <v>6</v>
       </c>
       <c r="P59" s="106" t="n">
         <v>8496</v>
       </c>
-      <c r="Q59" s="365" t="n">
+      <c r="Q59" s="382" t="n">
         <v>6</v>
       </c>
       <c r="R59" s="106" t="n">
         <v>6310</v>
       </c>
-      <c r="S59" s="365" t="n">
+      <c r="S59" s="382" t="n">
         <v>6</v>
       </c>
       <c r="T59" s="106" t="n">
@@ -4428,15 +4436,15 @@
       </c>
     </row>
     <row r="60">
-      <c r="A60" s="369" t="inlineStr">
+      <c r="A60" s="386" t="inlineStr">
         <is>
           <t>#P2CPRPQU</t>
         </is>
       </c>
-      <c r="B60" s="367" t="n">
+      <c r="B60" s="384" t="n">
         <v>2232</v>
       </c>
-      <c r="C60" s="356" t="n">
+      <c r="C60" s="373" t="n">
         <v>57</v>
       </c>
       <c r="D60" s="115" t="inlineStr">
@@ -4444,29 +4452,29 @@
           <t>The Drift King</t>
         </is>
       </c>
-      <c r="E60" s="367" t="n"/>
+      <c r="E60" s="384" t="n"/>
       <c r="F60" s="115" t="n"/>
-      <c r="G60" s="367" t="n"/>
+      <c r="G60" s="384" t="n"/>
       <c r="H60" s="115" t="n"/>
-      <c r="I60" s="367" t="n"/>
+      <c r="I60" s="384" t="n"/>
       <c r="J60" s="115" t="n"/>
-      <c r="K60" s="367" t="n"/>
+      <c r="K60" s="384" t="n"/>
       <c r="L60" s="115" t="n"/>
-      <c r="M60" s="367" t="n"/>
+      <c r="M60" s="384" t="n"/>
       <c r="N60" s="115" t="n"/>
-      <c r="O60" s="368" t="n">
+      <c r="O60" s="385" t="n">
         <v>6</v>
       </c>
       <c r="P60" s="112" t="n">
         <v>8023</v>
       </c>
-      <c r="Q60" s="368" t="n">
+      <c r="Q60" s="385" t="n">
         <v>6</v>
       </c>
       <c r="R60" s="112" t="n">
         <v>7625</v>
       </c>
-      <c r="S60" s="368" t="n">
+      <c r="S60" s="385" t="n">
         <v>6</v>
       </c>
       <c r="T60" s="112" t="n">
@@ -4474,15 +4482,15 @@
       </c>
     </row>
     <row r="61">
-      <c r="A61" s="366" t="inlineStr">
+      <c r="A61" s="383" t="inlineStr">
         <is>
           <t>#QJVL0LYQQ</t>
         </is>
       </c>
-      <c r="B61" s="364" t="n">
+      <c r="B61" s="381" t="n">
         <v>921</v>
       </c>
-      <c r="C61" s="360" t="n">
+      <c r="C61" s="377" t="n">
         <v>58</v>
       </c>
       <c r="D61" s="109" t="inlineStr">
@@ -4490,29 +4498,29 @@
           <t>mobbb341</t>
         </is>
       </c>
-      <c r="E61" s="364" t="n"/>
+      <c r="E61" s="381" t="n"/>
       <c r="F61" s="109" t="n"/>
-      <c r="G61" s="364" t="n"/>
+      <c r="G61" s="381" t="n"/>
       <c r="H61" s="109" t="n"/>
-      <c r="I61" s="364" t="n"/>
+      <c r="I61" s="381" t="n"/>
       <c r="J61" s="109" t="n"/>
-      <c r="K61" s="364" t="n"/>
+      <c r="K61" s="381" t="n"/>
       <c r="L61" s="109" t="n"/>
-      <c r="M61" s="364" t="n"/>
+      <c r="M61" s="381" t="n"/>
       <c r="N61" s="109" t="n"/>
-      <c r="O61" s="365" t="n">
+      <c r="O61" s="382" t="n">
         <v>6</v>
       </c>
       <c r="P61" s="106" t="n">
         <v>7710</v>
       </c>
-      <c r="Q61" s="365" t="n">
+      <c r="Q61" s="382" t="n">
         <v>6</v>
       </c>
       <c r="R61" s="106" t="n">
         <v>8810</v>
       </c>
-      <c r="S61" s="365" t="n">
+      <c r="S61" s="382" t="n">
         <v>6</v>
       </c>
       <c r="T61" s="118" t="n">
@@ -4520,15 +4528,15 @@
       </c>
     </row>
     <row r="62">
-      <c r="A62" s="369" t="inlineStr">
+      <c r="A62" s="386" t="inlineStr">
         <is>
           <t>#L8R82C8VC</t>
         </is>
       </c>
-      <c r="B62" s="367" t="n">
+      <c r="B62" s="384" t="n">
         <v>1162</v>
       </c>
-      <c r="C62" s="356" t="n">
+      <c r="C62" s="373" t="n">
         <v>59</v>
       </c>
       <c r="D62" s="115" t="inlineStr">
@@ -4536,29 +4544,29 @@
           <t>caden asue</t>
         </is>
       </c>
-      <c r="E62" s="367" t="n"/>
+      <c r="E62" s="384" t="n"/>
       <c r="F62" s="115" t="n"/>
-      <c r="G62" s="367" t="n"/>
+      <c r="G62" s="384" t="n"/>
       <c r="H62" s="115" t="n"/>
-      <c r="I62" s="367" t="n"/>
+      <c r="I62" s="384" t="n"/>
       <c r="J62" s="115" t="n"/>
-      <c r="K62" s="367" t="n"/>
+      <c r="K62" s="384" t="n"/>
       <c r="L62" s="115" t="n"/>
-      <c r="M62" s="367" t="n"/>
+      <c r="M62" s="384" t="n"/>
       <c r="N62" s="115" t="n"/>
-      <c r="O62" s="368" t="n">
+      <c r="O62" s="385" t="n">
         <v>6</v>
       </c>
       <c r="P62" s="117" t="n">
         <v>5112</v>
       </c>
-      <c r="Q62" s="368" t="n">
+      <c r="Q62" s="385" t="n">
         <v>6</v>
       </c>
       <c r="R62" s="117" t="n">
         <v>4283</v>
       </c>
-      <c r="S62" s="368" t="n">
+      <c r="S62" s="385" t="n">
         <v>6</v>
       </c>
       <c r="T62" s="117" t="n">
@@ -4566,15 +4574,15 @@
       </c>
     </row>
     <row r="63">
-      <c r="A63" s="366" t="inlineStr">
+      <c r="A63" s="383" t="inlineStr">
         <is>
           <t>#L9Q8VLLQG</t>
         </is>
       </c>
-      <c r="B63" s="364" t="n">
+      <c r="B63" s="381" t="n">
         <v>1130</v>
       </c>
-      <c r="C63" s="360" t="n">
+      <c r="C63" s="377" t="n">
         <v>60</v>
       </c>
       <c r="D63" s="109" t="inlineStr">
@@ -4582,21 +4590,21 @@
           <t>cat</t>
         </is>
       </c>
-      <c r="E63" s="364" t="n"/>
+      <c r="E63" s="381" t="n"/>
       <c r="F63" s="109" t="n"/>
-      <c r="G63" s="364" t="n"/>
+      <c r="G63" s="381" t="n"/>
       <c r="H63" s="109" t="n"/>
-      <c r="I63" s="364" t="n"/>
+      <c r="I63" s="381" t="n"/>
       <c r="J63" s="109" t="n"/>
-      <c r="K63" s="364" t="n"/>
+      <c r="K63" s="381" t="n"/>
       <c r="L63" s="109" t="n"/>
-      <c r="M63" s="364" t="n"/>
+      <c r="M63" s="381" t="n"/>
       <c r="N63" s="109" t="n"/>
-      <c r="O63" s="364" t="n"/>
+      <c r="O63" s="381" t="n"/>
       <c r="P63" s="109" t="n"/>
-      <c r="Q63" s="364" t="n"/>
+      <c r="Q63" s="381" t="n"/>
       <c r="R63" s="109" t="n"/>
-      <c r="S63" s="365" t="n">
+      <c r="S63" s="382" t="n">
         <v>6</v>
       </c>
       <c r="T63" s="118" t="n">
@@ -4604,15 +4612,15 @@
       </c>
     </row>
     <row r="64">
-      <c r="A64" s="369" t="inlineStr">
+      <c r="A64" s="386" t="inlineStr">
         <is>
           <t>#QV0PQC9JU</t>
         </is>
       </c>
-      <c r="B64" s="367" t="n">
+      <c r="B64" s="384" t="n">
         <v>539</v>
       </c>
-      <c r="C64" s="356" t="n">
+      <c r="C64" s="373" t="n">
         <v>61</v>
       </c>
       <c r="D64" s="115" t="inlineStr">
@@ -4620,21 +4628,21 @@
           <t>Superman</t>
         </is>
       </c>
-      <c r="E64" s="367" t="n"/>
+      <c r="E64" s="384" t="n"/>
       <c r="F64" s="115" t="n"/>
-      <c r="G64" s="367" t="n"/>
+      <c r="G64" s="384" t="n"/>
       <c r="H64" s="115" t="n"/>
-      <c r="I64" s="367" t="n"/>
+      <c r="I64" s="384" t="n"/>
       <c r="J64" s="115" t="n"/>
-      <c r="K64" s="367" t="n"/>
+      <c r="K64" s="384" t="n"/>
       <c r="L64" s="115" t="n"/>
-      <c r="M64" s="367" t="n"/>
+      <c r="M64" s="384" t="n"/>
       <c r="N64" s="115" t="n"/>
-      <c r="O64" s="367" t="n"/>
+      <c r="O64" s="384" t="n"/>
       <c r="P64" s="115" t="n"/>
-      <c r="Q64" s="367" t="n"/>
+      <c r="Q64" s="384" t="n"/>
       <c r="R64" s="115" t="n"/>
-      <c r="S64" s="368" t="n">
+      <c r="S64" s="385" t="n">
         <v>6</v>
       </c>
       <c r="T64" s="117" t="n">
@@ -4642,15 +4650,15 @@
       </c>
     </row>
     <row r="65">
-      <c r="A65" s="366" t="inlineStr">
+      <c r="A65" s="383" t="inlineStr">
         <is>
           <t>#LU0CRP09L</t>
         </is>
       </c>
-      <c r="B65" s="364" t="n">
+      <c r="B65" s="381" t="n">
         <v>809</v>
       </c>
-      <c r="C65" s="360" t="n">
+      <c r="C65" s="377" t="n">
         <v>62</v>
       </c>
       <c r="D65" s="109" t="inlineStr">
@@ -4658,21 +4666,21 @@
           <t>I Dont Know</t>
         </is>
       </c>
-      <c r="E65" s="364" t="n"/>
+      <c r="E65" s="381" t="n"/>
       <c r="F65" s="109" t="n"/>
-      <c r="G65" s="364" t="n"/>
+      <c r="G65" s="381" t="n"/>
       <c r="H65" s="109" t="n"/>
-      <c r="I65" s="364" t="n"/>
+      <c r="I65" s="381" t="n"/>
       <c r="J65" s="109" t="n"/>
-      <c r="K65" s="364" t="n"/>
+      <c r="K65" s="381" t="n"/>
       <c r="L65" s="109" t="n"/>
-      <c r="M65" s="364" t="n"/>
+      <c r="M65" s="381" t="n"/>
       <c r="N65" s="109" t="n"/>
-      <c r="O65" s="364" t="n"/>
+      <c r="O65" s="381" t="n"/>
       <c r="P65" s="109" t="n"/>
-      <c r="Q65" s="364" t="n"/>
+      <c r="Q65" s="381" t="n"/>
       <c r="R65" s="109" t="n"/>
-      <c r="S65" s="370" t="n">
+      <c r="S65" s="387" t="n">
         <v>3</v>
       </c>
       <c r="T65" s="110" t="n">
@@ -4680,15 +4688,15 @@
       </c>
     </row>
     <row r="66">
-      <c r="A66" s="369" t="inlineStr">
+      <c r="A66" s="386" t="inlineStr">
         <is>
           <t>#YCPP0QPP8</t>
         </is>
       </c>
-      <c r="B66" s="367" t="n">
+      <c r="B66" s="384" t="n">
         <v>3327</v>
       </c>
-      <c r="C66" s="356" t="n">
+      <c r="C66" s="373" t="n">
         <v>63</v>
       </c>
       <c r="D66" s="115" t="inlineStr">
@@ -4696,21 +4704,21 @@
           <t>Coach</t>
         </is>
       </c>
-      <c r="E66" s="367" t="n"/>
+      <c r="E66" s="384" t="n"/>
       <c r="F66" s="115" t="n"/>
-      <c r="G66" s="367" t="n"/>
+      <c r="G66" s="384" t="n"/>
       <c r="H66" s="115" t="n"/>
-      <c r="I66" s="367" t="n"/>
+      <c r="I66" s="384" t="n"/>
       <c r="J66" s="115" t="n"/>
-      <c r="K66" s="367" t="n"/>
+      <c r="K66" s="384" t="n"/>
       <c r="L66" s="115" t="n"/>
-      <c r="M66" s="367" t="n"/>
+      <c r="M66" s="384" t="n"/>
       <c r="N66" s="115" t="n"/>
-      <c r="O66" s="367" t="n"/>
+      <c r="O66" s="384" t="n"/>
       <c r="P66" s="115" t="n"/>
-      <c r="Q66" s="367" t="n"/>
+      <c r="Q66" s="384" t="n"/>
       <c r="R66" s="115" t="n"/>
-      <c r="S66" s="369" t="n">
+      <c r="S66" s="386" t="n">
         <v>0</v>
       </c>
       <c r="T66" s="116" t="n">

</xml_diff>

<commit_message>
updating the clash file from bat automatic run
</commit_message>
<xml_diff>
--- a/Clash.xlsx
+++ b/Clash.xlsx
@@ -223,7 +223,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="29">
+  <borders count="30">
     <border>
       <left/>
       <right/>
@@ -332,11 +332,12 @@
     <border/>
     <border/>
     <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9"/>
   </cellStyleXfs>
-  <cellXfs count="391">
+  <cellXfs count="408">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -830,6 +831,27 @@
     <xf numFmtId="164" fontId="8" fillId="31" borderId="28" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="8" fillId="26" borderId="12" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="8" fillId="26" borderId="13" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="7" fillId="25" borderId="29" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="25" borderId="29" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="26" borderId="29" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="7" fillId="27" borderId="29" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="7" fillId="28" borderId="29" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="28" borderId="29" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="29" borderId="29" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="7" fillId="30" borderId="29" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="7" fillId="31" borderId="29" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="8" fillId="28" borderId="29" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="8" fillId="29" borderId="29" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="8" fillId="30" borderId="29" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="8" fillId="25" borderId="29" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="8" fillId="26" borderId="29" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="8" fillId="27" borderId="29" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="8" fillId="32" borderId="29" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="8" fillId="31" borderId="29" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1428,15 +1450,15 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="372" t="inlineStr">
+      <c r="A4" s="391" t="inlineStr">
         <is>
           <t>#G0QPVJY9L</t>
         </is>
       </c>
-      <c r="B4" s="372" t="n">
+      <c r="B4" s="391" t="n">
         <v>779</v>
       </c>
-      <c r="C4" s="373" t="n">
+      <c r="C4" s="392" t="n">
         <v>1</v>
       </c>
       <c r="D4" s="95" t="inlineStr">
@@ -1444,49 +1466,49 @@
           <t>Zoro</t>
         </is>
       </c>
-      <c r="E4" s="374" t="n">
+      <c r="E4" s="393" t="n">
         <v>6</v>
       </c>
       <c r="F4" s="95" t="n">
         <v>13801</v>
       </c>
-      <c r="G4" s="375" t="n">
+      <c r="G4" s="394" t="n">
         <v>0</v>
       </c>
       <c r="H4" s="98" t="n">
         <v>0</v>
       </c>
-      <c r="I4" s="374" t="n">
+      <c r="I4" s="393" t="n">
         <v>6</v>
       </c>
       <c r="J4" s="95" t="n">
         <v>12116</v>
       </c>
-      <c r="K4" s="374" t="n">
+      <c r="K4" s="393" t="n">
         <v>6</v>
       </c>
       <c r="L4" s="95" t="n">
         <v>13432</v>
       </c>
-      <c r="M4" s="374" t="n">
+      <c r="M4" s="393" t="n">
         <v>6</v>
       </c>
       <c r="N4" s="95" t="n">
         <v>8855</v>
       </c>
-      <c r="O4" s="374" t="n">
+      <c r="O4" s="393" t="n">
         <v>6</v>
       </c>
       <c r="P4" s="95" t="n">
         <v>10965</v>
       </c>
-      <c r="Q4" s="374" t="n">
+      <c r="Q4" s="393" t="n">
         <v>6</v>
       </c>
       <c r="R4" s="95" t="n">
         <v>7905</v>
       </c>
-      <c r="S4" s="374" t="n">
+      <c r="S4" s="393" t="n">
         <v>6</v>
       </c>
       <c r="T4" s="95" t="n">
@@ -1494,15 +1516,15 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="376" t="inlineStr">
+      <c r="A5" s="395" t="inlineStr">
         <is>
           <t>#YRGRRJQCY</t>
         </is>
       </c>
-      <c r="B5" s="376" t="n">
+      <c r="B5" s="395" t="n">
         <v>1306</v>
       </c>
-      <c r="C5" s="377" t="n">
+      <c r="C5" s="396" t="n">
         <v>2</v>
       </c>
       <c r="D5" s="101" t="inlineStr">
@@ -1510,49 +1532,49 @@
           <t>DoubleSpice</t>
         </is>
       </c>
-      <c r="E5" s="378" t="n">
+      <c r="E5" s="397" t="n">
         <v>6</v>
       </c>
       <c r="F5" s="101" t="n">
         <v>13656</v>
       </c>
-      <c r="G5" s="379" t="n">
+      <c r="G5" s="398" t="n">
         <v>0</v>
       </c>
       <c r="H5" s="104" t="n">
         <v>0</v>
       </c>
-      <c r="I5" s="378" t="n">
+      <c r="I5" s="397" t="n">
         <v>6</v>
       </c>
       <c r="J5" s="101" t="n">
         <v>10016</v>
       </c>
-      <c r="K5" s="378" t="n">
+      <c r="K5" s="397" t="n">
         <v>6</v>
       </c>
       <c r="L5" s="101" t="n">
         <v>11620</v>
       </c>
-      <c r="M5" s="378" t="n">
+      <c r="M5" s="397" t="n">
         <v>6</v>
       </c>
       <c r="N5" s="101" t="n">
         <v>14095</v>
       </c>
-      <c r="O5" s="378" t="n">
+      <c r="O5" s="397" t="n">
         <v>6</v>
       </c>
       <c r="P5" s="101" t="n">
         <v>12379</v>
       </c>
-      <c r="Q5" s="378" t="n">
+      <c r="Q5" s="397" t="n">
         <v>6</v>
       </c>
       <c r="R5" s="101" t="n">
         <v>8256</v>
       </c>
-      <c r="S5" s="378" t="n">
+      <c r="S5" s="397" t="n">
         <v>6</v>
       </c>
       <c r="T5" s="101" t="n">
@@ -1560,15 +1582,15 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="372" t="inlineStr">
+      <c r="A6" s="391" t="inlineStr">
         <is>
           <t>#90U0VPU9U</t>
         </is>
       </c>
-      <c r="B6" s="372" t="n">
+      <c r="B6" s="391" t="n">
         <v>2597</v>
       </c>
-      <c r="C6" s="373" t="n">
+      <c r="C6" s="392" t="n">
         <v>3</v>
       </c>
       <c r="D6" s="95" t="inlineStr">
@@ -1576,49 +1598,49 @@
           <t>KYANI7E</t>
         </is>
       </c>
-      <c r="E6" s="374" t="n">
+      <c r="E6" s="393" t="n">
         <v>6</v>
       </c>
       <c r="F6" s="95" t="n">
         <v>13278</v>
       </c>
-      <c r="G6" s="380" t="n">
+      <c r="G6" s="399" t="n">
         <v>141</v>
       </c>
       <c r="H6" s="98" t="n">
         <v>0</v>
       </c>
-      <c r="I6" s="374" t="n">
+      <c r="I6" s="393" t="n">
         <v>6</v>
       </c>
       <c r="J6" s="95" t="n">
         <v>12477</v>
       </c>
-      <c r="K6" s="374" t="n">
+      <c r="K6" s="393" t="n">
         <v>6</v>
       </c>
       <c r="L6" s="95" t="n">
         <v>13260</v>
       </c>
-      <c r="M6" s="374" t="n">
+      <c r="M6" s="393" t="n">
         <v>6</v>
       </c>
       <c r="N6" s="95" t="n">
         <v>12144</v>
       </c>
-      <c r="O6" s="374" t="n">
+      <c r="O6" s="393" t="n">
         <v>6</v>
       </c>
       <c r="P6" s="95" t="n">
         <v>12835</v>
       </c>
-      <c r="Q6" s="374" t="n">
+      <c r="Q6" s="393" t="n">
         <v>6</v>
       </c>
       <c r="R6" s="95" t="n">
         <v>7696</v>
       </c>
-      <c r="S6" s="374" t="n">
+      <c r="S6" s="393" t="n">
         <v>6</v>
       </c>
       <c r="T6" s="95" t="n">
@@ -1626,15 +1648,15 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="376" t="inlineStr">
+      <c r="A7" s="395" t="inlineStr">
         <is>
           <t>#YJ20CRJYQ</t>
         </is>
       </c>
-      <c r="B7" s="376" t="n">
-        <v>1255</v>
-      </c>
-      <c r="C7" s="377" t="n">
+      <c r="B7" s="395" t="n">
+        <v>1244</v>
+      </c>
+      <c r="C7" s="396" t="n">
         <v>4</v>
       </c>
       <c r="D7" s="101" t="inlineStr">
@@ -1642,49 +1664,49 @@
           <t>UnluckGod</t>
         </is>
       </c>
-      <c r="E7" s="378" t="n">
+      <c r="E7" s="397" t="n">
         <v>6</v>
       </c>
       <c r="F7" s="101" t="n">
         <v>13062</v>
       </c>
-      <c r="G7" s="379" t="n">
+      <c r="G7" s="398" t="n">
         <v>0</v>
       </c>
       <c r="H7" s="104" t="n">
         <v>0</v>
       </c>
-      <c r="I7" s="378" t="n">
+      <c r="I7" s="397" t="n">
         <v>6</v>
       </c>
       <c r="J7" s="101" t="n">
         <v>8886</v>
       </c>
-      <c r="K7" s="378" t="n">
+      <c r="K7" s="397" t="n">
         <v>6</v>
       </c>
       <c r="L7" s="101" t="n">
         <v>12824</v>
       </c>
-      <c r="M7" s="378" t="n">
+      <c r="M7" s="397" t="n">
         <v>6</v>
       </c>
       <c r="N7" s="101" t="n">
         <v>11999</v>
       </c>
-      <c r="O7" s="378" t="n">
+      <c r="O7" s="397" t="n">
         <v>6</v>
       </c>
       <c r="P7" s="101" t="n">
         <v>12972</v>
       </c>
-      <c r="Q7" s="378" t="n">
+      <c r="Q7" s="397" t="n">
         <v>6</v>
       </c>
       <c r="R7" s="101" t="n">
         <v>8286</v>
       </c>
-      <c r="S7" s="378" t="n">
+      <c r="S7" s="397" t="n">
         <v>6</v>
       </c>
       <c r="T7" s="101" t="n">
@@ -1692,15 +1714,15 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="372" t="inlineStr">
+      <c r="A8" s="391" t="inlineStr">
         <is>
           <t>#QUYG0PQC8</t>
         </is>
       </c>
-      <c r="B8" s="372" t="n">
-        <v>854</v>
-      </c>
-      <c r="C8" s="373" t="n">
+      <c r="B8" s="391" t="n">
+        <v>830</v>
+      </c>
+      <c r="C8" s="392" t="n">
         <v>5</v>
       </c>
       <c r="D8" s="95" t="inlineStr">
@@ -1708,49 +1730,49 @@
           <t>Luffy</t>
         </is>
       </c>
-      <c r="E8" s="374" t="n">
+      <c r="E8" s="393" t="n">
         <v>6</v>
       </c>
       <c r="F8" s="95" t="n">
         <v>12820</v>
       </c>
-      <c r="G8" s="375" t="n">
+      <c r="G8" s="394" t="n">
         <v>0</v>
       </c>
       <c r="H8" s="98" t="n">
         <v>0</v>
       </c>
-      <c r="I8" s="374" t="n">
+      <c r="I8" s="393" t="n">
         <v>6</v>
       </c>
       <c r="J8" s="95" t="n">
         <v>11357</v>
       </c>
-      <c r="K8" s="374" t="n">
+      <c r="K8" s="393" t="n">
         <v>6</v>
       </c>
       <c r="L8" s="95" t="n">
         <v>10879</v>
       </c>
-      <c r="M8" s="374" t="n">
+      <c r="M8" s="393" t="n">
         <v>6</v>
       </c>
       <c r="N8" s="95" t="n">
         <v>9114</v>
       </c>
-      <c r="O8" s="374" t="n">
+      <c r="O8" s="393" t="n">
         <v>6</v>
       </c>
       <c r="P8" s="95" t="n">
         <v>13385</v>
       </c>
-      <c r="Q8" s="374" t="n">
+      <c r="Q8" s="393" t="n">
         <v>6</v>
       </c>
       <c r="R8" s="95" t="n">
         <v>7877</v>
       </c>
-      <c r="S8" s="374" t="n">
+      <c r="S8" s="393" t="n">
         <v>6</v>
       </c>
       <c r="T8" s="95" t="n">
@@ -1758,15 +1780,15 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="381" t="inlineStr">
+      <c r="A9" s="400" t="inlineStr">
         <is>
           <t>#LPCLQUCCY</t>
         </is>
       </c>
-      <c r="B9" s="381" t="n">
-        <v>1024</v>
-      </c>
-      <c r="C9" s="377" t="n">
+      <c r="B9" s="400" t="n">
+        <v>1003</v>
+      </c>
+      <c r="C9" s="396" t="n">
         <v>6</v>
       </c>
       <c r="D9" s="106" t="inlineStr">
@@ -1774,49 +1796,49 @@
           <t>Zodiac</t>
         </is>
       </c>
-      <c r="E9" s="382" t="n">
+      <c r="E9" s="401" t="n">
         <v>6</v>
       </c>
       <c r="F9" s="106" t="n">
         <v>12035</v>
       </c>
-      <c r="G9" s="383" t="n">
+      <c r="G9" s="402" t="n">
         <v>0</v>
       </c>
       <c r="H9" s="109" t="n">
         <v>0</v>
       </c>
-      <c r="I9" s="382" t="n">
+      <c r="I9" s="401" t="n">
         <v>6</v>
       </c>
       <c r="J9" s="106" t="n">
         <v>7463</v>
       </c>
-      <c r="K9" s="383" t="n">
+      <c r="K9" s="402" t="n">
         <v>0</v>
       </c>
       <c r="L9" s="110" t="n">
         <v>0</v>
       </c>
-      <c r="M9" s="381" t="n"/>
+      <c r="M9" s="400" t="n"/>
       <c r="N9" s="109" t="n"/>
-      <c r="O9" s="381" t="n"/>
+      <c r="O9" s="400" t="n"/>
       <c r="P9" s="109" t="n"/>
-      <c r="Q9" s="381" t="n"/>
+      <c r="Q9" s="400" t="n"/>
       <c r="R9" s="109" t="n"/>
-      <c r="S9" s="381" t="n"/>
+      <c r="S9" s="400" t="n"/>
       <c r="T9" s="109" t="n"/>
     </row>
     <row r="10">
-      <c r="A10" s="372" t="inlineStr">
+      <c r="A10" s="391" t="inlineStr">
         <is>
           <t>#QUV2GP88U</t>
         </is>
       </c>
-      <c r="B10" s="372" t="n">
-        <v>777</v>
-      </c>
-      <c r="C10" s="373" t="n">
+      <c r="B10" s="391" t="n">
+        <v>800</v>
+      </c>
+      <c r="C10" s="392" t="n">
         <v>7</v>
       </c>
       <c r="D10" s="95" t="inlineStr">
@@ -1824,49 +1846,49 @@
           <t>Nico Robin</t>
         </is>
       </c>
-      <c r="E10" s="374" t="n">
+      <c r="E10" s="393" t="n">
         <v>6</v>
       </c>
       <c r="F10" s="95" t="n">
         <v>11670</v>
       </c>
-      <c r="G10" s="375" t="n">
+      <c r="G10" s="394" t="n">
         <v>0</v>
       </c>
       <c r="H10" s="98" t="n">
         <v>0</v>
       </c>
-      <c r="I10" s="374" t="n">
+      <c r="I10" s="393" t="n">
         <v>6</v>
       </c>
       <c r="J10" s="95" t="n">
         <v>10389</v>
       </c>
-      <c r="K10" s="374" t="n">
+      <c r="K10" s="393" t="n">
         <v>6</v>
       </c>
       <c r="L10" s="95" t="n">
         <v>12612</v>
       </c>
-      <c r="M10" s="374" t="n">
+      <c r="M10" s="393" t="n">
         <v>6</v>
       </c>
       <c r="N10" s="95" t="n">
         <v>11338</v>
       </c>
-      <c r="O10" s="374" t="n">
+      <c r="O10" s="393" t="n">
         <v>6</v>
       </c>
       <c r="P10" s="95" t="n">
         <v>10997</v>
       </c>
-      <c r="Q10" s="374" t="n">
+      <c r="Q10" s="393" t="n">
         <v>6</v>
       </c>
       <c r="R10" s="95" t="n">
         <v>11087</v>
       </c>
-      <c r="S10" s="374" t="n">
+      <c r="S10" s="393" t="n">
         <v>6</v>
       </c>
       <c r="T10" s="95" t="n">
@@ -1874,15 +1896,15 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="376" t="inlineStr">
+      <c r="A11" s="395" t="inlineStr">
         <is>
           <t>#QCV22VP0G</t>
         </is>
       </c>
-      <c r="B11" s="376" t="n">
+      <c r="B11" s="395" t="n">
         <v>774</v>
       </c>
-      <c r="C11" s="377" t="n">
+      <c r="C11" s="396" t="n">
         <v>8</v>
       </c>
       <c r="D11" s="101" t="inlineStr">
@@ -1890,49 +1912,49 @@
           <t>Nami</t>
         </is>
       </c>
-      <c r="E11" s="378" t="n">
+      <c r="E11" s="397" t="n">
         <v>6</v>
       </c>
       <c r="F11" s="101" t="n">
         <v>11484</v>
       </c>
-      <c r="G11" s="379" t="n">
+      <c r="G11" s="398" t="n">
         <v>0</v>
       </c>
       <c r="H11" s="104" t="n">
         <v>0</v>
       </c>
-      <c r="I11" s="378" t="n">
+      <c r="I11" s="397" t="n">
         <v>6</v>
       </c>
       <c r="J11" s="101" t="n">
         <v>11657</v>
       </c>
-      <c r="K11" s="378" t="n">
+      <c r="K11" s="397" t="n">
         <v>6</v>
       </c>
       <c r="L11" s="101" t="n">
         <v>11795</v>
       </c>
-      <c r="M11" s="378" t="n">
+      <c r="M11" s="397" t="n">
         <v>6</v>
       </c>
       <c r="N11" s="101" t="n">
         <v>10769</v>
       </c>
-      <c r="O11" s="378" t="n">
+      <c r="O11" s="397" t="n">
         <v>6</v>
       </c>
       <c r="P11" s="101" t="n">
         <v>12486</v>
       </c>
-      <c r="Q11" s="378" t="n">
+      <c r="Q11" s="397" t="n">
         <v>6</v>
       </c>
       <c r="R11" s="101" t="n">
         <v>8472</v>
       </c>
-      <c r="S11" s="378" t="n">
+      <c r="S11" s="397" t="n">
         <v>6</v>
       </c>
       <c r="T11" s="101" t="n">
@@ -1940,15 +1962,15 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="372" t="inlineStr">
+      <c r="A12" s="391" t="inlineStr">
         <is>
           <t>#QLR088LC9</t>
         </is>
       </c>
-      <c r="B12" s="372" t="n">
-        <v>814</v>
-      </c>
-      <c r="C12" s="373" t="n">
+      <c r="B12" s="391" t="n">
+        <v>799</v>
+      </c>
+      <c r="C12" s="392" t="n">
         <v>9</v>
       </c>
       <c r="D12" s="95" t="inlineStr">
@@ -1956,49 +1978,49 @@
           <t>Sanji</t>
         </is>
       </c>
-      <c r="E12" s="374" t="n">
+      <c r="E12" s="393" t="n">
         <v>6</v>
       </c>
       <c r="F12" s="95" t="n">
         <v>11473</v>
       </c>
-      <c r="G12" s="375" t="n">
+      <c r="G12" s="394" t="n">
         <v>0</v>
       </c>
       <c r="H12" s="98" t="n">
         <v>0</v>
       </c>
-      <c r="I12" s="374" t="n">
+      <c r="I12" s="393" t="n">
         <v>6</v>
       </c>
       <c r="J12" s="95" t="n">
         <v>11960</v>
       </c>
-      <c r="K12" s="374" t="n">
+      <c r="K12" s="393" t="n">
         <v>6</v>
       </c>
       <c r="L12" s="95" t="n">
         <v>10910</v>
       </c>
-      <c r="M12" s="374" t="n">
+      <c r="M12" s="393" t="n">
         <v>6</v>
       </c>
       <c r="N12" s="95" t="n">
         <v>9550</v>
       </c>
-      <c r="O12" s="374" t="n">
+      <c r="O12" s="393" t="n">
         <v>6</v>
       </c>
       <c r="P12" s="95" t="n">
         <v>9138</v>
       </c>
-      <c r="Q12" s="374" t="n">
+      <c r="Q12" s="393" t="n">
         <v>6</v>
       </c>
       <c r="R12" s="95" t="n">
         <v>8897</v>
       </c>
-      <c r="S12" s="374" t="n">
+      <c r="S12" s="393" t="n">
         <v>6</v>
       </c>
       <c r="T12" s="95" t="n">
@@ -2006,15 +2028,15 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="376" t="inlineStr">
+      <c r="A13" s="395" t="inlineStr">
         <is>
           <t>#QLJ2U20Y2</t>
         </is>
       </c>
-      <c r="B13" s="376" t="n">
-        <v>1484</v>
-      </c>
-      <c r="C13" s="377" t="n">
+      <c r="B13" s="395" t="n">
+        <v>1461</v>
+      </c>
+      <c r="C13" s="396" t="n">
         <v>10</v>
       </c>
       <c r="D13" s="101" t="inlineStr">
@@ -2022,49 +2044,49 @@
           <t>DeadLeaf</t>
         </is>
       </c>
-      <c r="E13" s="378" t="n">
+      <c r="E13" s="397" t="n">
         <v>6</v>
       </c>
       <c r="F13" s="101" t="n">
         <v>11433</v>
       </c>
-      <c r="G13" s="379" t="n">
+      <c r="G13" s="398" t="n">
         <v>0</v>
       </c>
       <c r="H13" s="104" t="n">
         <v>0</v>
       </c>
-      <c r="I13" s="378" t="n">
+      <c r="I13" s="397" t="n">
         <v>6</v>
       </c>
       <c r="J13" s="101" t="n">
         <v>12676</v>
       </c>
-      <c r="K13" s="378" t="n">
+      <c r="K13" s="397" t="n">
         <v>6</v>
       </c>
       <c r="L13" s="101" t="n">
         <v>13763</v>
       </c>
-      <c r="M13" s="378" t="n">
+      <c r="M13" s="397" t="n">
         <v>6</v>
       </c>
       <c r="N13" s="101" t="n">
         <v>11140</v>
       </c>
-      <c r="O13" s="378" t="n">
+      <c r="O13" s="397" t="n">
         <v>6</v>
       </c>
       <c r="P13" s="101" t="n">
         <v>15509</v>
       </c>
-      <c r="Q13" s="378" t="n">
+      <c r="Q13" s="397" t="n">
         <v>6</v>
       </c>
       <c r="R13" s="101" t="n">
         <v>8567</v>
       </c>
-      <c r="S13" s="378" t="n">
+      <c r="S13" s="397" t="n">
         <v>6</v>
       </c>
       <c r="T13" s="101" t="n">
@@ -2072,15 +2094,15 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="372" t="inlineStr">
+      <c r="A14" s="391" t="inlineStr">
         <is>
           <t>#Q8CLCUCC2</t>
         </is>
       </c>
-      <c r="B14" s="372" t="n">
-        <v>1409</v>
-      </c>
-      <c r="C14" s="373" t="n">
+      <c r="B14" s="391" t="n">
+        <v>1431</v>
+      </c>
+      <c r="C14" s="392" t="n">
         <v>11</v>
       </c>
       <c r="D14" s="95" t="inlineStr">
@@ -2088,49 +2110,49 @@
           <t>Moxxi</t>
         </is>
       </c>
-      <c r="E14" s="374" t="n">
+      <c r="E14" s="393" t="n">
         <v>6</v>
       </c>
       <c r="F14" s="95" t="n">
         <v>10777</v>
       </c>
-      <c r="G14" s="375" t="n">
+      <c r="G14" s="394" t="n">
         <v>0</v>
       </c>
       <c r="H14" s="98" t="n">
         <v>0</v>
       </c>
-      <c r="I14" s="374" t="n">
+      <c r="I14" s="393" t="n">
         <v>6</v>
       </c>
       <c r="J14" s="95" t="n">
         <v>12912</v>
       </c>
-      <c r="K14" s="374" t="n">
+      <c r="K14" s="393" t="n">
         <v>6</v>
       </c>
       <c r="L14" s="95" t="n">
         <v>8015</v>
       </c>
-      <c r="M14" s="374" t="n">
+      <c r="M14" s="393" t="n">
         <v>6</v>
       </c>
       <c r="N14" s="95" t="n">
         <v>11010</v>
       </c>
-      <c r="O14" s="374" t="n">
+      <c r="O14" s="393" t="n">
         <v>6</v>
       </c>
       <c r="P14" s="95" t="n">
         <v>13857</v>
       </c>
-      <c r="Q14" s="374" t="n">
+      <c r="Q14" s="393" t="n">
         <v>6</v>
       </c>
       <c r="R14" s="95" t="n">
         <v>7905</v>
       </c>
-      <c r="S14" s="374" t="n">
+      <c r="S14" s="393" t="n">
         <v>6</v>
       </c>
       <c r="T14" s="95" t="n">
@@ -2138,15 +2160,15 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="376" t="inlineStr">
+      <c r="A15" s="395" t="inlineStr">
         <is>
           <t>#QUG8QQJ92</t>
         </is>
       </c>
-      <c r="B15" s="376" t="n">
+      <c r="B15" s="395" t="n">
         <v>894</v>
       </c>
-      <c r="C15" s="377" t="n">
+      <c r="C15" s="396" t="n">
         <v>12</v>
       </c>
       <c r="D15" s="101" t="inlineStr">
@@ -2154,49 +2176,49 @@
           <t>Karma</t>
         </is>
       </c>
-      <c r="E15" s="378" t="n">
+      <c r="E15" s="397" t="n">
         <v>6</v>
       </c>
       <c r="F15" s="101" t="n">
         <v>10105</v>
       </c>
-      <c r="G15" s="379" t="n">
+      <c r="G15" s="398" t="n">
         <v>0</v>
       </c>
       <c r="H15" s="104" t="n">
         <v>0</v>
       </c>
-      <c r="I15" s="378" t="n">
+      <c r="I15" s="397" t="n">
         <v>6</v>
       </c>
       <c r="J15" s="101" t="n">
         <v>12204</v>
       </c>
-      <c r="K15" s="378" t="n">
+      <c r="K15" s="397" t="n">
         <v>6</v>
       </c>
       <c r="L15" s="101" t="n">
         <v>11355</v>
       </c>
-      <c r="M15" s="378" t="n">
+      <c r="M15" s="397" t="n">
         <v>6</v>
       </c>
       <c r="N15" s="101" t="n">
         <v>10003</v>
       </c>
-      <c r="O15" s="378" t="n">
+      <c r="O15" s="397" t="n">
         <v>6</v>
       </c>
       <c r="P15" s="101" t="n">
         <v>10595</v>
       </c>
-      <c r="Q15" s="378" t="n">
+      <c r="Q15" s="397" t="n">
         <v>6</v>
       </c>
       <c r="R15" s="101" t="n">
         <v>9240</v>
       </c>
-      <c r="S15" s="378" t="n">
+      <c r="S15" s="397" t="n">
         <v>6</v>
       </c>
       <c r="T15" s="101" t="n">
@@ -2204,15 +2226,15 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="384" t="inlineStr">
+      <c r="A16" s="403" t="inlineStr">
         <is>
           <t>#QUGYGY88C</t>
         </is>
       </c>
-      <c r="B16" s="384" t="n">
-        <v>971</v>
-      </c>
-      <c r="C16" s="373" t="n">
+      <c r="B16" s="403" t="n">
+        <v>960</v>
+      </c>
+      <c r="C16" s="392" t="n">
         <v>13</v>
       </c>
       <c r="D16" s="112" t="inlineStr">
@@ -2220,49 +2242,49 @@
           <t>Kingsman</t>
         </is>
       </c>
-      <c r="E16" s="385" t="n">
+      <c r="E16" s="404" t="n">
         <v>6</v>
       </c>
       <c r="F16" s="112" t="n">
         <v>9948</v>
       </c>
-      <c r="G16" s="386" t="n">
+      <c r="G16" s="405" t="n">
         <v>0</v>
       </c>
       <c r="H16" s="115" t="n">
         <v>0</v>
       </c>
-      <c r="I16" s="386" t="n">
+      <c r="I16" s="405" t="n">
         <v>0</v>
       </c>
       <c r="J16" s="116" t="n">
         <v>0</v>
       </c>
-      <c r="K16" s="386" t="n">
+      <c r="K16" s="405" t="n">
         <v>0</v>
       </c>
       <c r="L16" s="116" t="n">
         <v>0</v>
       </c>
-      <c r="M16" s="384" t="n"/>
+      <c r="M16" s="403" t="n"/>
       <c r="N16" s="115" t="n"/>
-      <c r="O16" s="384" t="n"/>
+      <c r="O16" s="403" t="n"/>
       <c r="P16" s="115" t="n"/>
-      <c r="Q16" s="384" t="n"/>
+      <c r="Q16" s="403" t="n"/>
       <c r="R16" s="115" t="n"/>
-      <c r="S16" s="384" t="n"/>
+      <c r="S16" s="403" t="n"/>
       <c r="T16" s="115" t="n"/>
     </row>
     <row r="17">
-      <c r="A17" s="381" t="inlineStr">
+      <c r="A17" s="400" t="inlineStr">
         <is>
           <t>#98JG2UJQL</t>
         </is>
       </c>
-      <c r="B17" s="381" t="n">
-        <v>3030</v>
-      </c>
-      <c r="C17" s="377" t="n">
+      <c r="B17" s="400" t="n">
+        <v>3023</v>
+      </c>
+      <c r="C17" s="396" t="n">
         <v>14</v>
       </c>
       <c r="D17" s="106" t="inlineStr">
@@ -2270,49 +2292,49 @@
           <t>Dragonux</t>
         </is>
       </c>
-      <c r="E17" s="382" t="n">
+      <c r="E17" s="401" t="n">
         <v>6</v>
       </c>
       <c r="F17" s="106" t="n">
         <v>8745</v>
       </c>
-      <c r="G17" s="383" t="n">
+      <c r="G17" s="402" t="n">
         <v>0</v>
       </c>
       <c r="H17" s="109" t="n">
         <v>0</v>
       </c>
-      <c r="I17" s="382" t="n">
+      <c r="I17" s="401" t="n">
         <v>6</v>
       </c>
       <c r="J17" s="106" t="n">
         <v>10385</v>
       </c>
-      <c r="K17" s="382" t="n">
+      <c r="K17" s="401" t="n">
         <v>6</v>
       </c>
       <c r="L17" s="106" t="n">
         <v>10910</v>
       </c>
-      <c r="M17" s="382" t="n">
+      <c r="M17" s="401" t="n">
         <v>6</v>
       </c>
       <c r="N17" s="106" t="n">
         <v>8750</v>
       </c>
-      <c r="O17" s="382" t="n">
+      <c r="O17" s="401" t="n">
         <v>6</v>
       </c>
       <c r="P17" s="106" t="n">
         <v>10865</v>
       </c>
-      <c r="Q17" s="382" t="n">
+      <c r="Q17" s="401" t="n">
         <v>6</v>
       </c>
       <c r="R17" s="106" t="n">
         <v>8025</v>
       </c>
-      <c r="S17" s="382" t="n">
+      <c r="S17" s="401" t="n">
         <v>6</v>
       </c>
       <c r="T17" s="106" t="n">
@@ -2320,15 +2342,15 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="384" t="inlineStr">
+      <c r="A18" s="403" t="inlineStr">
         <is>
           <t>#G0JPUQGYR</t>
         </is>
       </c>
-      <c r="B18" s="384" t="n">
-        <v>1540</v>
-      </c>
-      <c r="C18" s="373" t="n">
+      <c r="B18" s="403" t="n">
+        <v>1589</v>
+      </c>
+      <c r="C18" s="392" t="n">
         <v>15</v>
       </c>
       <c r="D18" s="112" t="inlineStr">
@@ -2336,49 +2358,49 @@
           <t>Collin</t>
         </is>
       </c>
-      <c r="E18" s="385" t="n">
+      <c r="E18" s="404" t="n">
         <v>6</v>
       </c>
       <c r="F18" s="112" t="n">
         <v>8725</v>
       </c>
-      <c r="G18" s="386" t="n">
+      <c r="G18" s="405" t="n">
         <v>0</v>
       </c>
       <c r="H18" s="115" t="n">
         <v>0</v>
       </c>
-      <c r="I18" s="385" t="n">
+      <c r="I18" s="404" t="n">
         <v>6</v>
       </c>
       <c r="J18" s="112" t="n">
         <v>10299</v>
       </c>
-      <c r="K18" s="385" t="n">
+      <c r="K18" s="404" t="n">
         <v>6</v>
       </c>
       <c r="L18" s="112" t="n">
         <v>8833</v>
       </c>
-      <c r="M18" s="385" t="n">
+      <c r="M18" s="404" t="n">
         <v>6</v>
       </c>
       <c r="N18" s="112" t="n">
         <v>9238</v>
       </c>
-      <c r="O18" s="385" t="n">
+      <c r="O18" s="404" t="n">
         <v>6</v>
       </c>
       <c r="P18" s="112" t="n">
         <v>7756</v>
       </c>
-      <c r="Q18" s="385" t="n">
+      <c r="Q18" s="404" t="n">
         <v>6</v>
       </c>
       <c r="R18" s="117" t="n">
         <v>5943</v>
       </c>
-      <c r="S18" s="385" t="n">
+      <c r="S18" s="404" t="n">
         <v>6</v>
       </c>
       <c r="T18" s="112" t="n">
@@ -2386,15 +2408,15 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="381" t="inlineStr">
+      <c r="A19" s="400" t="inlineStr">
         <is>
           <t>#8U9CRC8G</t>
         </is>
       </c>
-      <c r="B19" s="381" t="n">
+      <c r="B19" s="400" t="n">
         <v>1773</v>
       </c>
-      <c r="C19" s="377" t="n">
+      <c r="C19" s="396" t="n">
         <v>16</v>
       </c>
       <c r="D19" s="106" t="inlineStr">
@@ -2402,49 +2424,49 @@
           <t>CEO JACK</t>
         </is>
       </c>
-      <c r="E19" s="382" t="n">
+      <c r="E19" s="401" t="n">
         <v>6</v>
       </c>
       <c r="F19" s="106" t="n">
         <v>8657</v>
       </c>
-      <c r="G19" s="387" t="n">
+      <c r="G19" s="406" t="n">
         <v>16</v>
       </c>
       <c r="H19" s="109" t="n">
         <v>132</v>
       </c>
-      <c r="I19" s="382" t="n">
+      <c r="I19" s="401" t="n">
         <v>6</v>
       </c>
       <c r="J19" s="106" t="n">
         <v>6980</v>
       </c>
-      <c r="K19" s="383" t="n">
+      <c r="K19" s="402" t="n">
         <v>0</v>
       </c>
       <c r="L19" s="110" t="n">
         <v>0</v>
       </c>
-      <c r="M19" s="381" t="n"/>
+      <c r="M19" s="400" t="n"/>
       <c r="N19" s="109" t="n"/>
-      <c r="O19" s="381" t="n"/>
+      <c r="O19" s="400" t="n"/>
       <c r="P19" s="109" t="n"/>
-      <c r="Q19" s="381" t="n"/>
+      <c r="Q19" s="400" t="n"/>
       <c r="R19" s="109" t="n"/>
-      <c r="S19" s="381" t="n"/>
+      <c r="S19" s="400" t="n"/>
       <c r="T19" s="109" t="n"/>
     </row>
     <row r="20">
-      <c r="A20" s="384" t="inlineStr">
+      <c r="A20" s="403" t="inlineStr">
         <is>
           <t>#LLQQ8CGPV</t>
         </is>
       </c>
-      <c r="B20" s="384" t="n">
-        <v>1405</v>
-      </c>
-      <c r="C20" s="373" t="n">
+      <c r="B20" s="403" t="n">
+        <v>1427</v>
+      </c>
+      <c r="C20" s="392" t="n">
         <v>17</v>
       </c>
       <c r="D20" s="112" t="inlineStr">
@@ -2452,41 +2474,41 @@
           <t>jojomoonky</t>
         </is>
       </c>
-      <c r="E20" s="385" t="n">
+      <c r="E20" s="404" t="n">
         <v>6</v>
       </c>
       <c r="F20" s="112" t="n">
         <v>8465</v>
       </c>
-      <c r="G20" s="386" t="n">
+      <c r="G20" s="405" t="n">
         <v>0</v>
       </c>
       <c r="H20" s="115" t="n">
         <v>0</v>
       </c>
-      <c r="I20" s="384" t="n"/>
+      <c r="I20" s="403" t="n"/>
       <c r="J20" s="115" t="n"/>
-      <c r="K20" s="384" t="n"/>
+      <c r="K20" s="403" t="n"/>
       <c r="L20" s="115" t="n"/>
-      <c r="M20" s="384" t="n"/>
+      <c r="M20" s="403" t="n"/>
       <c r="N20" s="115" t="n"/>
-      <c r="O20" s="384" t="n"/>
+      <c r="O20" s="403" t="n"/>
       <c r="P20" s="115" t="n"/>
-      <c r="Q20" s="384" t="n"/>
+      <c r="Q20" s="403" t="n"/>
       <c r="R20" s="115" t="n"/>
-      <c r="S20" s="384" t="n"/>
+      <c r="S20" s="403" t="n"/>
       <c r="T20" s="115" t="n"/>
     </row>
     <row r="21">
-      <c r="A21" s="381" t="inlineStr">
+      <c r="A21" s="400" t="inlineStr">
         <is>
           <t>#QRPRYR8LL</t>
         </is>
       </c>
-      <c r="B21" s="381" t="n">
-        <v>1216</v>
-      </c>
-      <c r="C21" s="377" t="n">
+      <c r="B21" s="400" t="n">
+        <v>1201</v>
+      </c>
+      <c r="C21" s="396" t="n">
         <v>18</v>
       </c>
       <c r="D21" s="106" t="inlineStr">
@@ -2494,49 +2516,49 @@
           <t>FidelCashflow</t>
         </is>
       </c>
-      <c r="E21" s="382" t="n">
+      <c r="E21" s="401" t="n">
         <v>6</v>
       </c>
       <c r="F21" s="106" t="n">
         <v>8263</v>
       </c>
-      <c r="G21" s="383" t="n">
+      <c r="G21" s="402" t="n">
         <v>0</v>
       </c>
       <c r="H21" s="109" t="n">
         <v>0</v>
       </c>
-      <c r="I21" s="382" t="n">
+      <c r="I21" s="401" t="n">
         <v>6</v>
       </c>
       <c r="J21" s="106" t="n">
         <v>8298</v>
       </c>
-      <c r="K21" s="382" t="n">
+      <c r="K21" s="401" t="n">
         <v>6</v>
       </c>
       <c r="L21" s="106" t="n">
         <v>6415</v>
       </c>
-      <c r="M21" s="382" t="n">
+      <c r="M21" s="401" t="n">
         <v>6</v>
       </c>
       <c r="N21" s="106" t="n">
         <v>6547</v>
       </c>
-      <c r="O21" s="382" t="n">
+      <c r="O21" s="401" t="n">
         <v>6</v>
       </c>
       <c r="P21" s="106" t="n">
         <v>6811</v>
       </c>
-      <c r="Q21" s="382" t="n">
+      <c r="Q21" s="401" t="n">
         <v>6</v>
       </c>
       <c r="R21" s="118" t="n">
         <v>4239</v>
       </c>
-      <c r="S21" s="382" t="n">
+      <c r="S21" s="401" t="n">
         <v>6</v>
       </c>
       <c r="T21" s="118" t="n">
@@ -2544,15 +2566,15 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="384" t="inlineStr">
+      <c r="A22" s="403" t="inlineStr">
         <is>
           <t>#QLGUYQPL0</t>
         </is>
       </c>
-      <c r="B22" s="384" t="n">
-        <v>1529</v>
-      </c>
-      <c r="C22" s="373" t="n">
+      <c r="B22" s="403" t="n">
+        <v>1521</v>
+      </c>
+      <c r="C22" s="392" t="n">
         <v>19</v>
       </c>
       <c r="D22" s="112" t="inlineStr">
@@ -2560,45 +2582,45 @@
           <t>i got time</t>
         </is>
       </c>
-      <c r="E22" s="385" t="n">
+      <c r="E22" s="404" t="n">
         <v>6</v>
       </c>
       <c r="F22" s="112" t="n">
         <v>8087</v>
       </c>
-      <c r="G22" s="386" t="n">
+      <c r="G22" s="405" t="n">
         <v>0</v>
       </c>
       <c r="H22" s="115" t="n">
         <v>0</v>
       </c>
-      <c r="I22" s="386" t="n">
+      <c r="I22" s="405" t="n">
         <v>1</v>
       </c>
       <c r="J22" s="116" t="n">
         <v>1435</v>
       </c>
-      <c r="K22" s="384" t="n"/>
+      <c r="K22" s="403" t="n"/>
       <c r="L22" s="115" t="n"/>
-      <c r="M22" s="384" t="n"/>
+      <c r="M22" s="403" t="n"/>
       <c r="N22" s="115" t="n"/>
-      <c r="O22" s="384" t="n"/>
+      <c r="O22" s="403" t="n"/>
       <c r="P22" s="115" t="n"/>
-      <c r="Q22" s="384" t="n"/>
+      <c r="Q22" s="403" t="n"/>
       <c r="R22" s="115" t="n"/>
-      <c r="S22" s="384" t="n"/>
+      <c r="S22" s="403" t="n"/>
       <c r="T22" s="115" t="n"/>
     </row>
     <row r="23">
-      <c r="A23" s="381" t="inlineStr">
+      <c r="A23" s="400" t="inlineStr">
         <is>
           <t>#G0LJCVR2P</t>
         </is>
       </c>
-      <c r="B23" s="381" t="n">
-        <v>1188</v>
-      </c>
-      <c r="C23" s="377" t="n">
+      <c r="B23" s="400" t="n">
+        <v>1236</v>
+      </c>
+      <c r="C23" s="396" t="n">
         <v>20</v>
       </c>
       <c r="D23" s="106" t="inlineStr">
@@ -2606,45 +2628,45 @@
           <t>DaddyChill</t>
         </is>
       </c>
-      <c r="E23" s="382" t="n">
+      <c r="E23" s="401" t="n">
         <v>6</v>
       </c>
       <c r="F23" s="106" t="n">
         <v>7874</v>
       </c>
-      <c r="G23" s="383" t="n">
+      <c r="G23" s="402" t="n">
         <v>0</v>
       </c>
       <c r="H23" s="109" t="n">
         <v>0</v>
       </c>
-      <c r="I23" s="383" t="n">
+      <c r="I23" s="402" t="n">
         <v>0</v>
       </c>
       <c r="J23" s="110" t="n">
         <v>0</v>
       </c>
-      <c r="K23" s="381" t="n"/>
+      <c r="K23" s="400" t="n"/>
       <c r="L23" s="109" t="n"/>
-      <c r="M23" s="381" t="n"/>
+      <c r="M23" s="400" t="n"/>
       <c r="N23" s="109" t="n"/>
-      <c r="O23" s="381" t="n"/>
+      <c r="O23" s="400" t="n"/>
       <c r="P23" s="109" t="n"/>
-      <c r="Q23" s="381" t="n"/>
+      <c r="Q23" s="400" t="n"/>
       <c r="R23" s="109" t="n"/>
-      <c r="S23" s="381" t="n"/>
+      <c r="S23" s="400" t="n"/>
       <c r="T23" s="109" t="n"/>
     </row>
     <row r="24">
-      <c r="A24" s="384" t="inlineStr">
+      <c r="A24" s="403" t="inlineStr">
         <is>
           <t>#QU0U2Q99G</t>
         </is>
       </c>
-      <c r="B24" s="384" t="n">
-        <v>1010</v>
-      </c>
-      <c r="C24" s="373" t="n">
+      <c r="B24" s="403" t="n">
+        <v>1014</v>
+      </c>
+      <c r="C24" s="392" t="n">
         <v>21</v>
       </c>
       <c r="D24" s="112" t="inlineStr">
@@ -2652,57 +2674,57 @@
           <t>big coc</t>
         </is>
       </c>
-      <c r="E24" s="385" t="n">
+      <c r="E24" s="404" t="n">
         <v>6</v>
       </c>
       <c r="F24" s="112" t="n">
         <v>7550</v>
       </c>
-      <c r="G24" s="386" t="n">
+      <c r="G24" s="405" t="n">
         <v>0</v>
       </c>
       <c r="H24" s="115" t="n">
         <v>0</v>
       </c>
-      <c r="I24" s="385" t="n">
+      <c r="I24" s="404" t="n">
         <v>6</v>
       </c>
       <c r="J24" s="112" t="n">
         <v>7115</v>
       </c>
-      <c r="K24" s="385" t="n">
+      <c r="K24" s="404" t="n">
         <v>6</v>
       </c>
       <c r="L24" s="112" t="n">
         <v>7420</v>
       </c>
-      <c r="M24" s="385" t="n">
+      <c r="M24" s="404" t="n">
         <v>5</v>
       </c>
       <c r="N24" s="117" t="n">
         <v>5150</v>
       </c>
-      <c r="O24" s="385" t="n">
+      <c r="O24" s="404" t="n">
         <v>6</v>
       </c>
       <c r="P24" s="112" t="n">
         <v>9075</v>
       </c>
-      <c r="Q24" s="384" t="n"/>
+      <c r="Q24" s="403" t="n"/>
       <c r="R24" s="115" t="n"/>
-      <c r="S24" s="384" t="n"/>
+      <c r="S24" s="403" t="n"/>
       <c r="T24" s="115" t="n"/>
     </row>
     <row r="25">
-      <c r="A25" s="381" t="inlineStr">
+      <c r="A25" s="400" t="inlineStr">
         <is>
           <t>#QUVJGC0VQ</t>
         </is>
       </c>
-      <c r="B25" s="381" t="n">
-        <v>1413</v>
-      </c>
-      <c r="C25" s="377" t="n">
+      <c r="B25" s="400" t="n">
+        <v>1403</v>
+      </c>
+      <c r="C25" s="396" t="n">
         <v>22</v>
       </c>
       <c r="D25" s="106" t="inlineStr">
@@ -2710,49 +2732,49 @@
           <t>Cam</t>
         </is>
       </c>
-      <c r="E25" s="382" t="n">
+      <c r="E25" s="401" t="n">
         <v>6</v>
       </c>
       <c r="F25" s="118" t="n">
         <v>5361</v>
       </c>
-      <c r="G25" s="383" t="n">
+      <c r="G25" s="402" t="n">
         <v>0</v>
       </c>
       <c r="H25" s="109" t="n">
         <v>0</v>
       </c>
-      <c r="I25" s="382" t="n">
+      <c r="I25" s="401" t="n">
         <v>6</v>
       </c>
       <c r="J25" s="106" t="n">
         <v>8080</v>
       </c>
-      <c r="K25" s="383" t="n">
+      <c r="K25" s="402" t="n">
         <v>0</v>
       </c>
       <c r="L25" s="110" t="n">
         <v>0</v>
       </c>
-      <c r="M25" s="381" t="n"/>
+      <c r="M25" s="400" t="n"/>
       <c r="N25" s="109" t="n"/>
-      <c r="O25" s="381" t="n"/>
+      <c r="O25" s="400" t="n"/>
       <c r="P25" s="109" t="n"/>
-      <c r="Q25" s="381" t="n"/>
+      <c r="Q25" s="400" t="n"/>
       <c r="R25" s="109" t="n"/>
-      <c r="S25" s="381" t="n"/>
+      <c r="S25" s="400" t="n"/>
       <c r="T25" s="109" t="n"/>
     </row>
     <row r="26">
-      <c r="A26" s="384" t="inlineStr">
+      <c r="A26" s="403" t="inlineStr">
         <is>
           <t>#QJQV82JG0</t>
         </is>
       </c>
-      <c r="B26" s="384" t="n">
+      <c r="B26" s="403" t="n">
         <v>1036</v>
       </c>
-      <c r="C26" s="373" t="n">
+      <c r="C26" s="392" t="n">
         <v>23</v>
       </c>
       <c r="D26" s="112" t="inlineStr">
@@ -2760,45 +2782,45 @@
           <t>The UnknownYT</t>
         </is>
       </c>
-      <c r="E26" s="385" t="n">
+      <c r="E26" s="404" t="n">
         <v>6</v>
       </c>
       <c r="F26" s="117" t="n">
         <v>5005</v>
       </c>
-      <c r="G26" s="386" t="n">
+      <c r="G26" s="405" t="n">
         <v>0</v>
       </c>
       <c r="H26" s="115" t="n">
         <v>0</v>
       </c>
-      <c r="I26" s="386" t="n">
+      <c r="I26" s="405" t="n">
         <v>0</v>
       </c>
       <c r="J26" s="116" t="n">
         <v>0</v>
       </c>
-      <c r="K26" s="384" t="n"/>
+      <c r="K26" s="403" t="n"/>
       <c r="L26" s="115" t="n"/>
-      <c r="M26" s="384" t="n"/>
+      <c r="M26" s="403" t="n"/>
       <c r="N26" s="115" t="n"/>
-      <c r="O26" s="384" t="n"/>
+      <c r="O26" s="403" t="n"/>
       <c r="P26" s="115" t="n"/>
-      <c r="Q26" s="384" t="n"/>
+      <c r="Q26" s="403" t="n"/>
       <c r="R26" s="115" t="n"/>
-      <c r="S26" s="384" t="n"/>
+      <c r="S26" s="403" t="n"/>
       <c r="T26" s="115" t="n"/>
     </row>
     <row r="27">
-      <c r="A27" s="381" t="inlineStr">
+      <c r="A27" s="400" t="inlineStr">
         <is>
           <t>#LC9GUPJJG</t>
         </is>
       </c>
-      <c r="B27" s="381" t="n">
-        <v>1054</v>
-      </c>
-      <c r="C27" s="377" t="n">
+      <c r="B27" s="400" t="n">
+        <v>1032</v>
+      </c>
+      <c r="C27" s="396" t="n">
         <v>24</v>
       </c>
       <c r="D27" s="106" t="inlineStr">
@@ -2806,53 +2828,53 @@
           <t>raptor2222a</t>
         </is>
       </c>
-      <c r="E27" s="382" t="n">
+      <c r="E27" s="401" t="n">
         <v>5</v>
       </c>
       <c r="F27" s="118" t="n">
         <v>4940</v>
       </c>
-      <c r="G27" s="383" t="n">
+      <c r="G27" s="402" t="n">
         <v>0</v>
       </c>
       <c r="H27" s="109" t="n">
         <v>0</v>
       </c>
-      <c r="I27" s="382" t="n">
+      <c r="I27" s="401" t="n">
         <v>6</v>
       </c>
       <c r="J27" s="106" t="n">
         <v>6971</v>
       </c>
-      <c r="K27" s="382" t="n">
+      <c r="K27" s="401" t="n">
         <v>5</v>
       </c>
       <c r="L27" s="118" t="n">
         <v>4350</v>
       </c>
-      <c r="M27" s="383" t="n">
+      <c r="M27" s="402" t="n">
         <v>0</v>
       </c>
       <c r="N27" s="110" t="n">
         <v>0</v>
       </c>
-      <c r="O27" s="381" t="n"/>
+      <c r="O27" s="400" t="n"/>
       <c r="P27" s="109" t="n"/>
-      <c r="Q27" s="381" t="n"/>
+      <c r="Q27" s="400" t="n"/>
       <c r="R27" s="109" t="n"/>
-      <c r="S27" s="381" t="n"/>
+      <c r="S27" s="400" t="n"/>
       <c r="T27" s="109" t="n"/>
     </row>
     <row r="28">
-      <c r="A28" s="384" t="inlineStr">
+      <c r="A28" s="403" t="inlineStr">
         <is>
           <t>#82QLQCJRJ</t>
         </is>
       </c>
-      <c r="B28" s="384" t="n">
+      <c r="B28" s="403" t="n">
         <v>3004</v>
       </c>
-      <c r="C28" s="373" t="n">
+      <c r="C28" s="392" t="n">
         <v>25</v>
       </c>
       <c r="D28" s="117" t="inlineStr">
@@ -2860,49 +2882,49 @@
           <t>Raging Fury</t>
         </is>
       </c>
-      <c r="E28" s="388" t="n">
+      <c r="E28" s="407" t="n">
         <v>4</v>
       </c>
       <c r="F28" s="117" t="n">
         <v>4850</v>
       </c>
-      <c r="G28" s="386" t="n">
+      <c r="G28" s="405" t="n">
         <v>0</v>
       </c>
       <c r="H28" s="115" t="n">
         <v>0</v>
       </c>
-      <c r="I28" s="385" t="n">
+      <c r="I28" s="404" t="n">
         <v>6</v>
       </c>
       <c r="J28" s="112" t="n">
         <v>6145</v>
       </c>
-      <c r="K28" s="385" t="n">
+      <c r="K28" s="404" t="n">
         <v>6</v>
       </c>
       <c r="L28" s="112" t="n">
         <v>8055</v>
       </c>
-      <c r="M28" s="385" t="n">
+      <c r="M28" s="404" t="n">
         <v>6</v>
       </c>
       <c r="N28" s="112" t="n">
         <v>7115</v>
       </c>
-      <c r="O28" s="386" t="n">
+      <c r="O28" s="405" t="n">
         <v>2</v>
       </c>
       <c r="P28" s="116" t="n">
         <v>2320</v>
       </c>
-      <c r="Q28" s="385" t="n">
+      <c r="Q28" s="404" t="n">
         <v>6</v>
       </c>
       <c r="R28" s="117" t="n">
         <v>4920</v>
       </c>
-      <c r="S28" s="385" t="n">
+      <c r="S28" s="404" t="n">
         <v>6</v>
       </c>
       <c r="T28" s="117" t="n">
@@ -2916,7 +2938,7 @@
         </is>
       </c>
       <c r="B29" s="120" t="n">
-        <v>977</v>
+        <v>962</v>
       </c>
       <c r="C29" s="121" t="n">
         <v>26</v>
@@ -2952,15 +2974,15 @@
       <c r="T29" s="124" t="n"/>
     </row>
     <row r="30">
-      <c r="A30" s="384" t="inlineStr">
+      <c r="A30" s="403" t="inlineStr">
         <is>
           <t>#G288QGVQ2</t>
         </is>
       </c>
-      <c r="B30" s="384" t="n">
+      <c r="B30" s="403" t="n">
         <v>909</v>
       </c>
-      <c r="C30" s="373" t="n">
+      <c r="C30" s="392" t="n">
         <v>27</v>
       </c>
       <c r="D30" s="116" t="inlineStr">
@@ -2968,41 +2990,41 @@
           <t>Sehaj123</t>
         </is>
       </c>
-      <c r="E30" s="386" t="n">
+      <c r="E30" s="405" t="n">
         <v>0</v>
       </c>
       <c r="F30" s="116" t="n">
         <v>0</v>
       </c>
-      <c r="G30" s="388" t="n">
+      <c r="G30" s="407" t="n">
         <v>21</v>
       </c>
       <c r="H30" s="115" t="n">
         <v>0</v>
       </c>
-      <c r="I30" s="384" t="n"/>
+      <c r="I30" s="403" t="n"/>
       <c r="J30" s="115" t="n"/>
-      <c r="K30" s="384" t="n"/>
+      <c r="K30" s="403" t="n"/>
       <c r="L30" s="115" t="n"/>
-      <c r="M30" s="384" t="n"/>
+      <c r="M30" s="403" t="n"/>
       <c r="N30" s="115" t="n"/>
-      <c r="O30" s="384" t="n"/>
+      <c r="O30" s="403" t="n"/>
       <c r="P30" s="115" t="n"/>
-      <c r="Q30" s="384" t="n"/>
+      <c r="Q30" s="403" t="n"/>
       <c r="R30" s="115" t="n"/>
-      <c r="S30" s="384" t="n"/>
+      <c r="S30" s="403" t="n"/>
       <c r="T30" s="115" t="n"/>
     </row>
     <row r="31">
-      <c r="A31" s="381" t="inlineStr">
+      <c r="A31" s="400" t="inlineStr">
         <is>
           <t>#QRUQQUPLV</t>
         </is>
       </c>
-      <c r="B31" s="381" t="n">
+      <c r="B31" s="400" t="n">
         <v>906</v>
       </c>
-      <c r="C31" s="377" t="n">
+      <c r="C31" s="396" t="n">
         <v>28</v>
       </c>
       <c r="D31" s="110" t="inlineStr">
@@ -3010,41 +3032,41 @@
           <t>datka/56</t>
         </is>
       </c>
-      <c r="E31" s="383" t="n">
+      <c r="E31" s="402" t="n">
         <v>0</v>
       </c>
       <c r="F31" s="110" t="n">
         <v>0</v>
       </c>
-      <c r="G31" s="383" t="n">
+      <c r="G31" s="402" t="n">
         <v>0</v>
       </c>
       <c r="H31" s="109" t="n">
         <v>0</v>
       </c>
-      <c r="I31" s="381" t="n"/>
+      <c r="I31" s="400" t="n"/>
       <c r="J31" s="109" t="n"/>
-      <c r="K31" s="381" t="n"/>
+      <c r="K31" s="400" t="n"/>
       <c r="L31" s="109" t="n"/>
-      <c r="M31" s="381" t="n"/>
+      <c r="M31" s="400" t="n"/>
       <c r="N31" s="109" t="n"/>
-      <c r="O31" s="381" t="n"/>
+      <c r="O31" s="400" t="n"/>
       <c r="P31" s="109" t="n"/>
-      <c r="Q31" s="381" t="n"/>
+      <c r="Q31" s="400" t="n"/>
       <c r="R31" s="109" t="n"/>
-      <c r="S31" s="381" t="n"/>
+      <c r="S31" s="400" t="n"/>
       <c r="T31" s="109" t="n"/>
     </row>
     <row r="32">
-      <c r="A32" s="384" t="inlineStr">
+      <c r="A32" s="403" t="inlineStr">
         <is>
           <t>#LGCVY0L9P</t>
         </is>
       </c>
-      <c r="B32" s="384" t="n">
+      <c r="B32" s="403" t="n">
         <v>873</v>
       </c>
-      <c r="C32" s="373" t="n">
+      <c r="C32" s="392" t="n">
         <v>29</v>
       </c>
       <c r="D32" s="116" t="inlineStr">
@@ -3052,45 +3074,45 @@
           <t>Death1wolf</t>
         </is>
       </c>
-      <c r="E32" s="386" t="n">
+      <c r="E32" s="405" t="n">
         <v>0</v>
       </c>
       <c r="F32" s="116" t="n">
         <v>0</v>
       </c>
-      <c r="G32" s="386" t="n">
+      <c r="G32" s="405" t="n">
         <v>0</v>
       </c>
       <c r="H32" s="115" t="n">
         <v>0</v>
       </c>
-      <c r="I32" s="385" t="n">
+      <c r="I32" s="404" t="n">
         <v>6</v>
       </c>
       <c r="J32" s="112" t="n">
         <v>7998</v>
       </c>
-      <c r="K32" s="384" t="n"/>
+      <c r="K32" s="403" t="n"/>
       <c r="L32" s="115" t="n"/>
-      <c r="M32" s="384" t="n"/>
+      <c r="M32" s="403" t="n"/>
       <c r="N32" s="115" t="n"/>
-      <c r="O32" s="384" t="n"/>
+      <c r="O32" s="403" t="n"/>
       <c r="P32" s="115" t="n"/>
-      <c r="Q32" s="384" t="n"/>
+      <c r="Q32" s="403" t="n"/>
       <c r="R32" s="115" t="n"/>
-      <c r="S32" s="384" t="n"/>
+      <c r="S32" s="403" t="n"/>
       <c r="T32" s="115" t="n"/>
     </row>
     <row r="33">
-      <c r="A33" s="381" t="inlineStr">
+      <c r="A33" s="400" t="inlineStr">
         <is>
           <t>#Q9QUUVQ02</t>
         </is>
       </c>
-      <c r="B33" s="381" t="n">
-        <v>1438</v>
-      </c>
-      <c r="C33" s="377" t="n">
+      <c r="B33" s="400" t="n">
+        <v>1428</v>
+      </c>
+      <c r="C33" s="396" t="n">
         <v>30</v>
       </c>
       <c r="D33" s="110" t="inlineStr">
@@ -3098,45 +3120,45 @@
           <t>zach</t>
         </is>
       </c>
-      <c r="E33" s="383" t="n">
+      <c r="E33" s="402" t="n">
         <v>0</v>
       </c>
       <c r="F33" s="110" t="n">
         <v>0</v>
       </c>
-      <c r="G33" s="383" t="n">
+      <c r="G33" s="402" t="n">
         <v>0</v>
       </c>
       <c r="H33" s="109" t="n">
         <v>0</v>
       </c>
-      <c r="I33" s="382" t="n">
+      <c r="I33" s="401" t="n">
         <v>6</v>
       </c>
       <c r="J33" s="106" t="n">
         <v>6106</v>
       </c>
-      <c r="K33" s="381" t="n"/>
+      <c r="K33" s="400" t="n"/>
       <c r="L33" s="109" t="n"/>
-      <c r="M33" s="381" t="n"/>
+      <c r="M33" s="400" t="n"/>
       <c r="N33" s="109" t="n"/>
-      <c r="O33" s="381" t="n"/>
+      <c r="O33" s="400" t="n"/>
       <c r="P33" s="109" t="n"/>
-      <c r="Q33" s="381" t="n"/>
+      <c r="Q33" s="400" t="n"/>
       <c r="R33" s="109" t="n"/>
-      <c r="S33" s="381" t="n"/>
+      <c r="S33" s="400" t="n"/>
       <c r="T33" s="109" t="n"/>
     </row>
     <row r="34">
-      <c r="A34" s="384" t="inlineStr">
+      <c r="A34" s="403" t="inlineStr">
         <is>
           <t>#VGG9LYL0</t>
         </is>
       </c>
-      <c r="B34" s="384" t="n">
+      <c r="B34" s="403" t="n">
         <v>1035</v>
       </c>
-      <c r="C34" s="373" t="n">
+      <c r="C34" s="392" t="n">
         <v>31</v>
       </c>
       <c r="D34" s="116" t="inlineStr">
@@ -3144,49 +3166,49 @@
           <t>ptripp1048</t>
         </is>
       </c>
-      <c r="E34" s="386" t="n">
+      <c r="E34" s="405" t="n">
         <v>0</v>
       </c>
       <c r="F34" s="116" t="n">
         <v>0</v>
       </c>
-      <c r="G34" s="386" t="n">
+      <c r="G34" s="405" t="n">
         <v>0</v>
       </c>
       <c r="H34" s="115" t="n">
         <v>0</v>
       </c>
-      <c r="I34" s="385" t="n">
+      <c r="I34" s="404" t="n">
         <v>6</v>
       </c>
       <c r="J34" s="112" t="n">
         <v>6023</v>
       </c>
-      <c r="K34" s="386" t="n">
+      <c r="K34" s="405" t="n">
         <v>0</v>
       </c>
       <c r="L34" s="116" t="n">
         <v>0</v>
       </c>
-      <c r="M34" s="384" t="n"/>
+      <c r="M34" s="403" t="n"/>
       <c r="N34" s="115" t="n"/>
-      <c r="O34" s="384" t="n"/>
+      <c r="O34" s="403" t="n"/>
       <c r="P34" s="115" t="n"/>
-      <c r="Q34" s="384" t="n"/>
+      <c r="Q34" s="403" t="n"/>
       <c r="R34" s="115" t="n"/>
-      <c r="S34" s="384" t="n"/>
+      <c r="S34" s="403" t="n"/>
       <c r="T34" s="115" t="n"/>
     </row>
     <row r="35">
-      <c r="A35" s="381" t="inlineStr">
+      <c r="A35" s="400" t="inlineStr">
         <is>
           <t>#QLG0VJG2J</t>
         </is>
       </c>
-      <c r="B35" s="381" t="n">
-        <v>1463</v>
-      </c>
-      <c r="C35" s="377" t="n">
+      <c r="B35" s="400" t="n">
+        <v>1444</v>
+      </c>
+      <c r="C35" s="396" t="n">
         <v>32</v>
       </c>
       <c r="D35" s="110" t="inlineStr">
@@ -3194,53 +3216,53 @@
           <t>PocketRocket</t>
         </is>
       </c>
-      <c r="E35" s="383" t="n">
+      <c r="E35" s="402" t="n">
         <v>0</v>
       </c>
       <c r="F35" s="110" t="n">
         <v>0</v>
       </c>
-      <c r="G35" s="383" t="n">
+      <c r="G35" s="402" t="n">
         <v>0</v>
       </c>
       <c r="H35" s="109" t="n">
         <v>0</v>
       </c>
-      <c r="I35" s="382" t="n">
+      <c r="I35" s="401" t="n">
         <v>6</v>
       </c>
       <c r="J35" s="118" t="n">
         <v>5660</v>
       </c>
-      <c r="K35" s="387" t="n">
+      <c r="K35" s="406" t="n">
         <v>4</v>
       </c>
       <c r="L35" s="118" t="n">
         <v>4327</v>
       </c>
-      <c r="M35" s="387" t="n">
+      <c r="M35" s="406" t="n">
         <v>4</v>
       </c>
       <c r="N35" s="118" t="n">
         <v>5215</v>
       </c>
-      <c r="O35" s="381" t="n"/>
+      <c r="O35" s="400" t="n"/>
       <c r="P35" s="109" t="n"/>
-      <c r="Q35" s="381" t="n"/>
+      <c r="Q35" s="400" t="n"/>
       <c r="R35" s="109" t="n"/>
-      <c r="S35" s="381" t="n"/>
+      <c r="S35" s="400" t="n"/>
       <c r="T35" s="109" t="n"/>
     </row>
     <row r="36">
-      <c r="A36" s="384" t="inlineStr">
+      <c r="A36" s="403" t="inlineStr">
         <is>
           <t>#QLUV29GGJ</t>
         </is>
       </c>
-      <c r="B36" s="384" t="n">
-        <v>1040</v>
-      </c>
-      <c r="C36" s="373" t="n">
+      <c r="B36" s="403" t="n">
+        <v>1018</v>
+      </c>
+      <c r="C36" s="392" t="n">
         <v>33</v>
       </c>
       <c r="D36" s="116" t="inlineStr">
@@ -3248,45 +3270,45 @@
           <t>Kukoshibo</t>
         </is>
       </c>
-      <c r="E36" s="386" t="n">
+      <c r="E36" s="405" t="n">
         <v>0</v>
       </c>
       <c r="F36" s="116" t="n">
         <v>0</v>
       </c>
-      <c r="G36" s="386" t="n">
+      <c r="G36" s="405" t="n">
         <v>0</v>
       </c>
       <c r="H36" s="115" t="n">
         <v>0</v>
       </c>
-      <c r="I36" s="386" t="n">
+      <c r="I36" s="405" t="n">
         <v>0</v>
       </c>
       <c r="J36" s="116" t="n">
         <v>0</v>
       </c>
-      <c r="K36" s="384" t="n"/>
+      <c r="K36" s="403" t="n"/>
       <c r="L36" s="115" t="n"/>
-      <c r="M36" s="384" t="n"/>
+      <c r="M36" s="403" t="n"/>
       <c r="N36" s="115" t="n"/>
-      <c r="O36" s="384" t="n"/>
+      <c r="O36" s="403" t="n"/>
       <c r="P36" s="115" t="n"/>
-      <c r="Q36" s="384" t="n"/>
+      <c r="Q36" s="403" t="n"/>
       <c r="R36" s="115" t="n"/>
-      <c r="S36" s="384" t="n"/>
+      <c r="S36" s="403" t="n"/>
       <c r="T36" s="115" t="n"/>
     </row>
     <row r="37">
-      <c r="A37" s="381" t="inlineStr">
+      <c r="A37" s="400" t="inlineStr">
         <is>
           <t>#Q0U0CRCGJ</t>
         </is>
       </c>
-      <c r="B37" s="381" t="n">
-        <v>691</v>
-      </c>
-      <c r="C37" s="377" t="n">
+      <c r="B37" s="400" t="n">
+        <v>680</v>
+      </c>
+      <c r="C37" s="396" t="n">
         <v>34</v>
       </c>
       <c r="D37" s="110" t="inlineStr">
@@ -3294,45 +3316,45 @@
           <t>Sn0wc0ne</t>
         </is>
       </c>
-      <c r="E37" s="383" t="n">
+      <c r="E37" s="402" t="n">
         <v>0</v>
       </c>
       <c r="F37" s="110" t="n">
         <v>0</v>
       </c>
-      <c r="G37" s="383" t="n">
+      <c r="G37" s="402" t="n">
         <v>0</v>
       </c>
       <c r="H37" s="109" t="n">
         <v>0</v>
       </c>
-      <c r="I37" s="383" t="n">
+      <c r="I37" s="402" t="n">
         <v>0</v>
       </c>
       <c r="J37" s="110" t="n">
         <v>0</v>
       </c>
-      <c r="K37" s="381" t="n"/>
+      <c r="K37" s="400" t="n"/>
       <c r="L37" s="109" t="n"/>
-      <c r="M37" s="381" t="n"/>
+      <c r="M37" s="400" t="n"/>
       <c r="N37" s="109" t="n"/>
-      <c r="O37" s="381" t="n"/>
+      <c r="O37" s="400" t="n"/>
       <c r="P37" s="109" t="n"/>
-      <c r="Q37" s="381" t="n"/>
+      <c r="Q37" s="400" t="n"/>
       <c r="R37" s="109" t="n"/>
-      <c r="S37" s="381" t="n"/>
+      <c r="S37" s="400" t="n"/>
       <c r="T37" s="109" t="n"/>
     </row>
     <row r="38">
-      <c r="A38" s="384" t="inlineStr">
+      <c r="A38" s="403" t="inlineStr">
         <is>
           <t>#QY0VGPQGQ</t>
         </is>
       </c>
-      <c r="B38" s="384" t="n">
+      <c r="B38" s="403" t="n">
         <v>613</v>
       </c>
-      <c r="C38" s="373" t="n">
+      <c r="C38" s="392" t="n">
         <v>35</v>
       </c>
       <c r="D38" s="116" t="inlineStr">
@@ -3340,49 +3362,49 @@
           <t>killerjones</t>
         </is>
       </c>
-      <c r="E38" s="386" t="n">
+      <c r="E38" s="405" t="n">
         <v>0</v>
       </c>
       <c r="F38" s="116" t="n">
         <v>0</v>
       </c>
-      <c r="G38" s="386" t="n">
+      <c r="G38" s="405" t="n">
         <v>0</v>
       </c>
       <c r="H38" s="115" t="n">
         <v>0</v>
       </c>
-      <c r="I38" s="386" t="n">
+      <c r="I38" s="405" t="n">
         <v>0</v>
       </c>
       <c r="J38" s="116" t="n">
         <v>0</v>
       </c>
-      <c r="K38" s="385" t="n">
+      <c r="K38" s="404" t="n">
         <v>6</v>
       </c>
       <c r="L38" s="112" t="n">
         <v>6320</v>
       </c>
-      <c r="M38" s="384" t="n"/>
+      <c r="M38" s="403" t="n"/>
       <c r="N38" s="115" t="n"/>
-      <c r="O38" s="384" t="n"/>
+      <c r="O38" s="403" t="n"/>
       <c r="P38" s="115" t="n"/>
-      <c r="Q38" s="384" t="n"/>
+      <c r="Q38" s="403" t="n"/>
       <c r="R38" s="115" t="n"/>
-      <c r="S38" s="384" t="n"/>
+      <c r="S38" s="403" t="n"/>
       <c r="T38" s="115" t="n"/>
     </row>
     <row r="39">
-      <c r="A39" s="381" t="inlineStr">
+      <c r="A39" s="400" t="inlineStr">
         <is>
           <t>#QL8LVLYG8</t>
         </is>
       </c>
-      <c r="B39" s="381" t="n">
-        <v>971</v>
-      </c>
-      <c r="C39" s="377" t="n">
+      <c r="B39" s="400" t="n">
+        <v>955</v>
+      </c>
+      <c r="C39" s="396" t="n">
         <v>36</v>
       </c>
       <c r="D39" s="110" t="inlineStr">
@@ -3390,49 +3412,49 @@
           <t>Some guy</t>
         </is>
       </c>
-      <c r="E39" s="383" t="n">
+      <c r="E39" s="402" t="n">
         <v>0</v>
       </c>
       <c r="F39" s="110" t="n">
         <v>0</v>
       </c>
-      <c r="G39" s="383" t="n">
+      <c r="G39" s="402" t="n">
         <v>0</v>
       </c>
       <c r="H39" s="109" t="n">
         <v>0</v>
       </c>
-      <c r="I39" s="383" t="n">
+      <c r="I39" s="402" t="n">
         <v>0</v>
       </c>
       <c r="J39" s="110" t="n">
         <v>0</v>
       </c>
-      <c r="K39" s="383" t="n">
+      <c r="K39" s="402" t="n">
         <v>2</v>
       </c>
       <c r="L39" s="110" t="n">
         <v>2650</v>
       </c>
-      <c r="M39" s="383" t="n">
+      <c r="M39" s="402" t="n">
         <v>0</v>
       </c>
       <c r="N39" s="110" t="n">
         <v>0</v>
       </c>
-      <c r="O39" s="382" t="n">
+      <c r="O39" s="401" t="n">
         <v>6</v>
       </c>
       <c r="P39" s="106" t="n">
         <v>6917</v>
       </c>
-      <c r="Q39" s="383" t="n">
+      <c r="Q39" s="402" t="n">
         <v>0</v>
       </c>
       <c r="R39" s="110" t="n">
         <v>0</v>
       </c>
-      <c r="S39" s="383" t="n">
+      <c r="S39" s="402" t="n">
         <v>2</v>
       </c>
       <c r="T39" s="110" t="n">
@@ -3440,165 +3462,165 @@
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="384" t="inlineStr">
+      <c r="A40" s="403" t="inlineStr">
+        <is>
+          <t>#QQL28Y2UL</t>
+        </is>
+      </c>
+      <c r="B40" s="403" t="n">
+        <v>1085</v>
+      </c>
+      <c r="C40" s="392" t="n">
+        <v>37</v>
+      </c>
+      <c r="D40" s="116" t="inlineStr">
+        <is>
+          <t>SUPoT</t>
+        </is>
+      </c>
+      <c r="E40" s="405" t="n">
+        <v>0</v>
+      </c>
+      <c r="F40" s="116" t="n">
+        <v>0</v>
+      </c>
+      <c r="G40" s="405" t="n">
+        <v>0</v>
+      </c>
+      <c r="H40" s="115" t="n">
+        <v>31</v>
+      </c>
+      <c r="I40" s="405" t="n">
+        <v>0</v>
+      </c>
+      <c r="J40" s="116" t="n">
+        <v>0</v>
+      </c>
+      <c r="K40" s="405" t="n">
+        <v>0</v>
+      </c>
+      <c r="L40" s="116" t="n">
+        <v>0</v>
+      </c>
+      <c r="M40" s="403" t="n"/>
+      <c r="N40" s="115" t="n"/>
+      <c r="O40" s="403" t="n"/>
+      <c r="P40" s="115" t="n"/>
+      <c r="Q40" s="403" t="n"/>
+      <c r="R40" s="115" t="n"/>
+      <c r="S40" s="403" t="n"/>
+      <c r="T40" s="115" t="n"/>
+    </row>
+    <row r="41">
+      <c r="A41" s="400" t="inlineStr">
+        <is>
+          <t>#QV8RY9UC8</t>
+        </is>
+      </c>
+      <c r="B41" s="400" t="n">
+        <v>747</v>
+      </c>
+      <c r="C41" s="396" t="n">
+        <v>38</v>
+      </c>
+      <c r="D41" s="110" t="inlineStr">
+        <is>
+          <t>Apollo</t>
+        </is>
+      </c>
+      <c r="E41" s="402" t="n">
+        <v>0</v>
+      </c>
+      <c r="F41" s="110" t="n">
+        <v>0</v>
+      </c>
+      <c r="G41" s="402" t="n">
+        <v>0</v>
+      </c>
+      <c r="H41" s="109" t="n">
+        <v>0</v>
+      </c>
+      <c r="I41" s="402" t="n">
+        <v>0</v>
+      </c>
+      <c r="J41" s="110" t="n">
+        <v>0</v>
+      </c>
+      <c r="K41" s="402" t="n">
+        <v>0</v>
+      </c>
+      <c r="L41" s="110" t="n">
+        <v>0</v>
+      </c>
+      <c r="M41" s="400" t="n"/>
+      <c r="N41" s="109" t="n"/>
+      <c r="O41" s="400" t="n"/>
+      <c r="P41" s="109" t="n"/>
+      <c r="Q41" s="400" t="n"/>
+      <c r="R41" s="109" t="n"/>
+      <c r="S41" s="400" t="n"/>
+      <c r="T41" s="109" t="n"/>
+    </row>
+    <row r="42">
+      <c r="A42" s="403" t="inlineStr">
         <is>
           <t>#QLGYRVPU0</t>
         </is>
       </c>
-      <c r="B40" s="384" t="n">
-        <v>1198</v>
-      </c>
-      <c r="C40" s="373" t="n">
-        <v>37</v>
-      </c>
-      <c r="D40" s="116" t="inlineStr">
+      <c r="B42" s="403" t="n">
+        <v>1182</v>
+      </c>
+      <c r="C42" s="392" t="n">
+        <v>39</v>
+      </c>
+      <c r="D42" s="116" t="inlineStr">
         <is>
           <t>Black.Boy.</t>
         </is>
       </c>
-      <c r="E40" s="386" t="n">
-        <v>0</v>
-      </c>
-      <c r="F40" s="116" t="n">
-        <v>0</v>
-      </c>
-      <c r="G40" s="386" t="n">
-        <v>0</v>
-      </c>
-      <c r="H40" s="115" t="n">
+      <c r="E42" s="405" t="n">
+        <v>0</v>
+      </c>
+      <c r="F42" s="116" t="n">
+        <v>0</v>
+      </c>
+      <c r="G42" s="405" t="n">
+        <v>0</v>
+      </c>
+      <c r="H42" s="115" t="n">
         <v>15</v>
       </c>
-      <c r="I40" s="386" t="n">
-        <v>0</v>
-      </c>
-      <c r="J40" s="116" t="n">
-        <v>0</v>
-      </c>
-      <c r="K40" s="386" t="n">
-        <v>0</v>
-      </c>
-      <c r="L40" s="116" t="n">
-        <v>0</v>
-      </c>
-      <c r="M40" s="384" t="n"/>
-      <c r="N40" s="115" t="n"/>
-      <c r="O40" s="384" t="n"/>
-      <c r="P40" s="115" t="n"/>
-      <c r="Q40" s="384" t="n"/>
-      <c r="R40" s="115" t="n"/>
-      <c r="S40" s="384" t="n"/>
-      <c r="T40" s="115" t="n"/>
-    </row>
-    <row r="41">
-      <c r="A41" s="381" t="inlineStr">
-        <is>
-          <t>#QV8RY9UC8</t>
-        </is>
-      </c>
-      <c r="B41" s="381" t="n">
-        <v>747</v>
-      </c>
-      <c r="C41" s="377" t="n">
-        <v>38</v>
-      </c>
-      <c r="D41" s="110" t="inlineStr">
-        <is>
-          <t>Apollo</t>
-        </is>
-      </c>
-      <c r="E41" s="383" t="n">
-        <v>0</v>
-      </c>
-      <c r="F41" s="110" t="n">
-        <v>0</v>
-      </c>
-      <c r="G41" s="383" t="n">
-        <v>0</v>
-      </c>
-      <c r="H41" s="109" t="n">
-        <v>0</v>
-      </c>
-      <c r="I41" s="383" t="n">
-        <v>0</v>
-      </c>
-      <c r="J41" s="110" t="n">
-        <v>0</v>
-      </c>
-      <c r="K41" s="383" t="n">
-        <v>0</v>
-      </c>
-      <c r="L41" s="110" t="n">
-        <v>0</v>
-      </c>
-      <c r="M41" s="381" t="n"/>
-      <c r="N41" s="109" t="n"/>
-      <c r="O41" s="381" t="n"/>
-      <c r="P41" s="109" t="n"/>
-      <c r="Q41" s="381" t="n"/>
-      <c r="R41" s="109" t="n"/>
-      <c r="S41" s="381" t="n"/>
-      <c r="T41" s="109" t="n"/>
-    </row>
-    <row r="42">
-      <c r="A42" s="384" t="inlineStr">
-        <is>
-          <t>#QQL28Y2UL</t>
-        </is>
-      </c>
-      <c r="B42" s="384" t="n">
-        <v>1085</v>
-      </c>
-      <c r="C42" s="373" t="n">
-        <v>39</v>
-      </c>
-      <c r="D42" s="116" t="inlineStr">
-        <is>
-          <t>SUPoT</t>
-        </is>
-      </c>
-      <c r="E42" s="386" t="n">
-        <v>0</v>
-      </c>
-      <c r="F42" s="116" t="n">
-        <v>0</v>
-      </c>
-      <c r="G42" s="386" t="n">
-        <v>0</v>
-      </c>
-      <c r="H42" s="115" t="n">
-        <v>31</v>
-      </c>
-      <c r="I42" s="386" t="n">
+      <c r="I42" s="405" t="n">
         <v>0</v>
       </c>
       <c r="J42" s="116" t="n">
         <v>0</v>
       </c>
-      <c r="K42" s="386" t="n">
+      <c r="K42" s="405" t="n">
         <v>0</v>
       </c>
       <c r="L42" s="116" t="n">
         <v>0</v>
       </c>
-      <c r="M42" s="384" t="n"/>
+      <c r="M42" s="403" t="n"/>
       <c r="N42" s="115" t="n"/>
-      <c r="O42" s="384" t="n"/>
+      <c r="O42" s="403" t="n"/>
       <c r="P42" s="115" t="n"/>
-      <c r="Q42" s="384" t="n"/>
+      <c r="Q42" s="403" t="n"/>
       <c r="R42" s="115" t="n"/>
-      <c r="S42" s="384" t="n"/>
+      <c r="S42" s="403" t="n"/>
       <c r="T42" s="115" t="n"/>
     </row>
     <row r="43">
-      <c r="A43" s="381" t="inlineStr">
+      <c r="A43" s="400" t="inlineStr">
         <is>
           <t>#QJC8LQU9U</t>
         </is>
       </c>
-      <c r="B43" s="381" t="n">
+      <c r="B43" s="400" t="n">
         <v>998</v>
       </c>
-      <c r="C43" s="377" t="n">
+      <c r="C43" s="396" t="n">
         <v>40</v>
       </c>
       <c r="D43" s="110" t="inlineStr">
@@ -3606,49 +3628,49 @@
           <t>Master01</t>
         </is>
       </c>
-      <c r="E43" s="383" t="n">
+      <c r="E43" s="402" t="n">
         <v>0</v>
       </c>
       <c r="F43" s="110" t="n">
         <v>0</v>
       </c>
-      <c r="G43" s="383" t="n">
+      <c r="G43" s="402" t="n">
         <v>0</v>
       </c>
       <c r="H43" s="109" t="n">
         <v>0</v>
       </c>
-      <c r="I43" s="383" t="n">
+      <c r="I43" s="402" t="n">
         <v>0</v>
       </c>
       <c r="J43" s="110" t="n">
         <v>0</v>
       </c>
-      <c r="K43" s="383" t="n">
+      <c r="K43" s="402" t="n">
         <v>0</v>
       </c>
       <c r="L43" s="110" t="n">
         <v>0</v>
       </c>
-      <c r="M43" s="383" t="n">
+      <c r="M43" s="402" t="n">
         <v>0</v>
       </c>
       <c r="N43" s="110" t="n">
         <v>0</v>
       </c>
-      <c r="O43" s="382" t="n">
+      <c r="O43" s="401" t="n">
         <v>6</v>
       </c>
       <c r="P43" s="118" t="n">
         <v>5415</v>
       </c>
-      <c r="Q43" s="382" t="n">
+      <c r="Q43" s="401" t="n">
         <v>6</v>
       </c>
       <c r="R43" s="118" t="n">
         <v>4835</v>
       </c>
-      <c r="S43" s="382" t="n">
+      <c r="S43" s="401" t="n">
         <v>5</v>
       </c>
       <c r="T43" s="118" t="n">
@@ -3656,15 +3678,15 @@
       </c>
     </row>
     <row r="44">
-      <c r="A44" s="384" t="inlineStr">
+      <c r="A44" s="403" t="inlineStr">
         <is>
           <t>#QV8JJ0URU</t>
         </is>
       </c>
-      <c r="B44" s="384" t="n">
+      <c r="B44" s="403" t="n">
         <v>741</v>
       </c>
-      <c r="C44" s="373" t="n">
+      <c r="C44" s="392" t="n">
         <v>41</v>
       </c>
       <c r="D44" s="116" t="inlineStr">
@@ -3672,49 +3694,49 @@
           <t>✨Jacob</t>
         </is>
       </c>
-      <c r="E44" s="386" t="n">
+      <c r="E44" s="405" t="n">
         <v>0</v>
       </c>
       <c r="F44" s="116" t="n">
         <v>0</v>
       </c>
-      <c r="G44" s="386" t="n">
+      <c r="G44" s="405" t="n">
         <v>0</v>
       </c>
       <c r="H44" s="115" t="n">
         <v>0</v>
       </c>
-      <c r="I44" s="386" t="n">
+      <c r="I44" s="405" t="n">
         <v>0</v>
       </c>
       <c r="J44" s="116" t="n">
         <v>0</v>
       </c>
-      <c r="K44" s="386" t="n">
+      <c r="K44" s="405" t="n">
         <v>0</v>
       </c>
       <c r="L44" s="116" t="n">
         <v>0</v>
       </c>
-      <c r="M44" s="386" t="n">
+      <c r="M44" s="405" t="n">
         <v>0</v>
       </c>
       <c r="N44" s="116" t="n">
         <v>0</v>
       </c>
-      <c r="O44" s="386" t="n">
+      <c r="O44" s="405" t="n">
         <v>0</v>
       </c>
       <c r="P44" s="116" t="n">
         <v>0</v>
       </c>
-      <c r="Q44" s="385" t="n">
+      <c r="Q44" s="404" t="n">
         <v>6</v>
       </c>
       <c r="R44" s="112" t="n">
         <v>7385</v>
       </c>
-      <c r="S44" s="385" t="n">
+      <c r="S44" s="404" t="n">
         <v>6</v>
       </c>
       <c r="T44" s="112" t="n">
@@ -3722,15 +3744,15 @@
       </c>
     </row>
     <row r="45">
-      <c r="A45" s="381" t="inlineStr">
+      <c r="A45" s="400" t="inlineStr">
         <is>
           <t>#QY8L2GLUR</t>
         </is>
       </c>
-      <c r="B45" s="381" t="n">
+      <c r="B45" s="400" t="n">
         <v>907</v>
       </c>
-      <c r="C45" s="377" t="n">
+      <c r="C45" s="396" t="n">
         <v>42</v>
       </c>
       <c r="D45" s="110" t="inlineStr">
@@ -3738,49 +3760,49 @@
           <t>Huy</t>
         </is>
       </c>
-      <c r="E45" s="383" t="n">
+      <c r="E45" s="402" t="n">
         <v>0</v>
       </c>
       <c r="F45" s="110" t="n">
         <v>0</v>
       </c>
-      <c r="G45" s="383" t="n">
+      <c r="G45" s="402" t="n">
         <v>0</v>
       </c>
       <c r="H45" s="109" t="n">
         <v>0</v>
       </c>
-      <c r="I45" s="383" t="n">
+      <c r="I45" s="402" t="n">
         <v>0</v>
       </c>
       <c r="J45" s="110" t="n">
         <v>0</v>
       </c>
-      <c r="K45" s="383" t="n">
+      <c r="K45" s="402" t="n">
         <v>0</v>
       </c>
       <c r="L45" s="110" t="n">
         <v>0</v>
       </c>
-      <c r="M45" s="383" t="n">
+      <c r="M45" s="402" t="n">
         <v>0</v>
       </c>
       <c r="N45" s="110" t="n">
         <v>0</v>
       </c>
-      <c r="O45" s="383" t="n">
+      <c r="O45" s="402" t="n">
         <v>0</v>
       </c>
       <c r="P45" s="110" t="n">
         <v>0</v>
       </c>
-      <c r="Q45" s="382" t="n">
+      <c r="Q45" s="401" t="n">
         <v>6</v>
       </c>
       <c r="R45" s="106" t="n">
         <v>6995</v>
       </c>
-      <c r="S45" s="382" t="n">
+      <c r="S45" s="401" t="n">
         <v>6</v>
       </c>
       <c r="T45" s="106" t="n">
@@ -3788,15 +3810,15 @@
       </c>
     </row>
     <row r="46">
-      <c r="A46" s="384" t="inlineStr">
+      <c r="A46" s="403" t="inlineStr">
         <is>
           <t>#L2QQL9QVJ</t>
         </is>
       </c>
-      <c r="B46" s="384" t="n">
+      <c r="B46" s="403" t="n">
         <v>1450</v>
       </c>
-      <c r="C46" s="373" t="n">
+      <c r="C46" s="392" t="n">
         <v>43</v>
       </c>
       <c r="D46" s="116" t="inlineStr">
@@ -3804,49 +3826,49 @@
           <t>JustPre10d</t>
         </is>
       </c>
-      <c r="E46" s="386" t="n">
+      <c r="E46" s="405" t="n">
         <v>0</v>
       </c>
       <c r="F46" s="116" t="n">
         <v>0</v>
       </c>
-      <c r="G46" s="386" t="n">
+      <c r="G46" s="405" t="n">
         <v>0</v>
       </c>
       <c r="H46" s="115" t="n">
         <v>0</v>
       </c>
-      <c r="I46" s="386" t="n">
+      <c r="I46" s="405" t="n">
         <v>0</v>
       </c>
       <c r="J46" s="116" t="n">
         <v>0</v>
       </c>
-      <c r="K46" s="386" t="n">
+      <c r="K46" s="405" t="n">
         <v>0</v>
       </c>
       <c r="L46" s="116" t="n">
         <v>0</v>
       </c>
-      <c r="M46" s="386" t="n">
+      <c r="M46" s="405" t="n">
         <v>0</v>
       </c>
       <c r="N46" s="116" t="n">
         <v>0</v>
       </c>
-      <c r="O46" s="386" t="n">
+      <c r="O46" s="405" t="n">
         <v>0</v>
       </c>
       <c r="P46" s="116" t="n">
         <v>0</v>
       </c>
-      <c r="Q46" s="385" t="n">
+      <c r="Q46" s="404" t="n">
         <v>6</v>
       </c>
       <c r="R46" s="112" t="n">
         <v>6655</v>
       </c>
-      <c r="S46" s="385" t="n">
+      <c r="S46" s="404" t="n">
         <v>6</v>
       </c>
       <c r="T46" s="112" t="n">
@@ -3854,15 +3876,15 @@
       </c>
     </row>
     <row r="47">
-      <c r="A47" s="381" t="inlineStr">
+      <c r="A47" s="400" t="inlineStr">
         <is>
           <t>#LPR9RPCY9</t>
         </is>
       </c>
-      <c r="B47" s="381" t="n">
-        <v>980</v>
-      </c>
-      <c r="C47" s="377" t="n">
+      <c r="B47" s="400" t="n">
+        <v>970</v>
+      </c>
+      <c r="C47" s="396" t="n">
         <v>44</v>
       </c>
       <c r="D47" s="110" t="inlineStr">
@@ -3870,49 +3892,49 @@
           <t>sayhuss17</t>
         </is>
       </c>
-      <c r="E47" s="383" t="n">
+      <c r="E47" s="402" t="n">
         <v>0</v>
       </c>
       <c r="F47" s="110" t="n">
         <v>0</v>
       </c>
-      <c r="G47" s="383" t="n">
+      <c r="G47" s="402" t="n">
         <v>0</v>
       </c>
       <c r="H47" s="109" t="n">
         <v>0</v>
       </c>
-      <c r="I47" s="383" t="n">
+      <c r="I47" s="402" t="n">
         <v>0</v>
       </c>
       <c r="J47" s="110" t="n">
         <v>0</v>
       </c>
-      <c r="K47" s="383" t="n">
+      <c r="K47" s="402" t="n">
         <v>0</v>
       </c>
       <c r="L47" s="110" t="n">
         <v>0</v>
       </c>
-      <c r="M47" s="383" t="n">
+      <c r="M47" s="402" t="n">
         <v>0</v>
       </c>
       <c r="N47" s="110" t="n">
         <v>0</v>
       </c>
-      <c r="O47" s="383" t="n">
+      <c r="O47" s="402" t="n">
         <v>0</v>
       </c>
       <c r="P47" s="110" t="n">
         <v>0</v>
       </c>
-      <c r="Q47" s="387" t="n">
+      <c r="Q47" s="406" t="n">
         <v>4</v>
       </c>
       <c r="R47" s="118" t="n">
         <v>4240</v>
       </c>
-      <c r="S47" s="381" t="n"/>
+      <c r="S47" s="400" t="n"/>
       <c r="T47" s="109" t="n"/>
     </row>
     <row r="48">
@@ -3974,15 +3996,15 @@
       </c>
     </row>
     <row r="49">
-      <c r="A49" s="383" t="inlineStr">
+      <c r="A49" s="402" t="inlineStr">
         <is>
           <t>#L9QL9YQQY</t>
         </is>
       </c>
-      <c r="B49" s="381" t="n">
+      <c r="B49" s="400" t="n">
         <v>975</v>
       </c>
-      <c r="C49" s="377" t="n">
+      <c r="C49" s="396" t="n">
         <v>46</v>
       </c>
       <c r="D49" s="109" t="inlineStr">
@@ -3990,41 +4012,41 @@
           <t>Ima Chad</t>
         </is>
       </c>
-      <c r="E49" s="381" t="n"/>
+      <c r="E49" s="400" t="n"/>
       <c r="F49" s="109" t="n"/>
-      <c r="G49" s="381" t="n"/>
+      <c r="G49" s="400" t="n"/>
       <c r="H49" s="109" t="n"/>
-      <c r="I49" s="383" t="n">
+      <c r="I49" s="402" t="n">
         <v>0</v>
       </c>
       <c r="J49" s="110" t="n">
         <v>0</v>
       </c>
-      <c r="K49" s="383" t="n">
+      <c r="K49" s="402" t="n">
         <v>0</v>
       </c>
       <c r="L49" s="110" t="n">
         <v>0</v>
       </c>
-      <c r="M49" s="383" t="n">
+      <c r="M49" s="402" t="n">
         <v>0</v>
       </c>
       <c r="N49" s="110" t="n">
         <v>0</v>
       </c>
-      <c r="O49" s="383" t="n">
+      <c r="O49" s="402" t="n">
         <v>0</v>
       </c>
       <c r="P49" s="110" t="n">
         <v>0</v>
       </c>
-      <c r="Q49" s="383" t="n">
+      <c r="Q49" s="402" t="n">
         <v>0</v>
       </c>
       <c r="R49" s="110" t="n">
         <v>0</v>
       </c>
-      <c r="S49" s="382" t="n">
+      <c r="S49" s="401" t="n">
         <v>5</v>
       </c>
       <c r="T49" s="110" t="n">
@@ -4032,15 +4054,15 @@
       </c>
     </row>
     <row r="50">
-      <c r="A50" s="386" t="inlineStr">
+      <c r="A50" s="405" t="inlineStr">
         <is>
           <t>#PJYVV989R</t>
         </is>
       </c>
-      <c r="B50" s="384" t="n">
+      <c r="B50" s="403" t="n">
         <v>1574</v>
       </c>
-      <c r="C50" s="373" t="n">
+      <c r="C50" s="392" t="n">
         <v>47</v>
       </c>
       <c r="D50" s="115" t="inlineStr">
@@ -4048,53 +4070,53 @@
           <t>nx</t>
         </is>
       </c>
-      <c r="E50" s="384" t="n"/>
+      <c r="E50" s="403" t="n"/>
       <c r="F50" s="115" t="n"/>
-      <c r="G50" s="384" t="n"/>
+      <c r="G50" s="403" t="n"/>
       <c r="H50" s="115" t="n"/>
-      <c r="I50" s="386" t="n">
+      <c r="I50" s="405" t="n">
         <v>0</v>
       </c>
       <c r="J50" s="116" t="n">
         <v>0</v>
       </c>
-      <c r="K50" s="386" t="n">
+      <c r="K50" s="405" t="n">
         <v>0</v>
       </c>
       <c r="L50" s="116" t="n">
         <v>0</v>
       </c>
-      <c r="M50" s="386" t="n">
+      <c r="M50" s="405" t="n">
         <v>0</v>
       </c>
       <c r="N50" s="116" t="n">
         <v>0</v>
       </c>
-      <c r="O50" s="386" t="n">
+      <c r="O50" s="405" t="n">
         <v>0</v>
       </c>
       <c r="P50" s="116" t="n">
         <v>0</v>
       </c>
-      <c r="Q50" s="386" t="n">
+      <c r="Q50" s="405" t="n">
         <v>0</v>
       </c>
       <c r="R50" s="116" t="n">
         <v>0</v>
       </c>
-      <c r="S50" s="384" t="n"/>
+      <c r="S50" s="403" t="n"/>
       <c r="T50" s="115" t="n"/>
     </row>
     <row r="51">
-      <c r="A51" s="383" t="inlineStr">
+      <c r="A51" s="402" t="inlineStr">
         <is>
           <t>#L9JJQY992</t>
         </is>
       </c>
-      <c r="B51" s="381" t="n">
+      <c r="B51" s="400" t="n">
         <v>773</v>
       </c>
-      <c r="C51" s="377" t="n">
+      <c r="C51" s="396" t="n">
         <v>48</v>
       </c>
       <c r="D51" s="109" t="inlineStr">
@@ -4102,53 +4124,53 @@
           <t>Fisted_Waffle</t>
         </is>
       </c>
-      <c r="E51" s="381" t="n"/>
+      <c r="E51" s="400" t="n"/>
       <c r="F51" s="109" t="n"/>
-      <c r="G51" s="381" t="n"/>
+      <c r="G51" s="400" t="n"/>
       <c r="H51" s="109" t="n"/>
-      <c r="I51" s="383" t="n">
+      <c r="I51" s="402" t="n">
         <v>0</v>
       </c>
       <c r="J51" s="110" t="n">
         <v>0</v>
       </c>
-      <c r="K51" s="383" t="n">
+      <c r="K51" s="402" t="n">
         <v>0</v>
       </c>
       <c r="L51" s="110" t="n">
         <v>0</v>
       </c>
-      <c r="M51" s="383" t="n">
+      <c r="M51" s="402" t="n">
         <v>0</v>
       </c>
       <c r="N51" s="110" t="n">
         <v>0</v>
       </c>
-      <c r="O51" s="383" t="n">
+      <c r="O51" s="402" t="n">
         <v>0</v>
       </c>
       <c r="P51" s="110" t="n">
         <v>0</v>
       </c>
-      <c r="Q51" s="383" t="n">
+      <c r="Q51" s="402" t="n">
         <v>0</v>
       </c>
       <c r="R51" s="110" t="n">
         <v>0</v>
       </c>
-      <c r="S51" s="381" t="n"/>
+      <c r="S51" s="400" t="n"/>
       <c r="T51" s="109" t="n"/>
     </row>
     <row r="52">
-      <c r="A52" s="386" t="inlineStr">
+      <c r="A52" s="405" t="inlineStr">
         <is>
           <t>#9JUR0JQV2</t>
         </is>
       </c>
-      <c r="B52" s="384" t="n">
+      <c r="B52" s="403" t="n">
         <v>1134</v>
       </c>
-      <c r="C52" s="373" t="n">
+      <c r="C52" s="392" t="n">
         <v>49</v>
       </c>
       <c r="D52" s="115" t="inlineStr">
@@ -4156,37 +4178,37 @@
           <t>atley</t>
         </is>
       </c>
-      <c r="E52" s="384" t="n"/>
+      <c r="E52" s="403" t="n"/>
       <c r="F52" s="115" t="n"/>
-      <c r="G52" s="384" t="n"/>
+      <c r="G52" s="403" t="n"/>
       <c r="H52" s="115" t="n"/>
-      <c r="I52" s="388" t="n">
+      <c r="I52" s="407" t="n">
         <v>3</v>
       </c>
       <c r="J52" s="117" t="n">
         <v>5277</v>
       </c>
-      <c r="K52" s="384" t="n"/>
+      <c r="K52" s="403" t="n"/>
       <c r="L52" s="115" t="n"/>
-      <c r="M52" s="384" t="n"/>
+      <c r="M52" s="403" t="n"/>
       <c r="N52" s="115" t="n"/>
-      <c r="O52" s="384" t="n"/>
+      <c r="O52" s="403" t="n"/>
       <c r="P52" s="115" t="n"/>
-      <c r="Q52" s="384" t="n"/>
+      <c r="Q52" s="403" t="n"/>
       <c r="R52" s="115" t="n"/>
-      <c r="S52" s="384" t="n"/>
+      <c r="S52" s="403" t="n"/>
       <c r="T52" s="115" t="n"/>
     </row>
     <row r="53">
-      <c r="A53" s="383" t="inlineStr">
+      <c r="A53" s="402" t="inlineStr">
         <is>
           <t>#QUCCVCCJ0</t>
         </is>
       </c>
-      <c r="B53" s="381" t="n">
+      <c r="B53" s="400" t="n">
         <v>783</v>
       </c>
-      <c r="C53" s="377" t="n">
+      <c r="C53" s="396" t="n">
         <v>50</v>
       </c>
       <c r="D53" s="109" t="inlineStr">
@@ -4194,33 +4216,33 @@
           <t>koi</t>
         </is>
       </c>
-      <c r="E53" s="381" t="n"/>
+      <c r="E53" s="400" t="n"/>
       <c r="F53" s="109" t="n"/>
-      <c r="G53" s="381" t="n"/>
+      <c r="G53" s="400" t="n"/>
       <c r="H53" s="109" t="n"/>
-      <c r="I53" s="381" t="n"/>
+      <c r="I53" s="400" t="n"/>
       <c r="J53" s="109" t="n"/>
-      <c r="K53" s="381" t="n"/>
+      <c r="K53" s="400" t="n"/>
       <c r="L53" s="109" t="n"/>
-      <c r="M53" s="381" t="n"/>
+      <c r="M53" s="400" t="n"/>
       <c r="N53" s="109" t="n"/>
-      <c r="O53" s="381" t="n"/>
+      <c r="O53" s="400" t="n"/>
       <c r="P53" s="109" t="n"/>
-      <c r="Q53" s="381" t="n"/>
+      <c r="Q53" s="400" t="n"/>
       <c r="R53" s="109" t="n"/>
-      <c r="S53" s="381" t="n"/>
+      <c r="S53" s="400" t="n"/>
       <c r="T53" s="109" t="n"/>
     </row>
     <row r="54">
-      <c r="A54" s="386" t="inlineStr">
+      <c r="A54" s="405" t="inlineStr">
         <is>
           <t>#QPRYCJVJL</t>
         </is>
       </c>
-      <c r="B54" s="384" t="n">
+      <c r="B54" s="403" t="n">
         <v>693</v>
       </c>
-      <c r="C54" s="373" t="n">
+      <c r="C54" s="392" t="n">
         <v>51</v>
       </c>
       <c r="D54" s="115" t="inlineStr">
@@ -4228,33 +4250,33 @@
           <t>cris</t>
         </is>
       </c>
-      <c r="E54" s="384" t="n"/>
+      <c r="E54" s="403" t="n"/>
       <c r="F54" s="115" t="n"/>
-      <c r="G54" s="384" t="n"/>
+      <c r="G54" s="403" t="n"/>
       <c r="H54" s="115" t="n"/>
-      <c r="I54" s="384" t="n"/>
+      <c r="I54" s="403" t="n"/>
       <c r="J54" s="115" t="n"/>
-      <c r="K54" s="384" t="n"/>
+      <c r="K54" s="403" t="n"/>
       <c r="L54" s="115" t="n"/>
-      <c r="M54" s="384" t="n"/>
+      <c r="M54" s="403" t="n"/>
       <c r="N54" s="115" t="n"/>
-      <c r="O54" s="384" t="n"/>
+      <c r="O54" s="403" t="n"/>
       <c r="P54" s="115" t="n"/>
-      <c r="Q54" s="384" t="n"/>
+      <c r="Q54" s="403" t="n"/>
       <c r="R54" s="115" t="n"/>
-      <c r="S54" s="384" t="n"/>
+      <c r="S54" s="403" t="n"/>
       <c r="T54" s="115" t="n"/>
     </row>
     <row r="55">
-      <c r="A55" s="383" t="inlineStr">
+      <c r="A55" s="402" t="inlineStr">
         <is>
           <t>#QQLVRJCGQ</t>
         </is>
       </c>
-      <c r="B55" s="381" t="n">
+      <c r="B55" s="400" t="n">
         <v>1240</v>
       </c>
-      <c r="C55" s="377" t="n">
+      <c r="C55" s="396" t="n">
         <v>52</v>
       </c>
       <c r="D55" s="109" t="inlineStr">
@@ -4262,33 +4284,33 @@
           <t>khant</t>
         </is>
       </c>
-      <c r="E55" s="381" t="n"/>
+      <c r="E55" s="400" t="n"/>
       <c r="F55" s="109" t="n"/>
-      <c r="G55" s="381" t="n"/>
+      <c r="G55" s="400" t="n"/>
       <c r="H55" s="109" t="n"/>
-      <c r="I55" s="381" t="n"/>
+      <c r="I55" s="400" t="n"/>
       <c r="J55" s="109" t="n"/>
-      <c r="K55" s="381" t="n"/>
+      <c r="K55" s="400" t="n"/>
       <c r="L55" s="109" t="n"/>
-      <c r="M55" s="381" t="n"/>
+      <c r="M55" s="400" t="n"/>
       <c r="N55" s="109" t="n"/>
-      <c r="O55" s="381" t="n"/>
+      <c r="O55" s="400" t="n"/>
       <c r="P55" s="109" t="n"/>
-      <c r="Q55" s="381" t="n"/>
+      <c r="Q55" s="400" t="n"/>
       <c r="R55" s="109" t="n"/>
-      <c r="S55" s="381" t="n"/>
+      <c r="S55" s="400" t="n"/>
       <c r="T55" s="109" t="n"/>
     </row>
     <row r="56">
-      <c r="A56" s="386" t="inlineStr">
+      <c r="A56" s="405" t="inlineStr">
         <is>
           <t>#QLL0PVCRV</t>
         </is>
       </c>
-      <c r="B56" s="384" t="n">
+      <c r="B56" s="403" t="n">
         <v>1704</v>
       </c>
-      <c r="C56" s="373" t="n">
+      <c r="C56" s="392" t="n">
         <v>53</v>
       </c>
       <c r="D56" s="115" t="inlineStr">
@@ -4296,33 +4318,33 @@
           <t>Harsh chhillar</t>
         </is>
       </c>
-      <c r="E56" s="384" t="n"/>
+      <c r="E56" s="403" t="n"/>
       <c r="F56" s="115" t="n"/>
-      <c r="G56" s="384" t="n"/>
+      <c r="G56" s="403" t="n"/>
       <c r="H56" s="115" t="n"/>
-      <c r="I56" s="384" t="n"/>
+      <c r="I56" s="403" t="n"/>
       <c r="J56" s="115" t="n"/>
-      <c r="K56" s="384" t="n"/>
+      <c r="K56" s="403" t="n"/>
       <c r="L56" s="115" t="n"/>
-      <c r="M56" s="384" t="n"/>
+      <c r="M56" s="403" t="n"/>
       <c r="N56" s="115" t="n"/>
-      <c r="O56" s="384" t="n"/>
+      <c r="O56" s="403" t="n"/>
       <c r="P56" s="115" t="n"/>
-      <c r="Q56" s="384" t="n"/>
+      <c r="Q56" s="403" t="n"/>
       <c r="R56" s="115" t="n"/>
-      <c r="S56" s="384" t="n"/>
+      <c r="S56" s="403" t="n"/>
       <c r="T56" s="115" t="n"/>
     </row>
     <row r="57">
-      <c r="A57" s="383" t="inlineStr">
+      <c r="A57" s="402" t="inlineStr">
         <is>
           <t>#Q8YP9P8UJ</t>
         </is>
       </c>
-      <c r="B57" s="381" t="n">
+      <c r="B57" s="400" t="n">
         <v>945</v>
       </c>
-      <c r="C57" s="377" t="n">
+      <c r="C57" s="396" t="n">
         <v>54</v>
       </c>
       <c r="D57" s="109" t="inlineStr">
@@ -4330,37 +4352,37 @@
           <t>Ranger</t>
         </is>
       </c>
-      <c r="E57" s="381" t="n"/>
+      <c r="E57" s="400" t="n"/>
       <c r="F57" s="109" t="n"/>
-      <c r="G57" s="381" t="n"/>
+      <c r="G57" s="400" t="n"/>
       <c r="H57" s="109" t="n"/>
-      <c r="I57" s="381" t="n"/>
+      <c r="I57" s="400" t="n"/>
       <c r="J57" s="109" t="n"/>
-      <c r="K57" s="381" t="n"/>
+      <c r="K57" s="400" t="n"/>
       <c r="L57" s="109" t="n"/>
-      <c r="M57" s="382" t="n">
+      <c r="M57" s="401" t="n">
         <v>5</v>
       </c>
       <c r="N57" s="118" t="n">
         <v>4680</v>
       </c>
-      <c r="O57" s="381" t="n"/>
+      <c r="O57" s="400" t="n"/>
       <c r="P57" s="109" t="n"/>
-      <c r="Q57" s="381" t="n"/>
+      <c r="Q57" s="400" t="n"/>
       <c r="R57" s="109" t="n"/>
-      <c r="S57" s="381" t="n"/>
+      <c r="S57" s="400" t="n"/>
       <c r="T57" s="109" t="n"/>
     </row>
     <row r="58">
-      <c r="A58" s="386" t="inlineStr">
+      <c r="A58" s="405" t="inlineStr">
         <is>
           <t>#Q0JG2RJQ8</t>
         </is>
       </c>
-      <c r="B58" s="384" t="n">
+      <c r="B58" s="403" t="n">
         <v>997</v>
       </c>
-      <c r="C58" s="373" t="n">
+      <c r="C58" s="392" t="n">
         <v>55</v>
       </c>
       <c r="D58" s="115" t="inlineStr">
@@ -4368,37 +4390,37 @@
           <t>bozo</t>
         </is>
       </c>
-      <c r="E58" s="384" t="n"/>
+      <c r="E58" s="403" t="n"/>
       <c r="F58" s="115" t="n"/>
-      <c r="G58" s="384" t="n"/>
+      <c r="G58" s="403" t="n"/>
       <c r="H58" s="115" t="n"/>
-      <c r="I58" s="384" t="n"/>
+      <c r="I58" s="403" t="n"/>
       <c r="J58" s="115" t="n"/>
-      <c r="K58" s="384" t="n"/>
+      <c r="K58" s="403" t="n"/>
       <c r="L58" s="115" t="n"/>
-      <c r="M58" s="384" t="n"/>
+      <c r="M58" s="403" t="n"/>
       <c r="N58" s="115" t="n"/>
-      <c r="O58" s="385" t="n">
+      <c r="O58" s="404" t="n">
         <v>6</v>
       </c>
       <c r="P58" s="112" t="n">
         <v>6495</v>
       </c>
-      <c r="Q58" s="384" t="n"/>
+      <c r="Q58" s="403" t="n"/>
       <c r="R58" s="115" t="n"/>
-      <c r="S58" s="384" t="n"/>
+      <c r="S58" s="403" t="n"/>
       <c r="T58" s="115" t="n"/>
     </row>
     <row r="59">
-      <c r="A59" s="383" t="inlineStr">
+      <c r="A59" s="402" t="inlineStr">
         <is>
           <t>#UVCCQC02</t>
         </is>
       </c>
-      <c r="B59" s="381" t="n">
+      <c r="B59" s="400" t="n">
         <v>1806</v>
       </c>
-      <c r="C59" s="377" t="n">
+      <c r="C59" s="396" t="n">
         <v>56</v>
       </c>
       <c r="D59" s="109" t="inlineStr">
@@ -4406,29 +4428,29 @@
           <t>lordshisha</t>
         </is>
       </c>
-      <c r="E59" s="381" t="n"/>
+      <c r="E59" s="400" t="n"/>
       <c r="F59" s="109" t="n"/>
-      <c r="G59" s="381" t="n"/>
+      <c r="G59" s="400" t="n"/>
       <c r="H59" s="109" t="n"/>
-      <c r="I59" s="381" t="n"/>
+      <c r="I59" s="400" t="n"/>
       <c r="J59" s="109" t="n"/>
-      <c r="K59" s="381" t="n"/>
+      <c r="K59" s="400" t="n"/>
       <c r="L59" s="109" t="n"/>
-      <c r="M59" s="381" t="n"/>
+      <c r="M59" s="400" t="n"/>
       <c r="N59" s="109" t="n"/>
-      <c r="O59" s="382" t="n">
+      <c r="O59" s="401" t="n">
         <v>6</v>
       </c>
       <c r="P59" s="106" t="n">
         <v>8496</v>
       </c>
-      <c r="Q59" s="382" t="n">
+      <c r="Q59" s="401" t="n">
         <v>6</v>
       </c>
       <c r="R59" s="106" t="n">
         <v>6310</v>
       </c>
-      <c r="S59" s="382" t="n">
+      <c r="S59" s="401" t="n">
         <v>6</v>
       </c>
       <c r="T59" s="106" t="n">
@@ -4436,15 +4458,15 @@
       </c>
     </row>
     <row r="60">
-      <c r="A60" s="386" t="inlineStr">
+      <c r="A60" s="405" t="inlineStr">
         <is>
           <t>#P2CPRPQU</t>
         </is>
       </c>
-      <c r="B60" s="384" t="n">
+      <c r="B60" s="403" t="n">
         <v>2232</v>
       </c>
-      <c r="C60" s="373" t="n">
+      <c r="C60" s="392" t="n">
         <v>57</v>
       </c>
       <c r="D60" s="115" t="inlineStr">
@@ -4452,29 +4474,29 @@
           <t>The Drift King</t>
         </is>
       </c>
-      <c r="E60" s="384" t="n"/>
+      <c r="E60" s="403" t="n"/>
       <c r="F60" s="115" t="n"/>
-      <c r="G60" s="384" t="n"/>
+      <c r="G60" s="403" t="n"/>
       <c r="H60" s="115" t="n"/>
-      <c r="I60" s="384" t="n"/>
+      <c r="I60" s="403" t="n"/>
       <c r="J60" s="115" t="n"/>
-      <c r="K60" s="384" t="n"/>
+      <c r="K60" s="403" t="n"/>
       <c r="L60" s="115" t="n"/>
-      <c r="M60" s="384" t="n"/>
+      <c r="M60" s="403" t="n"/>
       <c r="N60" s="115" t="n"/>
-      <c r="O60" s="385" t="n">
+      <c r="O60" s="404" t="n">
         <v>6</v>
       </c>
       <c r="P60" s="112" t="n">
         <v>8023</v>
       </c>
-      <c r="Q60" s="385" t="n">
+      <c r="Q60" s="404" t="n">
         <v>6</v>
       </c>
       <c r="R60" s="112" t="n">
         <v>7625</v>
       </c>
-      <c r="S60" s="385" t="n">
+      <c r="S60" s="404" t="n">
         <v>6</v>
       </c>
       <c r="T60" s="112" t="n">
@@ -4482,15 +4504,15 @@
       </c>
     </row>
     <row r="61">
-      <c r="A61" s="383" t="inlineStr">
+      <c r="A61" s="402" t="inlineStr">
         <is>
           <t>#QJVL0LYQQ</t>
         </is>
       </c>
-      <c r="B61" s="381" t="n">
+      <c r="B61" s="400" t="n">
         <v>921</v>
       </c>
-      <c r="C61" s="377" t="n">
+      <c r="C61" s="396" t="n">
         <v>58</v>
       </c>
       <c r="D61" s="109" t="inlineStr">
@@ -4498,29 +4520,29 @@
           <t>mobbb341</t>
         </is>
       </c>
-      <c r="E61" s="381" t="n"/>
+      <c r="E61" s="400" t="n"/>
       <c r="F61" s="109" t="n"/>
-      <c r="G61" s="381" t="n"/>
+      <c r="G61" s="400" t="n"/>
       <c r="H61" s="109" t="n"/>
-      <c r="I61" s="381" t="n"/>
+      <c r="I61" s="400" t="n"/>
       <c r="J61" s="109" t="n"/>
-      <c r="K61" s="381" t="n"/>
+      <c r="K61" s="400" t="n"/>
       <c r="L61" s="109" t="n"/>
-      <c r="M61" s="381" t="n"/>
+      <c r="M61" s="400" t="n"/>
       <c r="N61" s="109" t="n"/>
-      <c r="O61" s="382" t="n">
+      <c r="O61" s="401" t="n">
         <v>6</v>
       </c>
       <c r="P61" s="106" t="n">
         <v>7710</v>
       </c>
-      <c r="Q61" s="382" t="n">
+      <c r="Q61" s="401" t="n">
         <v>6</v>
       </c>
       <c r="R61" s="106" t="n">
         <v>8810</v>
       </c>
-      <c r="S61" s="382" t="n">
+      <c r="S61" s="401" t="n">
         <v>6</v>
       </c>
       <c r="T61" s="118" t="n">
@@ -4528,15 +4550,15 @@
       </c>
     </row>
     <row r="62">
-      <c r="A62" s="386" t="inlineStr">
+      <c r="A62" s="405" t="inlineStr">
         <is>
           <t>#L8R82C8VC</t>
         </is>
       </c>
-      <c r="B62" s="384" t="n">
+      <c r="B62" s="403" t="n">
         <v>1162</v>
       </c>
-      <c r="C62" s="373" t="n">
+      <c r="C62" s="392" t="n">
         <v>59</v>
       </c>
       <c r="D62" s="115" t="inlineStr">
@@ -4544,29 +4566,29 @@
           <t>caden asue</t>
         </is>
       </c>
-      <c r="E62" s="384" t="n"/>
+      <c r="E62" s="403" t="n"/>
       <c r="F62" s="115" t="n"/>
-      <c r="G62" s="384" t="n"/>
+      <c r="G62" s="403" t="n"/>
       <c r="H62" s="115" t="n"/>
-      <c r="I62" s="384" t="n"/>
+      <c r="I62" s="403" t="n"/>
       <c r="J62" s="115" t="n"/>
-      <c r="K62" s="384" t="n"/>
+      <c r="K62" s="403" t="n"/>
       <c r="L62" s="115" t="n"/>
-      <c r="M62" s="384" t="n"/>
+      <c r="M62" s="403" t="n"/>
       <c r="N62" s="115" t="n"/>
-      <c r="O62" s="385" t="n">
+      <c r="O62" s="404" t="n">
         <v>6</v>
       </c>
       <c r="P62" s="117" t="n">
         <v>5112</v>
       </c>
-      <c r="Q62" s="385" t="n">
+      <c r="Q62" s="404" t="n">
         <v>6</v>
       </c>
       <c r="R62" s="117" t="n">
         <v>4283</v>
       </c>
-      <c r="S62" s="385" t="n">
+      <c r="S62" s="404" t="n">
         <v>6</v>
       </c>
       <c r="T62" s="117" t="n">
@@ -4574,15 +4596,15 @@
       </c>
     </row>
     <row r="63">
-      <c r="A63" s="383" t="inlineStr">
+      <c r="A63" s="402" t="inlineStr">
         <is>
           <t>#L9Q8VLLQG</t>
         </is>
       </c>
-      <c r="B63" s="381" t="n">
+      <c r="B63" s="400" t="n">
         <v>1130</v>
       </c>
-      <c r="C63" s="377" t="n">
+      <c r="C63" s="396" t="n">
         <v>60</v>
       </c>
       <c r="D63" s="109" t="inlineStr">
@@ -4590,21 +4612,21 @@
           <t>cat</t>
         </is>
       </c>
-      <c r="E63" s="381" t="n"/>
+      <c r="E63" s="400" t="n"/>
       <c r="F63" s="109" t="n"/>
-      <c r="G63" s="381" t="n"/>
+      <c r="G63" s="400" t="n"/>
       <c r="H63" s="109" t="n"/>
-      <c r="I63" s="381" t="n"/>
+      <c r="I63" s="400" t="n"/>
       <c r="J63" s="109" t="n"/>
-      <c r="K63" s="381" t="n"/>
+      <c r="K63" s="400" t="n"/>
       <c r="L63" s="109" t="n"/>
-      <c r="M63" s="381" t="n"/>
+      <c r="M63" s="400" t="n"/>
       <c r="N63" s="109" t="n"/>
-      <c r="O63" s="381" t="n"/>
+      <c r="O63" s="400" t="n"/>
       <c r="P63" s="109" t="n"/>
-      <c r="Q63" s="381" t="n"/>
+      <c r="Q63" s="400" t="n"/>
       <c r="R63" s="109" t="n"/>
-      <c r="S63" s="382" t="n">
+      <c r="S63" s="401" t="n">
         <v>6</v>
       </c>
       <c r="T63" s="118" t="n">
@@ -4612,15 +4634,15 @@
       </c>
     </row>
     <row r="64">
-      <c r="A64" s="386" t="inlineStr">
+      <c r="A64" s="405" t="inlineStr">
         <is>
           <t>#QV0PQC9JU</t>
         </is>
       </c>
-      <c r="B64" s="384" t="n">
+      <c r="B64" s="403" t="n">
         <v>539</v>
       </c>
-      <c r="C64" s="373" t="n">
+      <c r="C64" s="392" t="n">
         <v>61</v>
       </c>
       <c r="D64" s="115" t="inlineStr">
@@ -4628,21 +4650,21 @@
           <t>Superman</t>
         </is>
       </c>
-      <c r="E64" s="384" t="n"/>
+      <c r="E64" s="403" t="n"/>
       <c r="F64" s="115" t="n"/>
-      <c r="G64" s="384" t="n"/>
+      <c r="G64" s="403" t="n"/>
       <c r="H64" s="115" t="n"/>
-      <c r="I64" s="384" t="n"/>
+      <c r="I64" s="403" t="n"/>
       <c r="J64" s="115" t="n"/>
-      <c r="K64" s="384" t="n"/>
+      <c r="K64" s="403" t="n"/>
       <c r="L64" s="115" t="n"/>
-      <c r="M64" s="384" t="n"/>
+      <c r="M64" s="403" t="n"/>
       <c r="N64" s="115" t="n"/>
-      <c r="O64" s="384" t="n"/>
+      <c r="O64" s="403" t="n"/>
       <c r="P64" s="115" t="n"/>
-      <c r="Q64" s="384" t="n"/>
+      <c r="Q64" s="403" t="n"/>
       <c r="R64" s="115" t="n"/>
-      <c r="S64" s="385" t="n">
+      <c r="S64" s="404" t="n">
         <v>6</v>
       </c>
       <c r="T64" s="117" t="n">
@@ -4650,15 +4672,15 @@
       </c>
     </row>
     <row r="65">
-      <c r="A65" s="383" t="inlineStr">
+      <c r="A65" s="402" t="inlineStr">
         <is>
           <t>#LU0CRP09L</t>
         </is>
       </c>
-      <c r="B65" s="381" t="n">
+      <c r="B65" s="400" t="n">
         <v>809</v>
       </c>
-      <c r="C65" s="377" t="n">
+      <c r="C65" s="396" t="n">
         <v>62</v>
       </c>
       <c r="D65" s="109" t="inlineStr">
@@ -4666,21 +4688,21 @@
           <t>I Dont Know</t>
         </is>
       </c>
-      <c r="E65" s="381" t="n"/>
+      <c r="E65" s="400" t="n"/>
       <c r="F65" s="109" t="n"/>
-      <c r="G65" s="381" t="n"/>
+      <c r="G65" s="400" t="n"/>
       <c r="H65" s="109" t="n"/>
-      <c r="I65" s="381" t="n"/>
+      <c r="I65" s="400" t="n"/>
       <c r="J65" s="109" t="n"/>
-      <c r="K65" s="381" t="n"/>
+      <c r="K65" s="400" t="n"/>
       <c r="L65" s="109" t="n"/>
-      <c r="M65" s="381" t="n"/>
+      <c r="M65" s="400" t="n"/>
       <c r="N65" s="109" t="n"/>
-      <c r="O65" s="381" t="n"/>
+      <c r="O65" s="400" t="n"/>
       <c r="P65" s="109" t="n"/>
-      <c r="Q65" s="381" t="n"/>
+      <c r="Q65" s="400" t="n"/>
       <c r="R65" s="109" t="n"/>
-      <c r="S65" s="387" t="n">
+      <c r="S65" s="406" t="n">
         <v>3</v>
       </c>
       <c r="T65" s="110" t="n">
@@ -4688,15 +4710,15 @@
       </c>
     </row>
     <row r="66">
-      <c r="A66" s="386" t="inlineStr">
+      <c r="A66" s="405" t="inlineStr">
         <is>
           <t>#YCPP0QPP8</t>
         </is>
       </c>
-      <c r="B66" s="384" t="n">
+      <c r="B66" s="403" t="n">
         <v>3327</v>
       </c>
-      <c r="C66" s="373" t="n">
+      <c r="C66" s="392" t="n">
         <v>63</v>
       </c>
       <c r="D66" s="115" t="inlineStr">
@@ -4704,21 +4726,21 @@
           <t>Coach</t>
         </is>
       </c>
-      <c r="E66" s="384" t="n"/>
+      <c r="E66" s="403" t="n"/>
       <c r="F66" s="115" t="n"/>
-      <c r="G66" s="384" t="n"/>
+      <c r="G66" s="403" t="n"/>
       <c r="H66" s="115" t="n"/>
-      <c r="I66" s="384" t="n"/>
+      <c r="I66" s="403" t="n"/>
       <c r="J66" s="115" t="n"/>
-      <c r="K66" s="384" t="n"/>
+      <c r="K66" s="403" t="n"/>
       <c r="L66" s="115" t="n"/>
-      <c r="M66" s="384" t="n"/>
+      <c r="M66" s="403" t="n"/>
       <c r="N66" s="115" t="n"/>
-      <c r="O66" s="384" t="n"/>
+      <c r="O66" s="403" t="n"/>
       <c r="P66" s="115" t="n"/>
-      <c r="Q66" s="384" t="n"/>
+      <c r="Q66" s="403" t="n"/>
       <c r="R66" s="115" t="n"/>
-      <c r="S66" s="386" t="n">
+      <c r="S66" s="405" t="n">
         <v>0</v>
       </c>
       <c r="T66" s="116" t="n">

</xml_diff>